<commit_message>
Router,PC fixes, we now have WiFi with password and a website, but DNS not working yet. Website IP: 192.168.1.233; WiFi passwords: 123456_[floor(0,1,2)]
</commit_message>
<xml_diff>
--- a/Kisvállalat létszám.xlsx
+++ b/Kisvállalat létszám.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\School\11.o\Hálózat\projekt\fluffy-system\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Izumi\Documents\github-repos\fluffy-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD064A95-E522-4D8B-8F3C-1C8CF0465616}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4708724C-AED9-434C-A648-EA0DE6C659F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18195" yWindow="945" windowWidth="9810" windowHeight="14205" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alap" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="61">
   <si>
     <t>I.em</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>Vlan</t>
+  </si>
+  <si>
+    <t>Szerver IP</t>
   </si>
 </sst>
 </file>
@@ -871,29 +874,47 @@
     <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -903,9 +924,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -920,40 +938,25 @@
     <xf numFmtId="0" fontId="5" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -1252,7 +1255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1343,8 +1346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12CB4148-414F-422C-94F5-AFDA695DCD79}">
   <dimension ref="A1:I257"/>
   <sheetViews>
-    <sheetView topLeftCell="A178" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I203" sqref="I203"/>
+    <sheetView tabSelected="1" topLeftCell="A217" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I235" sqref="I235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1383,7 +1386,7 @@
       <c r="C2" s="54"/>
       <c r="D2" s="54"/>
       <c r="E2" s="54"/>
-      <c r="F2" s="55" t="s">
+      <c r="F2" s="80" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="54"/>
@@ -1402,7 +1405,7 @@
       <c r="C3" s="54"/>
       <c r="D3" s="54"/>
       <c r="E3" s="54"/>
-      <c r="F3" s="55"/>
+      <c r="F3" s="80"/>
       <c r="G3" s="54"/>
       <c r="H3" s="54"/>
       <c r="I3" s="43"/>
@@ -1417,7 +1420,7 @@
       <c r="C4" s="54"/>
       <c r="D4" s="54"/>
       <c r="E4" s="54"/>
-      <c r="F4" s="55"/>
+      <c r="F4" s="80"/>
       <c r="G4" s="54"/>
       <c r="H4" s="54"/>
       <c r="I4" s="43"/>
@@ -1432,7 +1435,7 @@
       <c r="C5" s="54"/>
       <c r="D5" s="54"/>
       <c r="E5" s="54"/>
-      <c r="F5" s="55"/>
+      <c r="F5" s="80"/>
       <c r="G5" s="54"/>
       <c r="H5" s="54"/>
       <c r="I5" s="43"/>
@@ -1447,7 +1450,7 @@
       <c r="C6" s="54"/>
       <c r="D6" s="54"/>
       <c r="E6" s="54"/>
-      <c r="F6" s="55"/>
+      <c r="F6" s="80"/>
       <c r="G6" s="54"/>
       <c r="H6" s="54"/>
       <c r="I6" s="43"/>
@@ -1462,7 +1465,7 @@
       <c r="C7" s="54"/>
       <c r="D7" s="54"/>
       <c r="E7" s="54"/>
-      <c r="F7" s="55"/>
+      <c r="F7" s="80"/>
       <c r="G7" s="54"/>
       <c r="H7" s="54"/>
       <c r="I7" s="43"/>
@@ -1477,7 +1480,7 @@
       <c r="C8" s="54"/>
       <c r="D8" s="54"/>
       <c r="E8" s="54"/>
-      <c r="F8" s="55"/>
+      <c r="F8" s="80"/>
       <c r="G8" s="54"/>
       <c r="H8" s="54"/>
       <c r="I8" s="43"/>
@@ -1492,7 +1495,7 @@
       <c r="C9" s="54"/>
       <c r="D9" s="54"/>
       <c r="E9" s="54"/>
-      <c r="F9" s="55"/>
+      <c r="F9" s="80"/>
       <c r="G9" s="54"/>
       <c r="H9" s="54"/>
       <c r="I9" s="43"/>
@@ -1507,7 +1510,7 @@
       <c r="C10" s="54"/>
       <c r="D10" s="54"/>
       <c r="E10" s="54"/>
-      <c r="F10" s="55"/>
+      <c r="F10" s="80"/>
       <c r="G10" s="54"/>
       <c r="H10" s="54"/>
       <c r="I10" s="43"/>
@@ -1522,7 +1525,7 @@
       <c r="C11" s="54"/>
       <c r="D11" s="54"/>
       <c r="E11" s="54"/>
-      <c r="F11" s="55"/>
+      <c r="F11" s="80"/>
       <c r="G11" s="54"/>
       <c r="H11" s="54"/>
       <c r="I11" s="43"/>
@@ -1537,7 +1540,7 @@
       <c r="C12" s="54"/>
       <c r="D12" s="54"/>
       <c r="E12" s="54"/>
-      <c r="F12" s="55"/>
+      <c r="F12" s="80"/>
       <c r="G12" s="54"/>
       <c r="H12" s="54"/>
       <c r="I12" s="43"/>
@@ -1552,7 +1555,7 @@
       <c r="C13" s="54"/>
       <c r="D13" s="54"/>
       <c r="E13" s="54"/>
-      <c r="F13" s="55"/>
+      <c r="F13" s="80"/>
       <c r="G13" s="54"/>
       <c r="H13" s="54"/>
       <c r="I13" s="43"/>
@@ -1567,7 +1570,7 @@
       <c r="C14" s="54"/>
       <c r="D14" s="54"/>
       <c r="E14" s="54"/>
-      <c r="F14" s="55"/>
+      <c r="F14" s="80"/>
       <c r="G14" s="54"/>
       <c r="H14" s="54"/>
       <c r="I14" s="43"/>
@@ -1582,7 +1585,7 @@
       <c r="C15" s="54"/>
       <c r="D15" s="54"/>
       <c r="E15" s="54"/>
-      <c r="F15" s="55"/>
+      <c r="F15" s="80"/>
       <c r="G15" s="54"/>
       <c r="H15" s="54"/>
       <c r="I15" s="43"/>
@@ -1597,7 +1600,7 @@
       <c r="C16" s="54"/>
       <c r="D16" s="54"/>
       <c r="E16" s="54"/>
-      <c r="F16" s="55"/>
+      <c r="F16" s="80"/>
       <c r="G16" s="54"/>
       <c r="H16" s="54"/>
       <c r="I16" s="43"/>
@@ -1612,7 +1615,7 @@
       <c r="C17" s="54"/>
       <c r="D17" s="54"/>
       <c r="E17" s="54"/>
-      <c r="F17" s="55"/>
+      <c r="F17" s="80"/>
       <c r="G17" s="54"/>
       <c r="H17" s="54"/>
       <c r="I17" s="43"/>
@@ -1627,7 +1630,7 @@
       <c r="C18" s="54"/>
       <c r="D18" s="54"/>
       <c r="E18" s="54"/>
-      <c r="F18" s="55"/>
+      <c r="F18" s="80"/>
       <c r="G18" s="54"/>
       <c r="H18" s="54"/>
       <c r="I18" s="43"/>
@@ -1642,7 +1645,7 @@
       <c r="C19" s="54"/>
       <c r="D19" s="54"/>
       <c r="E19" s="54"/>
-      <c r="F19" s="55"/>
+      <c r="F19" s="80"/>
       <c r="G19" s="54"/>
       <c r="H19" s="54"/>
       <c r="I19" s="43"/>
@@ -1657,7 +1660,7 @@
       <c r="C20" s="54"/>
       <c r="D20" s="54"/>
       <c r="E20" s="54"/>
-      <c r="F20" s="55"/>
+      <c r="F20" s="80"/>
       <c r="G20" s="54"/>
       <c r="H20" s="54"/>
       <c r="I20" s="43"/>
@@ -1672,7 +1675,7 @@
       <c r="C21" s="54"/>
       <c r="D21" s="54"/>
       <c r="E21" s="54"/>
-      <c r="F21" s="55"/>
+      <c r="F21" s="80"/>
       <c r="G21" s="54"/>
       <c r="H21" s="54"/>
       <c r="I21" s="43"/>
@@ -1687,7 +1690,7 @@
       <c r="C22" s="54"/>
       <c r="D22" s="54"/>
       <c r="E22" s="54"/>
-      <c r="F22" s="55"/>
+      <c r="F22" s="80"/>
       <c r="G22" s="54"/>
       <c r="H22" s="54"/>
       <c r="I22" s="43"/>
@@ -1702,7 +1705,7 @@
       <c r="C23" s="54"/>
       <c r="D23" s="54"/>
       <c r="E23" s="54"/>
-      <c r="F23" s="55"/>
+      <c r="F23" s="80"/>
       <c r="G23" s="54"/>
       <c r="H23" s="54"/>
       <c r="I23" s="43"/>
@@ -1717,7 +1720,7 @@
       <c r="C24" s="54"/>
       <c r="D24" s="54"/>
       <c r="E24" s="54"/>
-      <c r="F24" s="55"/>
+      <c r="F24" s="80"/>
       <c r="G24" s="54"/>
       <c r="H24" s="54"/>
       <c r="I24" s="43"/>
@@ -1732,7 +1735,7 @@
       <c r="C25" s="54"/>
       <c r="D25" s="54"/>
       <c r="E25" s="54"/>
-      <c r="F25" s="55"/>
+      <c r="F25" s="80"/>
       <c r="G25" s="54"/>
       <c r="H25" s="54"/>
       <c r="I25" s="43"/>
@@ -1747,7 +1750,7 @@
       <c r="C26" s="54"/>
       <c r="D26" s="54"/>
       <c r="E26" s="54"/>
-      <c r="F26" s="55"/>
+      <c r="F26" s="80"/>
       <c r="G26" s="54"/>
       <c r="H26" s="54"/>
       <c r="I26" s="43"/>
@@ -1762,7 +1765,7 @@
       <c r="C27" s="54"/>
       <c r="D27" s="54"/>
       <c r="E27" s="54"/>
-      <c r="F27" s="55"/>
+      <c r="F27" s="80"/>
       <c r="G27" s="54"/>
       <c r="H27" s="54"/>
       <c r="I27" s="43"/>
@@ -1777,7 +1780,7 @@
       <c r="C28" s="54"/>
       <c r="D28" s="54"/>
       <c r="E28" s="54"/>
-      <c r="F28" s="55"/>
+      <c r="F28" s="80"/>
       <c r="G28" s="54"/>
       <c r="H28" s="54"/>
       <c r="I28" s="43"/>
@@ -1792,7 +1795,7 @@
       <c r="C29" s="54"/>
       <c r="D29" s="54"/>
       <c r="E29" s="54"/>
-      <c r="F29" s="55"/>
+      <c r="F29" s="80"/>
       <c r="G29" s="54"/>
       <c r="H29" s="54"/>
       <c r="I29" s="43"/>
@@ -1807,7 +1810,7 @@
       <c r="C30" s="54"/>
       <c r="D30" s="54"/>
       <c r="E30" s="54"/>
-      <c r="F30" s="55"/>
+      <c r="F30" s="80"/>
       <c r="G30" s="54"/>
       <c r="H30" s="54"/>
       <c r="I30" s="43"/>
@@ -1822,7 +1825,7 @@
       <c r="C31" s="54"/>
       <c r="D31" s="54"/>
       <c r="E31" s="54"/>
-      <c r="F31" s="55"/>
+      <c r="F31" s="80"/>
       <c r="G31" s="54"/>
       <c r="H31" s="54"/>
       <c r="I31" s="43"/>
@@ -1837,7 +1840,7 @@
       <c r="C32" s="54"/>
       <c r="D32" s="54"/>
       <c r="E32" s="54"/>
-      <c r="F32" s="55"/>
+      <c r="F32" s="80"/>
       <c r="G32" s="54"/>
       <c r="H32" s="54"/>
       <c r="I32" s="43" t="s">
@@ -1854,7 +1857,7 @@
       <c r="C33" s="54"/>
       <c r="D33" s="54"/>
       <c r="E33" s="54"/>
-      <c r="F33" s="55"/>
+      <c r="F33" s="80"/>
       <c r="G33" s="54"/>
       <c r="H33" s="54"/>
       <c r="I33" s="43" t="s">
@@ -1870,7 +1873,7 @@
       </c>
       <c r="C34" s="54"/>
       <c r="D34" s="54"/>
-      <c r="E34" s="58" t="s">
+      <c r="E34" s="79" t="s">
         <v>16</v>
       </c>
       <c r="F34" s="54"/>
@@ -1889,7 +1892,7 @@
       </c>
       <c r="C35" s="54"/>
       <c r="D35" s="54"/>
-      <c r="E35" s="58"/>
+      <c r="E35" s="79"/>
       <c r="F35" s="54"/>
       <c r="G35" s="54"/>
       <c r="H35" s="54"/>
@@ -1904,7 +1907,7 @@
       </c>
       <c r="C36" s="54"/>
       <c r="D36" s="54"/>
-      <c r="E36" s="58"/>
+      <c r="E36" s="79"/>
       <c r="F36" s="54"/>
       <c r="G36" s="54"/>
       <c r="H36" s="54"/>
@@ -1919,7 +1922,7 @@
       </c>
       <c r="C37" s="54"/>
       <c r="D37" s="54"/>
-      <c r="E37" s="58"/>
+      <c r="E37" s="79"/>
       <c r="F37" s="54"/>
       <c r="G37" s="54"/>
       <c r="H37" s="54"/>
@@ -1934,7 +1937,7 @@
       </c>
       <c r="C38" s="54"/>
       <c r="D38" s="54"/>
-      <c r="E38" s="58"/>
+      <c r="E38" s="79"/>
       <c r="F38" s="54"/>
       <c r="G38" s="54"/>
       <c r="H38" s="54"/>
@@ -1949,7 +1952,7 @@
       </c>
       <c r="C39" s="54"/>
       <c r="D39" s="54"/>
-      <c r="E39" s="58"/>
+      <c r="E39" s="79"/>
       <c r="F39" s="54"/>
       <c r="G39" s="54"/>
       <c r="H39" s="54"/>
@@ -1964,7 +1967,7 @@
       </c>
       <c r="C40" s="54"/>
       <c r="D40" s="54"/>
-      <c r="E40" s="58"/>
+      <c r="E40" s="79"/>
       <c r="F40" s="54"/>
       <c r="G40" s="54"/>
       <c r="H40" s="54"/>
@@ -1979,7 +1982,7 @@
       </c>
       <c r="C41" s="54"/>
       <c r="D41" s="54"/>
-      <c r="E41" s="58"/>
+      <c r="E41" s="79"/>
       <c r="F41" s="54"/>
       <c r="G41" s="54"/>
       <c r="H41" s="54"/>
@@ -1994,7 +1997,7 @@
       </c>
       <c r="C42" s="54"/>
       <c r="D42" s="54"/>
-      <c r="E42" s="58"/>
+      <c r="E42" s="79"/>
       <c r="F42" s="54"/>
       <c r="G42" s="54"/>
       <c r="H42" s="54"/>
@@ -2009,7 +2012,7 @@
       </c>
       <c r="C43" s="54"/>
       <c r="D43" s="54"/>
-      <c r="E43" s="58"/>
+      <c r="E43" s="79"/>
       <c r="F43" s="54"/>
       <c r="G43" s="54"/>
       <c r="H43" s="54"/>
@@ -2024,7 +2027,7 @@
       </c>
       <c r="C44" s="54"/>
       <c r="D44" s="54"/>
-      <c r="E44" s="58"/>
+      <c r="E44" s="79"/>
       <c r="F44" s="54"/>
       <c r="G44" s="54"/>
       <c r="H44" s="54"/>
@@ -2039,7 +2042,7 @@
       </c>
       <c r="C45" s="54"/>
       <c r="D45" s="54"/>
-      <c r="E45" s="58"/>
+      <c r="E45" s="79"/>
       <c r="F45" s="54"/>
       <c r="G45" s="54"/>
       <c r="H45" s="54"/>
@@ -2054,7 +2057,7 @@
       </c>
       <c r="C46" s="54"/>
       <c r="D46" s="54"/>
-      <c r="E46" s="58"/>
+      <c r="E46" s="79"/>
       <c r="F46" s="54"/>
       <c r="G46" s="54"/>
       <c r="H46" s="54"/>
@@ -2069,7 +2072,7 @@
       </c>
       <c r="C47" s="54"/>
       <c r="D47" s="54"/>
-      <c r="E47" s="58"/>
+      <c r="E47" s="79"/>
       <c r="F47" s="54"/>
       <c r="G47" s="54"/>
       <c r="H47" s="54"/>
@@ -2084,7 +2087,7 @@
       </c>
       <c r="C48" s="54"/>
       <c r="D48" s="54"/>
-      <c r="E48" s="58"/>
+      <c r="E48" s="79"/>
       <c r="F48" s="54"/>
       <c r="G48" s="54"/>
       <c r="H48" s="54"/>
@@ -2101,7 +2104,7 @@
       </c>
       <c r="C49" s="54"/>
       <c r="D49" s="54"/>
-      <c r="E49" s="58"/>
+      <c r="E49" s="79"/>
       <c r="F49" s="54"/>
       <c r="G49" s="54"/>
       <c r="H49" s="54"/>
@@ -2118,7 +2121,7 @@
       </c>
       <c r="C50" s="54"/>
       <c r="D50" s="54"/>
-      <c r="E50" s="56" t="s">
+      <c r="E50" s="77" t="s">
         <v>17</v>
       </c>
       <c r="F50" s="54"/>
@@ -2137,7 +2140,7 @@
       </c>
       <c r="C51" s="54"/>
       <c r="D51" s="54"/>
-      <c r="E51" s="56"/>
+      <c r="E51" s="77"/>
       <c r="F51" s="54"/>
       <c r="G51" s="54"/>
       <c r="H51" s="54"/>
@@ -2152,7 +2155,7 @@
       </c>
       <c r="C52" s="54"/>
       <c r="D52" s="54"/>
-      <c r="E52" s="56"/>
+      <c r="E52" s="77"/>
       <c r="F52" s="54"/>
       <c r="G52" s="54"/>
       <c r="H52" s="54"/>
@@ -2167,7 +2170,7 @@
       </c>
       <c r="C53" s="54"/>
       <c r="D53" s="54"/>
-      <c r="E53" s="56"/>
+      <c r="E53" s="77"/>
       <c r="F53" s="54"/>
       <c r="G53" s="54"/>
       <c r="H53" s="54"/>
@@ -2182,7 +2185,7 @@
       </c>
       <c r="C54" s="54"/>
       <c r="D54" s="54"/>
-      <c r="E54" s="56"/>
+      <c r="E54" s="77"/>
       <c r="F54" s="54"/>
       <c r="G54" s="54"/>
       <c r="H54" s="54"/>
@@ -2197,7 +2200,7 @@
       </c>
       <c r="C55" s="54"/>
       <c r="D55" s="54"/>
-      <c r="E55" s="56"/>
+      <c r="E55" s="77"/>
       <c r="F55" s="54"/>
       <c r="G55" s="54"/>
       <c r="H55" s="54"/>
@@ -2212,7 +2215,7 @@
       </c>
       <c r="C56" s="54"/>
       <c r="D56" s="54"/>
-      <c r="E56" s="56"/>
+      <c r="E56" s="77"/>
       <c r="F56" s="54"/>
       <c r="G56" s="54"/>
       <c r="H56" s="54"/>
@@ -2227,7 +2230,7 @@
       </c>
       <c r="C57" s="54"/>
       <c r="D57" s="54"/>
-      <c r="E57" s="56"/>
+      <c r="E57" s="77"/>
       <c r="F57" s="54"/>
       <c r="G57" s="54"/>
       <c r="H57" s="54"/>
@@ -2242,7 +2245,7 @@
       </c>
       <c r="C58" s="54"/>
       <c r="D58" s="54"/>
-      <c r="E58" s="56"/>
+      <c r="E58" s="77"/>
       <c r="F58" s="54"/>
       <c r="G58" s="54"/>
       <c r="H58" s="54"/>
@@ -2257,7 +2260,7 @@
       </c>
       <c r="C59" s="54"/>
       <c r="D59" s="54"/>
-      <c r="E59" s="56"/>
+      <c r="E59" s="77"/>
       <c r="F59" s="54"/>
       <c r="G59" s="54"/>
       <c r="H59" s="54"/>
@@ -2272,7 +2275,7 @@
       </c>
       <c r="C60" s="54"/>
       <c r="D60" s="54"/>
-      <c r="E60" s="56"/>
+      <c r="E60" s="77"/>
       <c r="F60" s="54"/>
       <c r="G60" s="54"/>
       <c r="H60" s="54"/>
@@ -2287,7 +2290,7 @@
       </c>
       <c r="C61" s="54"/>
       <c r="D61" s="54"/>
-      <c r="E61" s="56"/>
+      <c r="E61" s="77"/>
       <c r="F61" s="54"/>
       <c r="G61" s="54"/>
       <c r="H61" s="54"/>
@@ -2302,7 +2305,7 @@
       </c>
       <c r="C62" s="54"/>
       <c r="D62" s="54"/>
-      <c r="E62" s="56"/>
+      <c r="E62" s="77"/>
       <c r="F62" s="54"/>
       <c r="G62" s="54"/>
       <c r="H62" s="54"/>
@@ -2317,7 +2320,7 @@
       </c>
       <c r="C63" s="54"/>
       <c r="D63" s="54"/>
-      <c r="E63" s="56"/>
+      <c r="E63" s="77"/>
       <c r="F63" s="54"/>
       <c r="G63" s="54"/>
       <c r="H63" s="54"/>
@@ -2332,7 +2335,7 @@
       </c>
       <c r="C64" s="54"/>
       <c r="D64" s="54"/>
-      <c r="E64" s="56"/>
+      <c r="E64" s="77"/>
       <c r="F64" s="54"/>
       <c r="G64" s="54"/>
       <c r="H64" s="54"/>
@@ -2349,7 +2352,7 @@
       </c>
       <c r="C65" s="54"/>
       <c r="D65" s="54"/>
-      <c r="E65" s="56"/>
+      <c r="E65" s="77"/>
       <c r="F65" s="54"/>
       <c r="G65" s="54"/>
       <c r="H65" s="54"/>
@@ -2366,7 +2369,7 @@
       </c>
       <c r="C66" s="54"/>
       <c r="D66" s="54"/>
-      <c r="E66" s="57" t="s">
+      <c r="E66" s="78" t="s">
         <v>18</v>
       </c>
       <c r="F66" s="54"/>
@@ -2385,7 +2388,7 @@
       </c>
       <c r="C67" s="54"/>
       <c r="D67" s="54"/>
-      <c r="E67" s="57"/>
+      <c r="E67" s="78"/>
       <c r="F67" s="54"/>
       <c r="G67" s="54"/>
       <c r="H67" s="54"/>
@@ -2400,7 +2403,7 @@
       </c>
       <c r="C68" s="54"/>
       <c r="D68" s="54"/>
-      <c r="E68" s="57"/>
+      <c r="E68" s="78"/>
       <c r="F68" s="54"/>
       <c r="G68" s="54"/>
       <c r="H68" s="54"/>
@@ -2415,7 +2418,7 @@
       </c>
       <c r="C69" s="54"/>
       <c r="D69" s="54"/>
-      <c r="E69" s="57"/>
+      <c r="E69" s="78"/>
       <c r="F69" s="54"/>
       <c r="G69" s="54"/>
       <c r="H69" s="54"/>
@@ -2430,7 +2433,7 @@
       </c>
       <c r="C70" s="54"/>
       <c r="D70" s="54"/>
-      <c r="E70" s="57"/>
+      <c r="E70" s="78"/>
       <c r="F70" s="54"/>
       <c r="G70" s="54"/>
       <c r="H70" s="54"/>
@@ -2445,7 +2448,7 @@
       </c>
       <c r="C71" s="54"/>
       <c r="D71" s="54"/>
-      <c r="E71" s="57"/>
+      <c r="E71" s="78"/>
       <c r="F71" s="54"/>
       <c r="G71" s="54"/>
       <c r="H71" s="54"/>
@@ -2460,7 +2463,7 @@
       </c>
       <c r="C72" s="54"/>
       <c r="D72" s="54"/>
-      <c r="E72" s="57"/>
+      <c r="E72" s="78"/>
       <c r="F72" s="54"/>
       <c r="G72" s="54"/>
       <c r="H72" s="54"/>
@@ -2475,7 +2478,7 @@
       </c>
       <c r="C73" s="54"/>
       <c r="D73" s="54"/>
-      <c r="E73" s="57"/>
+      <c r="E73" s="78"/>
       <c r="F73" s="54"/>
       <c r="G73" s="54"/>
       <c r="H73" s="54"/>
@@ -2490,7 +2493,7 @@
       </c>
       <c r="C74" s="54"/>
       <c r="D74" s="54"/>
-      <c r="E74" s="57"/>
+      <c r="E74" s="78"/>
       <c r="F74" s="54"/>
       <c r="G74" s="54"/>
       <c r="H74" s="54"/>
@@ -2505,7 +2508,7 @@
       </c>
       <c r="C75" s="54"/>
       <c r="D75" s="54"/>
-      <c r="E75" s="57"/>
+      <c r="E75" s="78"/>
       <c r="F75" s="54"/>
       <c r="G75" s="54"/>
       <c r="H75" s="54"/>
@@ -2520,7 +2523,7 @@
       </c>
       <c r="C76" s="54"/>
       <c r="D76" s="54"/>
-      <c r="E76" s="57"/>
+      <c r="E76" s="78"/>
       <c r="F76" s="54"/>
       <c r="G76" s="54"/>
       <c r="H76" s="54"/>
@@ -2535,7 +2538,7 @@
       </c>
       <c r="C77" s="54"/>
       <c r="D77" s="54"/>
-      <c r="E77" s="57"/>
+      <c r="E77" s="78"/>
       <c r="F77" s="54"/>
       <c r="G77" s="54"/>
       <c r="H77" s="54"/>
@@ -2550,7 +2553,7 @@
       </c>
       <c r="C78" s="54"/>
       <c r="D78" s="54"/>
-      <c r="E78" s="57"/>
+      <c r="E78" s="78"/>
       <c r="F78" s="54"/>
       <c r="G78" s="54"/>
       <c r="H78" s="54"/>
@@ -2565,7 +2568,7 @@
       </c>
       <c r="C79" s="54"/>
       <c r="D79" s="54"/>
-      <c r="E79" s="57"/>
+      <c r="E79" s="78"/>
       <c r="F79" s="54"/>
       <c r="G79" s="54"/>
       <c r="H79" s="54"/>
@@ -2580,7 +2583,7 @@
       </c>
       <c r="C80" s="54"/>
       <c r="D80" s="54"/>
-      <c r="E80" s="57"/>
+      <c r="E80" s="78"/>
       <c r="F80" s="54"/>
       <c r="G80" s="54"/>
       <c r="H80" s="54"/>
@@ -2597,7 +2600,7 @@
       </c>
       <c r="C81" s="54"/>
       <c r="D81" s="54"/>
-      <c r="E81" s="57"/>
+      <c r="E81" s="78"/>
       <c r="F81" s="54"/>
       <c r="G81" s="54"/>
       <c r="H81" s="54"/>
@@ -2614,7 +2617,7 @@
       </c>
       <c r="C82" s="54"/>
       <c r="D82" s="54"/>
-      <c r="E82" s="60" t="s">
+      <c r="E82" s="76" t="s">
         <v>19</v>
       </c>
       <c r="F82" s="54"/>
@@ -2633,7 +2636,7 @@
       </c>
       <c r="C83" s="54"/>
       <c r="D83" s="54"/>
-      <c r="E83" s="60"/>
+      <c r="E83" s="76"/>
       <c r="F83" s="54"/>
       <c r="G83" s="54"/>
       <c r="H83" s="54"/>
@@ -2648,7 +2651,7 @@
       </c>
       <c r="C84" s="54"/>
       <c r="D84" s="54"/>
-      <c r="E84" s="60"/>
+      <c r="E84" s="76"/>
       <c r="F84" s="54"/>
       <c r="G84" s="54"/>
       <c r="H84" s="54"/>
@@ -2663,7 +2666,7 @@
       </c>
       <c r="C85" s="54"/>
       <c r="D85" s="54"/>
-      <c r="E85" s="60"/>
+      <c r="E85" s="76"/>
       <c r="F85" s="54"/>
       <c r="G85" s="54"/>
       <c r="H85" s="54"/>
@@ -2678,7 +2681,7 @@
       </c>
       <c r="C86" s="54"/>
       <c r="D86" s="54"/>
-      <c r="E86" s="60"/>
+      <c r="E86" s="76"/>
       <c r="F86" s="54"/>
       <c r="G86" s="54"/>
       <c r="H86" s="54"/>
@@ -2693,7 +2696,7 @@
       </c>
       <c r="C87" s="54"/>
       <c r="D87" s="54"/>
-      <c r="E87" s="60"/>
+      <c r="E87" s="76"/>
       <c r="F87" s="54"/>
       <c r="G87" s="54"/>
       <c r="H87" s="54"/>
@@ -2708,7 +2711,7 @@
       </c>
       <c r="C88" s="54"/>
       <c r="D88" s="54"/>
-      <c r="E88" s="60"/>
+      <c r="E88" s="76"/>
       <c r="F88" s="54"/>
       <c r="G88" s="54"/>
       <c r="H88" s="54"/>
@@ -2723,7 +2726,7 @@
       </c>
       <c r="C89" s="54"/>
       <c r="D89" s="54"/>
-      <c r="E89" s="60"/>
+      <c r="E89" s="76"/>
       <c r="F89" s="54"/>
       <c r="G89" s="54"/>
       <c r="H89" s="54"/>
@@ -2738,7 +2741,7 @@
       </c>
       <c r="C90" s="54"/>
       <c r="D90" s="54"/>
-      <c r="E90" s="60"/>
+      <c r="E90" s="76"/>
       <c r="F90" s="54"/>
       <c r="G90" s="54"/>
       <c r="H90" s="54"/>
@@ -2753,7 +2756,7 @@
       </c>
       <c r="C91" s="54"/>
       <c r="D91" s="54"/>
-      <c r="E91" s="60"/>
+      <c r="E91" s="76"/>
       <c r="F91" s="54"/>
       <c r="G91" s="54"/>
       <c r="H91" s="54"/>
@@ -2768,7 +2771,7 @@
       </c>
       <c r="C92" s="54"/>
       <c r="D92" s="54"/>
-      <c r="E92" s="60"/>
+      <c r="E92" s="76"/>
       <c r="F92" s="54"/>
       <c r="G92" s="54"/>
       <c r="H92" s="54"/>
@@ -2783,7 +2786,7 @@
       </c>
       <c r="C93" s="54"/>
       <c r="D93" s="54"/>
-      <c r="E93" s="60"/>
+      <c r="E93" s="76"/>
       <c r="F93" s="54"/>
       <c r="G93" s="54"/>
       <c r="H93" s="54"/>
@@ -2798,7 +2801,7 @@
       </c>
       <c r="C94" s="54"/>
       <c r="D94" s="54"/>
-      <c r="E94" s="60"/>
+      <c r="E94" s="76"/>
       <c r="F94" s="54"/>
       <c r="G94" s="54"/>
       <c r="H94" s="54"/>
@@ -2813,7 +2816,7 @@
       </c>
       <c r="C95" s="54"/>
       <c r="D95" s="54"/>
-      <c r="E95" s="60"/>
+      <c r="E95" s="76"/>
       <c r="F95" s="54"/>
       <c r="G95" s="54"/>
       <c r="H95" s="54"/>
@@ -2828,7 +2831,7 @@
       </c>
       <c r="C96" s="54"/>
       <c r="D96" s="54"/>
-      <c r="E96" s="60"/>
+      <c r="E96" s="76"/>
       <c r="F96" s="54"/>
       <c r="G96" s="54"/>
       <c r="H96" s="54"/>
@@ -2845,7 +2848,7 @@
       </c>
       <c r="C97" s="54"/>
       <c r="D97" s="54"/>
-      <c r="E97" s="60"/>
+      <c r="E97" s="76"/>
       <c r="F97" s="54"/>
       <c r="G97" s="54"/>
       <c r="H97" s="54"/>
@@ -2862,7 +2865,7 @@
       </c>
       <c r="C98" s="54"/>
       <c r="D98" s="54"/>
-      <c r="E98" s="59" t="s">
+      <c r="E98" s="75" t="s">
         <v>20</v>
       </c>
       <c r="F98" s="54"/>
@@ -2881,7 +2884,7 @@
       </c>
       <c r="C99" s="54"/>
       <c r="D99" s="54"/>
-      <c r="E99" s="59"/>
+      <c r="E99" s="75"/>
       <c r="F99" s="54"/>
       <c r="G99" s="54"/>
       <c r="H99" s="54"/>
@@ -2896,7 +2899,7 @@
       </c>
       <c r="C100" s="54"/>
       <c r="D100" s="54"/>
-      <c r="E100" s="59"/>
+      <c r="E100" s="75"/>
       <c r="F100" s="54"/>
       <c r="G100" s="54"/>
       <c r="H100" s="54"/>
@@ -2911,7 +2914,7 @@
       </c>
       <c r="C101" s="54"/>
       <c r="D101" s="54"/>
-      <c r="E101" s="59"/>
+      <c r="E101" s="75"/>
       <c r="F101" s="54"/>
       <c r="G101" s="54"/>
       <c r="H101" s="54"/>
@@ -2926,7 +2929,7 @@
       </c>
       <c r="C102" s="54"/>
       <c r="D102" s="54"/>
-      <c r="E102" s="59"/>
+      <c r="E102" s="75"/>
       <c r="F102" s="54"/>
       <c r="G102" s="54"/>
       <c r="H102" s="54"/>
@@ -2941,7 +2944,7 @@
       </c>
       <c r="C103" s="54"/>
       <c r="D103" s="54"/>
-      <c r="E103" s="59"/>
+      <c r="E103" s="75"/>
       <c r="F103" s="54"/>
       <c r="G103" s="54"/>
       <c r="H103" s="54"/>
@@ -2956,7 +2959,7 @@
       </c>
       <c r="C104" s="54"/>
       <c r="D104" s="54"/>
-      <c r="E104" s="59"/>
+      <c r="E104" s="75"/>
       <c r="F104" s="54"/>
       <c r="G104" s="54"/>
       <c r="H104" s="54"/>
@@ -2971,7 +2974,7 @@
       </c>
       <c r="C105" s="54"/>
       <c r="D105" s="54"/>
-      <c r="E105" s="59"/>
+      <c r="E105" s="75"/>
       <c r="F105" s="54"/>
       <c r="G105" s="54"/>
       <c r="H105" s="54"/>
@@ -2986,7 +2989,7 @@
       </c>
       <c r="C106" s="54"/>
       <c r="D106" s="54"/>
-      <c r="E106" s="59"/>
+      <c r="E106" s="75"/>
       <c r="F106" s="54"/>
       <c r="G106" s="54"/>
       <c r="H106" s="54"/>
@@ -3001,7 +3004,7 @@
       </c>
       <c r="C107" s="54"/>
       <c r="D107" s="54"/>
-      <c r="E107" s="59"/>
+      <c r="E107" s="75"/>
       <c r="F107" s="54"/>
       <c r="G107" s="54"/>
       <c r="H107" s="54"/>
@@ -3016,7 +3019,7 @@
       </c>
       <c r="C108" s="54"/>
       <c r="D108" s="54"/>
-      <c r="E108" s="59"/>
+      <c r="E108" s="75"/>
       <c r="F108" s="54"/>
       <c r="G108" s="54"/>
       <c r="H108" s="54"/>
@@ -3031,7 +3034,7 @@
       </c>
       <c r="C109" s="54"/>
       <c r="D109" s="54"/>
-      <c r="E109" s="59"/>
+      <c r="E109" s="75"/>
       <c r="F109" s="54"/>
       <c r="G109" s="54"/>
       <c r="H109" s="54"/>
@@ -3046,7 +3049,7 @@
       </c>
       <c r="C110" s="54"/>
       <c r="D110" s="54"/>
-      <c r="E110" s="59"/>
+      <c r="E110" s="75"/>
       <c r="F110" s="54"/>
       <c r="G110" s="54"/>
       <c r="H110" s="54"/>
@@ -3061,7 +3064,7 @@
       </c>
       <c r="C111" s="54"/>
       <c r="D111" s="54"/>
-      <c r="E111" s="59"/>
+      <c r="E111" s="75"/>
       <c r="F111" s="54"/>
       <c r="G111" s="54"/>
       <c r="H111" s="54"/>
@@ -3076,7 +3079,7 @@
       </c>
       <c r="C112" s="54"/>
       <c r="D112" s="54"/>
-      <c r="E112" s="59"/>
+      <c r="E112" s="75"/>
       <c r="F112" s="54"/>
       <c r="G112" s="54"/>
       <c r="H112" s="54"/>
@@ -3093,7 +3096,7 @@
       </c>
       <c r="C113" s="54"/>
       <c r="D113" s="54"/>
-      <c r="E113" s="59"/>
+      <c r="E113" s="75"/>
       <c r="F113" s="54"/>
       <c r="G113" s="54"/>
       <c r="H113" s="54"/>
@@ -3110,7 +3113,7 @@
       </c>
       <c r="C114" s="54"/>
       <c r="D114" s="54"/>
-      <c r="E114" s="64" t="s">
+      <c r="E114" s="74" t="s">
         <v>21</v>
       </c>
       <c r="F114" s="54"/>
@@ -3129,7 +3132,7 @@
       </c>
       <c r="C115" s="54"/>
       <c r="D115" s="54"/>
-      <c r="E115" s="64"/>
+      <c r="E115" s="74"/>
       <c r="F115" s="54"/>
       <c r="G115" s="54"/>
       <c r="H115" s="54"/>
@@ -3144,7 +3147,7 @@
       </c>
       <c r="C116" s="54"/>
       <c r="D116" s="54"/>
-      <c r="E116" s="64"/>
+      <c r="E116" s="74"/>
       <c r="F116" s="54"/>
       <c r="G116" s="54"/>
       <c r="H116" s="54"/>
@@ -3159,7 +3162,7 @@
       </c>
       <c r="C117" s="54"/>
       <c r="D117" s="54"/>
-      <c r="E117" s="64"/>
+      <c r="E117" s="74"/>
       <c r="F117" s="54"/>
       <c r="G117" s="54"/>
       <c r="H117" s="54"/>
@@ -3174,7 +3177,7 @@
       </c>
       <c r="C118" s="54"/>
       <c r="D118" s="54"/>
-      <c r="E118" s="64"/>
+      <c r="E118" s="74"/>
       <c r="F118" s="54"/>
       <c r="G118" s="54"/>
       <c r="H118" s="54"/>
@@ -3189,7 +3192,7 @@
       </c>
       <c r="C119" s="54"/>
       <c r="D119" s="54"/>
-      <c r="E119" s="64"/>
+      <c r="E119" s="74"/>
       <c r="F119" s="54"/>
       <c r="G119" s="54"/>
       <c r="H119" s="54"/>
@@ -3204,7 +3207,7 @@
       </c>
       <c r="C120" s="54"/>
       <c r="D120" s="54"/>
-      <c r="E120" s="64"/>
+      <c r="E120" s="74"/>
       <c r="F120" s="54"/>
       <c r="G120" s="54"/>
       <c r="H120" s="54"/>
@@ -3219,7 +3222,7 @@
       </c>
       <c r="C121" s="54"/>
       <c r="D121" s="54"/>
-      <c r="E121" s="64"/>
+      <c r="E121" s="74"/>
       <c r="F121" s="54"/>
       <c r="G121" s="54"/>
       <c r="H121" s="54"/>
@@ -3234,7 +3237,7 @@
       </c>
       <c r="C122" s="54"/>
       <c r="D122" s="54"/>
-      <c r="E122" s="64"/>
+      <c r="E122" s="74"/>
       <c r="F122" s="54"/>
       <c r="G122" s="54"/>
       <c r="H122" s="54"/>
@@ -3249,7 +3252,7 @@
       </c>
       <c r="C123" s="54"/>
       <c r="D123" s="54"/>
-      <c r="E123" s="64"/>
+      <c r="E123" s="74"/>
       <c r="F123" s="54"/>
       <c r="G123" s="54"/>
       <c r="H123" s="54"/>
@@ -3264,7 +3267,7 @@
       </c>
       <c r="C124" s="54"/>
       <c r="D124" s="54"/>
-      <c r="E124" s="64"/>
+      <c r="E124" s="74"/>
       <c r="F124" s="54"/>
       <c r="G124" s="54"/>
       <c r="H124" s="54"/>
@@ -3279,7 +3282,7 @@
       </c>
       <c r="C125" s="54"/>
       <c r="D125" s="54"/>
-      <c r="E125" s="64"/>
+      <c r="E125" s="74"/>
       <c r="F125" s="54"/>
       <c r="G125" s="54"/>
       <c r="H125" s="54"/>
@@ -3294,7 +3297,7 @@
       </c>
       <c r="C126" s="54"/>
       <c r="D126" s="54"/>
-      <c r="E126" s="64"/>
+      <c r="E126" s="74"/>
       <c r="F126" s="54"/>
       <c r="G126" s="54"/>
       <c r="H126" s="54"/>
@@ -3309,7 +3312,7 @@
       </c>
       <c r="C127" s="54"/>
       <c r="D127" s="54"/>
-      <c r="E127" s="64"/>
+      <c r="E127" s="74"/>
       <c r="F127" s="54"/>
       <c r="G127" s="54"/>
       <c r="H127" s="54"/>
@@ -3324,7 +3327,7 @@
       </c>
       <c r="C128" s="54"/>
       <c r="D128" s="54"/>
-      <c r="E128" s="64"/>
+      <c r="E128" s="74"/>
       <c r="F128" s="54"/>
       <c r="G128" s="54"/>
       <c r="H128" s="54"/>
@@ -3341,7 +3344,7 @@
       </c>
       <c r="C129" s="54"/>
       <c r="D129" s="54"/>
-      <c r="E129" s="64"/>
+      <c r="E129" s="74"/>
       <c r="F129" s="54"/>
       <c r="G129" s="54"/>
       <c r="H129" s="54"/>
@@ -3358,7 +3361,7 @@
       </c>
       <c r="C130" s="54"/>
       <c r="D130" s="54"/>
-      <c r="E130" s="61" t="s">
+      <c r="E130" s="67" t="s">
         <v>22</v>
       </c>
       <c r="F130" s="54"/>
@@ -3377,7 +3380,7 @@
       </c>
       <c r="C131" s="54"/>
       <c r="D131" s="54"/>
-      <c r="E131" s="62"/>
+      <c r="E131" s="68"/>
       <c r="F131" s="54"/>
       <c r="G131" s="54"/>
       <c r="H131" s="54"/>
@@ -3392,7 +3395,7 @@
       </c>
       <c r="C132" s="54"/>
       <c r="D132" s="54"/>
-      <c r="E132" s="62"/>
+      <c r="E132" s="68"/>
       <c r="F132" s="54"/>
       <c r="G132" s="54"/>
       <c r="H132" s="54"/>
@@ -3407,7 +3410,7 @@
       </c>
       <c r="C133" s="54"/>
       <c r="D133" s="54"/>
-      <c r="E133" s="62"/>
+      <c r="E133" s="68"/>
       <c r="F133" s="54"/>
       <c r="G133" s="54"/>
       <c r="H133" s="54"/>
@@ -3422,7 +3425,7 @@
       </c>
       <c r="C134" s="54"/>
       <c r="D134" s="54"/>
-      <c r="E134" s="62"/>
+      <c r="E134" s="68"/>
       <c r="F134" s="54"/>
       <c r="G134" s="54"/>
       <c r="H134" s="54"/>
@@ -3437,7 +3440,7 @@
       </c>
       <c r="C135" s="54"/>
       <c r="D135" s="54"/>
-      <c r="E135" s="62"/>
+      <c r="E135" s="68"/>
       <c r="F135" s="54"/>
       <c r="G135" s="54"/>
       <c r="H135" s="54"/>
@@ -3452,7 +3455,7 @@
       </c>
       <c r="C136" s="54"/>
       <c r="D136" s="54"/>
-      <c r="E136" s="62"/>
+      <c r="E136" s="68"/>
       <c r="F136" s="54"/>
       <c r="G136" s="54"/>
       <c r="H136" s="54"/>
@@ -3467,7 +3470,7 @@
       </c>
       <c r="C137" s="54"/>
       <c r="D137" s="54"/>
-      <c r="E137" s="62"/>
+      <c r="E137" s="68"/>
       <c r="F137" s="54"/>
       <c r="G137" s="54"/>
       <c r="H137" s="54"/>
@@ -3482,7 +3485,7 @@
       </c>
       <c r="C138" s="54"/>
       <c r="D138" s="54"/>
-      <c r="E138" s="62"/>
+      <c r="E138" s="68"/>
       <c r="F138" s="54"/>
       <c r="G138" s="54"/>
       <c r="H138" s="54"/>
@@ -3497,7 +3500,7 @@
       </c>
       <c r="C139" s="54"/>
       <c r="D139" s="54"/>
-      <c r="E139" s="62"/>
+      <c r="E139" s="68"/>
       <c r="F139" s="54"/>
       <c r="G139" s="54"/>
       <c r="H139" s="54"/>
@@ -3512,7 +3515,7 @@
       </c>
       <c r="C140" s="54"/>
       <c r="D140" s="54"/>
-      <c r="E140" s="62"/>
+      <c r="E140" s="68"/>
       <c r="F140" s="54"/>
       <c r="G140" s="54"/>
       <c r="H140" s="54"/>
@@ -3527,7 +3530,7 @@
       </c>
       <c r="C141" s="54"/>
       <c r="D141" s="54"/>
-      <c r="E141" s="62"/>
+      <c r="E141" s="68"/>
       <c r="F141" s="54"/>
       <c r="G141" s="54"/>
       <c r="H141" s="54"/>
@@ -3542,7 +3545,7 @@
       </c>
       <c r="C142" s="54"/>
       <c r="D142" s="54"/>
-      <c r="E142" s="62"/>
+      <c r="E142" s="68"/>
       <c r="F142" s="54"/>
       <c r="G142" s="54"/>
       <c r="H142" s="54"/>
@@ -3557,7 +3560,7 @@
       </c>
       <c r="C143" s="54"/>
       <c r="D143" s="54"/>
-      <c r="E143" s="62"/>
+      <c r="E143" s="68"/>
       <c r="F143" s="54"/>
       <c r="G143" s="54"/>
       <c r="H143" s="54"/>
@@ -3572,7 +3575,7 @@
       </c>
       <c r="C144" s="54"/>
       <c r="D144" s="54"/>
-      <c r="E144" s="62"/>
+      <c r="E144" s="68"/>
       <c r="F144" s="54"/>
       <c r="G144" s="54"/>
       <c r="H144" s="54"/>
@@ -3589,7 +3592,7 @@
       </c>
       <c r="C145" s="54"/>
       <c r="D145" s="54"/>
-      <c r="E145" s="63"/>
+      <c r="E145" s="69"/>
       <c r="F145" s="54"/>
       <c r="G145" s="54"/>
       <c r="H145" s="54"/>
@@ -3606,7 +3609,7 @@
       </c>
       <c r="C146" s="54"/>
       <c r="D146" s="54"/>
-      <c r="E146" s="61" t="s">
+      <c r="E146" s="67" t="s">
         <v>23</v>
       </c>
       <c r="F146" s="54"/>
@@ -3625,7 +3628,7 @@
       </c>
       <c r="C147" s="54"/>
       <c r="D147" s="54"/>
-      <c r="E147" s="62"/>
+      <c r="E147" s="68"/>
       <c r="F147" s="54"/>
       <c r="G147" s="54"/>
       <c r="H147" s="54"/>
@@ -3640,7 +3643,7 @@
       </c>
       <c r="C148" s="54"/>
       <c r="D148" s="54"/>
-      <c r="E148" s="62"/>
+      <c r="E148" s="68"/>
       <c r="F148" s="54"/>
       <c r="G148" s="54"/>
       <c r="H148" s="54"/>
@@ -3655,7 +3658,7 @@
       </c>
       <c r="C149" s="54"/>
       <c r="D149" s="54"/>
-      <c r="E149" s="62"/>
+      <c r="E149" s="68"/>
       <c r="F149" s="54"/>
       <c r="G149" s="54"/>
       <c r="H149" s="54"/>
@@ -3670,7 +3673,7 @@
       </c>
       <c r="C150" s="54"/>
       <c r="D150" s="54"/>
-      <c r="E150" s="62"/>
+      <c r="E150" s="68"/>
       <c r="F150" s="54"/>
       <c r="G150" s="54"/>
       <c r="H150" s="54"/>
@@ -3685,7 +3688,7 @@
       </c>
       <c r="C151" s="54"/>
       <c r="D151" s="54"/>
-      <c r="E151" s="62"/>
+      <c r="E151" s="68"/>
       <c r="F151" s="54"/>
       <c r="G151" s="54"/>
       <c r="H151" s="54"/>
@@ -3700,7 +3703,7 @@
       </c>
       <c r="C152" s="54"/>
       <c r="D152" s="54"/>
-      <c r="E152" s="62"/>
+      <c r="E152" s="68"/>
       <c r="F152" s="54"/>
       <c r="G152" s="54"/>
       <c r="H152" s="54"/>
@@ -3715,7 +3718,7 @@
       </c>
       <c r="C153" s="54"/>
       <c r="D153" s="54"/>
-      <c r="E153" s="62"/>
+      <c r="E153" s="68"/>
       <c r="F153" s="54"/>
       <c r="G153" s="54"/>
       <c r="H153" s="54"/>
@@ -3730,7 +3733,7 @@
       </c>
       <c r="C154" s="54"/>
       <c r="D154" s="54"/>
-      <c r="E154" s="62"/>
+      <c r="E154" s="68"/>
       <c r="F154" s="54"/>
       <c r="G154" s="54"/>
       <c r="H154" s="54"/>
@@ -3745,7 +3748,7 @@
       </c>
       <c r="C155" s="54"/>
       <c r="D155" s="54"/>
-      <c r="E155" s="62"/>
+      <c r="E155" s="68"/>
       <c r="F155" s="54"/>
       <c r="G155" s="54"/>
       <c r="H155" s="54"/>
@@ -3760,7 +3763,7 @@
       </c>
       <c r="C156" s="54"/>
       <c r="D156" s="54"/>
-      <c r="E156" s="62"/>
+      <c r="E156" s="68"/>
       <c r="F156" s="54"/>
       <c r="G156" s="54"/>
       <c r="H156" s="54"/>
@@ -3775,7 +3778,7 @@
       </c>
       <c r="C157" s="54"/>
       <c r="D157" s="54"/>
-      <c r="E157" s="62"/>
+      <c r="E157" s="68"/>
       <c r="F157" s="54"/>
       <c r="G157" s="54"/>
       <c r="H157" s="54"/>
@@ -3790,7 +3793,7 @@
       </c>
       <c r="C158" s="54"/>
       <c r="D158" s="54"/>
-      <c r="E158" s="62"/>
+      <c r="E158" s="68"/>
       <c r="F158" s="54"/>
       <c r="G158" s="54"/>
       <c r="H158" s="54"/>
@@ -3805,7 +3808,7 @@
       </c>
       <c r="C159" s="54"/>
       <c r="D159" s="54"/>
-      <c r="E159" s="62"/>
+      <c r="E159" s="68"/>
       <c r="F159" s="54"/>
       <c r="G159" s="54"/>
       <c r="H159" s="54"/>
@@ -3820,7 +3823,7 @@
       </c>
       <c r="C160" s="54"/>
       <c r="D160" s="54"/>
-      <c r="E160" s="62"/>
+      <c r="E160" s="68"/>
       <c r="F160" s="54"/>
       <c r="G160" s="54"/>
       <c r="H160" s="54"/>
@@ -3837,7 +3840,7 @@
       </c>
       <c r="C161" s="54"/>
       <c r="D161" s="54"/>
-      <c r="E161" s="63"/>
+      <c r="E161" s="69"/>
       <c r="F161" s="54"/>
       <c r="G161" s="54"/>
       <c r="H161" s="54"/>
@@ -3854,7 +3857,7 @@
       </c>
       <c r="C162" s="54"/>
       <c r="D162" s="54"/>
-      <c r="E162" s="69" t="s">
+      <c r="E162" s="61" t="s">
         <v>26</v>
       </c>
       <c r="F162" s="54"/>
@@ -3873,7 +3876,7 @@
       </c>
       <c r="C163" s="54"/>
       <c r="D163" s="54"/>
-      <c r="E163" s="70"/>
+      <c r="E163" s="62"/>
       <c r="F163" s="54"/>
       <c r="G163" s="54"/>
       <c r="H163" s="54"/>
@@ -3888,7 +3891,7 @@
       </c>
       <c r="C164" s="54"/>
       <c r="D164" s="54"/>
-      <c r="E164" s="70"/>
+      <c r="E164" s="62"/>
       <c r="F164" s="54"/>
       <c r="G164" s="54"/>
       <c r="H164" s="54"/>
@@ -3903,7 +3906,7 @@
       </c>
       <c r="C165" s="54"/>
       <c r="D165" s="54"/>
-      <c r="E165" s="70"/>
+      <c r="E165" s="62"/>
       <c r="F165" s="54"/>
       <c r="G165" s="54"/>
       <c r="H165" s="54"/>
@@ -3918,7 +3921,7 @@
       </c>
       <c r="C166" s="54"/>
       <c r="D166" s="54"/>
-      <c r="E166" s="70"/>
+      <c r="E166" s="62"/>
       <c r="F166" s="54"/>
       <c r="G166" s="54"/>
       <c r="H166" s="54"/>
@@ -3933,7 +3936,7 @@
       </c>
       <c r="C167" s="54"/>
       <c r="D167" s="54"/>
-      <c r="E167" s="70"/>
+      <c r="E167" s="62"/>
       <c r="F167" s="54"/>
       <c r="G167" s="54"/>
       <c r="H167" s="54"/>
@@ -3948,7 +3951,7 @@
       </c>
       <c r="C168" s="54"/>
       <c r="D168" s="54"/>
-      <c r="E168" s="70"/>
+      <c r="E168" s="62"/>
       <c r="F168" s="54"/>
       <c r="G168" s="54"/>
       <c r="H168" s="54"/>
@@ -3963,7 +3966,7 @@
       </c>
       <c r="C169" s="54"/>
       <c r="D169" s="54"/>
-      <c r="E169" s="70"/>
+      <c r="E169" s="62"/>
       <c r="F169" s="54"/>
       <c r="G169" s="54"/>
       <c r="H169" s="54"/>
@@ -3978,7 +3981,7 @@
       </c>
       <c r="C170" s="54"/>
       <c r="D170" s="54"/>
-      <c r="E170" s="70"/>
+      <c r="E170" s="62"/>
       <c r="F170" s="54"/>
       <c r="G170" s="54"/>
       <c r="H170" s="54"/>
@@ -3993,7 +3996,7 @@
       </c>
       <c r="C171" s="54"/>
       <c r="D171" s="54"/>
-      <c r="E171" s="70"/>
+      <c r="E171" s="62"/>
       <c r="F171" s="54"/>
       <c r="G171" s="54"/>
       <c r="H171" s="54"/>
@@ -4008,7 +4011,7 @@
       </c>
       <c r="C172" s="54"/>
       <c r="D172" s="54"/>
-      <c r="E172" s="70"/>
+      <c r="E172" s="62"/>
       <c r="F172" s="54"/>
       <c r="G172" s="54"/>
       <c r="H172" s="54"/>
@@ -4023,7 +4026,7 @@
       </c>
       <c r="C173" s="54"/>
       <c r="D173" s="54"/>
-      <c r="E173" s="70"/>
+      <c r="E173" s="62"/>
       <c r="F173" s="54"/>
       <c r="G173" s="54"/>
       <c r="H173" s="54"/>
@@ -4038,7 +4041,7 @@
       </c>
       <c r="C174" s="54"/>
       <c r="D174" s="54"/>
-      <c r="E174" s="70"/>
+      <c r="E174" s="62"/>
       <c r="F174" s="54"/>
       <c r="G174" s="54"/>
       <c r="H174" s="54"/>
@@ -4053,7 +4056,7 @@
       </c>
       <c r="C175" s="54"/>
       <c r="D175" s="54"/>
-      <c r="E175" s="70"/>
+      <c r="E175" s="62"/>
       <c r="F175" s="54"/>
       <c r="G175" s="54"/>
       <c r="H175" s="54"/>
@@ -4068,7 +4071,7 @@
       </c>
       <c r="C176" s="54"/>
       <c r="D176" s="54"/>
-      <c r="E176" s="70"/>
+      <c r="E176" s="62"/>
       <c r="F176" s="54"/>
       <c r="G176" s="54"/>
       <c r="H176" s="54"/>
@@ -4085,7 +4088,7 @@
       </c>
       <c r="C177" s="54"/>
       <c r="D177" s="54"/>
-      <c r="E177" s="71"/>
+      <c r="E177" s="63"/>
       <c r="F177" s="54"/>
       <c r="G177" s="54"/>
       <c r="H177" s="54"/>
@@ -4102,7 +4105,7 @@
       </c>
       <c r="C178" s="54"/>
       <c r="D178" s="54"/>
-      <c r="E178" s="65" t="s">
+      <c r="E178" s="70" t="s">
         <v>27</v>
       </c>
       <c r="F178" s="54"/>
@@ -4121,7 +4124,7 @@
       </c>
       <c r="C179" s="54"/>
       <c r="D179" s="54"/>
-      <c r="E179" s="65"/>
+      <c r="E179" s="70"/>
       <c r="F179" s="54"/>
       <c r="G179" s="54"/>
       <c r="H179" s="54"/>
@@ -4136,7 +4139,7 @@
       </c>
       <c r="C180" s="54"/>
       <c r="D180" s="54"/>
-      <c r="E180" s="65"/>
+      <c r="E180" s="70"/>
       <c r="F180" s="54"/>
       <c r="G180" s="54"/>
       <c r="H180" s="54"/>
@@ -4151,7 +4154,7 @@
       </c>
       <c r="C181" s="54"/>
       <c r="D181" s="54"/>
-      <c r="E181" s="65"/>
+      <c r="E181" s="70"/>
       <c r="F181" s="54"/>
       <c r="G181" s="54"/>
       <c r="H181" s="54"/>
@@ -4166,7 +4169,7 @@
       </c>
       <c r="C182" s="54"/>
       <c r="D182" s="54"/>
-      <c r="E182" s="65"/>
+      <c r="E182" s="70"/>
       <c r="F182" s="54"/>
       <c r="G182" s="54"/>
       <c r="H182" s="54"/>
@@ -4181,7 +4184,7 @@
       </c>
       <c r="C183" s="54"/>
       <c r="D183" s="54"/>
-      <c r="E183" s="65"/>
+      <c r="E183" s="70"/>
       <c r="F183" s="54"/>
       <c r="G183" s="54"/>
       <c r="H183" s="54"/>
@@ -4196,7 +4199,7 @@
       </c>
       <c r="C184" s="54"/>
       <c r="D184" s="54"/>
-      <c r="E184" s="65"/>
+      <c r="E184" s="70"/>
       <c r="F184" s="54"/>
       <c r="G184" s="54"/>
       <c r="H184" s="54"/>
@@ -4211,7 +4214,7 @@
       </c>
       <c r="C185" s="54"/>
       <c r="D185" s="54"/>
-      <c r="E185" s="65"/>
+      <c r="E185" s="70"/>
       <c r="F185" s="54"/>
       <c r="G185" s="54"/>
       <c r="H185" s="54"/>
@@ -4226,7 +4229,7 @@
       </c>
       <c r="C186" s="54"/>
       <c r="D186" s="54"/>
-      <c r="E186" s="65"/>
+      <c r="E186" s="70"/>
       <c r="F186" s="54"/>
       <c r="G186" s="54"/>
       <c r="H186" s="54"/>
@@ -4241,7 +4244,7 @@
       </c>
       <c r="C187" s="54"/>
       <c r="D187" s="54"/>
-      <c r="E187" s="65"/>
+      <c r="E187" s="70"/>
       <c r="F187" s="54"/>
       <c r="G187" s="54"/>
       <c r="H187" s="54"/>
@@ -4256,7 +4259,7 @@
       </c>
       <c r="C188" s="54"/>
       <c r="D188" s="54"/>
-      <c r="E188" s="65"/>
+      <c r="E188" s="70"/>
       <c r="F188" s="54"/>
       <c r="G188" s="54"/>
       <c r="H188" s="54"/>
@@ -4271,7 +4274,7 @@
       </c>
       <c r="C189" s="54"/>
       <c r="D189" s="54"/>
-      <c r="E189" s="65"/>
+      <c r="E189" s="70"/>
       <c r="F189" s="54"/>
       <c r="G189" s="54"/>
       <c r="H189" s="54"/>
@@ -4286,7 +4289,7 @@
       </c>
       <c r="C190" s="54"/>
       <c r="D190" s="54"/>
-      <c r="E190" s="65"/>
+      <c r="E190" s="70"/>
       <c r="F190" s="54"/>
       <c r="G190" s="54"/>
       <c r="H190" s="54"/>
@@ -4301,7 +4304,7 @@
       </c>
       <c r="C191" s="54"/>
       <c r="D191" s="54"/>
-      <c r="E191" s="65"/>
+      <c r="E191" s="70"/>
       <c r="F191" s="54"/>
       <c r="G191" s="54"/>
       <c r="H191" s="54"/>
@@ -4316,7 +4319,7 @@
       </c>
       <c r="C192" s="54"/>
       <c r="D192" s="54"/>
-      <c r="E192" s="65"/>
+      <c r="E192" s="70"/>
       <c r="F192" s="54"/>
       <c r="G192" s="54"/>
       <c r="H192" s="54"/>
@@ -4333,7 +4336,7 @@
       </c>
       <c r="C193" s="54"/>
       <c r="D193" s="54"/>
-      <c r="E193" s="65"/>
+      <c r="E193" s="70"/>
       <c r="F193" s="54"/>
       <c r="G193" s="54"/>
       <c r="H193" s="54"/>
@@ -4349,7 +4352,7 @@
         <v>192</v>
       </c>
       <c r="C194" s="54"/>
-      <c r="D194" s="66" t="s">
+      <c r="D194" s="71" t="s">
         <v>25</v>
       </c>
       <c r="E194" s="54"/>
@@ -4368,7 +4371,7 @@
         <v>193</v>
       </c>
       <c r="C195" s="54"/>
-      <c r="D195" s="67"/>
+      <c r="D195" s="72"/>
       <c r="E195" s="54"/>
       <c r="F195" s="54"/>
       <c r="G195" s="54"/>
@@ -4383,7 +4386,7 @@
         <v>194</v>
       </c>
       <c r="C196" s="54"/>
-      <c r="D196" s="67"/>
+      <c r="D196" s="72"/>
       <c r="E196" s="54"/>
       <c r="F196" s="54"/>
       <c r="G196" s="54"/>
@@ -4398,7 +4401,7 @@
         <v>195</v>
       </c>
       <c r="C197" s="54"/>
-      <c r="D197" s="67"/>
+      <c r="D197" s="72"/>
       <c r="E197" s="54"/>
       <c r="F197" s="54"/>
       <c r="G197" s="54"/>
@@ -4413,7 +4416,7 @@
         <v>196</v>
       </c>
       <c r="C198" s="54"/>
-      <c r="D198" s="67"/>
+      <c r="D198" s="72"/>
       <c r="E198" s="54"/>
       <c r="F198" s="54"/>
       <c r="G198" s="54"/>
@@ -4428,7 +4431,7 @@
         <v>197</v>
       </c>
       <c r="C199" s="54"/>
-      <c r="D199" s="67"/>
+      <c r="D199" s="72"/>
       <c r="E199" s="54"/>
       <c r="F199" s="54"/>
       <c r="G199" s="54"/>
@@ -4443,7 +4446,7 @@
         <v>198</v>
       </c>
       <c r="C200" s="54"/>
-      <c r="D200" s="67"/>
+      <c r="D200" s="72"/>
       <c r="E200" s="54"/>
       <c r="F200" s="54"/>
       <c r="G200" s="54"/>
@@ -4460,7 +4463,7 @@
         <v>199</v>
       </c>
       <c r="C201" s="54"/>
-      <c r="D201" s="68"/>
+      <c r="D201" s="73"/>
       <c r="E201" s="54"/>
       <c r="F201" s="54"/>
       <c r="G201" s="54"/>
@@ -4477,7 +4480,7 @@
         <v>200</v>
       </c>
       <c r="C202" s="54"/>
-      <c r="D202" s="75" t="s">
+      <c r="D202" s="55" t="s">
         <v>24</v>
       </c>
       <c r="E202" s="54"/>
@@ -4496,7 +4499,7 @@
         <v>201</v>
       </c>
       <c r="C203" s="54"/>
-      <c r="D203" s="75"/>
+      <c r="D203" s="55"/>
       <c r="E203" s="54"/>
       <c r="F203" s="54"/>
       <c r="G203" s="54"/>
@@ -4511,7 +4514,7 @@
         <v>202</v>
       </c>
       <c r="C204" s="54"/>
-      <c r="D204" s="75"/>
+      <c r="D204" s="55"/>
       <c r="E204" s="54"/>
       <c r="F204" s="54"/>
       <c r="G204" s="54"/>
@@ -4526,7 +4529,7 @@
         <v>203</v>
       </c>
       <c r="C205" s="54"/>
-      <c r="D205" s="75"/>
+      <c r="D205" s="55"/>
       <c r="E205" s="54"/>
       <c r="F205" s="54"/>
       <c r="G205" s="54"/>
@@ -4541,7 +4544,7 @@
         <v>204</v>
       </c>
       <c r="C206" s="54"/>
-      <c r="D206" s="75"/>
+      <c r="D206" s="55"/>
       <c r="E206" s="54"/>
       <c r="F206" s="54"/>
       <c r="G206" s="54"/>
@@ -4556,7 +4559,7 @@
         <v>205</v>
       </c>
       <c r="C207" s="54"/>
-      <c r="D207" s="75"/>
+      <c r="D207" s="55"/>
       <c r="E207" s="54"/>
       <c r="F207" s="54"/>
       <c r="G207" s="54"/>
@@ -4571,7 +4574,7 @@
         <v>206</v>
       </c>
       <c r="C208" s="54"/>
-      <c r="D208" s="75"/>
+      <c r="D208" s="55"/>
       <c r="E208" s="54"/>
       <c r="F208" s="54"/>
       <c r="G208" s="54"/>
@@ -4588,7 +4591,7 @@
         <v>207</v>
       </c>
       <c r="C209" s="54"/>
-      <c r="D209" s="75"/>
+      <c r="D209" s="55"/>
       <c r="E209" s="54"/>
       <c r="F209" s="54"/>
       <c r="G209" s="54"/>
@@ -4604,9 +4607,9 @@
       <c r="B210" s="32">
         <v>208</v>
       </c>
-      <c r="C210" s="76"/>
-      <c r="D210" s="77"/>
-      <c r="E210" s="78" t="s">
+      <c r="C210" s="56"/>
+      <c r="D210" s="57"/>
+      <c r="E210" s="58" t="s">
         <v>34</v>
       </c>
       <c r="F210" s="54"/>
@@ -4623,9 +4626,9 @@
       <c r="B211" s="32">
         <v>209</v>
       </c>
-      <c r="C211" s="76"/>
-      <c r="D211" s="77"/>
-      <c r="E211" s="78"/>
+      <c r="C211" s="56"/>
+      <c r="D211" s="57"/>
+      <c r="E211" s="58"/>
       <c r="F211" s="54"/>
       <c r="G211" s="54"/>
       <c r="H211" s="54"/>
@@ -4640,9 +4643,9 @@
       <c r="B212" s="32">
         <v>210</v>
       </c>
-      <c r="C212" s="76"/>
-      <c r="D212" s="77"/>
-      <c r="E212" s="78"/>
+      <c r="C212" s="56"/>
+      <c r="D212" s="57"/>
+      <c r="E212" s="58"/>
       <c r="F212" s="54"/>
       <c r="G212" s="54"/>
       <c r="H212" s="54"/>
@@ -4657,9 +4660,9 @@
       <c r="B213" s="32">
         <v>211</v>
       </c>
-      <c r="C213" s="76"/>
-      <c r="D213" s="77"/>
-      <c r="E213" s="78"/>
+      <c r="C213" s="56"/>
+      <c r="D213" s="57"/>
+      <c r="E213" s="58"/>
       <c r="F213" s="54"/>
       <c r="G213" s="54"/>
       <c r="H213" s="54"/>
@@ -4674,9 +4677,9 @@
       <c r="B214" s="32">
         <v>212</v>
       </c>
-      <c r="C214" s="76"/>
-      <c r="D214" s="77"/>
-      <c r="E214" s="78"/>
+      <c r="C214" s="56"/>
+      <c r="D214" s="57"/>
+      <c r="E214" s="58"/>
       <c r="F214" s="54"/>
       <c r="G214" s="54"/>
       <c r="H214" s="54"/>
@@ -4691,9 +4694,9 @@
       <c r="B215" s="32">
         <v>213</v>
       </c>
-      <c r="C215" s="76"/>
-      <c r="D215" s="77"/>
-      <c r="E215" s="78"/>
+      <c r="C215" s="56"/>
+      <c r="D215" s="57"/>
+      <c r="E215" s="58"/>
       <c r="F215" s="54"/>
       <c r="G215" s="54"/>
       <c r="H215" s="54"/>
@@ -4708,9 +4711,9 @@
       <c r="B216" s="32">
         <v>214</v>
       </c>
-      <c r="C216" s="76"/>
-      <c r="D216" s="77"/>
-      <c r="E216" s="78"/>
+      <c r="C216" s="56"/>
+      <c r="D216" s="57"/>
+      <c r="E216" s="58"/>
       <c r="F216" s="54"/>
       <c r="G216" s="54"/>
       <c r="H216" s="54"/>
@@ -4725,9 +4728,9 @@
       <c r="B217" s="32">
         <v>215</v>
       </c>
-      <c r="C217" s="76"/>
-      <c r="D217" s="77"/>
-      <c r="E217" s="78"/>
+      <c r="C217" s="56"/>
+      <c r="D217" s="57"/>
+      <c r="E217" s="58"/>
       <c r="F217" s="54"/>
       <c r="G217" s="54"/>
       <c r="H217" s="54"/>
@@ -4741,8 +4744,8 @@
         <v>216</v>
       </c>
       <c r="C218" s="54"/>
-      <c r="D218" s="72"/>
-      <c r="E218" s="78"/>
+      <c r="D218" s="64"/>
+      <c r="E218" s="58"/>
       <c r="F218" s="54"/>
       <c r="G218" s="54"/>
       <c r="H218" s="54"/>
@@ -4756,8 +4759,8 @@
         <v>217</v>
       </c>
       <c r="C219" s="54"/>
-      <c r="D219" s="72"/>
-      <c r="E219" s="78"/>
+      <c r="D219" s="64"/>
+      <c r="E219" s="58"/>
       <c r="F219" s="54"/>
       <c r="G219" s="54"/>
       <c r="H219" s="54"/>
@@ -4771,8 +4774,8 @@
         <v>218</v>
       </c>
       <c r="C220" s="54"/>
-      <c r="D220" s="72"/>
-      <c r="E220" s="78"/>
+      <c r="D220" s="64"/>
+      <c r="E220" s="58"/>
       <c r="F220" s="54"/>
       <c r="G220" s="54"/>
       <c r="H220" s="54"/>
@@ -4786,8 +4789,8 @@
         <v>219</v>
       </c>
       <c r="C221" s="54"/>
-      <c r="D221" s="72"/>
-      <c r="E221" s="78"/>
+      <c r="D221" s="64"/>
+      <c r="E221" s="58"/>
       <c r="F221" s="54"/>
       <c r="G221" s="54"/>
       <c r="H221" s="54"/>
@@ -4801,8 +4804,8 @@
         <v>220</v>
       </c>
       <c r="C222" s="54"/>
-      <c r="D222" s="72"/>
-      <c r="E222" s="78"/>
+      <c r="D222" s="64"/>
+      <c r="E222" s="58"/>
       <c r="F222" s="54"/>
       <c r="G222" s="54"/>
       <c r="H222" s="54"/>
@@ -4816,8 +4819,8 @@
         <v>221</v>
       </c>
       <c r="C223" s="54"/>
-      <c r="D223" s="72"/>
-      <c r="E223" s="78"/>
+      <c r="D223" s="64"/>
+      <c r="E223" s="58"/>
       <c r="F223" s="54"/>
       <c r="G223" s="54"/>
       <c r="H223" s="54"/>
@@ -4831,8 +4834,8 @@
         <v>222</v>
       </c>
       <c r="C224" s="54"/>
-      <c r="D224" s="72"/>
-      <c r="E224" s="78"/>
+      <c r="D224" s="64"/>
+      <c r="E224" s="58"/>
       <c r="F224" s="54"/>
       <c r="G224" s="54"/>
       <c r="H224" s="54"/>
@@ -4846,8 +4849,8 @@
         <v>223</v>
       </c>
       <c r="C225" s="54"/>
-      <c r="D225" s="72"/>
-      <c r="E225" s="78"/>
+      <c r="D225" s="64"/>
+      <c r="E225" s="58"/>
       <c r="F225" s="54"/>
       <c r="G225" s="54"/>
       <c r="H225" s="54"/>
@@ -4862,8 +4865,8 @@
       <c r="B226" s="51">
         <v>224</v>
       </c>
-      <c r="C226" s="73"/>
-      <c r="D226" s="74" t="s">
+      <c r="C226" s="65"/>
+      <c r="D226" s="66" t="s">
         <v>29</v>
       </c>
       <c r="E226" s="54"/>
@@ -4881,8 +4884,8 @@
       <c r="B227" s="51">
         <v>225</v>
       </c>
-      <c r="C227" s="73"/>
-      <c r="D227" s="74"/>
+      <c r="C227" s="65"/>
+      <c r="D227" s="66"/>
       <c r="E227" s="54"/>
       <c r="F227" s="54"/>
       <c r="G227" s="54"/>
@@ -4896,8 +4899,8 @@
       <c r="B228" s="51">
         <v>226</v>
       </c>
-      <c r="C228" s="73"/>
-      <c r="D228" s="74"/>
+      <c r="C228" s="65"/>
+      <c r="D228" s="66"/>
       <c r="E228" s="54"/>
       <c r="F228" s="54"/>
       <c r="G228" s="54"/>
@@ -4911,8 +4914,8 @@
       <c r="B229" s="51">
         <v>227</v>
       </c>
-      <c r="C229" s="73"/>
-      <c r="D229" s="74"/>
+      <c r="C229" s="65"/>
+      <c r="D229" s="66"/>
       <c r="E229" s="54"/>
       <c r="F229" s="54"/>
       <c r="G229" s="54"/>
@@ -4926,8 +4929,8 @@
       <c r="B230" s="51">
         <v>228</v>
       </c>
-      <c r="C230" s="79"/>
-      <c r="D230" s="74"/>
+      <c r="C230" s="59"/>
+      <c r="D230" s="66"/>
       <c r="E230" s="54"/>
       <c r="F230" s="54"/>
       <c r="G230" s="54"/>
@@ -4941,8 +4944,8 @@
       <c r="B231" s="51">
         <v>229</v>
       </c>
-      <c r="C231" s="79"/>
-      <c r="D231" s="74"/>
+      <c r="C231" s="59"/>
+      <c r="D231" s="66"/>
       <c r="E231" s="54"/>
       <c r="F231" s="54"/>
       <c r="G231" s="54"/>
@@ -4956,8 +4959,8 @@
       <c r="B232" s="51">
         <v>230</v>
       </c>
-      <c r="C232" s="79"/>
-      <c r="D232" s="74"/>
+      <c r="C232" s="59"/>
+      <c r="D232" s="66"/>
       <c r="E232" s="54"/>
       <c r="F232" s="54"/>
       <c r="G232" s="54"/>
@@ -4971,8 +4974,8 @@
       <c r="B233" s="51">
         <v>231</v>
       </c>
-      <c r="C233" s="79"/>
-      <c r="D233" s="74"/>
+      <c r="C233" s="59"/>
+      <c r="D233" s="66"/>
       <c r="E233" s="54"/>
       <c r="F233" s="54"/>
       <c r="G233" s="54"/>
@@ -4988,7 +4991,7 @@
       <c r="B234" s="47">
         <v>232</v>
       </c>
-      <c r="C234" s="80" t="s">
+      <c r="C234" s="60" t="s">
         <v>30</v>
       </c>
       <c r="D234" s="54"/>
@@ -5007,13 +5010,15 @@
       <c r="B235" s="47">
         <v>233</v>
       </c>
-      <c r="C235" s="80"/>
+      <c r="C235" s="60"/>
       <c r="D235" s="54"/>
       <c r="E235" s="54"/>
       <c r="F235" s="54"/>
       <c r="G235" s="54"/>
       <c r="H235" s="54"/>
-      <c r="I235" s="49"/>
+      <c r="I235" s="49" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" s="47" t="s">
@@ -5022,13 +5027,15 @@
       <c r="B236" s="47">
         <v>234</v>
       </c>
-      <c r="C236" s="80"/>
+      <c r="C236" s="60"/>
       <c r="D236" s="54"/>
       <c r="E236" s="54"/>
       <c r="F236" s="54"/>
       <c r="G236" s="54"/>
       <c r="H236" s="54"/>
-      <c r="I236" s="49"/>
+      <c r="I236" s="49" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" s="47" t="s">
@@ -5037,7 +5044,7 @@
       <c r="B237" s="47">
         <v>235</v>
       </c>
-      <c r="C237" s="80"/>
+      <c r="C237" s="60"/>
       <c r="D237" s="54"/>
       <c r="E237" s="54"/>
       <c r="F237" s="54"/>
@@ -5349,38 +5356,76 @@
     </row>
   </sheetData>
   <mergeCells count="126">
-    <mergeCell ref="F194:F225"/>
-    <mergeCell ref="G194:G257"/>
-    <mergeCell ref="C198:C201"/>
-    <mergeCell ref="C202:C205"/>
-    <mergeCell ref="D202:D209"/>
-    <mergeCell ref="C206:C209"/>
-    <mergeCell ref="C210:C213"/>
-    <mergeCell ref="D210:D217"/>
-    <mergeCell ref="E210:E225"/>
-    <mergeCell ref="C214:C217"/>
-    <mergeCell ref="D250:D257"/>
-    <mergeCell ref="C254:C257"/>
-    <mergeCell ref="F226:F257"/>
-    <mergeCell ref="C230:C233"/>
-    <mergeCell ref="C234:C237"/>
-    <mergeCell ref="D234:D241"/>
-    <mergeCell ref="C238:C241"/>
-    <mergeCell ref="C242:C245"/>
-    <mergeCell ref="D242:D249"/>
-    <mergeCell ref="E242:E257"/>
-    <mergeCell ref="C246:C249"/>
-    <mergeCell ref="C250:C253"/>
-    <mergeCell ref="E194:E209"/>
-    <mergeCell ref="C162:C165"/>
-    <mergeCell ref="D162:D169"/>
-    <mergeCell ref="E162:E177"/>
-    <mergeCell ref="C218:C221"/>
-    <mergeCell ref="D218:D225"/>
-    <mergeCell ref="C222:C225"/>
-    <mergeCell ref="C226:C229"/>
-    <mergeCell ref="D226:D233"/>
-    <mergeCell ref="E226:E241"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D9"/>
+    <mergeCell ref="E2:E17"/>
+    <mergeCell ref="F2:F33"/>
+    <mergeCell ref="G2:G65"/>
+    <mergeCell ref="H2:H129"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="F34:F65"/>
+    <mergeCell ref="C38:C41"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="D42:D49"/>
+    <mergeCell ref="C46:C49"/>
+    <mergeCell ref="C50:C53"/>
+    <mergeCell ref="D50:D57"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D25"/>
+    <mergeCell ref="E18:E33"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D26:D33"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="E50:E65"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="D58:D65"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="D66:D73"/>
+    <mergeCell ref="E66:E81"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="D34:D41"/>
+    <mergeCell ref="E34:E49"/>
+    <mergeCell ref="C90:C93"/>
+    <mergeCell ref="D90:D97"/>
+    <mergeCell ref="C94:C97"/>
+    <mergeCell ref="C98:C101"/>
+    <mergeCell ref="D98:D105"/>
+    <mergeCell ref="E98:E113"/>
+    <mergeCell ref="F66:F97"/>
+    <mergeCell ref="G66:G129"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="C74:C77"/>
+    <mergeCell ref="D74:D81"/>
+    <mergeCell ref="C78:C81"/>
+    <mergeCell ref="C82:C85"/>
+    <mergeCell ref="D82:D89"/>
+    <mergeCell ref="E82:E97"/>
+    <mergeCell ref="C86:C89"/>
+    <mergeCell ref="D122:D129"/>
+    <mergeCell ref="C126:C129"/>
+    <mergeCell ref="C130:C133"/>
+    <mergeCell ref="D130:D137"/>
+    <mergeCell ref="E130:E145"/>
+    <mergeCell ref="F130:F161"/>
+    <mergeCell ref="C154:C157"/>
+    <mergeCell ref="D154:D161"/>
+    <mergeCell ref="C158:C161"/>
+    <mergeCell ref="F98:F129"/>
+    <mergeCell ref="C102:C105"/>
+    <mergeCell ref="C106:C109"/>
+    <mergeCell ref="D106:D113"/>
+    <mergeCell ref="C110:C113"/>
+    <mergeCell ref="C114:C117"/>
+    <mergeCell ref="D114:D121"/>
+    <mergeCell ref="E114:E129"/>
+    <mergeCell ref="C118:C121"/>
+    <mergeCell ref="C122:C125"/>
     <mergeCell ref="F162:F193"/>
     <mergeCell ref="C166:C169"/>
     <mergeCell ref="C170:C173"/>
@@ -5405,76 +5450,38 @@
     <mergeCell ref="C190:C193"/>
     <mergeCell ref="C194:C197"/>
     <mergeCell ref="D194:D201"/>
-    <mergeCell ref="C130:C133"/>
-    <mergeCell ref="D130:D137"/>
-    <mergeCell ref="E130:E145"/>
-    <mergeCell ref="F130:F161"/>
-    <mergeCell ref="C154:C157"/>
-    <mergeCell ref="D154:D161"/>
-    <mergeCell ref="C158:C161"/>
-    <mergeCell ref="F98:F129"/>
-    <mergeCell ref="C102:C105"/>
-    <mergeCell ref="C106:C109"/>
-    <mergeCell ref="D106:D113"/>
-    <mergeCell ref="C110:C113"/>
-    <mergeCell ref="C114:C117"/>
-    <mergeCell ref="D114:D121"/>
-    <mergeCell ref="E114:E129"/>
-    <mergeCell ref="C118:C121"/>
-    <mergeCell ref="C122:C125"/>
-    <mergeCell ref="C90:C93"/>
-    <mergeCell ref="D90:D97"/>
-    <mergeCell ref="C94:C97"/>
-    <mergeCell ref="C98:C101"/>
-    <mergeCell ref="D98:D105"/>
-    <mergeCell ref="E98:E113"/>
-    <mergeCell ref="F66:F97"/>
-    <mergeCell ref="G66:G129"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="C74:C77"/>
-    <mergeCell ref="D74:D81"/>
-    <mergeCell ref="C78:C81"/>
-    <mergeCell ref="C82:C85"/>
-    <mergeCell ref="D82:D89"/>
-    <mergeCell ref="E82:E97"/>
-    <mergeCell ref="C86:C89"/>
-    <mergeCell ref="D122:D129"/>
-    <mergeCell ref="C126:C129"/>
-    <mergeCell ref="E50:E65"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="D58:D65"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="C66:C69"/>
-    <mergeCell ref="D66:D73"/>
-    <mergeCell ref="E66:E81"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="D34:D41"/>
-    <mergeCell ref="E34:E49"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="D2:D9"/>
-    <mergeCell ref="E2:E17"/>
-    <mergeCell ref="F2:F33"/>
-    <mergeCell ref="G2:G65"/>
-    <mergeCell ref="H2:H129"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="D10:D17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="F34:F65"/>
-    <mergeCell ref="C38:C41"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="D42:D49"/>
-    <mergeCell ref="C46:C49"/>
-    <mergeCell ref="C50:C53"/>
-    <mergeCell ref="D50:D57"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D25"/>
-    <mergeCell ref="E18:E33"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="D26:D33"/>
-    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="C162:C165"/>
+    <mergeCell ref="D162:D169"/>
+    <mergeCell ref="E162:E177"/>
+    <mergeCell ref="C218:C221"/>
+    <mergeCell ref="D218:D225"/>
+    <mergeCell ref="C222:C225"/>
+    <mergeCell ref="C226:C229"/>
+    <mergeCell ref="D226:D233"/>
+    <mergeCell ref="E226:E241"/>
+    <mergeCell ref="F194:F225"/>
+    <mergeCell ref="G194:G257"/>
+    <mergeCell ref="C198:C201"/>
+    <mergeCell ref="C202:C205"/>
+    <mergeCell ref="D202:D209"/>
+    <mergeCell ref="C206:C209"/>
+    <mergeCell ref="C210:C213"/>
+    <mergeCell ref="D210:D217"/>
+    <mergeCell ref="E210:E225"/>
+    <mergeCell ref="C214:C217"/>
+    <mergeCell ref="D250:D257"/>
+    <mergeCell ref="C254:C257"/>
+    <mergeCell ref="F226:F257"/>
+    <mergeCell ref="C230:C233"/>
+    <mergeCell ref="C234:C237"/>
+    <mergeCell ref="D234:D241"/>
+    <mergeCell ref="C238:C241"/>
+    <mergeCell ref="C242:C245"/>
+    <mergeCell ref="D242:D249"/>
+    <mergeCell ref="E242:E257"/>
+    <mergeCell ref="C246:C249"/>
+    <mergeCell ref="C250:C253"/>
+    <mergeCell ref="E194:E209"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Excel table fixes, now Switches and WiFi Routers are not in same subnets
</commit_message>
<xml_diff>
--- a/Kisvállalat létszám.xlsx
+++ b/Kisvállalat létszám.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Izumi\Documents\github-repos\fluffy-system\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\School\11.o\Hálózat\projekt\fluffy-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4708724C-AED9-434C-A648-EA0DE6C659F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3679D178-B854-4281-AFB1-D5D356EBFBF7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18195" yWindow="945" windowWidth="9810" windowHeight="14205" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alap" sheetId="1" r:id="rId1"/>
@@ -143,15 +143,6 @@
     <t>Wireless Router2</t>
   </si>
   <si>
-    <t>Switch0</t>
-  </si>
-  <si>
-    <t>Switch1</t>
-  </si>
-  <si>
-    <t>Switch2</t>
-  </si>
-  <si>
     <t>192.168.1</t>
   </si>
   <si>
@@ -210,6 +201,15 @@
   </si>
   <si>
     <t>Szerver IP</t>
+  </si>
+  <si>
+    <t>S0</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
   </si>
 </sst>
 </file>
@@ -881,22 +881,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -917,46 +941,22 @@
     <xf numFmtId="0" fontId="7" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -1346,8 +1346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12CB4148-414F-422C-94F5-AFDA695DCD79}">
   <dimension ref="A1:I257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A217" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I235" sqref="I235"/>
+    <sheetView tabSelected="1" topLeftCell="A184" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L201" sqref="L201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1378,7 +1378,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B2" s="33">
         <v>0</v>
@@ -1386,7 +1386,7 @@
       <c r="C2" s="54"/>
       <c r="D2" s="54"/>
       <c r="E2" s="54"/>
-      <c r="F2" s="80" t="s">
+      <c r="F2" s="55" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="54"/>
@@ -1397,7 +1397,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B3" s="33">
         <v>1</v>
@@ -1405,14 +1405,14 @@
       <c r="C3" s="54"/>
       <c r="D3" s="54"/>
       <c r="E3" s="54"/>
-      <c r="F3" s="80"/>
+      <c r="F3" s="55"/>
       <c r="G3" s="54"/>
       <c r="H3" s="54"/>
       <c r="I3" s="43"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B4" s="33">
         <v>2</v>
@@ -1420,14 +1420,14 @@
       <c r="C4" s="54"/>
       <c r="D4" s="54"/>
       <c r="E4" s="54"/>
-      <c r="F4" s="80"/>
+      <c r="F4" s="55"/>
       <c r="G4" s="54"/>
       <c r="H4" s="54"/>
       <c r="I4" s="43"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B5" s="33">
         <v>3</v>
@@ -1435,14 +1435,14 @@
       <c r="C5" s="54"/>
       <c r="D5" s="54"/>
       <c r="E5" s="54"/>
-      <c r="F5" s="80"/>
+      <c r="F5" s="55"/>
       <c r="G5" s="54"/>
       <c r="H5" s="54"/>
       <c r="I5" s="43"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B6" s="33">
         <v>4</v>
@@ -1450,14 +1450,14 @@
       <c r="C6" s="54"/>
       <c r="D6" s="54"/>
       <c r="E6" s="54"/>
-      <c r="F6" s="80"/>
+      <c r="F6" s="55"/>
       <c r="G6" s="54"/>
       <c r="H6" s="54"/>
       <c r="I6" s="43"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B7" s="33">
         <v>5</v>
@@ -1465,14 +1465,14 @@
       <c r="C7" s="54"/>
       <c r="D7" s="54"/>
       <c r="E7" s="54"/>
-      <c r="F7" s="80"/>
+      <c r="F7" s="55"/>
       <c r="G7" s="54"/>
       <c r="H7" s="54"/>
       <c r="I7" s="43"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B8" s="33">
         <v>6</v>
@@ -1480,14 +1480,14 @@
       <c r="C8" s="54"/>
       <c r="D8" s="54"/>
       <c r="E8" s="54"/>
-      <c r="F8" s="80"/>
+      <c r="F8" s="55"/>
       <c r="G8" s="54"/>
       <c r="H8" s="54"/>
       <c r="I8" s="43"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B9" s="33">
         <v>7</v>
@@ -1495,14 +1495,14 @@
       <c r="C9" s="54"/>
       <c r="D9" s="54"/>
       <c r="E9" s="54"/>
-      <c r="F9" s="80"/>
+      <c r="F9" s="55"/>
       <c r="G9" s="54"/>
       <c r="H9" s="54"/>
       <c r="I9" s="43"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B10" s="33">
         <v>8</v>
@@ -1510,14 +1510,14 @@
       <c r="C10" s="54"/>
       <c r="D10" s="54"/>
       <c r="E10" s="54"/>
-      <c r="F10" s="80"/>
+      <c r="F10" s="55"/>
       <c r="G10" s="54"/>
       <c r="H10" s="54"/>
       <c r="I10" s="43"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B11" s="33">
         <v>9</v>
@@ -1525,14 +1525,14 @@
       <c r="C11" s="54"/>
       <c r="D11" s="54"/>
       <c r="E11" s="54"/>
-      <c r="F11" s="80"/>
+      <c r="F11" s="55"/>
       <c r="G11" s="54"/>
       <c r="H11" s="54"/>
       <c r="I11" s="43"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B12" s="33">
         <v>10</v>
@@ -1540,14 +1540,14 @@
       <c r="C12" s="54"/>
       <c r="D12" s="54"/>
       <c r="E12" s="54"/>
-      <c r="F12" s="80"/>
+      <c r="F12" s="55"/>
       <c r="G12" s="54"/>
       <c r="H12" s="54"/>
       <c r="I12" s="43"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B13" s="33">
         <v>11</v>
@@ -1555,14 +1555,14 @@
       <c r="C13" s="54"/>
       <c r="D13" s="54"/>
       <c r="E13" s="54"/>
-      <c r="F13" s="80"/>
+      <c r="F13" s="55"/>
       <c r="G13" s="54"/>
       <c r="H13" s="54"/>
       <c r="I13" s="43"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B14" s="33">
         <v>12</v>
@@ -1570,14 +1570,14 @@
       <c r="C14" s="54"/>
       <c r="D14" s="54"/>
       <c r="E14" s="54"/>
-      <c r="F14" s="80"/>
+      <c r="F14" s="55"/>
       <c r="G14" s="54"/>
       <c r="H14" s="54"/>
       <c r="I14" s="43"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B15" s="33">
         <v>13</v>
@@ -1585,14 +1585,14 @@
       <c r="C15" s="54"/>
       <c r="D15" s="54"/>
       <c r="E15" s="54"/>
-      <c r="F15" s="80"/>
+      <c r="F15" s="55"/>
       <c r="G15" s="54"/>
       <c r="H15" s="54"/>
       <c r="I15" s="43"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B16" s="33">
         <v>14</v>
@@ -1600,14 +1600,14 @@
       <c r="C16" s="54"/>
       <c r="D16" s="54"/>
       <c r="E16" s="54"/>
-      <c r="F16" s="80"/>
+      <c r="F16" s="55"/>
       <c r="G16" s="54"/>
       <c r="H16" s="54"/>
       <c r="I16" s="43"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B17" s="33">
         <v>15</v>
@@ -1615,14 +1615,14 @@
       <c r="C17" s="54"/>
       <c r="D17" s="54"/>
       <c r="E17" s="54"/>
-      <c r="F17" s="80"/>
+      <c r="F17" s="55"/>
       <c r="G17" s="54"/>
       <c r="H17" s="54"/>
       <c r="I17" s="43"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B18" s="33">
         <v>16</v>
@@ -1630,14 +1630,14 @@
       <c r="C18" s="54"/>
       <c r="D18" s="54"/>
       <c r="E18" s="54"/>
-      <c r="F18" s="80"/>
+      <c r="F18" s="55"/>
       <c r="G18" s="54"/>
       <c r="H18" s="54"/>
       <c r="I18" s="43"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B19" s="33">
         <v>17</v>
@@ -1645,14 +1645,14 @@
       <c r="C19" s="54"/>
       <c r="D19" s="54"/>
       <c r="E19" s="54"/>
-      <c r="F19" s="80"/>
+      <c r="F19" s="55"/>
       <c r="G19" s="54"/>
       <c r="H19" s="54"/>
       <c r="I19" s="43"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B20" s="33">
         <v>18</v>
@@ -1660,14 +1660,14 @@
       <c r="C20" s="54"/>
       <c r="D20" s="54"/>
       <c r="E20" s="54"/>
-      <c r="F20" s="80"/>
+      <c r="F20" s="55"/>
       <c r="G20" s="54"/>
       <c r="H20" s="54"/>
       <c r="I20" s="43"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B21" s="33">
         <v>19</v>
@@ -1675,14 +1675,14 @@
       <c r="C21" s="54"/>
       <c r="D21" s="54"/>
       <c r="E21" s="54"/>
-      <c r="F21" s="80"/>
+      <c r="F21" s="55"/>
       <c r="G21" s="54"/>
       <c r="H21" s="54"/>
       <c r="I21" s="43"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B22" s="33">
         <v>20</v>
@@ -1690,14 +1690,14 @@
       <c r="C22" s="54"/>
       <c r="D22" s="54"/>
       <c r="E22" s="54"/>
-      <c r="F22" s="80"/>
+      <c r="F22" s="55"/>
       <c r="G22" s="54"/>
       <c r="H22" s="54"/>
       <c r="I22" s="43"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B23" s="33">
         <v>21</v>
@@ -1705,14 +1705,14 @@
       <c r="C23" s="54"/>
       <c r="D23" s="54"/>
       <c r="E23" s="54"/>
-      <c r="F23" s="80"/>
+      <c r="F23" s="55"/>
       <c r="G23" s="54"/>
       <c r="H23" s="54"/>
       <c r="I23" s="43"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B24" s="33">
         <v>22</v>
@@ -1720,14 +1720,14 @@
       <c r="C24" s="54"/>
       <c r="D24" s="54"/>
       <c r="E24" s="54"/>
-      <c r="F24" s="80"/>
+      <c r="F24" s="55"/>
       <c r="G24" s="54"/>
       <c r="H24" s="54"/>
       <c r="I24" s="43"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B25" s="33">
         <v>23</v>
@@ -1735,14 +1735,14 @@
       <c r="C25" s="54"/>
       <c r="D25" s="54"/>
       <c r="E25" s="54"/>
-      <c r="F25" s="80"/>
+      <c r="F25" s="55"/>
       <c r="G25" s="54"/>
       <c r="H25" s="54"/>
       <c r="I25" s="43"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B26" s="33">
         <v>24</v>
@@ -1750,14 +1750,14 @@
       <c r="C26" s="54"/>
       <c r="D26" s="54"/>
       <c r="E26" s="54"/>
-      <c r="F26" s="80"/>
+      <c r="F26" s="55"/>
       <c r="G26" s="54"/>
       <c r="H26" s="54"/>
       <c r="I26" s="43"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B27" s="33">
         <v>25</v>
@@ -1765,14 +1765,14 @@
       <c r="C27" s="54"/>
       <c r="D27" s="54"/>
       <c r="E27" s="54"/>
-      <c r="F27" s="80"/>
+      <c r="F27" s="55"/>
       <c r="G27" s="54"/>
       <c r="H27" s="54"/>
       <c r="I27" s="43"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B28" s="33">
         <v>26</v>
@@ -1780,14 +1780,14 @@
       <c r="C28" s="54"/>
       <c r="D28" s="54"/>
       <c r="E28" s="54"/>
-      <c r="F28" s="80"/>
+      <c r="F28" s="55"/>
       <c r="G28" s="54"/>
       <c r="H28" s="54"/>
       <c r="I28" s="43"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B29" s="33">
         <v>27</v>
@@ -1795,14 +1795,16 @@
       <c r="C29" s="54"/>
       <c r="D29" s="54"/>
       <c r="E29" s="54"/>
-      <c r="F29" s="80"/>
+      <c r="F29" s="55"/>
       <c r="G29" s="54"/>
       <c r="H29" s="54"/>
-      <c r="I29" s="43"/>
+      <c r="I29" s="43" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B30" s="33">
         <v>28</v>
@@ -1810,14 +1812,16 @@
       <c r="C30" s="54"/>
       <c r="D30" s="54"/>
       <c r="E30" s="54"/>
-      <c r="F30" s="80"/>
+      <c r="F30" s="55"/>
       <c r="G30" s="54"/>
       <c r="H30" s="54"/>
-      <c r="I30" s="43"/>
+      <c r="I30" s="43" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B31" s="33">
         <v>29</v>
@@ -1825,14 +1829,16 @@
       <c r="C31" s="54"/>
       <c r="D31" s="54"/>
       <c r="E31" s="54"/>
-      <c r="F31" s="80"/>
+      <c r="F31" s="55"/>
       <c r="G31" s="54"/>
       <c r="H31" s="54"/>
-      <c r="I31" s="43"/>
+      <c r="I31" s="43" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B32" s="33">
         <v>30</v>
@@ -1840,7 +1846,7 @@
       <c r="C32" s="54"/>
       <c r="D32" s="54"/>
       <c r="E32" s="54"/>
-      <c r="F32" s="80"/>
+      <c r="F32" s="55"/>
       <c r="G32" s="54"/>
       <c r="H32" s="54"/>
       <c r="I32" s="43" t="s">
@@ -1849,7 +1855,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B33" s="33">
         <v>31</v>
@@ -1857,7 +1863,7 @@
       <c r="C33" s="54"/>
       <c r="D33" s="54"/>
       <c r="E33" s="54"/>
-      <c r="F33" s="80"/>
+      <c r="F33" s="55"/>
       <c r="G33" s="54"/>
       <c r="H33" s="54"/>
       <c r="I33" s="43" t="s">
@@ -1866,14 +1872,14 @@
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B34" s="40">
         <v>32</v>
       </c>
       <c r="C34" s="54"/>
       <c r="D34" s="54"/>
-      <c r="E34" s="79" t="s">
+      <c r="E34" s="58" t="s">
         <v>16</v>
       </c>
       <c r="F34" s="54"/>
@@ -1885,14 +1891,14 @@
     </row>
     <row r="35" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B35" s="40">
         <v>33</v>
       </c>
       <c r="C35" s="54"/>
       <c r="D35" s="54"/>
-      <c r="E35" s="79"/>
+      <c r="E35" s="58"/>
       <c r="F35" s="54"/>
       <c r="G35" s="54"/>
       <c r="H35" s="54"/>
@@ -1900,14 +1906,14 @@
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B36" s="40">
         <v>34</v>
       </c>
       <c r="C36" s="54"/>
       <c r="D36" s="54"/>
-      <c r="E36" s="79"/>
+      <c r="E36" s="58"/>
       <c r="F36" s="54"/>
       <c r="G36" s="54"/>
       <c r="H36" s="54"/>
@@ -1915,14 +1921,14 @@
     </row>
     <row r="37" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B37" s="40">
         <v>35</v>
       </c>
       <c r="C37" s="54"/>
       <c r="D37" s="54"/>
-      <c r="E37" s="79"/>
+      <c r="E37" s="58"/>
       <c r="F37" s="54"/>
       <c r="G37" s="54"/>
       <c r="H37" s="54"/>
@@ -1930,14 +1936,14 @@
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B38" s="40">
         <v>36</v>
       </c>
       <c r="C38" s="54"/>
       <c r="D38" s="54"/>
-      <c r="E38" s="79"/>
+      <c r="E38" s="58"/>
       <c r="F38" s="54"/>
       <c r="G38" s="54"/>
       <c r="H38" s="54"/>
@@ -1945,14 +1951,14 @@
     </row>
     <row r="39" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B39" s="40">
         <v>37</v>
       </c>
       <c r="C39" s="54"/>
       <c r="D39" s="54"/>
-      <c r="E39" s="79"/>
+      <c r="E39" s="58"/>
       <c r="F39" s="54"/>
       <c r="G39" s="54"/>
       <c r="H39" s="54"/>
@@ -1960,14 +1966,14 @@
     </row>
     <row r="40" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B40" s="40">
         <v>38</v>
       </c>
       <c r="C40" s="54"/>
       <c r="D40" s="54"/>
-      <c r="E40" s="79"/>
+      <c r="E40" s="58"/>
       <c r="F40" s="54"/>
       <c r="G40" s="54"/>
       <c r="H40" s="54"/>
@@ -1975,14 +1981,14 @@
     </row>
     <row r="41" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B41" s="40">
         <v>39</v>
       </c>
       <c r="C41" s="54"/>
       <c r="D41" s="54"/>
-      <c r="E41" s="79"/>
+      <c r="E41" s="58"/>
       <c r="F41" s="54"/>
       <c r="G41" s="54"/>
       <c r="H41" s="54"/>
@@ -1990,14 +1996,14 @@
     </row>
     <row r="42" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B42" s="40">
         <v>40</v>
       </c>
       <c r="C42" s="54"/>
       <c r="D42" s="54"/>
-      <c r="E42" s="79"/>
+      <c r="E42" s="58"/>
       <c r="F42" s="54"/>
       <c r="G42" s="54"/>
       <c r="H42" s="54"/>
@@ -2005,14 +2011,14 @@
     </row>
     <row r="43" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B43" s="40">
         <v>41</v>
       </c>
       <c r="C43" s="54"/>
       <c r="D43" s="54"/>
-      <c r="E43" s="79"/>
+      <c r="E43" s="58"/>
       <c r="F43" s="54"/>
       <c r="G43" s="54"/>
       <c r="H43" s="54"/>
@@ -2020,14 +2026,14 @@
     </row>
     <row r="44" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B44" s="40">
         <v>42</v>
       </c>
       <c r="C44" s="54"/>
       <c r="D44" s="54"/>
-      <c r="E44" s="79"/>
+      <c r="E44" s="58"/>
       <c r="F44" s="54"/>
       <c r="G44" s="54"/>
       <c r="H44" s="54"/>
@@ -2035,14 +2041,14 @@
     </row>
     <row r="45" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B45" s="40">
         <v>43</v>
       </c>
       <c r="C45" s="54"/>
       <c r="D45" s="54"/>
-      <c r="E45" s="79"/>
+      <c r="E45" s="58"/>
       <c r="F45" s="54"/>
       <c r="G45" s="54"/>
       <c r="H45" s="54"/>
@@ -2050,14 +2056,14 @@
     </row>
     <row r="46" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B46" s="40">
         <v>44</v>
       </c>
       <c r="C46" s="54"/>
       <c r="D46" s="54"/>
-      <c r="E46" s="79"/>
+      <c r="E46" s="58"/>
       <c r="F46" s="54"/>
       <c r="G46" s="54"/>
       <c r="H46" s="54"/>
@@ -2065,14 +2071,14 @@
     </row>
     <row r="47" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B47" s="40">
         <v>45</v>
       </c>
       <c r="C47" s="54"/>
       <c r="D47" s="54"/>
-      <c r="E47" s="79"/>
+      <c r="E47" s="58"/>
       <c r="F47" s="54"/>
       <c r="G47" s="54"/>
       <c r="H47" s="54"/>
@@ -2080,14 +2086,14 @@
     </row>
     <row r="48" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B48" s="40">
         <v>46</v>
       </c>
       <c r="C48" s="54"/>
       <c r="D48" s="54"/>
-      <c r="E48" s="79"/>
+      <c r="E48" s="58"/>
       <c r="F48" s="54"/>
       <c r="G48" s="54"/>
       <c r="H48" s="54"/>
@@ -2097,14 +2103,14 @@
     </row>
     <row r="49" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B49" s="40">
         <v>47</v>
       </c>
       <c r="C49" s="54"/>
       <c r="D49" s="54"/>
-      <c r="E49" s="79"/>
+      <c r="E49" s="58"/>
       <c r="F49" s="54"/>
       <c r="G49" s="54"/>
       <c r="H49" s="54"/>
@@ -2114,14 +2120,14 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B50" s="40">
         <v>48</v>
       </c>
       <c r="C50" s="54"/>
       <c r="D50" s="54"/>
-      <c r="E50" s="77" t="s">
+      <c r="E50" s="56" t="s">
         <v>17</v>
       </c>
       <c r="F50" s="54"/>
@@ -2133,14 +2139,14 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B51" s="40">
         <v>49</v>
       </c>
       <c r="C51" s="54"/>
       <c r="D51" s="54"/>
-      <c r="E51" s="77"/>
+      <c r="E51" s="56"/>
       <c r="F51" s="54"/>
       <c r="G51" s="54"/>
       <c r="H51" s="54"/>
@@ -2148,14 +2154,14 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B52" s="40">
         <v>50</v>
       </c>
       <c r="C52" s="54"/>
       <c r="D52" s="54"/>
-      <c r="E52" s="77"/>
+      <c r="E52" s="56"/>
       <c r="F52" s="54"/>
       <c r="G52" s="54"/>
       <c r="H52" s="54"/>
@@ -2163,14 +2169,14 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B53" s="40">
         <v>51</v>
       </c>
       <c r="C53" s="54"/>
       <c r="D53" s="54"/>
-      <c r="E53" s="77"/>
+      <c r="E53" s="56"/>
       <c r="F53" s="54"/>
       <c r="G53" s="54"/>
       <c r="H53" s="54"/>
@@ -2178,14 +2184,14 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B54" s="40">
         <v>52</v>
       </c>
       <c r="C54" s="54"/>
       <c r="D54" s="54"/>
-      <c r="E54" s="77"/>
+      <c r="E54" s="56"/>
       <c r="F54" s="54"/>
       <c r="G54" s="54"/>
       <c r="H54" s="54"/>
@@ -2193,14 +2199,14 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B55" s="40">
         <v>53</v>
       </c>
       <c r="C55" s="54"/>
       <c r="D55" s="54"/>
-      <c r="E55" s="77"/>
+      <c r="E55" s="56"/>
       <c r="F55" s="54"/>
       <c r="G55" s="54"/>
       <c r="H55" s="54"/>
@@ -2208,14 +2214,14 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B56" s="40">
         <v>54</v>
       </c>
       <c r="C56" s="54"/>
       <c r="D56" s="54"/>
-      <c r="E56" s="77"/>
+      <c r="E56" s="56"/>
       <c r="F56" s="54"/>
       <c r="G56" s="54"/>
       <c r="H56" s="54"/>
@@ -2223,14 +2229,14 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B57" s="40">
         <v>55</v>
       </c>
       <c r="C57" s="54"/>
       <c r="D57" s="54"/>
-      <c r="E57" s="77"/>
+      <c r="E57" s="56"/>
       <c r="F57" s="54"/>
       <c r="G57" s="54"/>
       <c r="H57" s="54"/>
@@ -2238,14 +2244,14 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B58" s="40">
         <v>56</v>
       </c>
       <c r="C58" s="54"/>
       <c r="D58" s="54"/>
-      <c r="E58" s="77"/>
+      <c r="E58" s="56"/>
       <c r="F58" s="54"/>
       <c r="G58" s="54"/>
       <c r="H58" s="54"/>
@@ -2253,14 +2259,14 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B59" s="40">
         <v>57</v>
       </c>
       <c r="C59" s="54"/>
       <c r="D59" s="54"/>
-      <c r="E59" s="77"/>
+      <c r="E59" s="56"/>
       <c r="F59" s="54"/>
       <c r="G59" s="54"/>
       <c r="H59" s="54"/>
@@ -2268,14 +2274,14 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B60" s="40">
         <v>58</v>
       </c>
       <c r="C60" s="54"/>
       <c r="D60" s="54"/>
-      <c r="E60" s="77"/>
+      <c r="E60" s="56"/>
       <c r="F60" s="54"/>
       <c r="G60" s="54"/>
       <c r="H60" s="54"/>
@@ -2283,14 +2289,14 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B61" s="40">
         <v>59</v>
       </c>
       <c r="C61" s="54"/>
       <c r="D61" s="54"/>
-      <c r="E61" s="77"/>
+      <c r="E61" s="56"/>
       <c r="F61" s="54"/>
       <c r="G61" s="54"/>
       <c r="H61" s="54"/>
@@ -2298,14 +2304,14 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B62" s="40">
         <v>60</v>
       </c>
       <c r="C62" s="54"/>
       <c r="D62" s="54"/>
-      <c r="E62" s="77"/>
+      <c r="E62" s="56"/>
       <c r="F62" s="54"/>
       <c r="G62" s="54"/>
       <c r="H62" s="54"/>
@@ -2313,14 +2319,14 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B63" s="40">
         <v>61</v>
       </c>
       <c r="C63" s="54"/>
       <c r="D63" s="54"/>
-      <c r="E63" s="77"/>
+      <c r="E63" s="56"/>
       <c r="F63" s="54"/>
       <c r="G63" s="54"/>
       <c r="H63" s="54"/>
@@ -2328,14 +2334,14 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B64" s="40">
         <v>62</v>
       </c>
       <c r="C64" s="54"/>
       <c r="D64" s="54"/>
-      <c r="E64" s="77"/>
+      <c r="E64" s="56"/>
       <c r="F64" s="54"/>
       <c r="G64" s="54"/>
       <c r="H64" s="54"/>
@@ -2345,14 +2351,14 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B65" s="40">
         <v>63</v>
       </c>
       <c r="C65" s="54"/>
       <c r="D65" s="54"/>
-      <c r="E65" s="77"/>
+      <c r="E65" s="56"/>
       <c r="F65" s="54"/>
       <c r="G65" s="54"/>
       <c r="H65" s="54"/>
@@ -2362,14 +2368,14 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B66" s="41">
         <v>64</v>
       </c>
       <c r="C66" s="54"/>
       <c r="D66" s="54"/>
-      <c r="E66" s="78" t="s">
+      <c r="E66" s="57" t="s">
         <v>18</v>
       </c>
       <c r="F66" s="54"/>
@@ -2381,14 +2387,14 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B67" s="41">
         <v>65</v>
       </c>
       <c r="C67" s="54"/>
       <c r="D67" s="54"/>
-      <c r="E67" s="78"/>
+      <c r="E67" s="57"/>
       <c r="F67" s="54"/>
       <c r="G67" s="54"/>
       <c r="H67" s="54"/>
@@ -2396,14 +2402,14 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B68" s="41">
         <v>66</v>
       </c>
       <c r="C68" s="54"/>
       <c r="D68" s="54"/>
-      <c r="E68" s="78"/>
+      <c r="E68" s="57"/>
       <c r="F68" s="54"/>
       <c r="G68" s="54"/>
       <c r="H68" s="54"/>
@@ -2411,14 +2417,14 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B69" s="41">
         <v>67</v>
       </c>
       <c r="C69" s="54"/>
       <c r="D69" s="54"/>
-      <c r="E69" s="78"/>
+      <c r="E69" s="57"/>
       <c r="F69" s="54"/>
       <c r="G69" s="54"/>
       <c r="H69" s="54"/>
@@ -2426,14 +2432,14 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B70" s="41">
         <v>68</v>
       </c>
       <c r="C70" s="54"/>
       <c r="D70" s="54"/>
-      <c r="E70" s="78"/>
+      <c r="E70" s="57"/>
       <c r="F70" s="54"/>
       <c r="G70" s="54"/>
       <c r="H70" s="54"/>
@@ -2441,14 +2447,14 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B71" s="41">
         <v>69</v>
       </c>
       <c r="C71" s="54"/>
       <c r="D71" s="54"/>
-      <c r="E71" s="78"/>
+      <c r="E71" s="57"/>
       <c r="F71" s="54"/>
       <c r="G71" s="54"/>
       <c r="H71" s="54"/>
@@ -2456,14 +2462,14 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B72" s="41">
         <v>70</v>
       </c>
       <c r="C72" s="54"/>
       <c r="D72" s="54"/>
-      <c r="E72" s="78"/>
+      <c r="E72" s="57"/>
       <c r="F72" s="54"/>
       <c r="G72" s="54"/>
       <c r="H72" s="54"/>
@@ -2471,14 +2477,14 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B73" s="41">
         <v>71</v>
       </c>
       <c r="C73" s="54"/>
       <c r="D73" s="54"/>
-      <c r="E73" s="78"/>
+      <c r="E73" s="57"/>
       <c r="F73" s="54"/>
       <c r="G73" s="54"/>
       <c r="H73" s="54"/>
@@ -2486,14 +2492,14 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B74" s="41">
         <v>72</v>
       </c>
       <c r="C74" s="54"/>
       <c r="D74" s="54"/>
-      <c r="E74" s="78"/>
+      <c r="E74" s="57"/>
       <c r="F74" s="54"/>
       <c r="G74" s="54"/>
       <c r="H74" s="54"/>
@@ -2501,14 +2507,14 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B75" s="41">
         <v>73</v>
       </c>
       <c r="C75" s="54"/>
       <c r="D75" s="54"/>
-      <c r="E75" s="78"/>
+      <c r="E75" s="57"/>
       <c r="F75" s="54"/>
       <c r="G75" s="54"/>
       <c r="H75" s="54"/>
@@ -2516,14 +2522,14 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B76" s="41">
         <v>74</v>
       </c>
       <c r="C76" s="54"/>
       <c r="D76" s="54"/>
-      <c r="E76" s="78"/>
+      <c r="E76" s="57"/>
       <c r="F76" s="54"/>
       <c r="G76" s="54"/>
       <c r="H76" s="54"/>
@@ -2531,14 +2537,14 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B77" s="41">
         <v>75</v>
       </c>
       <c r="C77" s="54"/>
       <c r="D77" s="54"/>
-      <c r="E77" s="78"/>
+      <c r="E77" s="57"/>
       <c r="F77" s="54"/>
       <c r="G77" s="54"/>
       <c r="H77" s="54"/>
@@ -2546,14 +2552,14 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B78" s="41">
         <v>76</v>
       </c>
       <c r="C78" s="54"/>
       <c r="D78" s="54"/>
-      <c r="E78" s="78"/>
+      <c r="E78" s="57"/>
       <c r="F78" s="54"/>
       <c r="G78" s="54"/>
       <c r="H78" s="54"/>
@@ -2561,14 +2567,14 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B79" s="41">
         <v>77</v>
       </c>
       <c r="C79" s="54"/>
       <c r="D79" s="54"/>
-      <c r="E79" s="78"/>
+      <c r="E79" s="57"/>
       <c r="F79" s="54"/>
       <c r="G79" s="54"/>
       <c r="H79" s="54"/>
@@ -2576,14 +2582,14 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B80" s="41">
         <v>78</v>
       </c>
       <c r="C80" s="54"/>
       <c r="D80" s="54"/>
-      <c r="E80" s="78"/>
+      <c r="E80" s="57"/>
       <c r="F80" s="54"/>
       <c r="G80" s="54"/>
       <c r="H80" s="54"/>
@@ -2593,14 +2599,14 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B81" s="41">
         <v>79</v>
       </c>
       <c r="C81" s="54"/>
       <c r="D81" s="54"/>
-      <c r="E81" s="78"/>
+      <c r="E81" s="57"/>
       <c r="F81" s="54"/>
       <c r="G81" s="54"/>
       <c r="H81" s="54"/>
@@ -2610,14 +2616,14 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B82" s="41">
         <v>80</v>
       </c>
       <c r="C82" s="54"/>
       <c r="D82" s="54"/>
-      <c r="E82" s="76" t="s">
+      <c r="E82" s="60" t="s">
         <v>19</v>
       </c>
       <c r="F82" s="54"/>
@@ -2629,14 +2635,14 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B83" s="41">
         <v>81</v>
       </c>
       <c r="C83" s="54"/>
       <c r="D83" s="54"/>
-      <c r="E83" s="76"/>
+      <c r="E83" s="60"/>
       <c r="F83" s="54"/>
       <c r="G83" s="54"/>
       <c r="H83" s="54"/>
@@ -2644,14 +2650,14 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B84" s="41">
         <v>82</v>
       </c>
       <c r="C84" s="54"/>
       <c r="D84" s="54"/>
-      <c r="E84" s="76"/>
+      <c r="E84" s="60"/>
       <c r="F84" s="54"/>
       <c r="G84" s="54"/>
       <c r="H84" s="54"/>
@@ -2659,14 +2665,14 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B85" s="41">
         <v>83</v>
       </c>
       <c r="C85" s="54"/>
       <c r="D85" s="54"/>
-      <c r="E85" s="76"/>
+      <c r="E85" s="60"/>
       <c r="F85" s="54"/>
       <c r="G85" s="54"/>
       <c r="H85" s="54"/>
@@ -2674,14 +2680,14 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B86" s="41">
         <v>84</v>
       </c>
       <c r="C86" s="54"/>
       <c r="D86" s="54"/>
-      <c r="E86" s="76"/>
+      <c r="E86" s="60"/>
       <c r="F86" s="54"/>
       <c r="G86" s="54"/>
       <c r="H86" s="54"/>
@@ -2689,14 +2695,14 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B87" s="41">
         <v>85</v>
       </c>
       <c r="C87" s="54"/>
       <c r="D87" s="54"/>
-      <c r="E87" s="76"/>
+      <c r="E87" s="60"/>
       <c r="F87" s="54"/>
       <c r="G87" s="54"/>
       <c r="H87" s="54"/>
@@ -2704,14 +2710,14 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B88" s="41">
         <v>86</v>
       </c>
       <c r="C88" s="54"/>
       <c r="D88" s="54"/>
-      <c r="E88" s="76"/>
+      <c r="E88" s="60"/>
       <c r="F88" s="54"/>
       <c r="G88" s="54"/>
       <c r="H88" s="54"/>
@@ -2719,14 +2725,14 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B89" s="41">
         <v>87</v>
       </c>
       <c r="C89" s="54"/>
       <c r="D89" s="54"/>
-      <c r="E89" s="76"/>
+      <c r="E89" s="60"/>
       <c r="F89" s="54"/>
       <c r="G89" s="54"/>
       <c r="H89" s="54"/>
@@ -2734,14 +2740,14 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B90" s="41">
         <v>88</v>
       </c>
       <c r="C90" s="54"/>
       <c r="D90" s="54"/>
-      <c r="E90" s="76"/>
+      <c r="E90" s="60"/>
       <c r="F90" s="54"/>
       <c r="G90" s="54"/>
       <c r="H90" s="54"/>
@@ -2749,14 +2755,14 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B91" s="41">
         <v>89</v>
       </c>
       <c r="C91" s="54"/>
       <c r="D91" s="54"/>
-      <c r="E91" s="76"/>
+      <c r="E91" s="60"/>
       <c r="F91" s="54"/>
       <c r="G91" s="54"/>
       <c r="H91" s="54"/>
@@ -2764,14 +2770,14 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B92" s="41">
         <v>90</v>
       </c>
       <c r="C92" s="54"/>
       <c r="D92" s="54"/>
-      <c r="E92" s="76"/>
+      <c r="E92" s="60"/>
       <c r="F92" s="54"/>
       <c r="G92" s="54"/>
       <c r="H92" s="54"/>
@@ -2779,14 +2785,14 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B93" s="41">
         <v>91</v>
       </c>
       <c r="C93" s="54"/>
       <c r="D93" s="54"/>
-      <c r="E93" s="76"/>
+      <c r="E93" s="60"/>
       <c r="F93" s="54"/>
       <c r="G93" s="54"/>
       <c r="H93" s="54"/>
@@ -2794,14 +2800,14 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B94" s="41">
         <v>92</v>
       </c>
       <c r="C94" s="54"/>
       <c r="D94" s="54"/>
-      <c r="E94" s="76"/>
+      <c r="E94" s="60"/>
       <c r="F94" s="54"/>
       <c r="G94" s="54"/>
       <c r="H94" s="54"/>
@@ -2809,14 +2815,14 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B95" s="41">
         <v>93</v>
       </c>
       <c r="C95" s="54"/>
       <c r="D95" s="54"/>
-      <c r="E95" s="76"/>
+      <c r="E95" s="60"/>
       <c r="F95" s="54"/>
       <c r="G95" s="54"/>
       <c r="H95" s="54"/>
@@ -2824,14 +2830,14 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B96" s="41">
         <v>94</v>
       </c>
       <c r="C96" s="54"/>
       <c r="D96" s="54"/>
-      <c r="E96" s="76"/>
+      <c r="E96" s="60"/>
       <c r="F96" s="54"/>
       <c r="G96" s="54"/>
       <c r="H96" s="54"/>
@@ -2841,14 +2847,14 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B97" s="41">
         <v>95</v>
       </c>
       <c r="C97" s="54"/>
       <c r="D97" s="54"/>
-      <c r="E97" s="76"/>
+      <c r="E97" s="60"/>
       <c r="F97" s="54"/>
       <c r="G97" s="54"/>
       <c r="H97" s="54"/>
@@ -2858,14 +2864,14 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B98" s="42">
         <v>96</v>
       </c>
       <c r="C98" s="54"/>
       <c r="D98" s="54"/>
-      <c r="E98" s="75" t="s">
+      <c r="E98" s="59" t="s">
         <v>20</v>
       </c>
       <c r="F98" s="54"/>
@@ -2877,14 +2883,14 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B99" s="42">
         <v>97</v>
       </c>
       <c r="C99" s="54"/>
       <c r="D99" s="54"/>
-      <c r="E99" s="75"/>
+      <c r="E99" s="59"/>
       <c r="F99" s="54"/>
       <c r="G99" s="54"/>
       <c r="H99" s="54"/>
@@ -2892,14 +2898,14 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B100" s="42">
         <v>98</v>
       </c>
       <c r="C100" s="54"/>
       <c r="D100" s="54"/>
-      <c r="E100" s="75"/>
+      <c r="E100" s="59"/>
       <c r="F100" s="54"/>
       <c r="G100" s="54"/>
       <c r="H100" s="54"/>
@@ -2907,14 +2913,14 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B101" s="42">
         <v>99</v>
       </c>
       <c r="C101" s="54"/>
       <c r="D101" s="54"/>
-      <c r="E101" s="75"/>
+      <c r="E101" s="59"/>
       <c r="F101" s="54"/>
       <c r="G101" s="54"/>
       <c r="H101" s="54"/>
@@ -2922,14 +2928,14 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B102" s="42">
         <v>100</v>
       </c>
       <c r="C102" s="54"/>
       <c r="D102" s="54"/>
-      <c r="E102" s="75"/>
+      <c r="E102" s="59"/>
       <c r="F102" s="54"/>
       <c r="G102" s="54"/>
       <c r="H102" s="54"/>
@@ -2937,14 +2943,14 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B103" s="42">
         <v>101</v>
       </c>
       <c r="C103" s="54"/>
       <c r="D103" s="54"/>
-      <c r="E103" s="75"/>
+      <c r="E103" s="59"/>
       <c r="F103" s="54"/>
       <c r="G103" s="54"/>
       <c r="H103" s="54"/>
@@ -2952,14 +2958,14 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B104" s="42">
         <v>102</v>
       </c>
       <c r="C104" s="54"/>
       <c r="D104" s="54"/>
-      <c r="E104" s="75"/>
+      <c r="E104" s="59"/>
       <c r="F104" s="54"/>
       <c r="G104" s="54"/>
       <c r="H104" s="54"/>
@@ -2967,14 +2973,14 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B105" s="42">
         <v>103</v>
       </c>
       <c r="C105" s="54"/>
       <c r="D105" s="54"/>
-      <c r="E105" s="75"/>
+      <c r="E105" s="59"/>
       <c r="F105" s="54"/>
       <c r="G105" s="54"/>
       <c r="H105" s="54"/>
@@ -2982,14 +2988,14 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B106" s="42">
         <v>104</v>
       </c>
       <c r="C106" s="54"/>
       <c r="D106" s="54"/>
-      <c r="E106" s="75"/>
+      <c r="E106" s="59"/>
       <c r="F106" s="54"/>
       <c r="G106" s="54"/>
       <c r="H106" s="54"/>
@@ -2997,14 +3003,14 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B107" s="42">
         <v>105</v>
       </c>
       <c r="C107" s="54"/>
       <c r="D107" s="54"/>
-      <c r="E107" s="75"/>
+      <c r="E107" s="59"/>
       <c r="F107" s="54"/>
       <c r="G107" s="54"/>
       <c r="H107" s="54"/>
@@ -3012,14 +3018,14 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B108" s="42">
         <v>106</v>
       </c>
       <c r="C108" s="54"/>
       <c r="D108" s="54"/>
-      <c r="E108" s="75"/>
+      <c r="E108" s="59"/>
       <c r="F108" s="54"/>
       <c r="G108" s="54"/>
       <c r="H108" s="54"/>
@@ -3027,14 +3033,14 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B109" s="42">
         <v>107</v>
       </c>
       <c r="C109" s="54"/>
       <c r="D109" s="54"/>
-      <c r="E109" s="75"/>
+      <c r="E109" s="59"/>
       <c r="F109" s="54"/>
       <c r="G109" s="54"/>
       <c r="H109" s="54"/>
@@ -3042,14 +3048,14 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B110" s="42">
         <v>108</v>
       </c>
       <c r="C110" s="54"/>
       <c r="D110" s="54"/>
-      <c r="E110" s="75"/>
+      <c r="E110" s="59"/>
       <c r="F110" s="54"/>
       <c r="G110" s="54"/>
       <c r="H110" s="54"/>
@@ -3057,14 +3063,14 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B111" s="42">
         <v>109</v>
       </c>
       <c r="C111" s="54"/>
       <c r="D111" s="54"/>
-      <c r="E111" s="75"/>
+      <c r="E111" s="59"/>
       <c r="F111" s="54"/>
       <c r="G111" s="54"/>
       <c r="H111" s="54"/>
@@ -3072,14 +3078,14 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B112" s="42">
         <v>110</v>
       </c>
       <c r="C112" s="54"/>
       <c r="D112" s="54"/>
-      <c r="E112" s="75"/>
+      <c r="E112" s="59"/>
       <c r="F112" s="54"/>
       <c r="G112" s="54"/>
       <c r="H112" s="54"/>
@@ -3089,14 +3095,14 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B113" s="42">
         <v>111</v>
       </c>
       <c r="C113" s="54"/>
       <c r="D113" s="54"/>
-      <c r="E113" s="75"/>
+      <c r="E113" s="59"/>
       <c r="F113" s="54"/>
       <c r="G113" s="54"/>
       <c r="H113" s="54"/>
@@ -3106,14 +3112,14 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B114" s="42">
         <v>112</v>
       </c>
       <c r="C114" s="54"/>
       <c r="D114" s="54"/>
-      <c r="E114" s="74" t="s">
+      <c r="E114" s="64" t="s">
         <v>21</v>
       </c>
       <c r="F114" s="54"/>
@@ -3125,14 +3131,14 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B115" s="42">
         <v>113</v>
       </c>
       <c r="C115" s="54"/>
       <c r="D115" s="54"/>
-      <c r="E115" s="74"/>
+      <c r="E115" s="64"/>
       <c r="F115" s="54"/>
       <c r="G115" s="54"/>
       <c r="H115" s="54"/>
@@ -3140,14 +3146,14 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B116" s="42">
         <v>114</v>
       </c>
       <c r="C116" s="54"/>
       <c r="D116" s="54"/>
-      <c r="E116" s="74"/>
+      <c r="E116" s="64"/>
       <c r="F116" s="54"/>
       <c r="G116" s="54"/>
       <c r="H116" s="54"/>
@@ -3155,14 +3161,14 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B117" s="42">
         <v>115</v>
       </c>
       <c r="C117" s="54"/>
       <c r="D117" s="54"/>
-      <c r="E117" s="74"/>
+      <c r="E117" s="64"/>
       <c r="F117" s="54"/>
       <c r="G117" s="54"/>
       <c r="H117" s="54"/>
@@ -3170,14 +3176,14 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B118" s="42">
         <v>116</v>
       </c>
       <c r="C118" s="54"/>
       <c r="D118" s="54"/>
-      <c r="E118" s="74"/>
+      <c r="E118" s="64"/>
       <c r="F118" s="54"/>
       <c r="G118" s="54"/>
       <c r="H118" s="54"/>
@@ -3185,14 +3191,14 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B119" s="42">
         <v>117</v>
       </c>
       <c r="C119" s="54"/>
       <c r="D119" s="54"/>
-      <c r="E119" s="74"/>
+      <c r="E119" s="64"/>
       <c r="F119" s="54"/>
       <c r="G119" s="54"/>
       <c r="H119" s="54"/>
@@ -3200,14 +3206,14 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B120" s="42">
         <v>118</v>
       </c>
       <c r="C120" s="54"/>
       <c r="D120" s="54"/>
-      <c r="E120" s="74"/>
+      <c r="E120" s="64"/>
       <c r="F120" s="54"/>
       <c r="G120" s="54"/>
       <c r="H120" s="54"/>
@@ -3215,14 +3221,14 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B121" s="42">
         <v>119</v>
       </c>
       <c r="C121" s="54"/>
       <c r="D121" s="54"/>
-      <c r="E121" s="74"/>
+      <c r="E121" s="64"/>
       <c r="F121" s="54"/>
       <c r="G121" s="54"/>
       <c r="H121" s="54"/>
@@ -3230,14 +3236,14 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B122" s="42">
         <v>120</v>
       </c>
       <c r="C122" s="54"/>
       <c r="D122" s="54"/>
-      <c r="E122" s="74"/>
+      <c r="E122" s="64"/>
       <c r="F122" s="54"/>
       <c r="G122" s="54"/>
       <c r="H122" s="54"/>
@@ -3245,14 +3251,14 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B123" s="42">
         <v>121</v>
       </c>
       <c r="C123" s="54"/>
       <c r="D123" s="54"/>
-      <c r="E123" s="74"/>
+      <c r="E123" s="64"/>
       <c r="F123" s="54"/>
       <c r="G123" s="54"/>
       <c r="H123" s="54"/>
@@ -3260,14 +3266,14 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B124" s="42">
         <v>122</v>
       </c>
       <c r="C124" s="54"/>
       <c r="D124" s="54"/>
-      <c r="E124" s="74"/>
+      <c r="E124" s="64"/>
       <c r="F124" s="54"/>
       <c r="G124" s="54"/>
       <c r="H124" s="54"/>
@@ -3275,14 +3281,14 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B125" s="42">
         <v>123</v>
       </c>
       <c r="C125" s="54"/>
       <c r="D125" s="54"/>
-      <c r="E125" s="74"/>
+      <c r="E125" s="64"/>
       <c r="F125" s="54"/>
       <c r="G125" s="54"/>
       <c r="H125" s="54"/>
@@ -3290,14 +3296,14 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B126" s="42">
         <v>124</v>
       </c>
       <c r="C126" s="54"/>
       <c r="D126" s="54"/>
-      <c r="E126" s="74"/>
+      <c r="E126" s="64"/>
       <c r="F126" s="54"/>
       <c r="G126" s="54"/>
       <c r="H126" s="54"/>
@@ -3305,14 +3311,14 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B127" s="42">
         <v>125</v>
       </c>
       <c r="C127" s="54"/>
       <c r="D127" s="54"/>
-      <c r="E127" s="74"/>
+      <c r="E127" s="64"/>
       <c r="F127" s="54"/>
       <c r="G127" s="54"/>
       <c r="H127" s="54"/>
@@ -3320,14 +3326,14 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B128" s="42">
         <v>126</v>
       </c>
       <c r="C128" s="54"/>
       <c r="D128" s="54"/>
-      <c r="E128" s="74"/>
+      <c r="E128" s="64"/>
       <c r="F128" s="54"/>
       <c r="G128" s="54"/>
       <c r="H128" s="54"/>
@@ -3337,14 +3343,14 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B129" s="42">
         <v>127</v>
       </c>
       <c r="C129" s="54"/>
       <c r="D129" s="54"/>
-      <c r="E129" s="74"/>
+      <c r="E129" s="64"/>
       <c r="F129" s="54"/>
       <c r="G129" s="54"/>
       <c r="H129" s="54"/>
@@ -3354,14 +3360,14 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B130" s="39">
         <v>128</v>
       </c>
       <c r="C130" s="54"/>
       <c r="D130" s="54"/>
-      <c r="E130" s="67" t="s">
+      <c r="E130" s="61" t="s">
         <v>22</v>
       </c>
       <c r="F130" s="54"/>
@@ -3373,14 +3379,14 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B131" s="39">
         <v>129</v>
       </c>
       <c r="C131" s="54"/>
       <c r="D131" s="54"/>
-      <c r="E131" s="68"/>
+      <c r="E131" s="62"/>
       <c r="F131" s="54"/>
       <c r="G131" s="54"/>
       <c r="H131" s="54"/>
@@ -3388,14 +3394,14 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B132" s="39">
         <v>130</v>
       </c>
       <c r="C132" s="54"/>
       <c r="D132" s="54"/>
-      <c r="E132" s="68"/>
+      <c r="E132" s="62"/>
       <c r="F132" s="54"/>
       <c r="G132" s="54"/>
       <c r="H132" s="54"/>
@@ -3403,14 +3409,14 @@
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B133" s="39">
         <v>131</v>
       </c>
       <c r="C133" s="54"/>
       <c r="D133" s="54"/>
-      <c r="E133" s="68"/>
+      <c r="E133" s="62"/>
       <c r="F133" s="54"/>
       <c r="G133" s="54"/>
       <c r="H133" s="54"/>
@@ -3418,14 +3424,14 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B134" s="39">
         <v>132</v>
       </c>
       <c r="C134" s="54"/>
       <c r="D134" s="54"/>
-      <c r="E134" s="68"/>
+      <c r="E134" s="62"/>
       <c r="F134" s="54"/>
       <c r="G134" s="54"/>
       <c r="H134" s="54"/>
@@ -3433,14 +3439,14 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B135" s="39">
         <v>133</v>
       </c>
       <c r="C135" s="54"/>
       <c r="D135" s="54"/>
-      <c r="E135" s="68"/>
+      <c r="E135" s="62"/>
       <c r="F135" s="54"/>
       <c r="G135" s="54"/>
       <c r="H135" s="54"/>
@@ -3448,14 +3454,14 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B136" s="39">
         <v>134</v>
       </c>
       <c r="C136" s="54"/>
       <c r="D136" s="54"/>
-      <c r="E136" s="68"/>
+      <c r="E136" s="62"/>
       <c r="F136" s="54"/>
       <c r="G136" s="54"/>
       <c r="H136" s="54"/>
@@ -3463,14 +3469,14 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B137" s="39">
         <v>135</v>
       </c>
       <c r="C137" s="54"/>
       <c r="D137" s="54"/>
-      <c r="E137" s="68"/>
+      <c r="E137" s="62"/>
       <c r="F137" s="54"/>
       <c r="G137" s="54"/>
       <c r="H137" s="54"/>
@@ -3478,14 +3484,14 @@
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B138" s="39">
         <v>136</v>
       </c>
       <c r="C138" s="54"/>
       <c r="D138" s="54"/>
-      <c r="E138" s="68"/>
+      <c r="E138" s="62"/>
       <c r="F138" s="54"/>
       <c r="G138" s="54"/>
       <c r="H138" s="54"/>
@@ -3493,14 +3499,14 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B139" s="39">
         <v>137</v>
       </c>
       <c r="C139" s="54"/>
       <c r="D139" s="54"/>
-      <c r="E139" s="68"/>
+      <c r="E139" s="62"/>
       <c r="F139" s="54"/>
       <c r="G139" s="54"/>
       <c r="H139" s="54"/>
@@ -3508,14 +3514,14 @@
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B140" s="39">
         <v>138</v>
       </c>
       <c r="C140" s="54"/>
       <c r="D140" s="54"/>
-      <c r="E140" s="68"/>
+      <c r="E140" s="62"/>
       <c r="F140" s="54"/>
       <c r="G140" s="54"/>
       <c r="H140" s="54"/>
@@ -3523,14 +3529,14 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B141" s="39">
         <v>139</v>
       </c>
       <c r="C141" s="54"/>
       <c r="D141" s="54"/>
-      <c r="E141" s="68"/>
+      <c r="E141" s="62"/>
       <c r="F141" s="54"/>
       <c r="G141" s="54"/>
       <c r="H141" s="54"/>
@@ -3538,14 +3544,14 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B142" s="39">
         <v>140</v>
       </c>
       <c r="C142" s="54"/>
       <c r="D142" s="54"/>
-      <c r="E142" s="68"/>
+      <c r="E142" s="62"/>
       <c r="F142" s="54"/>
       <c r="G142" s="54"/>
       <c r="H142" s="54"/>
@@ -3553,14 +3559,14 @@
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B143" s="39">
         <v>141</v>
       </c>
       <c r="C143" s="54"/>
       <c r="D143" s="54"/>
-      <c r="E143" s="68"/>
+      <c r="E143" s="62"/>
       <c r="F143" s="54"/>
       <c r="G143" s="54"/>
       <c r="H143" s="54"/>
@@ -3568,14 +3574,14 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B144" s="39">
         <v>142</v>
       </c>
       <c r="C144" s="54"/>
       <c r="D144" s="54"/>
-      <c r="E144" s="68"/>
+      <c r="E144" s="62"/>
       <c r="F144" s="54"/>
       <c r="G144" s="54"/>
       <c r="H144" s="54"/>
@@ -3585,14 +3591,14 @@
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B145" s="39">
         <v>143</v>
       </c>
       <c r="C145" s="54"/>
       <c r="D145" s="54"/>
-      <c r="E145" s="69"/>
+      <c r="E145" s="63"/>
       <c r="F145" s="54"/>
       <c r="G145" s="54"/>
       <c r="H145" s="54"/>
@@ -3602,14 +3608,14 @@
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B146" s="39">
         <v>144</v>
       </c>
       <c r="C146" s="54"/>
       <c r="D146" s="54"/>
-      <c r="E146" s="67" t="s">
+      <c r="E146" s="61" t="s">
         <v>23</v>
       </c>
       <c r="F146" s="54"/>
@@ -3621,14 +3627,14 @@
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B147" s="39">
         <v>145</v>
       </c>
       <c r="C147" s="54"/>
       <c r="D147" s="54"/>
-      <c r="E147" s="68"/>
+      <c r="E147" s="62"/>
       <c r="F147" s="54"/>
       <c r="G147" s="54"/>
       <c r="H147" s="54"/>
@@ -3636,14 +3642,14 @@
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B148" s="39">
         <v>146</v>
       </c>
       <c r="C148" s="54"/>
       <c r="D148" s="54"/>
-      <c r="E148" s="68"/>
+      <c r="E148" s="62"/>
       <c r="F148" s="54"/>
       <c r="G148" s="54"/>
       <c r="H148" s="54"/>
@@ -3651,14 +3657,14 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B149" s="39">
         <v>147</v>
       </c>
       <c r="C149" s="54"/>
       <c r="D149" s="54"/>
-      <c r="E149" s="68"/>
+      <c r="E149" s="62"/>
       <c r="F149" s="54"/>
       <c r="G149" s="54"/>
       <c r="H149" s="54"/>
@@ -3666,14 +3672,14 @@
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B150" s="39">
         <v>148</v>
       </c>
       <c r="C150" s="54"/>
       <c r="D150" s="54"/>
-      <c r="E150" s="68"/>
+      <c r="E150" s="62"/>
       <c r="F150" s="54"/>
       <c r="G150" s="54"/>
       <c r="H150" s="54"/>
@@ -3681,14 +3687,14 @@
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B151" s="39">
         <v>149</v>
       </c>
       <c r="C151" s="54"/>
       <c r="D151" s="54"/>
-      <c r="E151" s="68"/>
+      <c r="E151" s="62"/>
       <c r="F151" s="54"/>
       <c r="G151" s="54"/>
       <c r="H151" s="54"/>
@@ -3696,14 +3702,14 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B152" s="39">
         <v>150</v>
       </c>
       <c r="C152" s="54"/>
       <c r="D152" s="54"/>
-      <c r="E152" s="68"/>
+      <c r="E152" s="62"/>
       <c r="F152" s="54"/>
       <c r="G152" s="54"/>
       <c r="H152" s="54"/>
@@ -3711,14 +3717,14 @@
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B153" s="39">
         <v>151</v>
       </c>
       <c r="C153" s="54"/>
       <c r="D153" s="54"/>
-      <c r="E153" s="68"/>
+      <c r="E153" s="62"/>
       <c r="F153" s="54"/>
       <c r="G153" s="54"/>
       <c r="H153" s="54"/>
@@ -3726,14 +3732,14 @@
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B154" s="39">
         <v>152</v>
       </c>
       <c r="C154" s="54"/>
       <c r="D154" s="54"/>
-      <c r="E154" s="68"/>
+      <c r="E154" s="62"/>
       <c r="F154" s="54"/>
       <c r="G154" s="54"/>
       <c r="H154" s="54"/>
@@ -3741,14 +3747,14 @@
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B155" s="39">
         <v>153</v>
       </c>
       <c r="C155" s="54"/>
       <c r="D155" s="54"/>
-      <c r="E155" s="68"/>
+      <c r="E155" s="62"/>
       <c r="F155" s="54"/>
       <c r="G155" s="54"/>
       <c r="H155" s="54"/>
@@ -3756,14 +3762,14 @@
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B156" s="39">
         <v>154</v>
       </c>
       <c r="C156" s="54"/>
       <c r="D156" s="54"/>
-      <c r="E156" s="68"/>
+      <c r="E156" s="62"/>
       <c r="F156" s="54"/>
       <c r="G156" s="54"/>
       <c r="H156" s="54"/>
@@ -3771,14 +3777,14 @@
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B157" s="39">
         <v>155</v>
       </c>
       <c r="C157" s="54"/>
       <c r="D157" s="54"/>
-      <c r="E157" s="68"/>
+      <c r="E157" s="62"/>
       <c r="F157" s="54"/>
       <c r="G157" s="54"/>
       <c r="H157" s="54"/>
@@ -3786,14 +3792,14 @@
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B158" s="39">
         <v>156</v>
       </c>
       <c r="C158" s="54"/>
       <c r="D158" s="54"/>
-      <c r="E158" s="68"/>
+      <c r="E158" s="62"/>
       <c r="F158" s="54"/>
       <c r="G158" s="54"/>
       <c r="H158" s="54"/>
@@ -3801,14 +3807,14 @@
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B159" s="39">
         <v>157</v>
       </c>
       <c r="C159" s="54"/>
       <c r="D159" s="54"/>
-      <c r="E159" s="68"/>
+      <c r="E159" s="62"/>
       <c r="F159" s="54"/>
       <c r="G159" s="54"/>
       <c r="H159" s="54"/>
@@ -3816,14 +3822,14 @@
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B160" s="39">
         <v>158</v>
       </c>
       <c r="C160" s="54"/>
       <c r="D160" s="54"/>
-      <c r="E160" s="68"/>
+      <c r="E160" s="62"/>
       <c r="F160" s="54"/>
       <c r="G160" s="54"/>
       <c r="H160" s="54"/>
@@ -3833,14 +3839,14 @@
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B161" s="39">
         <v>159</v>
       </c>
       <c r="C161" s="54"/>
       <c r="D161" s="54"/>
-      <c r="E161" s="69"/>
+      <c r="E161" s="63"/>
       <c r="F161" s="54"/>
       <c r="G161" s="54"/>
       <c r="H161" s="54"/>
@@ -3850,14 +3856,14 @@
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B162" s="37">
         <v>160</v>
       </c>
       <c r="C162" s="54"/>
       <c r="D162" s="54"/>
-      <c r="E162" s="61" t="s">
+      <c r="E162" s="69" t="s">
         <v>26</v>
       </c>
       <c r="F162" s="54"/>
@@ -3869,14 +3875,14 @@
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B163" s="37">
         <v>161</v>
       </c>
       <c r="C163" s="54"/>
       <c r="D163" s="54"/>
-      <c r="E163" s="62"/>
+      <c r="E163" s="70"/>
       <c r="F163" s="54"/>
       <c r="G163" s="54"/>
       <c r="H163" s="54"/>
@@ -3884,14 +3890,14 @@
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B164" s="37">
         <v>162</v>
       </c>
       <c r="C164" s="54"/>
       <c r="D164" s="54"/>
-      <c r="E164" s="62"/>
+      <c r="E164" s="70"/>
       <c r="F164" s="54"/>
       <c r="G164" s="54"/>
       <c r="H164" s="54"/>
@@ -3899,14 +3905,14 @@
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B165" s="37">
         <v>163</v>
       </c>
       <c r="C165" s="54"/>
       <c r="D165" s="54"/>
-      <c r="E165" s="62"/>
+      <c r="E165" s="70"/>
       <c r="F165" s="54"/>
       <c r="G165" s="54"/>
       <c r="H165" s="54"/>
@@ -3914,14 +3920,14 @@
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B166" s="37">
         <v>164</v>
       </c>
       <c r="C166" s="54"/>
       <c r="D166" s="54"/>
-      <c r="E166" s="62"/>
+      <c r="E166" s="70"/>
       <c r="F166" s="54"/>
       <c r="G166" s="54"/>
       <c r="H166" s="54"/>
@@ -3929,14 +3935,14 @@
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B167" s="37">
         <v>165</v>
       </c>
       <c r="C167" s="54"/>
       <c r="D167" s="54"/>
-      <c r="E167" s="62"/>
+      <c r="E167" s="70"/>
       <c r="F167" s="54"/>
       <c r="G167" s="54"/>
       <c r="H167" s="54"/>
@@ -3944,14 +3950,14 @@
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B168" s="37">
         <v>166</v>
       </c>
       <c r="C168" s="54"/>
       <c r="D168" s="54"/>
-      <c r="E168" s="62"/>
+      <c r="E168" s="70"/>
       <c r="F168" s="54"/>
       <c r="G168" s="54"/>
       <c r="H168" s="54"/>
@@ -3959,14 +3965,14 @@
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B169" s="37">
         <v>167</v>
       </c>
       <c r="C169" s="54"/>
       <c r="D169" s="54"/>
-      <c r="E169" s="62"/>
+      <c r="E169" s="70"/>
       <c r="F169" s="54"/>
       <c r="G169" s="54"/>
       <c r="H169" s="54"/>
@@ -3974,14 +3980,14 @@
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B170" s="37">
         <v>168</v>
       </c>
       <c r="C170" s="54"/>
       <c r="D170" s="54"/>
-      <c r="E170" s="62"/>
+      <c r="E170" s="70"/>
       <c r="F170" s="54"/>
       <c r="G170" s="54"/>
       <c r="H170" s="54"/>
@@ -3989,14 +3995,14 @@
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B171" s="37">
         <v>169</v>
       </c>
       <c r="C171" s="54"/>
       <c r="D171" s="54"/>
-      <c r="E171" s="62"/>
+      <c r="E171" s="70"/>
       <c r="F171" s="54"/>
       <c r="G171" s="54"/>
       <c r="H171" s="54"/>
@@ -4004,14 +4010,14 @@
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B172" s="37">
         <v>170</v>
       </c>
       <c r="C172" s="54"/>
       <c r="D172" s="54"/>
-      <c r="E172" s="62"/>
+      <c r="E172" s="70"/>
       <c r="F172" s="54"/>
       <c r="G172" s="54"/>
       <c r="H172" s="54"/>
@@ -4019,14 +4025,14 @@
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B173" s="37">
         <v>171</v>
       </c>
       <c r="C173" s="54"/>
       <c r="D173" s="54"/>
-      <c r="E173" s="62"/>
+      <c r="E173" s="70"/>
       <c r="F173" s="54"/>
       <c r="G173" s="54"/>
       <c r="H173" s="54"/>
@@ -4034,14 +4040,14 @@
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B174" s="37">
         <v>172</v>
       </c>
       <c r="C174" s="54"/>
       <c r="D174" s="54"/>
-      <c r="E174" s="62"/>
+      <c r="E174" s="70"/>
       <c r="F174" s="54"/>
       <c r="G174" s="54"/>
       <c r="H174" s="54"/>
@@ -4049,14 +4055,14 @@
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B175" s="37">
         <v>173</v>
       </c>
       <c r="C175" s="54"/>
       <c r="D175" s="54"/>
-      <c r="E175" s="62"/>
+      <c r="E175" s="70"/>
       <c r="F175" s="54"/>
       <c r="G175" s="54"/>
       <c r="H175" s="54"/>
@@ -4064,14 +4070,14 @@
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B176" s="37">
         <v>174</v>
       </c>
       <c r="C176" s="54"/>
       <c r="D176" s="54"/>
-      <c r="E176" s="62"/>
+      <c r="E176" s="70"/>
       <c r="F176" s="54"/>
       <c r="G176" s="54"/>
       <c r="H176" s="54"/>
@@ -4081,14 +4087,14 @@
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B177" s="37">
         <v>175</v>
       </c>
       <c r="C177" s="54"/>
       <c r="D177" s="54"/>
-      <c r="E177" s="63"/>
+      <c r="E177" s="71"/>
       <c r="F177" s="54"/>
       <c r="G177" s="54"/>
       <c r="H177" s="54"/>
@@ -4098,14 +4104,14 @@
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B178" s="37">
         <v>176</v>
       </c>
       <c r="C178" s="54"/>
       <c r="D178" s="54"/>
-      <c r="E178" s="70" t="s">
+      <c r="E178" s="65" t="s">
         <v>27</v>
       </c>
       <c r="F178" s="54"/>
@@ -4117,14 +4123,14 @@
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B179" s="37">
         <v>177</v>
       </c>
       <c r="C179" s="54"/>
       <c r="D179" s="54"/>
-      <c r="E179" s="70"/>
+      <c r="E179" s="65"/>
       <c r="F179" s="54"/>
       <c r="G179" s="54"/>
       <c r="H179" s="54"/>
@@ -4132,14 +4138,14 @@
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B180" s="37">
         <v>178</v>
       </c>
       <c r="C180" s="54"/>
       <c r="D180" s="54"/>
-      <c r="E180" s="70"/>
+      <c r="E180" s="65"/>
       <c r="F180" s="54"/>
       <c r="G180" s="54"/>
       <c r="H180" s="54"/>
@@ -4147,14 +4153,14 @@
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B181" s="37">
         <v>179</v>
       </c>
       <c r="C181" s="54"/>
       <c r="D181" s="54"/>
-      <c r="E181" s="70"/>
+      <c r="E181" s="65"/>
       <c r="F181" s="54"/>
       <c r="G181" s="54"/>
       <c r="H181" s="54"/>
@@ -4162,14 +4168,14 @@
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B182" s="37">
         <v>180</v>
       </c>
       <c r="C182" s="54"/>
       <c r="D182" s="54"/>
-      <c r="E182" s="70"/>
+      <c r="E182" s="65"/>
       <c r="F182" s="54"/>
       <c r="G182" s="54"/>
       <c r="H182" s="54"/>
@@ -4177,14 +4183,14 @@
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B183" s="37">
         <v>181</v>
       </c>
       <c r="C183" s="54"/>
       <c r="D183" s="54"/>
-      <c r="E183" s="70"/>
+      <c r="E183" s="65"/>
       <c r="F183" s="54"/>
       <c r="G183" s="54"/>
       <c r="H183" s="54"/>
@@ -4192,14 +4198,14 @@
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B184" s="37">
         <v>182</v>
       </c>
       <c r="C184" s="54"/>
       <c r="D184" s="54"/>
-      <c r="E184" s="70"/>
+      <c r="E184" s="65"/>
       <c r="F184" s="54"/>
       <c r="G184" s="54"/>
       <c r="H184" s="54"/>
@@ -4207,14 +4213,14 @@
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B185" s="37">
         <v>183</v>
       </c>
       <c r="C185" s="54"/>
       <c r="D185" s="54"/>
-      <c r="E185" s="70"/>
+      <c r="E185" s="65"/>
       <c r="F185" s="54"/>
       <c r="G185" s="54"/>
       <c r="H185" s="54"/>
@@ -4222,14 +4228,14 @@
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B186" s="37">
         <v>184</v>
       </c>
       <c r="C186" s="54"/>
       <c r="D186" s="54"/>
-      <c r="E186" s="70"/>
+      <c r="E186" s="65"/>
       <c r="F186" s="54"/>
       <c r="G186" s="54"/>
       <c r="H186" s="54"/>
@@ -4237,14 +4243,14 @@
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B187" s="37">
         <v>185</v>
       </c>
       <c r="C187" s="54"/>
       <c r="D187" s="54"/>
-      <c r="E187" s="70"/>
+      <c r="E187" s="65"/>
       <c r="F187" s="54"/>
       <c r="G187" s="54"/>
       <c r="H187" s="54"/>
@@ -4252,14 +4258,14 @@
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B188" s="37">
         <v>186</v>
       </c>
       <c r="C188" s="54"/>
       <c r="D188" s="54"/>
-      <c r="E188" s="70"/>
+      <c r="E188" s="65"/>
       <c r="F188" s="54"/>
       <c r="G188" s="54"/>
       <c r="H188" s="54"/>
@@ -4267,14 +4273,14 @@
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B189" s="37">
         <v>187</v>
       </c>
       <c r="C189" s="54"/>
       <c r="D189" s="54"/>
-      <c r="E189" s="70"/>
+      <c r="E189" s="65"/>
       <c r="F189" s="54"/>
       <c r="G189" s="54"/>
       <c r="H189" s="54"/>
@@ -4282,14 +4288,14 @@
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B190" s="37">
         <v>188</v>
       </c>
       <c r="C190" s="54"/>
       <c r="D190" s="54"/>
-      <c r="E190" s="70"/>
+      <c r="E190" s="65"/>
       <c r="F190" s="54"/>
       <c r="G190" s="54"/>
       <c r="H190" s="54"/>
@@ -4297,14 +4303,14 @@
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B191" s="37">
         <v>189</v>
       </c>
       <c r="C191" s="54"/>
       <c r="D191" s="54"/>
-      <c r="E191" s="70"/>
+      <c r="E191" s="65"/>
       <c r="F191" s="54"/>
       <c r="G191" s="54"/>
       <c r="H191" s="54"/>
@@ -4312,14 +4318,14 @@
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B192" s="37">
         <v>190</v>
       </c>
       <c r="C192" s="54"/>
       <c r="D192" s="54"/>
-      <c r="E192" s="70"/>
+      <c r="E192" s="65"/>
       <c r="F192" s="54"/>
       <c r="G192" s="54"/>
       <c r="H192" s="54"/>
@@ -4329,14 +4335,14 @@
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B193" s="37">
         <v>191</v>
       </c>
       <c r="C193" s="54"/>
       <c r="D193" s="54"/>
-      <c r="E193" s="70"/>
+      <c r="E193" s="65"/>
       <c r="F193" s="54"/>
       <c r="G193" s="54"/>
       <c r="H193" s="54"/>
@@ -4346,13 +4352,13 @@
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" s="35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B194" s="35">
         <v>192</v>
       </c>
       <c r="C194" s="54"/>
-      <c r="D194" s="71" t="s">
+      <c r="D194" s="66" t="s">
         <v>25</v>
       </c>
       <c r="E194" s="54"/>
@@ -4365,13 +4371,13 @@
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" s="35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B195" s="35">
         <v>193</v>
       </c>
       <c r="C195" s="54"/>
-      <c r="D195" s="72"/>
+      <c r="D195" s="67"/>
       <c r="E195" s="54"/>
       <c r="F195" s="54"/>
       <c r="G195" s="54"/>
@@ -4380,13 +4386,13 @@
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" s="35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B196" s="35">
         <v>194</v>
       </c>
       <c r="C196" s="54"/>
-      <c r="D196" s="72"/>
+      <c r="D196" s="67"/>
       <c r="E196" s="54"/>
       <c r="F196" s="54"/>
       <c r="G196" s="54"/>
@@ -4395,13 +4401,13 @@
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" s="35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B197" s="35">
         <v>195</v>
       </c>
       <c r="C197" s="54"/>
-      <c r="D197" s="72"/>
+      <c r="D197" s="67"/>
       <c r="E197" s="54"/>
       <c r="F197" s="54"/>
       <c r="G197" s="54"/>
@@ -4410,13 +4416,13 @@
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" s="35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B198" s="35">
         <v>196</v>
       </c>
       <c r="C198" s="54"/>
-      <c r="D198" s="72"/>
+      <c r="D198" s="67"/>
       <c r="E198" s="54"/>
       <c r="F198" s="54"/>
       <c r="G198" s="54"/>
@@ -4425,13 +4431,13 @@
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" s="35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B199" s="35">
         <v>197</v>
       </c>
       <c r="C199" s="54"/>
-      <c r="D199" s="72"/>
+      <c r="D199" s="67"/>
       <c r="E199" s="54"/>
       <c r="F199" s="54"/>
       <c r="G199" s="54"/>
@@ -4440,13 +4446,13 @@
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" s="35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B200" s="35">
         <v>198</v>
       </c>
       <c r="C200" s="54"/>
-      <c r="D200" s="72"/>
+      <c r="D200" s="67"/>
       <c r="E200" s="54"/>
       <c r="F200" s="54"/>
       <c r="G200" s="54"/>
@@ -4457,13 +4463,13 @@
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" s="35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B201" s="35">
         <v>199</v>
       </c>
       <c r="C201" s="54"/>
-      <c r="D201" s="73"/>
+      <c r="D201" s="68"/>
       <c r="E201" s="54"/>
       <c r="F201" s="54"/>
       <c r="G201" s="54"/>
@@ -4474,13 +4480,13 @@
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" s="35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B202" s="35">
         <v>200</v>
       </c>
       <c r="C202" s="54"/>
-      <c r="D202" s="55" t="s">
+      <c r="D202" s="75" t="s">
         <v>24</v>
       </c>
       <c r="E202" s="54"/>
@@ -4493,13 +4499,13 @@
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" s="35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B203" s="35">
         <v>201</v>
       </c>
       <c r="C203" s="54"/>
-      <c r="D203" s="55"/>
+      <c r="D203" s="75"/>
       <c r="E203" s="54"/>
       <c r="F203" s="54"/>
       <c r="G203" s="54"/>
@@ -4508,13 +4514,13 @@
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" s="35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B204" s="35">
         <v>202</v>
       </c>
       <c r="C204" s="54"/>
-      <c r="D204" s="55"/>
+      <c r="D204" s="75"/>
       <c r="E204" s="54"/>
       <c r="F204" s="54"/>
       <c r="G204" s="54"/>
@@ -4523,13 +4529,13 @@
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" s="35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B205" s="35">
         <v>203</v>
       </c>
       <c r="C205" s="54"/>
-      <c r="D205" s="55"/>
+      <c r="D205" s="75"/>
       <c r="E205" s="54"/>
       <c r="F205" s="54"/>
       <c r="G205" s="54"/>
@@ -4538,13 +4544,13 @@
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" s="35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B206" s="35">
         <v>204</v>
       </c>
       <c r="C206" s="54"/>
-      <c r="D206" s="55"/>
+      <c r="D206" s="75"/>
       <c r="E206" s="54"/>
       <c r="F206" s="54"/>
       <c r="G206" s="54"/>
@@ -4553,13 +4559,13 @@
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" s="35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B207" s="35">
         <v>205</v>
       </c>
       <c r="C207" s="54"/>
-      <c r="D207" s="55"/>
+      <c r="D207" s="75"/>
       <c r="E207" s="54"/>
       <c r="F207" s="54"/>
       <c r="G207" s="54"/>
@@ -4568,13 +4574,13 @@
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" s="35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B208" s="35">
         <v>206</v>
       </c>
       <c r="C208" s="54"/>
-      <c r="D208" s="55"/>
+      <c r="D208" s="75"/>
       <c r="E208" s="54"/>
       <c r="F208" s="54"/>
       <c r="G208" s="54"/>
@@ -4585,13 +4591,13 @@
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" s="35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B209" s="35">
         <v>207</v>
       </c>
       <c r="C209" s="54"/>
-      <c r="D209" s="55"/>
+      <c r="D209" s="75"/>
       <c r="E209" s="54"/>
       <c r="F209" s="54"/>
       <c r="G209" s="54"/>
@@ -4602,14 +4608,14 @@
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" s="32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B210" s="32">
         <v>208</v>
       </c>
-      <c r="C210" s="56"/>
-      <c r="D210" s="57"/>
-      <c r="E210" s="58" t="s">
+      <c r="C210" s="76"/>
+      <c r="D210" s="77"/>
+      <c r="E210" s="78" t="s">
         <v>34</v>
       </c>
       <c r="F210" s="54"/>
@@ -4621,116 +4627,110 @@
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" s="32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B211" s="32">
         <v>209</v>
       </c>
-      <c r="C211" s="56"/>
-      <c r="D211" s="57"/>
-      <c r="E211" s="58"/>
+      <c r="C211" s="76"/>
+      <c r="D211" s="77"/>
+      <c r="E211" s="78"/>
       <c r="F211" s="54"/>
       <c r="G211" s="54"/>
       <c r="H211" s="54"/>
       <c r="I211" s="31" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" s="32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B212" s="32">
         <v>210</v>
       </c>
-      <c r="C212" s="56"/>
-      <c r="D212" s="57"/>
-      <c r="E212" s="58"/>
+      <c r="C212" s="76"/>
+      <c r="D212" s="77"/>
+      <c r="E212" s="78"/>
       <c r="F212" s="54"/>
       <c r="G212" s="54"/>
       <c r="H212" s="54"/>
       <c r="I212" s="31" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" s="32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B213" s="32">
         <v>211</v>
       </c>
-      <c r="C213" s="56"/>
-      <c r="D213" s="57"/>
-      <c r="E213" s="58"/>
+      <c r="C213" s="76"/>
+      <c r="D213" s="77"/>
+      <c r="E213" s="78"/>
       <c r="F213" s="54"/>
       <c r="G213" s="54"/>
       <c r="H213" s="54"/>
       <c r="I213" s="31" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" s="32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B214" s="32">
         <v>212</v>
       </c>
-      <c r="C214" s="56"/>
-      <c r="D214" s="57"/>
-      <c r="E214" s="58"/>
+      <c r="C214" s="76"/>
+      <c r="D214" s="77"/>
+      <c r="E214" s="78"/>
       <c r="F214" s="54"/>
       <c r="G214" s="54"/>
       <c r="H214" s="54"/>
-      <c r="I214" s="31" t="s">
-        <v>38</v>
-      </c>
+      <c r="I214" s="31"/>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" s="32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B215" s="32">
         <v>213</v>
       </c>
-      <c r="C215" s="56"/>
-      <c r="D215" s="57"/>
-      <c r="E215" s="58"/>
+      <c r="C215" s="76"/>
+      <c r="D215" s="77"/>
+      <c r="E215" s="78"/>
       <c r="F215" s="54"/>
       <c r="G215" s="54"/>
       <c r="H215" s="54"/>
-      <c r="I215" s="31" t="s">
-        <v>39</v>
-      </c>
+      <c r="I215" s="31"/>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" s="32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B216" s="32">
         <v>214</v>
       </c>
-      <c r="C216" s="56"/>
-      <c r="D216" s="57"/>
-      <c r="E216" s="58"/>
+      <c r="C216" s="76"/>
+      <c r="D216" s="77"/>
+      <c r="E216" s="78"/>
       <c r="F216" s="54"/>
       <c r="G216" s="54"/>
       <c r="H216" s="54"/>
-      <c r="I216" s="31" t="s">
-        <v>40</v>
-      </c>
+      <c r="I216" s="31"/>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" s="32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B217" s="32">
         <v>215</v>
       </c>
-      <c r="C217" s="56"/>
-      <c r="D217" s="57"/>
-      <c r="E217" s="58"/>
+      <c r="C217" s="76"/>
+      <c r="D217" s="77"/>
+      <c r="E217" s="78"/>
       <c r="F217" s="54"/>
       <c r="G217" s="54"/>
       <c r="H217" s="54"/>
@@ -4738,14 +4738,14 @@
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" s="32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B218" s="32">
         <v>216</v>
       </c>
       <c r="C218" s="54"/>
-      <c r="D218" s="64"/>
-      <c r="E218" s="58"/>
+      <c r="D218" s="72"/>
+      <c r="E218" s="78"/>
       <c r="F218" s="54"/>
       <c r="G218" s="54"/>
       <c r="H218" s="54"/>
@@ -4753,14 +4753,14 @@
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" s="32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B219" s="32">
         <v>217</v>
       </c>
       <c r="C219" s="54"/>
-      <c r="D219" s="64"/>
-      <c r="E219" s="58"/>
+      <c r="D219" s="72"/>
+      <c r="E219" s="78"/>
       <c r="F219" s="54"/>
       <c r="G219" s="54"/>
       <c r="H219" s="54"/>
@@ -4768,14 +4768,14 @@
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" s="32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B220" s="32">
         <v>218</v>
       </c>
       <c r="C220" s="54"/>
-      <c r="D220" s="64"/>
-      <c r="E220" s="58"/>
+      <c r="D220" s="72"/>
+      <c r="E220" s="78"/>
       <c r="F220" s="54"/>
       <c r="G220" s="54"/>
       <c r="H220" s="54"/>
@@ -4783,14 +4783,14 @@
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" s="32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B221" s="32">
         <v>219</v>
       </c>
       <c r="C221" s="54"/>
-      <c r="D221" s="64"/>
-      <c r="E221" s="58"/>
+      <c r="D221" s="72"/>
+      <c r="E221" s="78"/>
       <c r="F221" s="54"/>
       <c r="G221" s="54"/>
       <c r="H221" s="54"/>
@@ -4798,14 +4798,14 @@
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" s="32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B222" s="32">
         <v>220</v>
       </c>
       <c r="C222" s="54"/>
-      <c r="D222" s="64"/>
-      <c r="E222" s="58"/>
+      <c r="D222" s="72"/>
+      <c r="E222" s="78"/>
       <c r="F222" s="54"/>
       <c r="G222" s="54"/>
       <c r="H222" s="54"/>
@@ -4813,14 +4813,14 @@
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" s="32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B223" s="32">
         <v>221</v>
       </c>
       <c r="C223" s="54"/>
-      <c r="D223" s="64"/>
-      <c r="E223" s="58"/>
+      <c r="D223" s="72"/>
+      <c r="E223" s="78"/>
       <c r="F223" s="54"/>
       <c r="G223" s="54"/>
       <c r="H223" s="54"/>
@@ -4828,14 +4828,14 @@
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" s="32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B224" s="32">
         <v>222</v>
       </c>
       <c r="C224" s="54"/>
-      <c r="D224" s="64"/>
-      <c r="E224" s="58"/>
+      <c r="D224" s="72"/>
+      <c r="E224" s="78"/>
       <c r="F224" s="54"/>
       <c r="G224" s="54"/>
       <c r="H224" s="54"/>
@@ -4843,14 +4843,14 @@
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" s="32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B225" s="32">
         <v>223</v>
       </c>
       <c r="C225" s="54"/>
-      <c r="D225" s="64"/>
-      <c r="E225" s="58"/>
+      <c r="D225" s="72"/>
+      <c r="E225" s="78"/>
       <c r="F225" s="54"/>
       <c r="G225" s="54"/>
       <c r="H225" s="54"/>
@@ -4860,13 +4860,13 @@
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" s="50" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B226" s="51">
         <v>224</v>
       </c>
-      <c r="C226" s="65"/>
-      <c r="D226" s="66" t="s">
+      <c r="C226" s="73"/>
+      <c r="D226" s="74" t="s">
         <v>29</v>
       </c>
       <c r="E226" s="54"/>
@@ -4879,13 +4879,13 @@
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" s="50" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B227" s="51">
         <v>225</v>
       </c>
-      <c r="C227" s="65"/>
-      <c r="D227" s="66"/>
+      <c r="C227" s="73"/>
+      <c r="D227" s="74"/>
       <c r="E227" s="54"/>
       <c r="F227" s="54"/>
       <c r="G227" s="54"/>
@@ -4894,13 +4894,13 @@
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" s="50" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B228" s="51">
         <v>226</v>
       </c>
-      <c r="C228" s="65"/>
-      <c r="D228" s="66"/>
+      <c r="C228" s="73"/>
+      <c r="D228" s="74"/>
       <c r="E228" s="54"/>
       <c r="F228" s="54"/>
       <c r="G228" s="54"/>
@@ -4909,13 +4909,13 @@
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" s="50" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B229" s="51">
         <v>227</v>
       </c>
-      <c r="C229" s="65"/>
-      <c r="D229" s="66"/>
+      <c r="C229" s="73"/>
+      <c r="D229" s="74"/>
       <c r="E229" s="54"/>
       <c r="F229" s="54"/>
       <c r="G229" s="54"/>
@@ -4924,13 +4924,13 @@
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" s="50" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B230" s="51">
         <v>228</v>
       </c>
-      <c r="C230" s="59"/>
-      <c r="D230" s="66"/>
+      <c r="C230" s="79"/>
+      <c r="D230" s="74"/>
       <c r="E230" s="54"/>
       <c r="F230" s="54"/>
       <c r="G230" s="54"/>
@@ -4939,13 +4939,13 @@
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" s="50" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B231" s="51">
         <v>229</v>
       </c>
-      <c r="C231" s="59"/>
-      <c r="D231" s="66"/>
+      <c r="C231" s="79"/>
+      <c r="D231" s="74"/>
       <c r="E231" s="54"/>
       <c r="F231" s="54"/>
       <c r="G231" s="54"/>
@@ -4954,13 +4954,13 @@
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" s="50" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B232" s="51">
         <v>230</v>
       </c>
-      <c r="C232" s="59"/>
-      <c r="D232" s="66"/>
+      <c r="C232" s="79"/>
+      <c r="D232" s="74"/>
       <c r="E232" s="54"/>
       <c r="F232" s="54"/>
       <c r="G232" s="54"/>
@@ -4969,13 +4969,13 @@
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" s="50" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B233" s="51">
         <v>231</v>
       </c>
-      <c r="C233" s="59"/>
-      <c r="D233" s="66"/>
+      <c r="C233" s="79"/>
+      <c r="D233" s="74"/>
       <c r="E233" s="54"/>
       <c r="F233" s="54"/>
       <c r="G233" s="54"/>
@@ -4986,12 +4986,12 @@
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" s="47" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B234" s="47">
         <v>232</v>
       </c>
-      <c r="C234" s="60" t="s">
+      <c r="C234" s="80" t="s">
         <v>30</v>
       </c>
       <c r="D234" s="54"/>
@@ -5005,29 +5005,29 @@
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" s="47" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B235" s="47">
         <v>233</v>
       </c>
-      <c r="C235" s="60"/>
+      <c r="C235" s="80"/>
       <c r="D235" s="54"/>
       <c r="E235" s="54"/>
       <c r="F235" s="54"/>
       <c r="G235" s="54"/>
       <c r="H235" s="54"/>
       <c r="I235" s="49" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" s="47" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B236" s="47">
         <v>234</v>
       </c>
-      <c r="C236" s="60"/>
+      <c r="C236" s="80"/>
       <c r="D236" s="54"/>
       <c r="E236" s="54"/>
       <c r="F236" s="54"/>
@@ -5039,12 +5039,12 @@
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" s="47" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B237" s="47">
         <v>235</v>
       </c>
-      <c r="C237" s="60"/>
+      <c r="C237" s="80"/>
       <c r="D237" s="54"/>
       <c r="E237" s="54"/>
       <c r="F237" s="54"/>
@@ -5356,6 +5356,108 @@
     </row>
   </sheetData>
   <mergeCells count="126">
+    <mergeCell ref="F194:F225"/>
+    <mergeCell ref="G194:G257"/>
+    <mergeCell ref="C198:C201"/>
+    <mergeCell ref="C202:C205"/>
+    <mergeCell ref="D202:D209"/>
+    <mergeCell ref="C206:C209"/>
+    <mergeCell ref="C210:C213"/>
+    <mergeCell ref="D210:D217"/>
+    <mergeCell ref="E210:E225"/>
+    <mergeCell ref="C214:C217"/>
+    <mergeCell ref="D250:D257"/>
+    <mergeCell ref="C254:C257"/>
+    <mergeCell ref="F226:F257"/>
+    <mergeCell ref="C230:C233"/>
+    <mergeCell ref="C234:C237"/>
+    <mergeCell ref="D234:D241"/>
+    <mergeCell ref="C238:C241"/>
+    <mergeCell ref="C242:C245"/>
+    <mergeCell ref="D242:D249"/>
+    <mergeCell ref="E242:E257"/>
+    <mergeCell ref="C246:C249"/>
+    <mergeCell ref="C250:C253"/>
+    <mergeCell ref="E194:E209"/>
+    <mergeCell ref="C162:C165"/>
+    <mergeCell ref="D162:D169"/>
+    <mergeCell ref="E162:E177"/>
+    <mergeCell ref="C218:C221"/>
+    <mergeCell ref="D218:D225"/>
+    <mergeCell ref="C222:C225"/>
+    <mergeCell ref="C226:C229"/>
+    <mergeCell ref="D226:D233"/>
+    <mergeCell ref="E226:E241"/>
+    <mergeCell ref="F162:F193"/>
+    <mergeCell ref="C166:C169"/>
+    <mergeCell ref="C170:C173"/>
+    <mergeCell ref="D170:D177"/>
+    <mergeCell ref="C174:C177"/>
+    <mergeCell ref="C178:C181"/>
+    <mergeCell ref="D178:D185"/>
+    <mergeCell ref="G130:G193"/>
+    <mergeCell ref="H130:H257"/>
+    <mergeCell ref="C134:C137"/>
+    <mergeCell ref="C138:C141"/>
+    <mergeCell ref="D138:D145"/>
+    <mergeCell ref="C142:C145"/>
+    <mergeCell ref="C146:C149"/>
+    <mergeCell ref="D146:D153"/>
+    <mergeCell ref="E146:E161"/>
+    <mergeCell ref="C150:C153"/>
+    <mergeCell ref="E178:E193"/>
+    <mergeCell ref="C182:C185"/>
+    <mergeCell ref="C186:C189"/>
+    <mergeCell ref="D186:D193"/>
+    <mergeCell ref="C190:C193"/>
+    <mergeCell ref="C194:C197"/>
+    <mergeCell ref="D194:D201"/>
+    <mergeCell ref="C130:C133"/>
+    <mergeCell ref="D130:D137"/>
+    <mergeCell ref="E130:E145"/>
+    <mergeCell ref="F130:F161"/>
+    <mergeCell ref="C154:C157"/>
+    <mergeCell ref="D154:D161"/>
+    <mergeCell ref="C158:C161"/>
+    <mergeCell ref="F98:F129"/>
+    <mergeCell ref="C102:C105"/>
+    <mergeCell ref="C106:C109"/>
+    <mergeCell ref="D106:D113"/>
+    <mergeCell ref="C110:C113"/>
+    <mergeCell ref="C114:C117"/>
+    <mergeCell ref="D114:D121"/>
+    <mergeCell ref="E114:E129"/>
+    <mergeCell ref="C118:C121"/>
+    <mergeCell ref="C122:C125"/>
+    <mergeCell ref="C90:C93"/>
+    <mergeCell ref="D90:D97"/>
+    <mergeCell ref="C94:C97"/>
+    <mergeCell ref="C98:C101"/>
+    <mergeCell ref="D98:D105"/>
+    <mergeCell ref="E98:E113"/>
+    <mergeCell ref="F66:F97"/>
+    <mergeCell ref="G66:G129"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="C74:C77"/>
+    <mergeCell ref="D74:D81"/>
+    <mergeCell ref="C78:C81"/>
+    <mergeCell ref="C82:C85"/>
+    <mergeCell ref="D82:D89"/>
+    <mergeCell ref="E82:E97"/>
+    <mergeCell ref="C86:C89"/>
+    <mergeCell ref="D122:D129"/>
+    <mergeCell ref="C126:C129"/>
+    <mergeCell ref="E50:E65"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="D58:D65"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="D66:D73"/>
+    <mergeCell ref="E66:E81"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="D34:D41"/>
+    <mergeCell ref="E34:E49"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="D2:D9"/>
     <mergeCell ref="E2:E17"/>
@@ -5380,108 +5482,6 @@
     <mergeCell ref="C26:C29"/>
     <mergeCell ref="D26:D33"/>
     <mergeCell ref="C30:C33"/>
-    <mergeCell ref="E50:E65"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="D58:D65"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="C66:C69"/>
-    <mergeCell ref="D66:D73"/>
-    <mergeCell ref="E66:E81"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="D34:D41"/>
-    <mergeCell ref="E34:E49"/>
-    <mergeCell ref="C90:C93"/>
-    <mergeCell ref="D90:D97"/>
-    <mergeCell ref="C94:C97"/>
-    <mergeCell ref="C98:C101"/>
-    <mergeCell ref="D98:D105"/>
-    <mergeCell ref="E98:E113"/>
-    <mergeCell ref="F66:F97"/>
-    <mergeCell ref="G66:G129"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="C74:C77"/>
-    <mergeCell ref="D74:D81"/>
-    <mergeCell ref="C78:C81"/>
-    <mergeCell ref="C82:C85"/>
-    <mergeCell ref="D82:D89"/>
-    <mergeCell ref="E82:E97"/>
-    <mergeCell ref="C86:C89"/>
-    <mergeCell ref="D122:D129"/>
-    <mergeCell ref="C126:C129"/>
-    <mergeCell ref="C130:C133"/>
-    <mergeCell ref="D130:D137"/>
-    <mergeCell ref="E130:E145"/>
-    <mergeCell ref="F130:F161"/>
-    <mergeCell ref="C154:C157"/>
-    <mergeCell ref="D154:D161"/>
-    <mergeCell ref="C158:C161"/>
-    <mergeCell ref="F98:F129"/>
-    <mergeCell ref="C102:C105"/>
-    <mergeCell ref="C106:C109"/>
-    <mergeCell ref="D106:D113"/>
-    <mergeCell ref="C110:C113"/>
-    <mergeCell ref="C114:C117"/>
-    <mergeCell ref="D114:D121"/>
-    <mergeCell ref="E114:E129"/>
-    <mergeCell ref="C118:C121"/>
-    <mergeCell ref="C122:C125"/>
-    <mergeCell ref="F162:F193"/>
-    <mergeCell ref="C166:C169"/>
-    <mergeCell ref="C170:C173"/>
-    <mergeCell ref="D170:D177"/>
-    <mergeCell ref="C174:C177"/>
-    <mergeCell ref="C178:C181"/>
-    <mergeCell ref="D178:D185"/>
-    <mergeCell ref="G130:G193"/>
-    <mergeCell ref="H130:H257"/>
-    <mergeCell ref="C134:C137"/>
-    <mergeCell ref="C138:C141"/>
-    <mergeCell ref="D138:D145"/>
-    <mergeCell ref="C142:C145"/>
-    <mergeCell ref="C146:C149"/>
-    <mergeCell ref="D146:D153"/>
-    <mergeCell ref="E146:E161"/>
-    <mergeCell ref="C150:C153"/>
-    <mergeCell ref="E178:E193"/>
-    <mergeCell ref="C182:C185"/>
-    <mergeCell ref="C186:C189"/>
-    <mergeCell ref="D186:D193"/>
-    <mergeCell ref="C190:C193"/>
-    <mergeCell ref="C194:C197"/>
-    <mergeCell ref="D194:D201"/>
-    <mergeCell ref="C162:C165"/>
-    <mergeCell ref="D162:D169"/>
-    <mergeCell ref="E162:E177"/>
-    <mergeCell ref="C218:C221"/>
-    <mergeCell ref="D218:D225"/>
-    <mergeCell ref="C222:C225"/>
-    <mergeCell ref="C226:C229"/>
-    <mergeCell ref="D226:D233"/>
-    <mergeCell ref="E226:E241"/>
-    <mergeCell ref="F194:F225"/>
-    <mergeCell ref="G194:G257"/>
-    <mergeCell ref="C198:C201"/>
-    <mergeCell ref="C202:C205"/>
-    <mergeCell ref="D202:D209"/>
-    <mergeCell ref="C206:C209"/>
-    <mergeCell ref="C210:C213"/>
-    <mergeCell ref="D210:D217"/>
-    <mergeCell ref="E210:E225"/>
-    <mergeCell ref="C214:C217"/>
-    <mergeCell ref="D250:D257"/>
-    <mergeCell ref="C254:C257"/>
-    <mergeCell ref="F226:F257"/>
-    <mergeCell ref="C230:C233"/>
-    <mergeCell ref="C234:C237"/>
-    <mergeCell ref="D234:D241"/>
-    <mergeCell ref="C238:C241"/>
-    <mergeCell ref="C242:C245"/>
-    <mergeCell ref="D242:D249"/>
-    <mergeCell ref="E242:E257"/>
-    <mergeCell ref="C246:C249"/>
-    <mergeCell ref="C250:C253"/>
-    <mergeCell ref="E194:E209"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5503,15 +5503,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="53" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B1" s="53" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B2" s="52">
         <v>1</v>
@@ -5519,7 +5519,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B3" s="29">
         <v>2</v>
@@ -5527,7 +5527,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B4" s="29">
         <v>10</v>
@@ -5535,7 +5535,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B5" s="29">
         <v>20</v>
@@ -5543,7 +5543,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B6" s="29">
         <v>21</v>
@@ -5551,7 +5551,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B7" s="29">
         <v>30</v>
@@ -5559,7 +5559,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B8" s="29">
         <v>31</v>
@@ -5567,7 +5567,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B9" s="29">
         <v>40</v>
@@ -5575,7 +5575,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B10" s="29">
         <v>41</v>
@@ -5583,7 +5583,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B11" s="29">
         <v>50</v>
@@ -5591,7 +5591,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B12" s="29">
         <v>51</v>
@@ -5599,7 +5599,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B13" s="29">
         <v>60</v>
@@ -5607,7 +5607,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B14" s="29">
         <v>61</v>
@@ -5615,7 +5615,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B15" s="29">
         <v>70</v>
@@ -5623,7 +5623,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B16" s="29">
         <v>80</v>
@@ -5631,7 +5631,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B17" s="29">
         <v>90</v>

</xml_diff>

<commit_message>
Vlsm táblázat javítása,wifi hálózat javítása
</commit_message>
<xml_diff>
--- a/Kisvállalat létszám.xlsx
+++ b/Kisvállalat létszám.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20396"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\School\11.o\Hálózat\projekt\fluffy-system\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\projekt\fluffy-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3679D178-B854-4281-AFB1-D5D356EBFBF7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D0B286-F70D-4F9D-8158-7DC99EA26B32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alap" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="66">
   <si>
     <t>I.em</t>
   </si>
@@ -210,6 +210,21 @@
   </si>
   <si>
     <t>S2</t>
+  </si>
+  <si>
+    <t>szórási</t>
+  </si>
+  <si>
+    <t>Wireless Router0-internet</t>
+  </si>
+  <si>
+    <t>Wireless Router1-internet</t>
+  </si>
+  <si>
+    <t>Wireless Router2-internet</t>
+  </si>
+  <si>
+    <t>Internet</t>
   </si>
 </sst>
 </file>
@@ -283,7 +298,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,6 +497,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="21">
     <border>
@@ -775,7 +796,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -881,46 +902,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -941,22 +938,51 @@
     <xf numFmtId="0" fontId="7" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -1346,8 +1372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12CB4148-414F-422C-94F5-AFDA695DCD79}">
   <dimension ref="A1:I257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L201" sqref="L201"/>
+    <sheetView tabSelected="1" topLeftCell="A213" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K241" sqref="K241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1386,7 +1412,7 @@
       <c r="C2" s="54"/>
       <c r="D2" s="54"/>
       <c r="E2" s="54"/>
-      <c r="F2" s="55" t="s">
+      <c r="F2" s="80" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="54"/>
@@ -1405,7 +1431,7 @@
       <c r="C3" s="54"/>
       <c r="D3" s="54"/>
       <c r="E3" s="54"/>
-      <c r="F3" s="55"/>
+      <c r="F3" s="80"/>
       <c r="G3" s="54"/>
       <c r="H3" s="54"/>
       <c r="I3" s="43"/>
@@ -1420,7 +1446,7 @@
       <c r="C4" s="54"/>
       <c r="D4" s="54"/>
       <c r="E4" s="54"/>
-      <c r="F4" s="55"/>
+      <c r="F4" s="80"/>
       <c r="G4" s="54"/>
       <c r="H4" s="54"/>
       <c r="I4" s="43"/>
@@ -1435,7 +1461,7 @@
       <c r="C5" s="54"/>
       <c r="D5" s="54"/>
       <c r="E5" s="54"/>
-      <c r="F5" s="55"/>
+      <c r="F5" s="80"/>
       <c r="G5" s="54"/>
       <c r="H5" s="54"/>
       <c r="I5" s="43"/>
@@ -1450,7 +1476,7 @@
       <c r="C6" s="54"/>
       <c r="D6" s="54"/>
       <c r="E6" s="54"/>
-      <c r="F6" s="55"/>
+      <c r="F6" s="80"/>
       <c r="G6" s="54"/>
       <c r="H6" s="54"/>
       <c r="I6" s="43"/>
@@ -1465,7 +1491,7 @@
       <c r="C7" s="54"/>
       <c r="D7" s="54"/>
       <c r="E7" s="54"/>
-      <c r="F7" s="55"/>
+      <c r="F7" s="80"/>
       <c r="G7" s="54"/>
       <c r="H7" s="54"/>
       <c r="I7" s="43"/>
@@ -1480,7 +1506,7 @@
       <c r="C8" s="54"/>
       <c r="D8" s="54"/>
       <c r="E8" s="54"/>
-      <c r="F8" s="55"/>
+      <c r="F8" s="80"/>
       <c r="G8" s="54"/>
       <c r="H8" s="54"/>
       <c r="I8" s="43"/>
@@ -1495,7 +1521,7 @@
       <c r="C9" s="54"/>
       <c r="D9" s="54"/>
       <c r="E9" s="54"/>
-      <c r="F9" s="55"/>
+      <c r="F9" s="80"/>
       <c r="G9" s="54"/>
       <c r="H9" s="54"/>
       <c r="I9" s="43"/>
@@ -1510,7 +1536,7 @@
       <c r="C10" s="54"/>
       <c r="D10" s="54"/>
       <c r="E10" s="54"/>
-      <c r="F10" s="55"/>
+      <c r="F10" s="80"/>
       <c r="G10" s="54"/>
       <c r="H10" s="54"/>
       <c r="I10" s="43"/>
@@ -1525,7 +1551,7 @@
       <c r="C11" s="54"/>
       <c r="D11" s="54"/>
       <c r="E11" s="54"/>
-      <c r="F11" s="55"/>
+      <c r="F11" s="80"/>
       <c r="G11" s="54"/>
       <c r="H11" s="54"/>
       <c r="I11" s="43"/>
@@ -1540,7 +1566,7 @@
       <c r="C12" s="54"/>
       <c r="D12" s="54"/>
       <c r="E12" s="54"/>
-      <c r="F12" s="55"/>
+      <c r="F12" s="80"/>
       <c r="G12" s="54"/>
       <c r="H12" s="54"/>
       <c r="I12" s="43"/>
@@ -1555,7 +1581,7 @@
       <c r="C13" s="54"/>
       <c r="D13" s="54"/>
       <c r="E13" s="54"/>
-      <c r="F13" s="55"/>
+      <c r="F13" s="80"/>
       <c r="G13" s="54"/>
       <c r="H13" s="54"/>
       <c r="I13" s="43"/>
@@ -1570,7 +1596,7 @@
       <c r="C14" s="54"/>
       <c r="D14" s="54"/>
       <c r="E14" s="54"/>
-      <c r="F14" s="55"/>
+      <c r="F14" s="80"/>
       <c r="G14" s="54"/>
       <c r="H14" s="54"/>
       <c r="I14" s="43"/>
@@ -1585,7 +1611,7 @@
       <c r="C15" s="54"/>
       <c r="D15" s="54"/>
       <c r="E15" s="54"/>
-      <c r="F15" s="55"/>
+      <c r="F15" s="80"/>
       <c r="G15" s="54"/>
       <c r="H15" s="54"/>
       <c r="I15" s="43"/>
@@ -1600,7 +1626,7 @@
       <c r="C16" s="54"/>
       <c r="D16" s="54"/>
       <c r="E16" s="54"/>
-      <c r="F16" s="55"/>
+      <c r="F16" s="80"/>
       <c r="G16" s="54"/>
       <c r="H16" s="54"/>
       <c r="I16" s="43"/>
@@ -1615,7 +1641,7 @@
       <c r="C17" s="54"/>
       <c r="D17" s="54"/>
       <c r="E17" s="54"/>
-      <c r="F17" s="55"/>
+      <c r="F17" s="80"/>
       <c r="G17" s="54"/>
       <c r="H17" s="54"/>
       <c r="I17" s="43"/>
@@ -1630,7 +1656,7 @@
       <c r="C18" s="54"/>
       <c r="D18" s="54"/>
       <c r="E18" s="54"/>
-      <c r="F18" s="55"/>
+      <c r="F18" s="80"/>
       <c r="G18" s="54"/>
       <c r="H18" s="54"/>
       <c r="I18" s="43"/>
@@ -1645,7 +1671,7 @@
       <c r="C19" s="54"/>
       <c r="D19" s="54"/>
       <c r="E19" s="54"/>
-      <c r="F19" s="55"/>
+      <c r="F19" s="80"/>
       <c r="G19" s="54"/>
       <c r="H19" s="54"/>
       <c r="I19" s="43"/>
@@ -1660,7 +1686,7 @@
       <c r="C20" s="54"/>
       <c r="D20" s="54"/>
       <c r="E20" s="54"/>
-      <c r="F20" s="55"/>
+      <c r="F20" s="80"/>
       <c r="G20" s="54"/>
       <c r="H20" s="54"/>
       <c r="I20" s="43"/>
@@ -1675,7 +1701,7 @@
       <c r="C21" s="54"/>
       <c r="D21" s="54"/>
       <c r="E21" s="54"/>
-      <c r="F21" s="55"/>
+      <c r="F21" s="80"/>
       <c r="G21" s="54"/>
       <c r="H21" s="54"/>
       <c r="I21" s="43"/>
@@ -1690,7 +1716,7 @@
       <c r="C22" s="54"/>
       <c r="D22" s="54"/>
       <c r="E22" s="54"/>
-      <c r="F22" s="55"/>
+      <c r="F22" s="80"/>
       <c r="G22" s="54"/>
       <c r="H22" s="54"/>
       <c r="I22" s="43"/>
@@ -1705,7 +1731,7 @@
       <c r="C23" s="54"/>
       <c r="D23" s="54"/>
       <c r="E23" s="54"/>
-      <c r="F23" s="55"/>
+      <c r="F23" s="80"/>
       <c r="G23" s="54"/>
       <c r="H23" s="54"/>
       <c r="I23" s="43"/>
@@ -1720,7 +1746,7 @@
       <c r="C24" s="54"/>
       <c r="D24" s="54"/>
       <c r="E24" s="54"/>
-      <c r="F24" s="55"/>
+      <c r="F24" s="80"/>
       <c r="G24" s="54"/>
       <c r="H24" s="54"/>
       <c r="I24" s="43"/>
@@ -1735,7 +1761,7 @@
       <c r="C25" s="54"/>
       <c r="D25" s="54"/>
       <c r="E25" s="54"/>
-      <c r="F25" s="55"/>
+      <c r="F25" s="80"/>
       <c r="G25" s="54"/>
       <c r="H25" s="54"/>
       <c r="I25" s="43"/>
@@ -1750,7 +1776,7 @@
       <c r="C26" s="54"/>
       <c r="D26" s="54"/>
       <c r="E26" s="54"/>
-      <c r="F26" s="55"/>
+      <c r="F26" s="80"/>
       <c r="G26" s="54"/>
       <c r="H26" s="54"/>
       <c r="I26" s="43"/>
@@ -1765,7 +1791,7 @@
       <c r="C27" s="54"/>
       <c r="D27" s="54"/>
       <c r="E27" s="54"/>
-      <c r="F27" s="55"/>
+      <c r="F27" s="80"/>
       <c r="G27" s="54"/>
       <c r="H27" s="54"/>
       <c r="I27" s="43"/>
@@ -1780,7 +1806,7 @@
       <c r="C28" s="54"/>
       <c r="D28" s="54"/>
       <c r="E28" s="54"/>
-      <c r="F28" s="55"/>
+      <c r="F28" s="80"/>
       <c r="G28" s="54"/>
       <c r="H28" s="54"/>
       <c r="I28" s="43"/>
@@ -1795,11 +1821,11 @@
       <c r="C29" s="54"/>
       <c r="D29" s="54"/>
       <c r="E29" s="54"/>
-      <c r="F29" s="55"/>
+      <c r="F29" s="80"/>
       <c r="G29" s="54"/>
       <c r="H29" s="54"/>
       <c r="I29" s="43" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1812,7 +1838,7 @@
       <c r="C30" s="54"/>
       <c r="D30" s="54"/>
       <c r="E30" s="54"/>
-      <c r="F30" s="55"/>
+      <c r="F30" s="80"/>
       <c r="G30" s="54"/>
       <c r="H30" s="54"/>
       <c r="I30" s="43" t="s">
@@ -1829,11 +1855,11 @@
       <c r="C31" s="54"/>
       <c r="D31" s="54"/>
       <c r="E31" s="54"/>
-      <c r="F31" s="55"/>
+      <c r="F31" s="80"/>
       <c r="G31" s="54"/>
       <c r="H31" s="54"/>
       <c r="I31" s="43" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1846,7 +1872,7 @@
       <c r="C32" s="54"/>
       <c r="D32" s="54"/>
       <c r="E32" s="54"/>
-      <c r="F32" s="55"/>
+      <c r="F32" s="80"/>
       <c r="G32" s="54"/>
       <c r="H32" s="54"/>
       <c r="I32" s="43" t="s">
@@ -1863,7 +1889,7 @@
       <c r="C33" s="54"/>
       <c r="D33" s="54"/>
       <c r="E33" s="54"/>
-      <c r="F33" s="55"/>
+      <c r="F33" s="80"/>
       <c r="G33" s="54"/>
       <c r="H33" s="54"/>
       <c r="I33" s="43" t="s">
@@ -1879,7 +1905,7 @@
       </c>
       <c r="C34" s="54"/>
       <c r="D34" s="54"/>
-      <c r="E34" s="58" t="s">
+      <c r="E34" s="79" t="s">
         <v>16</v>
       </c>
       <c r="F34" s="54"/>
@@ -1898,7 +1924,7 @@
       </c>
       <c r="C35" s="54"/>
       <c r="D35" s="54"/>
-      <c r="E35" s="58"/>
+      <c r="E35" s="79"/>
       <c r="F35" s="54"/>
       <c r="G35" s="54"/>
       <c r="H35" s="54"/>
@@ -1913,7 +1939,7 @@
       </c>
       <c r="C36" s="54"/>
       <c r="D36" s="54"/>
-      <c r="E36" s="58"/>
+      <c r="E36" s="79"/>
       <c r="F36" s="54"/>
       <c r="G36" s="54"/>
       <c r="H36" s="54"/>
@@ -1928,7 +1954,7 @@
       </c>
       <c r="C37" s="54"/>
       <c r="D37" s="54"/>
-      <c r="E37" s="58"/>
+      <c r="E37" s="79"/>
       <c r="F37" s="54"/>
       <c r="G37" s="54"/>
       <c r="H37" s="54"/>
@@ -1943,7 +1969,7 @@
       </c>
       <c r="C38" s="54"/>
       <c r="D38" s="54"/>
-      <c r="E38" s="58"/>
+      <c r="E38" s="79"/>
       <c r="F38" s="54"/>
       <c r="G38" s="54"/>
       <c r="H38" s="54"/>
@@ -1958,7 +1984,7 @@
       </c>
       <c r="C39" s="54"/>
       <c r="D39" s="54"/>
-      <c r="E39" s="58"/>
+      <c r="E39" s="79"/>
       <c r="F39" s="54"/>
       <c r="G39" s="54"/>
       <c r="H39" s="54"/>
@@ -1973,7 +1999,7 @@
       </c>
       <c r="C40" s="54"/>
       <c r="D40" s="54"/>
-      <c r="E40" s="58"/>
+      <c r="E40" s="79"/>
       <c r="F40" s="54"/>
       <c r="G40" s="54"/>
       <c r="H40" s="54"/>
@@ -1988,7 +2014,7 @@
       </c>
       <c r="C41" s="54"/>
       <c r="D41" s="54"/>
-      <c r="E41" s="58"/>
+      <c r="E41" s="79"/>
       <c r="F41" s="54"/>
       <c r="G41" s="54"/>
       <c r="H41" s="54"/>
@@ -2003,7 +2029,7 @@
       </c>
       <c r="C42" s="54"/>
       <c r="D42" s="54"/>
-      <c r="E42" s="58"/>
+      <c r="E42" s="79"/>
       <c r="F42" s="54"/>
       <c r="G42" s="54"/>
       <c r="H42" s="54"/>
@@ -2018,7 +2044,7 @@
       </c>
       <c r="C43" s="54"/>
       <c r="D43" s="54"/>
-      <c r="E43" s="58"/>
+      <c r="E43" s="79"/>
       <c r="F43" s="54"/>
       <c r="G43" s="54"/>
       <c r="H43" s="54"/>
@@ -2033,7 +2059,7 @@
       </c>
       <c r="C44" s="54"/>
       <c r="D44" s="54"/>
-      <c r="E44" s="58"/>
+      <c r="E44" s="79"/>
       <c r="F44" s="54"/>
       <c r="G44" s="54"/>
       <c r="H44" s="54"/>
@@ -2048,7 +2074,7 @@
       </c>
       <c r="C45" s="54"/>
       <c r="D45" s="54"/>
-      <c r="E45" s="58"/>
+      <c r="E45" s="79"/>
       <c r="F45" s="54"/>
       <c r="G45" s="54"/>
       <c r="H45" s="54"/>
@@ -2063,7 +2089,7 @@
       </c>
       <c r="C46" s="54"/>
       <c r="D46" s="54"/>
-      <c r="E46" s="58"/>
+      <c r="E46" s="79"/>
       <c r="F46" s="54"/>
       <c r="G46" s="54"/>
       <c r="H46" s="54"/>
@@ -2078,7 +2104,7 @@
       </c>
       <c r="C47" s="54"/>
       <c r="D47" s="54"/>
-      <c r="E47" s="58"/>
+      <c r="E47" s="79"/>
       <c r="F47" s="54"/>
       <c r="G47" s="54"/>
       <c r="H47" s="54"/>
@@ -2093,7 +2119,7 @@
       </c>
       <c r="C48" s="54"/>
       <c r="D48" s="54"/>
-      <c r="E48" s="58"/>
+      <c r="E48" s="79"/>
       <c r="F48" s="54"/>
       <c r="G48" s="54"/>
       <c r="H48" s="54"/>
@@ -2110,7 +2136,7 @@
       </c>
       <c r="C49" s="54"/>
       <c r="D49" s="54"/>
-      <c r="E49" s="58"/>
+      <c r="E49" s="79"/>
       <c r="F49" s="54"/>
       <c r="G49" s="54"/>
       <c r="H49" s="54"/>
@@ -2127,7 +2153,7 @@
       </c>
       <c r="C50" s="54"/>
       <c r="D50" s="54"/>
-      <c r="E50" s="56" t="s">
+      <c r="E50" s="77" t="s">
         <v>17</v>
       </c>
       <c r="F50" s="54"/>
@@ -2146,7 +2172,7 @@
       </c>
       <c r="C51" s="54"/>
       <c r="D51" s="54"/>
-      <c r="E51" s="56"/>
+      <c r="E51" s="77"/>
       <c r="F51" s="54"/>
       <c r="G51" s="54"/>
       <c r="H51" s="54"/>
@@ -2161,7 +2187,7 @@
       </c>
       <c r="C52" s="54"/>
       <c r="D52" s="54"/>
-      <c r="E52" s="56"/>
+      <c r="E52" s="77"/>
       <c r="F52" s="54"/>
       <c r="G52" s="54"/>
       <c r="H52" s="54"/>
@@ -2176,7 +2202,7 @@
       </c>
       <c r="C53" s="54"/>
       <c r="D53" s="54"/>
-      <c r="E53" s="56"/>
+      <c r="E53" s="77"/>
       <c r="F53" s="54"/>
       <c r="G53" s="54"/>
       <c r="H53" s="54"/>
@@ -2191,7 +2217,7 @@
       </c>
       <c r="C54" s="54"/>
       <c r="D54" s="54"/>
-      <c r="E54" s="56"/>
+      <c r="E54" s="77"/>
       <c r="F54" s="54"/>
       <c r="G54" s="54"/>
       <c r="H54" s="54"/>
@@ -2206,7 +2232,7 @@
       </c>
       <c r="C55" s="54"/>
       <c r="D55" s="54"/>
-      <c r="E55" s="56"/>
+      <c r="E55" s="77"/>
       <c r="F55" s="54"/>
       <c r="G55" s="54"/>
       <c r="H55" s="54"/>
@@ -2221,7 +2247,7 @@
       </c>
       <c r="C56" s="54"/>
       <c r="D56" s="54"/>
-      <c r="E56" s="56"/>
+      <c r="E56" s="77"/>
       <c r="F56" s="54"/>
       <c r="G56" s="54"/>
       <c r="H56" s="54"/>
@@ -2236,7 +2262,7 @@
       </c>
       <c r="C57" s="54"/>
       <c r="D57" s="54"/>
-      <c r="E57" s="56"/>
+      <c r="E57" s="77"/>
       <c r="F57" s="54"/>
       <c r="G57" s="54"/>
       <c r="H57" s="54"/>
@@ -2251,7 +2277,7 @@
       </c>
       <c r="C58" s="54"/>
       <c r="D58" s="54"/>
-      <c r="E58" s="56"/>
+      <c r="E58" s="77"/>
       <c r="F58" s="54"/>
       <c r="G58" s="54"/>
       <c r="H58" s="54"/>
@@ -2266,7 +2292,7 @@
       </c>
       <c r="C59" s="54"/>
       <c r="D59" s="54"/>
-      <c r="E59" s="56"/>
+      <c r="E59" s="77"/>
       <c r="F59" s="54"/>
       <c r="G59" s="54"/>
       <c r="H59" s="54"/>
@@ -2281,7 +2307,7 @@
       </c>
       <c r="C60" s="54"/>
       <c r="D60" s="54"/>
-      <c r="E60" s="56"/>
+      <c r="E60" s="77"/>
       <c r="F60" s="54"/>
       <c r="G60" s="54"/>
       <c r="H60" s="54"/>
@@ -2296,7 +2322,7 @@
       </c>
       <c r="C61" s="54"/>
       <c r="D61" s="54"/>
-      <c r="E61" s="56"/>
+      <c r="E61" s="77"/>
       <c r="F61" s="54"/>
       <c r="G61" s="54"/>
       <c r="H61" s="54"/>
@@ -2311,7 +2337,7 @@
       </c>
       <c r="C62" s="54"/>
       <c r="D62" s="54"/>
-      <c r="E62" s="56"/>
+      <c r="E62" s="77"/>
       <c r="F62" s="54"/>
       <c r="G62" s="54"/>
       <c r="H62" s="54"/>
@@ -2326,7 +2352,7 @@
       </c>
       <c r="C63" s="54"/>
       <c r="D63" s="54"/>
-      <c r="E63" s="56"/>
+      <c r="E63" s="77"/>
       <c r="F63" s="54"/>
       <c r="G63" s="54"/>
       <c r="H63" s="54"/>
@@ -2341,7 +2367,7 @@
       </c>
       <c r="C64" s="54"/>
       <c r="D64" s="54"/>
-      <c r="E64" s="56"/>
+      <c r="E64" s="77"/>
       <c r="F64" s="54"/>
       <c r="G64" s="54"/>
       <c r="H64" s="54"/>
@@ -2358,7 +2384,7 @@
       </c>
       <c r="C65" s="54"/>
       <c r="D65" s="54"/>
-      <c r="E65" s="56"/>
+      <c r="E65" s="77"/>
       <c r="F65" s="54"/>
       <c r="G65" s="54"/>
       <c r="H65" s="54"/>
@@ -2375,7 +2401,7 @@
       </c>
       <c r="C66" s="54"/>
       <c r="D66" s="54"/>
-      <c r="E66" s="57" t="s">
+      <c r="E66" s="78" t="s">
         <v>18</v>
       </c>
       <c r="F66" s="54"/>
@@ -2394,7 +2420,7 @@
       </c>
       <c r="C67" s="54"/>
       <c r="D67" s="54"/>
-      <c r="E67" s="57"/>
+      <c r="E67" s="78"/>
       <c r="F67" s="54"/>
       <c r="G67" s="54"/>
       <c r="H67" s="54"/>
@@ -2409,7 +2435,7 @@
       </c>
       <c r="C68" s="54"/>
       <c r="D68" s="54"/>
-      <c r="E68" s="57"/>
+      <c r="E68" s="78"/>
       <c r="F68" s="54"/>
       <c r="G68" s="54"/>
       <c r="H68" s="54"/>
@@ -2424,7 +2450,7 @@
       </c>
       <c r="C69" s="54"/>
       <c r="D69" s="54"/>
-      <c r="E69" s="57"/>
+      <c r="E69" s="78"/>
       <c r="F69" s="54"/>
       <c r="G69" s="54"/>
       <c r="H69" s="54"/>
@@ -2439,7 +2465,7 @@
       </c>
       <c r="C70" s="54"/>
       <c r="D70" s="54"/>
-      <c r="E70" s="57"/>
+      <c r="E70" s="78"/>
       <c r="F70" s="54"/>
       <c r="G70" s="54"/>
       <c r="H70" s="54"/>
@@ -2454,7 +2480,7 @@
       </c>
       <c r="C71" s="54"/>
       <c r="D71" s="54"/>
-      <c r="E71" s="57"/>
+      <c r="E71" s="78"/>
       <c r="F71" s="54"/>
       <c r="G71" s="54"/>
       <c r="H71" s="54"/>
@@ -2469,7 +2495,7 @@
       </c>
       <c r="C72" s="54"/>
       <c r="D72" s="54"/>
-      <c r="E72" s="57"/>
+      <c r="E72" s="78"/>
       <c r="F72" s="54"/>
       <c r="G72" s="54"/>
       <c r="H72" s="54"/>
@@ -2484,7 +2510,7 @@
       </c>
       <c r="C73" s="54"/>
       <c r="D73" s="54"/>
-      <c r="E73" s="57"/>
+      <c r="E73" s="78"/>
       <c r="F73" s="54"/>
       <c r="G73" s="54"/>
       <c r="H73" s="54"/>
@@ -2499,7 +2525,7 @@
       </c>
       <c r="C74" s="54"/>
       <c r="D74" s="54"/>
-      <c r="E74" s="57"/>
+      <c r="E74" s="78"/>
       <c r="F74" s="54"/>
       <c r="G74" s="54"/>
       <c r="H74" s="54"/>
@@ -2514,7 +2540,7 @@
       </c>
       <c r="C75" s="54"/>
       <c r="D75" s="54"/>
-      <c r="E75" s="57"/>
+      <c r="E75" s="78"/>
       <c r="F75" s="54"/>
       <c r="G75" s="54"/>
       <c r="H75" s="54"/>
@@ -2529,7 +2555,7 @@
       </c>
       <c r="C76" s="54"/>
       <c r="D76" s="54"/>
-      <c r="E76" s="57"/>
+      <c r="E76" s="78"/>
       <c r="F76" s="54"/>
       <c r="G76" s="54"/>
       <c r="H76" s="54"/>
@@ -2544,7 +2570,7 @@
       </c>
       <c r="C77" s="54"/>
       <c r="D77" s="54"/>
-      <c r="E77" s="57"/>
+      <c r="E77" s="78"/>
       <c r="F77" s="54"/>
       <c r="G77" s="54"/>
       <c r="H77" s="54"/>
@@ -2559,7 +2585,7 @@
       </c>
       <c r="C78" s="54"/>
       <c r="D78" s="54"/>
-      <c r="E78" s="57"/>
+      <c r="E78" s="78"/>
       <c r="F78" s="54"/>
       <c r="G78" s="54"/>
       <c r="H78" s="54"/>
@@ -2574,7 +2600,7 @@
       </c>
       <c r="C79" s="54"/>
       <c r="D79" s="54"/>
-      <c r="E79" s="57"/>
+      <c r="E79" s="78"/>
       <c r="F79" s="54"/>
       <c r="G79" s="54"/>
       <c r="H79" s="54"/>
@@ -2589,7 +2615,7 @@
       </c>
       <c r="C80" s="54"/>
       <c r="D80" s="54"/>
-      <c r="E80" s="57"/>
+      <c r="E80" s="78"/>
       <c r="F80" s="54"/>
       <c r="G80" s="54"/>
       <c r="H80" s="54"/>
@@ -2606,7 +2632,7 @@
       </c>
       <c r="C81" s="54"/>
       <c r="D81" s="54"/>
-      <c r="E81" s="57"/>
+      <c r="E81" s="78"/>
       <c r="F81" s="54"/>
       <c r="G81" s="54"/>
       <c r="H81" s="54"/>
@@ -2623,7 +2649,7 @@
       </c>
       <c r="C82" s="54"/>
       <c r="D82" s="54"/>
-      <c r="E82" s="60" t="s">
+      <c r="E82" s="76" t="s">
         <v>19</v>
       </c>
       <c r="F82" s="54"/>
@@ -2642,7 +2668,7 @@
       </c>
       <c r="C83" s="54"/>
       <c r="D83" s="54"/>
-      <c r="E83" s="60"/>
+      <c r="E83" s="76"/>
       <c r="F83" s="54"/>
       <c r="G83" s="54"/>
       <c r="H83" s="54"/>
@@ -2657,7 +2683,7 @@
       </c>
       <c r="C84" s="54"/>
       <c r="D84" s="54"/>
-      <c r="E84" s="60"/>
+      <c r="E84" s="76"/>
       <c r="F84" s="54"/>
       <c r="G84" s="54"/>
       <c r="H84" s="54"/>
@@ -2672,7 +2698,7 @@
       </c>
       <c r="C85" s="54"/>
       <c r="D85" s="54"/>
-      <c r="E85" s="60"/>
+      <c r="E85" s="76"/>
       <c r="F85" s="54"/>
       <c r="G85" s="54"/>
       <c r="H85" s="54"/>
@@ -2687,7 +2713,7 @@
       </c>
       <c r="C86" s="54"/>
       <c r="D86" s="54"/>
-      <c r="E86" s="60"/>
+      <c r="E86" s="76"/>
       <c r="F86" s="54"/>
       <c r="G86" s="54"/>
       <c r="H86" s="54"/>
@@ -2702,7 +2728,7 @@
       </c>
       <c r="C87" s="54"/>
       <c r="D87" s="54"/>
-      <c r="E87" s="60"/>
+      <c r="E87" s="76"/>
       <c r="F87" s="54"/>
       <c r="G87" s="54"/>
       <c r="H87" s="54"/>
@@ -2717,7 +2743,7 @@
       </c>
       <c r="C88" s="54"/>
       <c r="D88" s="54"/>
-      <c r="E88" s="60"/>
+      <c r="E88" s="76"/>
       <c r="F88" s="54"/>
       <c r="G88" s="54"/>
       <c r="H88" s="54"/>
@@ -2732,7 +2758,7 @@
       </c>
       <c r="C89" s="54"/>
       <c r="D89" s="54"/>
-      <c r="E89" s="60"/>
+      <c r="E89" s="76"/>
       <c r="F89" s="54"/>
       <c r="G89" s="54"/>
       <c r="H89" s="54"/>
@@ -2747,7 +2773,7 @@
       </c>
       <c r="C90" s="54"/>
       <c r="D90" s="54"/>
-      <c r="E90" s="60"/>
+      <c r="E90" s="76"/>
       <c r="F90" s="54"/>
       <c r="G90" s="54"/>
       <c r="H90" s="54"/>
@@ -2762,7 +2788,7 @@
       </c>
       <c r="C91" s="54"/>
       <c r="D91" s="54"/>
-      <c r="E91" s="60"/>
+      <c r="E91" s="76"/>
       <c r="F91" s="54"/>
       <c r="G91" s="54"/>
       <c r="H91" s="54"/>
@@ -2777,7 +2803,7 @@
       </c>
       <c r="C92" s="54"/>
       <c r="D92" s="54"/>
-      <c r="E92" s="60"/>
+      <c r="E92" s="76"/>
       <c r="F92" s="54"/>
       <c r="G92" s="54"/>
       <c r="H92" s="54"/>
@@ -2792,7 +2818,7 @@
       </c>
       <c r="C93" s="54"/>
       <c r="D93" s="54"/>
-      <c r="E93" s="60"/>
+      <c r="E93" s="76"/>
       <c r="F93" s="54"/>
       <c r="G93" s="54"/>
       <c r="H93" s="54"/>
@@ -2807,7 +2833,7 @@
       </c>
       <c r="C94" s="54"/>
       <c r="D94" s="54"/>
-      <c r="E94" s="60"/>
+      <c r="E94" s="76"/>
       <c r="F94" s="54"/>
       <c r="G94" s="54"/>
       <c r="H94" s="54"/>
@@ -2822,7 +2848,7 @@
       </c>
       <c r="C95" s="54"/>
       <c r="D95" s="54"/>
-      <c r="E95" s="60"/>
+      <c r="E95" s="76"/>
       <c r="F95" s="54"/>
       <c r="G95" s="54"/>
       <c r="H95" s="54"/>
@@ -2837,7 +2863,7 @@
       </c>
       <c r="C96" s="54"/>
       <c r="D96" s="54"/>
-      <c r="E96" s="60"/>
+      <c r="E96" s="76"/>
       <c r="F96" s="54"/>
       <c r="G96" s="54"/>
       <c r="H96" s="54"/>
@@ -2854,7 +2880,7 @@
       </c>
       <c r="C97" s="54"/>
       <c r="D97" s="54"/>
-      <c r="E97" s="60"/>
+      <c r="E97" s="76"/>
       <c r="F97" s="54"/>
       <c r="G97" s="54"/>
       <c r="H97" s="54"/>
@@ -2871,7 +2897,7 @@
       </c>
       <c r="C98" s="54"/>
       <c r="D98" s="54"/>
-      <c r="E98" s="59" t="s">
+      <c r="E98" s="75" t="s">
         <v>20</v>
       </c>
       <c r="F98" s="54"/>
@@ -2890,7 +2916,7 @@
       </c>
       <c r="C99" s="54"/>
       <c r="D99" s="54"/>
-      <c r="E99" s="59"/>
+      <c r="E99" s="75"/>
       <c r="F99" s="54"/>
       <c r="G99" s="54"/>
       <c r="H99" s="54"/>
@@ -2905,7 +2931,7 @@
       </c>
       <c r="C100" s="54"/>
       <c r="D100" s="54"/>
-      <c r="E100" s="59"/>
+      <c r="E100" s="75"/>
       <c r="F100" s="54"/>
       <c r="G100" s="54"/>
       <c r="H100" s="54"/>
@@ -2920,7 +2946,7 @@
       </c>
       <c r="C101" s="54"/>
       <c r="D101" s="54"/>
-      <c r="E101" s="59"/>
+      <c r="E101" s="75"/>
       <c r="F101" s="54"/>
       <c r="G101" s="54"/>
       <c r="H101" s="54"/>
@@ -2935,7 +2961,7 @@
       </c>
       <c r="C102" s="54"/>
       <c r="D102" s="54"/>
-      <c r="E102" s="59"/>
+      <c r="E102" s="75"/>
       <c r="F102" s="54"/>
       <c r="G102" s="54"/>
       <c r="H102" s="54"/>
@@ -2950,7 +2976,7 @@
       </c>
       <c r="C103" s="54"/>
       <c r="D103" s="54"/>
-      <c r="E103" s="59"/>
+      <c r="E103" s="75"/>
       <c r="F103" s="54"/>
       <c r="G103" s="54"/>
       <c r="H103" s="54"/>
@@ -2965,7 +2991,7 @@
       </c>
       <c r="C104" s="54"/>
       <c r="D104" s="54"/>
-      <c r="E104" s="59"/>
+      <c r="E104" s="75"/>
       <c r="F104" s="54"/>
       <c r="G104" s="54"/>
       <c r="H104" s="54"/>
@@ -2980,7 +3006,7 @@
       </c>
       <c r="C105" s="54"/>
       <c r="D105" s="54"/>
-      <c r="E105" s="59"/>
+      <c r="E105" s="75"/>
       <c r="F105" s="54"/>
       <c r="G105" s="54"/>
       <c r="H105" s="54"/>
@@ -2995,7 +3021,7 @@
       </c>
       <c r="C106" s="54"/>
       <c r="D106" s="54"/>
-      <c r="E106" s="59"/>
+      <c r="E106" s="75"/>
       <c r="F106" s="54"/>
       <c r="G106" s="54"/>
       <c r="H106" s="54"/>
@@ -3010,7 +3036,7 @@
       </c>
       <c r="C107" s="54"/>
       <c r="D107" s="54"/>
-      <c r="E107" s="59"/>
+      <c r="E107" s="75"/>
       <c r="F107" s="54"/>
       <c r="G107" s="54"/>
       <c r="H107" s="54"/>
@@ -3025,7 +3051,7 @@
       </c>
       <c r="C108" s="54"/>
       <c r="D108" s="54"/>
-      <c r="E108" s="59"/>
+      <c r="E108" s="75"/>
       <c r="F108" s="54"/>
       <c r="G108" s="54"/>
       <c r="H108" s="54"/>
@@ -3040,7 +3066,7 @@
       </c>
       <c r="C109" s="54"/>
       <c r="D109" s="54"/>
-      <c r="E109" s="59"/>
+      <c r="E109" s="75"/>
       <c r="F109" s="54"/>
       <c r="G109" s="54"/>
       <c r="H109" s="54"/>
@@ -3055,7 +3081,7 @@
       </c>
       <c r="C110" s="54"/>
       <c r="D110" s="54"/>
-      <c r="E110" s="59"/>
+      <c r="E110" s="75"/>
       <c r="F110" s="54"/>
       <c r="G110" s="54"/>
       <c r="H110" s="54"/>
@@ -3070,7 +3096,7 @@
       </c>
       <c r="C111" s="54"/>
       <c r="D111" s="54"/>
-      <c r="E111" s="59"/>
+      <c r="E111" s="75"/>
       <c r="F111" s="54"/>
       <c r="G111" s="54"/>
       <c r="H111" s="54"/>
@@ -3085,7 +3111,7 @@
       </c>
       <c r="C112" s="54"/>
       <c r="D112" s="54"/>
-      <c r="E112" s="59"/>
+      <c r="E112" s="75"/>
       <c r="F112" s="54"/>
       <c r="G112" s="54"/>
       <c r="H112" s="54"/>
@@ -3102,7 +3128,7 @@
       </c>
       <c r="C113" s="54"/>
       <c r="D113" s="54"/>
-      <c r="E113" s="59"/>
+      <c r="E113" s="75"/>
       <c r="F113" s="54"/>
       <c r="G113" s="54"/>
       <c r="H113" s="54"/>
@@ -3119,7 +3145,7 @@
       </c>
       <c r="C114" s="54"/>
       <c r="D114" s="54"/>
-      <c r="E114" s="64" t="s">
+      <c r="E114" s="74" t="s">
         <v>21</v>
       </c>
       <c r="F114" s="54"/>
@@ -3138,7 +3164,7 @@
       </c>
       <c r="C115" s="54"/>
       <c r="D115" s="54"/>
-      <c r="E115" s="64"/>
+      <c r="E115" s="74"/>
       <c r="F115" s="54"/>
       <c r="G115" s="54"/>
       <c r="H115" s="54"/>
@@ -3153,7 +3179,7 @@
       </c>
       <c r="C116" s="54"/>
       <c r="D116" s="54"/>
-      <c r="E116" s="64"/>
+      <c r="E116" s="74"/>
       <c r="F116" s="54"/>
       <c r="G116" s="54"/>
       <c r="H116" s="54"/>
@@ -3168,7 +3194,7 @@
       </c>
       <c r="C117" s="54"/>
       <c r="D117" s="54"/>
-      <c r="E117" s="64"/>
+      <c r="E117" s="74"/>
       <c r="F117" s="54"/>
       <c r="G117" s="54"/>
       <c r="H117" s="54"/>
@@ -3183,7 +3209,7 @@
       </c>
       <c r="C118" s="54"/>
       <c r="D118" s="54"/>
-      <c r="E118" s="64"/>
+      <c r="E118" s="74"/>
       <c r="F118" s="54"/>
       <c r="G118" s="54"/>
       <c r="H118" s="54"/>
@@ -3198,7 +3224,7 @@
       </c>
       <c r="C119" s="54"/>
       <c r="D119" s="54"/>
-      <c r="E119" s="64"/>
+      <c r="E119" s="74"/>
       <c r="F119" s="54"/>
       <c r="G119" s="54"/>
       <c r="H119" s="54"/>
@@ -3213,7 +3239,7 @@
       </c>
       <c r="C120" s="54"/>
       <c r="D120" s="54"/>
-      <c r="E120" s="64"/>
+      <c r="E120" s="74"/>
       <c r="F120" s="54"/>
       <c r="G120" s="54"/>
       <c r="H120" s="54"/>
@@ -3228,7 +3254,7 @@
       </c>
       <c r="C121" s="54"/>
       <c r="D121" s="54"/>
-      <c r="E121" s="64"/>
+      <c r="E121" s="74"/>
       <c r="F121" s="54"/>
       <c r="G121" s="54"/>
       <c r="H121" s="54"/>
@@ -3243,7 +3269,7 @@
       </c>
       <c r="C122" s="54"/>
       <c r="D122" s="54"/>
-      <c r="E122" s="64"/>
+      <c r="E122" s="74"/>
       <c r="F122" s="54"/>
       <c r="G122" s="54"/>
       <c r="H122" s="54"/>
@@ -3258,7 +3284,7 @@
       </c>
       <c r="C123" s="54"/>
       <c r="D123" s="54"/>
-      <c r="E123" s="64"/>
+      <c r="E123" s="74"/>
       <c r="F123" s="54"/>
       <c r="G123" s="54"/>
       <c r="H123" s="54"/>
@@ -3273,7 +3299,7 @@
       </c>
       <c r="C124" s="54"/>
       <c r="D124" s="54"/>
-      <c r="E124" s="64"/>
+      <c r="E124" s="74"/>
       <c r="F124" s="54"/>
       <c r="G124" s="54"/>
       <c r="H124" s="54"/>
@@ -3288,7 +3314,7 @@
       </c>
       <c r="C125" s="54"/>
       <c r="D125" s="54"/>
-      <c r="E125" s="64"/>
+      <c r="E125" s="74"/>
       <c r="F125" s="54"/>
       <c r="G125" s="54"/>
       <c r="H125" s="54"/>
@@ -3303,7 +3329,7 @@
       </c>
       <c r="C126" s="54"/>
       <c r="D126" s="54"/>
-      <c r="E126" s="64"/>
+      <c r="E126" s="74"/>
       <c r="F126" s="54"/>
       <c r="G126" s="54"/>
       <c r="H126" s="54"/>
@@ -3318,7 +3344,7 @@
       </c>
       <c r="C127" s="54"/>
       <c r="D127" s="54"/>
-      <c r="E127" s="64"/>
+      <c r="E127" s="74"/>
       <c r="F127" s="54"/>
       <c r="G127" s="54"/>
       <c r="H127" s="54"/>
@@ -3333,7 +3359,7 @@
       </c>
       <c r="C128" s="54"/>
       <c r="D128" s="54"/>
-      <c r="E128" s="64"/>
+      <c r="E128" s="74"/>
       <c r="F128" s="54"/>
       <c r="G128" s="54"/>
       <c r="H128" s="54"/>
@@ -3350,7 +3376,7 @@
       </c>
       <c r="C129" s="54"/>
       <c r="D129" s="54"/>
-      <c r="E129" s="64"/>
+      <c r="E129" s="74"/>
       <c r="F129" s="54"/>
       <c r="G129" s="54"/>
       <c r="H129" s="54"/>
@@ -3367,7 +3393,7 @@
       </c>
       <c r="C130" s="54"/>
       <c r="D130" s="54"/>
-      <c r="E130" s="61" t="s">
+      <c r="E130" s="67" t="s">
         <v>22</v>
       </c>
       <c r="F130" s="54"/>
@@ -3386,7 +3412,7 @@
       </c>
       <c r="C131" s="54"/>
       <c r="D131" s="54"/>
-      <c r="E131" s="62"/>
+      <c r="E131" s="68"/>
       <c r="F131" s="54"/>
       <c r="G131" s="54"/>
       <c r="H131" s="54"/>
@@ -3401,7 +3427,7 @@
       </c>
       <c r="C132" s="54"/>
       <c r="D132" s="54"/>
-      <c r="E132" s="62"/>
+      <c r="E132" s="68"/>
       <c r="F132" s="54"/>
       <c r="G132" s="54"/>
       <c r="H132" s="54"/>
@@ -3416,7 +3442,7 @@
       </c>
       <c r="C133" s="54"/>
       <c r="D133" s="54"/>
-      <c r="E133" s="62"/>
+      <c r="E133" s="68"/>
       <c r="F133" s="54"/>
       <c r="G133" s="54"/>
       <c r="H133" s="54"/>
@@ -3431,7 +3457,7 @@
       </c>
       <c r="C134" s="54"/>
       <c r="D134" s="54"/>
-      <c r="E134" s="62"/>
+      <c r="E134" s="68"/>
       <c r="F134" s="54"/>
       <c r="G134" s="54"/>
       <c r="H134" s="54"/>
@@ -3446,7 +3472,7 @@
       </c>
       <c r="C135" s="54"/>
       <c r="D135" s="54"/>
-      <c r="E135" s="62"/>
+      <c r="E135" s="68"/>
       <c r="F135" s="54"/>
       <c r="G135" s="54"/>
       <c r="H135" s="54"/>
@@ -3461,7 +3487,7 @@
       </c>
       <c r="C136" s="54"/>
       <c r="D136" s="54"/>
-      <c r="E136" s="62"/>
+      <c r="E136" s="68"/>
       <c r="F136" s="54"/>
       <c r="G136" s="54"/>
       <c r="H136" s="54"/>
@@ -3476,7 +3502,7 @@
       </c>
       <c r="C137" s="54"/>
       <c r="D137" s="54"/>
-      <c r="E137" s="62"/>
+      <c r="E137" s="68"/>
       <c r="F137" s="54"/>
       <c r="G137" s="54"/>
       <c r="H137" s="54"/>
@@ -3491,7 +3517,7 @@
       </c>
       <c r="C138" s="54"/>
       <c r="D138" s="54"/>
-      <c r="E138" s="62"/>
+      <c r="E138" s="68"/>
       <c r="F138" s="54"/>
       <c r="G138" s="54"/>
       <c r="H138" s="54"/>
@@ -3506,7 +3532,7 @@
       </c>
       <c r="C139" s="54"/>
       <c r="D139" s="54"/>
-      <c r="E139" s="62"/>
+      <c r="E139" s="68"/>
       <c r="F139" s="54"/>
       <c r="G139" s="54"/>
       <c r="H139" s="54"/>
@@ -3521,7 +3547,7 @@
       </c>
       <c r="C140" s="54"/>
       <c r="D140" s="54"/>
-      <c r="E140" s="62"/>
+      <c r="E140" s="68"/>
       <c r="F140" s="54"/>
       <c r="G140" s="54"/>
       <c r="H140" s="54"/>
@@ -3536,7 +3562,7 @@
       </c>
       <c r="C141" s="54"/>
       <c r="D141" s="54"/>
-      <c r="E141" s="62"/>
+      <c r="E141" s="68"/>
       <c r="F141" s="54"/>
       <c r="G141" s="54"/>
       <c r="H141" s="54"/>
@@ -3551,7 +3577,7 @@
       </c>
       <c r="C142" s="54"/>
       <c r="D142" s="54"/>
-      <c r="E142" s="62"/>
+      <c r="E142" s="68"/>
       <c r="F142" s="54"/>
       <c r="G142" s="54"/>
       <c r="H142" s="54"/>
@@ -3566,7 +3592,7 @@
       </c>
       <c r="C143" s="54"/>
       <c r="D143" s="54"/>
-      <c r="E143" s="62"/>
+      <c r="E143" s="68"/>
       <c r="F143" s="54"/>
       <c r="G143" s="54"/>
       <c r="H143" s="54"/>
@@ -3581,7 +3607,7 @@
       </c>
       <c r="C144" s="54"/>
       <c r="D144" s="54"/>
-      <c r="E144" s="62"/>
+      <c r="E144" s="68"/>
       <c r="F144" s="54"/>
       <c r="G144" s="54"/>
       <c r="H144" s="54"/>
@@ -3598,7 +3624,7 @@
       </c>
       <c r="C145" s="54"/>
       <c r="D145" s="54"/>
-      <c r="E145" s="63"/>
+      <c r="E145" s="69"/>
       <c r="F145" s="54"/>
       <c r="G145" s="54"/>
       <c r="H145" s="54"/>
@@ -3615,7 +3641,7 @@
       </c>
       <c r="C146" s="54"/>
       <c r="D146" s="54"/>
-      <c r="E146" s="61" t="s">
+      <c r="E146" s="67" t="s">
         <v>23</v>
       </c>
       <c r="F146" s="54"/>
@@ -3634,7 +3660,7 @@
       </c>
       <c r="C147" s="54"/>
       <c r="D147" s="54"/>
-      <c r="E147" s="62"/>
+      <c r="E147" s="68"/>
       <c r="F147" s="54"/>
       <c r="G147" s="54"/>
       <c r="H147" s="54"/>
@@ -3649,7 +3675,7 @@
       </c>
       <c r="C148" s="54"/>
       <c r="D148" s="54"/>
-      <c r="E148" s="62"/>
+      <c r="E148" s="68"/>
       <c r="F148" s="54"/>
       <c r="G148" s="54"/>
       <c r="H148" s="54"/>
@@ -3664,7 +3690,7 @@
       </c>
       <c r="C149" s="54"/>
       <c r="D149" s="54"/>
-      <c r="E149" s="62"/>
+      <c r="E149" s="68"/>
       <c r="F149" s="54"/>
       <c r="G149" s="54"/>
       <c r="H149" s="54"/>
@@ -3679,7 +3705,7 @@
       </c>
       <c r="C150" s="54"/>
       <c r="D150" s="54"/>
-      <c r="E150" s="62"/>
+      <c r="E150" s="68"/>
       <c r="F150" s="54"/>
       <c r="G150" s="54"/>
       <c r="H150" s="54"/>
@@ -3694,7 +3720,7 @@
       </c>
       <c r="C151" s="54"/>
       <c r="D151" s="54"/>
-      <c r="E151" s="62"/>
+      <c r="E151" s="68"/>
       <c r="F151" s="54"/>
       <c r="G151" s="54"/>
       <c r="H151" s="54"/>
@@ -3709,7 +3735,7 @@
       </c>
       <c r="C152" s="54"/>
       <c r="D152" s="54"/>
-      <c r="E152" s="62"/>
+      <c r="E152" s="68"/>
       <c r="F152" s="54"/>
       <c r="G152" s="54"/>
       <c r="H152" s="54"/>
@@ -3724,7 +3750,7 @@
       </c>
       <c r="C153" s="54"/>
       <c r="D153" s="54"/>
-      <c r="E153" s="62"/>
+      <c r="E153" s="68"/>
       <c r="F153" s="54"/>
       <c r="G153" s="54"/>
       <c r="H153" s="54"/>
@@ -3739,7 +3765,7 @@
       </c>
       <c r="C154" s="54"/>
       <c r="D154" s="54"/>
-      <c r="E154" s="62"/>
+      <c r="E154" s="68"/>
       <c r="F154" s="54"/>
       <c r="G154" s="54"/>
       <c r="H154" s="54"/>
@@ -3754,7 +3780,7 @@
       </c>
       <c r="C155" s="54"/>
       <c r="D155" s="54"/>
-      <c r="E155" s="62"/>
+      <c r="E155" s="68"/>
       <c r="F155" s="54"/>
       <c r="G155" s="54"/>
       <c r="H155" s="54"/>
@@ -3769,7 +3795,7 @@
       </c>
       <c r="C156" s="54"/>
       <c r="D156" s="54"/>
-      <c r="E156" s="62"/>
+      <c r="E156" s="68"/>
       <c r="F156" s="54"/>
       <c r="G156" s="54"/>
       <c r="H156" s="54"/>
@@ -3784,7 +3810,7 @@
       </c>
       <c r="C157" s="54"/>
       <c r="D157" s="54"/>
-      <c r="E157" s="62"/>
+      <c r="E157" s="68"/>
       <c r="F157" s="54"/>
       <c r="G157" s="54"/>
       <c r="H157" s="54"/>
@@ -3799,7 +3825,7 @@
       </c>
       <c r="C158" s="54"/>
       <c r="D158" s="54"/>
-      <c r="E158" s="62"/>
+      <c r="E158" s="68"/>
       <c r="F158" s="54"/>
       <c r="G158" s="54"/>
       <c r="H158" s="54"/>
@@ -3814,7 +3840,7 @@
       </c>
       <c r="C159" s="54"/>
       <c r="D159" s="54"/>
-      <c r="E159" s="62"/>
+      <c r="E159" s="68"/>
       <c r="F159" s="54"/>
       <c r="G159" s="54"/>
       <c r="H159" s="54"/>
@@ -3829,7 +3855,7 @@
       </c>
       <c r="C160" s="54"/>
       <c r="D160" s="54"/>
-      <c r="E160" s="62"/>
+      <c r="E160" s="68"/>
       <c r="F160" s="54"/>
       <c r="G160" s="54"/>
       <c r="H160" s="54"/>
@@ -3846,7 +3872,7 @@
       </c>
       <c r="C161" s="54"/>
       <c r="D161" s="54"/>
-      <c r="E161" s="63"/>
+      <c r="E161" s="69"/>
       <c r="F161" s="54"/>
       <c r="G161" s="54"/>
       <c r="H161" s="54"/>
@@ -3863,7 +3889,7 @@
       </c>
       <c r="C162" s="54"/>
       <c r="D162" s="54"/>
-      <c r="E162" s="69" t="s">
+      <c r="E162" s="61" t="s">
         <v>26</v>
       </c>
       <c r="F162" s="54"/>
@@ -3882,7 +3908,7 @@
       </c>
       <c r="C163" s="54"/>
       <c r="D163" s="54"/>
-      <c r="E163" s="70"/>
+      <c r="E163" s="62"/>
       <c r="F163" s="54"/>
       <c r="G163" s="54"/>
       <c r="H163" s="54"/>
@@ -3897,7 +3923,7 @@
       </c>
       <c r="C164" s="54"/>
       <c r="D164" s="54"/>
-      <c r="E164" s="70"/>
+      <c r="E164" s="62"/>
       <c r="F164" s="54"/>
       <c r="G164" s="54"/>
       <c r="H164" s="54"/>
@@ -3912,7 +3938,7 @@
       </c>
       <c r="C165" s="54"/>
       <c r="D165" s="54"/>
-      <c r="E165" s="70"/>
+      <c r="E165" s="62"/>
       <c r="F165" s="54"/>
       <c r="G165" s="54"/>
       <c r="H165" s="54"/>
@@ -3927,7 +3953,7 @@
       </c>
       <c r="C166" s="54"/>
       <c r="D166" s="54"/>
-      <c r="E166" s="70"/>
+      <c r="E166" s="62"/>
       <c r="F166" s="54"/>
       <c r="G166" s="54"/>
       <c r="H166" s="54"/>
@@ -3942,7 +3968,7 @@
       </c>
       <c r="C167" s="54"/>
       <c r="D167" s="54"/>
-      <c r="E167" s="70"/>
+      <c r="E167" s="62"/>
       <c r="F167" s="54"/>
       <c r="G167" s="54"/>
       <c r="H167" s="54"/>
@@ -3957,7 +3983,7 @@
       </c>
       <c r="C168" s="54"/>
       <c r="D168" s="54"/>
-      <c r="E168" s="70"/>
+      <c r="E168" s="62"/>
       <c r="F168" s="54"/>
       <c r="G168" s="54"/>
       <c r="H168" s="54"/>
@@ -3972,7 +3998,7 @@
       </c>
       <c r="C169" s="54"/>
       <c r="D169" s="54"/>
-      <c r="E169" s="70"/>
+      <c r="E169" s="62"/>
       <c r="F169" s="54"/>
       <c r="G169" s="54"/>
       <c r="H169" s="54"/>
@@ -3987,7 +4013,7 @@
       </c>
       <c r="C170" s="54"/>
       <c r="D170" s="54"/>
-      <c r="E170" s="70"/>
+      <c r="E170" s="62"/>
       <c r="F170" s="54"/>
       <c r="G170" s="54"/>
       <c r="H170" s="54"/>
@@ -4002,7 +4028,7 @@
       </c>
       <c r="C171" s="54"/>
       <c r="D171" s="54"/>
-      <c r="E171" s="70"/>
+      <c r="E171" s="62"/>
       <c r="F171" s="54"/>
       <c r="G171" s="54"/>
       <c r="H171" s="54"/>
@@ -4017,7 +4043,7 @@
       </c>
       <c r="C172" s="54"/>
       <c r="D172" s="54"/>
-      <c r="E172" s="70"/>
+      <c r="E172" s="62"/>
       <c r="F172" s="54"/>
       <c r="G172" s="54"/>
       <c r="H172" s="54"/>
@@ -4032,7 +4058,7 @@
       </c>
       <c r="C173" s="54"/>
       <c r="D173" s="54"/>
-      <c r="E173" s="70"/>
+      <c r="E173" s="62"/>
       <c r="F173" s="54"/>
       <c r="G173" s="54"/>
       <c r="H173" s="54"/>
@@ -4047,7 +4073,7 @@
       </c>
       <c r="C174" s="54"/>
       <c r="D174" s="54"/>
-      <c r="E174" s="70"/>
+      <c r="E174" s="62"/>
       <c r="F174" s="54"/>
       <c r="G174" s="54"/>
       <c r="H174" s="54"/>
@@ -4062,7 +4088,7 @@
       </c>
       <c r="C175" s="54"/>
       <c r="D175" s="54"/>
-      <c r="E175" s="70"/>
+      <c r="E175" s="62"/>
       <c r="F175" s="54"/>
       <c r="G175" s="54"/>
       <c r="H175" s="54"/>
@@ -4077,7 +4103,7 @@
       </c>
       <c r="C176" s="54"/>
       <c r="D176" s="54"/>
-      <c r="E176" s="70"/>
+      <c r="E176" s="62"/>
       <c r="F176" s="54"/>
       <c r="G176" s="54"/>
       <c r="H176" s="54"/>
@@ -4094,7 +4120,7 @@
       </c>
       <c r="C177" s="54"/>
       <c r="D177" s="54"/>
-      <c r="E177" s="71"/>
+      <c r="E177" s="63"/>
       <c r="F177" s="54"/>
       <c r="G177" s="54"/>
       <c r="H177" s="54"/>
@@ -4111,7 +4137,7 @@
       </c>
       <c r="C178" s="54"/>
       <c r="D178" s="54"/>
-      <c r="E178" s="65" t="s">
+      <c r="E178" s="70" t="s">
         <v>27</v>
       </c>
       <c r="F178" s="54"/>
@@ -4130,7 +4156,7 @@
       </c>
       <c r="C179" s="54"/>
       <c r="D179" s="54"/>
-      <c r="E179" s="65"/>
+      <c r="E179" s="70"/>
       <c r="F179" s="54"/>
       <c r="G179" s="54"/>
       <c r="H179" s="54"/>
@@ -4145,7 +4171,7 @@
       </c>
       <c r="C180" s="54"/>
       <c r="D180" s="54"/>
-      <c r="E180" s="65"/>
+      <c r="E180" s="70"/>
       <c r="F180" s="54"/>
       <c r="G180" s="54"/>
       <c r="H180" s="54"/>
@@ -4160,7 +4186,7 @@
       </c>
       <c r="C181" s="54"/>
       <c r="D181" s="54"/>
-      <c r="E181" s="65"/>
+      <c r="E181" s="70"/>
       <c r="F181" s="54"/>
       <c r="G181" s="54"/>
       <c r="H181" s="54"/>
@@ -4175,7 +4201,7 @@
       </c>
       <c r="C182" s="54"/>
       <c r="D182" s="54"/>
-      <c r="E182" s="65"/>
+      <c r="E182" s="70"/>
       <c r="F182" s="54"/>
       <c r="G182" s="54"/>
       <c r="H182" s="54"/>
@@ -4190,7 +4216,7 @@
       </c>
       <c r="C183" s="54"/>
       <c r="D183" s="54"/>
-      <c r="E183" s="65"/>
+      <c r="E183" s="70"/>
       <c r="F183" s="54"/>
       <c r="G183" s="54"/>
       <c r="H183" s="54"/>
@@ -4205,7 +4231,7 @@
       </c>
       <c r="C184" s="54"/>
       <c r="D184" s="54"/>
-      <c r="E184" s="65"/>
+      <c r="E184" s="70"/>
       <c r="F184" s="54"/>
       <c r="G184" s="54"/>
       <c r="H184" s="54"/>
@@ -4220,7 +4246,7 @@
       </c>
       <c r="C185" s="54"/>
       <c r="D185" s="54"/>
-      <c r="E185" s="65"/>
+      <c r="E185" s="70"/>
       <c r="F185" s="54"/>
       <c r="G185" s="54"/>
       <c r="H185" s="54"/>
@@ -4235,7 +4261,7 @@
       </c>
       <c r="C186" s="54"/>
       <c r="D186" s="54"/>
-      <c r="E186" s="65"/>
+      <c r="E186" s="70"/>
       <c r="F186" s="54"/>
       <c r="G186" s="54"/>
       <c r="H186" s="54"/>
@@ -4250,7 +4276,7 @@
       </c>
       <c r="C187" s="54"/>
       <c r="D187" s="54"/>
-      <c r="E187" s="65"/>
+      <c r="E187" s="70"/>
       <c r="F187" s="54"/>
       <c r="G187" s="54"/>
       <c r="H187" s="54"/>
@@ -4265,7 +4291,7 @@
       </c>
       <c r="C188" s="54"/>
       <c r="D188" s="54"/>
-      <c r="E188" s="65"/>
+      <c r="E188" s="70"/>
       <c r="F188" s="54"/>
       <c r="G188" s="54"/>
       <c r="H188" s="54"/>
@@ -4280,7 +4306,7 @@
       </c>
       <c r="C189" s="54"/>
       <c r="D189" s="54"/>
-      <c r="E189" s="65"/>
+      <c r="E189" s="70"/>
       <c r="F189" s="54"/>
       <c r="G189" s="54"/>
       <c r="H189" s="54"/>
@@ -4295,7 +4321,7 @@
       </c>
       <c r="C190" s="54"/>
       <c r="D190" s="54"/>
-      <c r="E190" s="65"/>
+      <c r="E190" s="70"/>
       <c r="F190" s="54"/>
       <c r="G190" s="54"/>
       <c r="H190" s="54"/>
@@ -4310,7 +4336,7 @@
       </c>
       <c r="C191" s="54"/>
       <c r="D191" s="54"/>
-      <c r="E191" s="65"/>
+      <c r="E191" s="70"/>
       <c r="F191" s="54"/>
       <c r="G191" s="54"/>
       <c r="H191" s="54"/>
@@ -4325,7 +4351,7 @@
       </c>
       <c r="C192" s="54"/>
       <c r="D192" s="54"/>
-      <c r="E192" s="65"/>
+      <c r="E192" s="70"/>
       <c r="F192" s="54"/>
       <c r="G192" s="54"/>
       <c r="H192" s="54"/>
@@ -4342,7 +4368,7 @@
       </c>
       <c r="C193" s="54"/>
       <c r="D193" s="54"/>
-      <c r="E193" s="65"/>
+      <c r="E193" s="70"/>
       <c r="F193" s="54"/>
       <c r="G193" s="54"/>
       <c r="H193" s="54"/>
@@ -4358,7 +4384,7 @@
         <v>192</v>
       </c>
       <c r="C194" s="54"/>
-      <c r="D194" s="66" t="s">
+      <c r="D194" s="71" t="s">
         <v>25</v>
       </c>
       <c r="E194" s="54"/>
@@ -4377,7 +4403,7 @@
         <v>193</v>
       </c>
       <c r="C195" s="54"/>
-      <c r="D195" s="67"/>
+      <c r="D195" s="72"/>
       <c r="E195" s="54"/>
       <c r="F195" s="54"/>
       <c r="G195" s="54"/>
@@ -4392,7 +4418,7 @@
         <v>194</v>
       </c>
       <c r="C196" s="54"/>
-      <c r="D196" s="67"/>
+      <c r="D196" s="72"/>
       <c r="E196" s="54"/>
       <c r="F196" s="54"/>
       <c r="G196" s="54"/>
@@ -4407,7 +4433,7 @@
         <v>195</v>
       </c>
       <c r="C197" s="54"/>
-      <c r="D197" s="67"/>
+      <c r="D197" s="72"/>
       <c r="E197" s="54"/>
       <c r="F197" s="54"/>
       <c r="G197" s="54"/>
@@ -4422,7 +4448,7 @@
         <v>196</v>
       </c>
       <c r="C198" s="54"/>
-      <c r="D198" s="67"/>
+      <c r="D198" s="72"/>
       <c r="E198" s="54"/>
       <c r="F198" s="54"/>
       <c r="G198" s="54"/>
@@ -4437,7 +4463,7 @@
         <v>197</v>
       </c>
       <c r="C199" s="54"/>
-      <c r="D199" s="67"/>
+      <c r="D199" s="72"/>
       <c r="E199" s="54"/>
       <c r="F199" s="54"/>
       <c r="G199" s="54"/>
@@ -4452,7 +4478,7 @@
         <v>198</v>
       </c>
       <c r="C200" s="54"/>
-      <c r="D200" s="67"/>
+      <c r="D200" s="72"/>
       <c r="E200" s="54"/>
       <c r="F200" s="54"/>
       <c r="G200" s="54"/>
@@ -4469,7 +4495,7 @@
         <v>199</v>
       </c>
       <c r="C201" s="54"/>
-      <c r="D201" s="68"/>
+      <c r="D201" s="73"/>
       <c r="E201" s="54"/>
       <c r="F201" s="54"/>
       <c r="G201" s="54"/>
@@ -4486,7 +4512,7 @@
         <v>200</v>
       </c>
       <c r="C202" s="54"/>
-      <c r="D202" s="75" t="s">
+      <c r="D202" s="55" t="s">
         <v>24</v>
       </c>
       <c r="E202" s="54"/>
@@ -4505,7 +4531,7 @@
         <v>201</v>
       </c>
       <c r="C203" s="54"/>
-      <c r="D203" s="75"/>
+      <c r="D203" s="55"/>
       <c r="E203" s="54"/>
       <c r="F203" s="54"/>
       <c r="G203" s="54"/>
@@ -4520,7 +4546,7 @@
         <v>202</v>
       </c>
       <c r="C204" s="54"/>
-      <c r="D204" s="75"/>
+      <c r="D204" s="55"/>
       <c r="E204" s="54"/>
       <c r="F204" s="54"/>
       <c r="G204" s="54"/>
@@ -4535,7 +4561,7 @@
         <v>203</v>
       </c>
       <c r="C205" s="54"/>
-      <c r="D205" s="75"/>
+      <c r="D205" s="55"/>
       <c r="E205" s="54"/>
       <c r="F205" s="54"/>
       <c r="G205" s="54"/>
@@ -4550,7 +4576,7 @@
         <v>204</v>
       </c>
       <c r="C206" s="54"/>
-      <c r="D206" s="75"/>
+      <c r="D206" s="55"/>
       <c r="E206" s="54"/>
       <c r="F206" s="54"/>
       <c r="G206" s="54"/>
@@ -4565,7 +4591,7 @@
         <v>205</v>
       </c>
       <c r="C207" s="54"/>
-      <c r="D207" s="75"/>
+      <c r="D207" s="55"/>
       <c r="E207" s="54"/>
       <c r="F207" s="54"/>
       <c r="G207" s="54"/>
@@ -4580,7 +4606,7 @@
         <v>206</v>
       </c>
       <c r="C208" s="54"/>
-      <c r="D208" s="75"/>
+      <c r="D208" s="55"/>
       <c r="E208" s="54"/>
       <c r="F208" s="54"/>
       <c r="G208" s="54"/>
@@ -4597,7 +4623,7 @@
         <v>207</v>
       </c>
       <c r="C209" s="54"/>
-      <c r="D209" s="75"/>
+      <c r="D209" s="55"/>
       <c r="E209" s="54"/>
       <c r="F209" s="54"/>
       <c r="G209" s="54"/>
@@ -4613,9 +4639,9 @@
       <c r="B210" s="32">
         <v>208</v>
       </c>
-      <c r="C210" s="76"/>
-      <c r="D210" s="77"/>
-      <c r="E210" s="78" t="s">
+      <c r="C210" s="56"/>
+      <c r="D210" s="57"/>
+      <c r="E210" s="58" t="s">
         <v>34</v>
       </c>
       <c r="F210" s="54"/>
@@ -4632,9 +4658,9 @@
       <c r="B211" s="32">
         <v>209</v>
       </c>
-      <c r="C211" s="76"/>
-      <c r="D211" s="77"/>
-      <c r="E211" s="78"/>
+      <c r="C211" s="56"/>
+      <c r="D211" s="57"/>
+      <c r="E211" s="58"/>
       <c r="F211" s="54"/>
       <c r="G211" s="54"/>
       <c r="H211" s="54"/>
@@ -4649,9 +4675,9 @@
       <c r="B212" s="32">
         <v>210</v>
       </c>
-      <c r="C212" s="76"/>
-      <c r="D212" s="77"/>
-      <c r="E212" s="78"/>
+      <c r="C212" s="56"/>
+      <c r="D212" s="57"/>
+      <c r="E212" s="58"/>
       <c r="F212" s="54"/>
       <c r="G212" s="54"/>
       <c r="H212" s="54"/>
@@ -4666,9 +4692,9 @@
       <c r="B213" s="32">
         <v>211</v>
       </c>
-      <c r="C213" s="76"/>
-      <c r="D213" s="77"/>
-      <c r="E213" s="78"/>
+      <c r="C213" s="56"/>
+      <c r="D213" s="57"/>
+      <c r="E213" s="58"/>
       <c r="F213" s="54"/>
       <c r="G213" s="54"/>
       <c r="H213" s="54"/>
@@ -4683,9 +4709,9 @@
       <c r="B214" s="32">
         <v>212</v>
       </c>
-      <c r="C214" s="76"/>
-      <c r="D214" s="77"/>
-      <c r="E214" s="78"/>
+      <c r="C214" s="56"/>
+      <c r="D214" s="57"/>
+      <c r="E214" s="58"/>
       <c r="F214" s="54"/>
       <c r="G214" s="54"/>
       <c r="H214" s="54"/>
@@ -4698,9 +4724,9 @@
       <c r="B215" s="32">
         <v>213</v>
       </c>
-      <c r="C215" s="76"/>
-      <c r="D215" s="77"/>
-      <c r="E215" s="78"/>
+      <c r="C215" s="56"/>
+      <c r="D215" s="57"/>
+      <c r="E215" s="58"/>
       <c r="F215" s="54"/>
       <c r="G215" s="54"/>
       <c r="H215" s="54"/>
@@ -4713,9 +4739,9 @@
       <c r="B216" s="32">
         <v>214</v>
       </c>
-      <c r="C216" s="76"/>
-      <c r="D216" s="77"/>
-      <c r="E216" s="78"/>
+      <c r="C216" s="56"/>
+      <c r="D216" s="57"/>
+      <c r="E216" s="58"/>
       <c r="F216" s="54"/>
       <c r="G216" s="54"/>
       <c r="H216" s="54"/>
@@ -4728,9 +4754,9 @@
       <c r="B217" s="32">
         <v>215</v>
       </c>
-      <c r="C217" s="76"/>
-      <c r="D217" s="77"/>
-      <c r="E217" s="78"/>
+      <c r="C217" s="56"/>
+      <c r="D217" s="57"/>
+      <c r="E217" s="58"/>
       <c r="F217" s="54"/>
       <c r="G217" s="54"/>
       <c r="H217" s="54"/>
@@ -4744,8 +4770,8 @@
         <v>216</v>
       </c>
       <c r="C218" s="54"/>
-      <c r="D218" s="72"/>
-      <c r="E218" s="78"/>
+      <c r="D218" s="64"/>
+      <c r="E218" s="58"/>
       <c r="F218" s="54"/>
       <c r="G218" s="54"/>
       <c r="H218" s="54"/>
@@ -4759,8 +4785,8 @@
         <v>217</v>
       </c>
       <c r="C219" s="54"/>
-      <c r="D219" s="72"/>
-      <c r="E219" s="78"/>
+      <c r="D219" s="64"/>
+      <c r="E219" s="58"/>
       <c r="F219" s="54"/>
       <c r="G219" s="54"/>
       <c r="H219" s="54"/>
@@ -4774,8 +4800,8 @@
         <v>218</v>
       </c>
       <c r="C220" s="54"/>
-      <c r="D220" s="72"/>
-      <c r="E220" s="78"/>
+      <c r="D220" s="64"/>
+      <c r="E220" s="58"/>
       <c r="F220" s="54"/>
       <c r="G220" s="54"/>
       <c r="H220" s="54"/>
@@ -4789,8 +4815,8 @@
         <v>219</v>
       </c>
       <c r="C221" s="54"/>
-      <c r="D221" s="72"/>
-      <c r="E221" s="78"/>
+      <c r="D221" s="64"/>
+      <c r="E221" s="58"/>
       <c r="F221" s="54"/>
       <c r="G221" s="54"/>
       <c r="H221" s="54"/>
@@ -4804,8 +4830,8 @@
         <v>220</v>
       </c>
       <c r="C222" s="54"/>
-      <c r="D222" s="72"/>
-      <c r="E222" s="78"/>
+      <c r="D222" s="64"/>
+      <c r="E222" s="58"/>
       <c r="F222" s="54"/>
       <c r="G222" s="54"/>
       <c r="H222" s="54"/>
@@ -4819,8 +4845,8 @@
         <v>221</v>
       </c>
       <c r="C223" s="54"/>
-      <c r="D223" s="72"/>
-      <c r="E223" s="78"/>
+      <c r="D223" s="64"/>
+      <c r="E223" s="58"/>
       <c r="F223" s="54"/>
       <c r="G223" s="54"/>
       <c r="H223" s="54"/>
@@ -4834,8 +4860,8 @@
         <v>222</v>
       </c>
       <c r="C224" s="54"/>
-      <c r="D224" s="72"/>
-      <c r="E224" s="78"/>
+      <c r="D224" s="64"/>
+      <c r="E224" s="58"/>
       <c r="F224" s="54"/>
       <c r="G224" s="54"/>
       <c r="H224" s="54"/>
@@ -4849,8 +4875,8 @@
         <v>223</v>
       </c>
       <c r="C225" s="54"/>
-      <c r="D225" s="72"/>
-      <c r="E225" s="78"/>
+      <c r="D225" s="64"/>
+      <c r="E225" s="58"/>
       <c r="F225" s="54"/>
       <c r="G225" s="54"/>
       <c r="H225" s="54"/>
@@ -4865,8 +4891,8 @@
       <c r="B226" s="51">
         <v>224</v>
       </c>
-      <c r="C226" s="73"/>
-      <c r="D226" s="74" t="s">
+      <c r="C226" s="65"/>
+      <c r="D226" s="66" t="s">
         <v>29</v>
       </c>
       <c r="E226" s="54"/>
@@ -4884,8 +4910,8 @@
       <c r="B227" s="51">
         <v>225</v>
       </c>
-      <c r="C227" s="73"/>
-      <c r="D227" s="74"/>
+      <c r="C227" s="65"/>
+      <c r="D227" s="66"/>
       <c r="E227" s="54"/>
       <c r="F227" s="54"/>
       <c r="G227" s="54"/>
@@ -4899,8 +4925,8 @@
       <c r="B228" s="51">
         <v>226</v>
       </c>
-      <c r="C228" s="73"/>
-      <c r="D228" s="74"/>
+      <c r="C228" s="65"/>
+      <c r="D228" s="66"/>
       <c r="E228" s="54"/>
       <c r="F228" s="54"/>
       <c r="G228" s="54"/>
@@ -4914,8 +4940,8 @@
       <c r="B229" s="51">
         <v>227</v>
       </c>
-      <c r="C229" s="73"/>
-      <c r="D229" s="74"/>
+      <c r="C229" s="65"/>
+      <c r="D229" s="66"/>
       <c r="E229" s="54"/>
       <c r="F229" s="54"/>
       <c r="G229" s="54"/>
@@ -4929,8 +4955,8 @@
       <c r="B230" s="51">
         <v>228</v>
       </c>
-      <c r="C230" s="79"/>
-      <c r="D230" s="74"/>
+      <c r="C230" s="59"/>
+      <c r="D230" s="66"/>
       <c r="E230" s="54"/>
       <c r="F230" s="54"/>
       <c r="G230" s="54"/>
@@ -4944,8 +4970,8 @@
       <c r="B231" s="51">
         <v>229</v>
       </c>
-      <c r="C231" s="79"/>
-      <c r="D231" s="74"/>
+      <c r="C231" s="59"/>
+      <c r="D231" s="66"/>
       <c r="E231" s="54"/>
       <c r="F231" s="54"/>
       <c r="G231" s="54"/>
@@ -4959,8 +4985,8 @@
       <c r="B232" s="51">
         <v>230</v>
       </c>
-      <c r="C232" s="79"/>
-      <c r="D232" s="74"/>
+      <c r="C232" s="59"/>
+      <c r="D232" s="66"/>
       <c r="E232" s="54"/>
       <c r="F232" s="54"/>
       <c r="G232" s="54"/>
@@ -4974,8 +5000,8 @@
       <c r="B233" s="51">
         <v>231</v>
       </c>
-      <c r="C233" s="79"/>
-      <c r="D233" s="74"/>
+      <c r="C233" s="59"/>
+      <c r="D233" s="66"/>
       <c r="E233" s="54"/>
       <c r="F233" s="54"/>
       <c r="G233" s="54"/>
@@ -4991,7 +5017,7 @@
       <c r="B234" s="47">
         <v>232</v>
       </c>
-      <c r="C234" s="80" t="s">
+      <c r="C234" s="60" t="s">
         <v>30</v>
       </c>
       <c r="D234" s="54"/>
@@ -5010,7 +5036,7 @@
       <c r="B235" s="47">
         <v>233</v>
       </c>
-      <c r="C235" s="80"/>
+      <c r="C235" s="60"/>
       <c r="D235" s="54"/>
       <c r="E235" s="54"/>
       <c r="F235" s="54"/>
@@ -5027,7 +5053,7 @@
       <c r="B236" s="47">
         <v>234</v>
       </c>
-      <c r="C236" s="80"/>
+      <c r="C236" s="60"/>
       <c r="D236" s="54"/>
       <c r="E236" s="54"/>
       <c r="F236" s="54"/>
@@ -5044,7 +5070,7 @@
       <c r="B237" s="47">
         <v>235</v>
       </c>
-      <c r="C237" s="80"/>
+      <c r="C237" s="60"/>
       <c r="D237" s="54"/>
       <c r="E237" s="54"/>
       <c r="F237" s="54"/>
@@ -5115,124 +5141,138 @@
       <c r="I241" s="29"/>
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A242" t="s">
+      <c r="A242" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="B242">
+      <c r="B242" s="82">
         <v>240</v>
       </c>
       <c r="C242" s="54"/>
-      <c r="D242" s="54"/>
+      <c r="D242" s="83" t="s">
+        <v>65</v>
+      </c>
       <c r="E242" s="54"/>
       <c r="F242" s="54"/>
       <c r="G242" s="54"/>
       <c r="H242" s="54"/>
-      <c r="I242" s="29"/>
+      <c r="I242" s="81" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A243" t="s">
+      <c r="A243" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="B243">
+      <c r="B243" s="82">
         <v>241</v>
       </c>
       <c r="C243" s="54"/>
-      <c r="D243" s="54"/>
+      <c r="D243" s="83"/>
       <c r="E243" s="54"/>
       <c r="F243" s="54"/>
       <c r="G243" s="54"/>
       <c r="H243" s="54"/>
-      <c r="I243" s="29"/>
+      <c r="I243" s="81" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A244" t="s">
+      <c r="A244" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="B244">
+      <c r="B244" s="82">
         <v>242</v>
       </c>
       <c r="C244" s="54"/>
-      <c r="D244" s="54"/>
+      <c r="D244" s="83"/>
       <c r="E244" s="54"/>
       <c r="F244" s="54"/>
       <c r="G244" s="54"/>
       <c r="H244" s="54"/>
-      <c r="I244" s="29"/>
+      <c r="I244" s="81" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A245" t="s">
+      <c r="A245" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="B245">
+      <c r="B245" s="82">
         <v>243</v>
       </c>
       <c r="C245" s="54"/>
-      <c r="D245" s="54"/>
+      <c r="D245" s="83"/>
       <c r="E245" s="54"/>
       <c r="F245" s="54"/>
       <c r="G245" s="54"/>
       <c r="H245" s="54"/>
-      <c r="I245" s="29"/>
+      <c r="I245" s="81" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A246" t="s">
+      <c r="A246" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="B246">
+      <c r="B246" s="82">
         <v>244</v>
       </c>
       <c r="C246" s="54"/>
-      <c r="D246" s="54"/>
+      <c r="D246" s="83"/>
       <c r="E246" s="54"/>
       <c r="F246" s="54"/>
       <c r="G246" s="54"/>
       <c r="H246" s="54"/>
-      <c r="I246" s="29"/>
+      <c r="I246" s="81"/>
     </row>
     <row r="247" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A247" t="s">
+      <c r="A247" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="B247">
+      <c r="B247" s="82">
         <v>245</v>
       </c>
       <c r="C247" s="54"/>
-      <c r="D247" s="54"/>
+      <c r="D247" s="83"/>
       <c r="E247" s="54"/>
       <c r="F247" s="54"/>
       <c r="G247" s="54"/>
       <c r="H247" s="54"/>
-      <c r="I247" s="29"/>
+      <c r="I247" s="81"/>
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A248" t="s">
+      <c r="A248" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="B248">
+      <c r="B248" s="82">
         <v>246</v>
       </c>
       <c r="C248" s="54"/>
-      <c r="D248" s="54"/>
+      <c r="D248" s="83"/>
       <c r="E248" s="54"/>
       <c r="F248" s="54"/>
       <c r="G248" s="54"/>
       <c r="H248" s="54"/>
-      <c r="I248" s="29"/>
+      <c r="I248" s="81" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A249" t="s">
+      <c r="A249" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="B249">
+      <c r="B249" s="82">
         <v>247</v>
       </c>
       <c r="C249" s="54"/>
-      <c r="D249" s="54"/>
+      <c r="D249" s="83"/>
       <c r="E249" s="54"/>
       <c r="F249" s="54"/>
       <c r="G249" s="54"/>
       <c r="H249" s="54"/>
-      <c r="I249" s="29"/>
+      <c r="I249" s="81" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
@@ -5356,38 +5396,76 @@
     </row>
   </sheetData>
   <mergeCells count="126">
-    <mergeCell ref="F194:F225"/>
-    <mergeCell ref="G194:G257"/>
-    <mergeCell ref="C198:C201"/>
-    <mergeCell ref="C202:C205"/>
-    <mergeCell ref="D202:D209"/>
-    <mergeCell ref="C206:C209"/>
-    <mergeCell ref="C210:C213"/>
-    <mergeCell ref="D210:D217"/>
-    <mergeCell ref="E210:E225"/>
-    <mergeCell ref="C214:C217"/>
-    <mergeCell ref="D250:D257"/>
-    <mergeCell ref="C254:C257"/>
-    <mergeCell ref="F226:F257"/>
-    <mergeCell ref="C230:C233"/>
-    <mergeCell ref="C234:C237"/>
-    <mergeCell ref="D234:D241"/>
-    <mergeCell ref="C238:C241"/>
-    <mergeCell ref="C242:C245"/>
-    <mergeCell ref="D242:D249"/>
-    <mergeCell ref="E242:E257"/>
-    <mergeCell ref="C246:C249"/>
-    <mergeCell ref="C250:C253"/>
-    <mergeCell ref="E194:E209"/>
-    <mergeCell ref="C162:C165"/>
-    <mergeCell ref="D162:D169"/>
-    <mergeCell ref="E162:E177"/>
-    <mergeCell ref="C218:C221"/>
-    <mergeCell ref="D218:D225"/>
-    <mergeCell ref="C222:C225"/>
-    <mergeCell ref="C226:C229"/>
-    <mergeCell ref="D226:D233"/>
-    <mergeCell ref="E226:E241"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D9"/>
+    <mergeCell ref="E2:E17"/>
+    <mergeCell ref="F2:F33"/>
+    <mergeCell ref="G2:G65"/>
+    <mergeCell ref="H2:H129"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="F34:F65"/>
+    <mergeCell ref="C38:C41"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="D42:D49"/>
+    <mergeCell ref="C46:C49"/>
+    <mergeCell ref="C50:C53"/>
+    <mergeCell ref="D50:D57"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D25"/>
+    <mergeCell ref="E18:E33"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D26:D33"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="E50:E65"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="D58:D65"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="D66:D73"/>
+    <mergeCell ref="E66:E81"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="D34:D41"/>
+    <mergeCell ref="E34:E49"/>
+    <mergeCell ref="C90:C93"/>
+    <mergeCell ref="D90:D97"/>
+    <mergeCell ref="C94:C97"/>
+    <mergeCell ref="C98:C101"/>
+    <mergeCell ref="D98:D105"/>
+    <mergeCell ref="E98:E113"/>
+    <mergeCell ref="F66:F97"/>
+    <mergeCell ref="G66:G129"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="C74:C77"/>
+    <mergeCell ref="D74:D81"/>
+    <mergeCell ref="C78:C81"/>
+    <mergeCell ref="C82:C85"/>
+    <mergeCell ref="D82:D89"/>
+    <mergeCell ref="E82:E97"/>
+    <mergeCell ref="C86:C89"/>
+    <mergeCell ref="D122:D129"/>
+    <mergeCell ref="C126:C129"/>
+    <mergeCell ref="C130:C133"/>
+    <mergeCell ref="D130:D137"/>
+    <mergeCell ref="E130:E145"/>
+    <mergeCell ref="F130:F161"/>
+    <mergeCell ref="C154:C157"/>
+    <mergeCell ref="D154:D161"/>
+    <mergeCell ref="C158:C161"/>
+    <mergeCell ref="F98:F129"/>
+    <mergeCell ref="C102:C105"/>
+    <mergeCell ref="C106:C109"/>
+    <mergeCell ref="D106:D113"/>
+    <mergeCell ref="C110:C113"/>
+    <mergeCell ref="C114:C117"/>
+    <mergeCell ref="D114:D121"/>
+    <mergeCell ref="E114:E129"/>
+    <mergeCell ref="C118:C121"/>
+    <mergeCell ref="C122:C125"/>
     <mergeCell ref="F162:F193"/>
     <mergeCell ref="C166:C169"/>
     <mergeCell ref="C170:C173"/>
@@ -5412,76 +5490,38 @@
     <mergeCell ref="C190:C193"/>
     <mergeCell ref="C194:C197"/>
     <mergeCell ref="D194:D201"/>
-    <mergeCell ref="C130:C133"/>
-    <mergeCell ref="D130:D137"/>
-    <mergeCell ref="E130:E145"/>
-    <mergeCell ref="F130:F161"/>
-    <mergeCell ref="C154:C157"/>
-    <mergeCell ref="D154:D161"/>
-    <mergeCell ref="C158:C161"/>
-    <mergeCell ref="F98:F129"/>
-    <mergeCell ref="C102:C105"/>
-    <mergeCell ref="C106:C109"/>
-    <mergeCell ref="D106:D113"/>
-    <mergeCell ref="C110:C113"/>
-    <mergeCell ref="C114:C117"/>
-    <mergeCell ref="D114:D121"/>
-    <mergeCell ref="E114:E129"/>
-    <mergeCell ref="C118:C121"/>
-    <mergeCell ref="C122:C125"/>
-    <mergeCell ref="C90:C93"/>
-    <mergeCell ref="D90:D97"/>
-    <mergeCell ref="C94:C97"/>
-    <mergeCell ref="C98:C101"/>
-    <mergeCell ref="D98:D105"/>
-    <mergeCell ref="E98:E113"/>
-    <mergeCell ref="F66:F97"/>
-    <mergeCell ref="G66:G129"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="C74:C77"/>
-    <mergeCell ref="D74:D81"/>
-    <mergeCell ref="C78:C81"/>
-    <mergeCell ref="C82:C85"/>
-    <mergeCell ref="D82:D89"/>
-    <mergeCell ref="E82:E97"/>
-    <mergeCell ref="C86:C89"/>
-    <mergeCell ref="D122:D129"/>
-    <mergeCell ref="C126:C129"/>
-    <mergeCell ref="E50:E65"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="D58:D65"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="C66:C69"/>
-    <mergeCell ref="D66:D73"/>
-    <mergeCell ref="E66:E81"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="D34:D41"/>
-    <mergeCell ref="E34:E49"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="D2:D9"/>
-    <mergeCell ref="E2:E17"/>
-    <mergeCell ref="F2:F33"/>
-    <mergeCell ref="G2:G65"/>
-    <mergeCell ref="H2:H129"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="D10:D17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="F34:F65"/>
-    <mergeCell ref="C38:C41"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="D42:D49"/>
-    <mergeCell ref="C46:C49"/>
-    <mergeCell ref="C50:C53"/>
-    <mergeCell ref="D50:D57"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D25"/>
-    <mergeCell ref="E18:E33"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="D26:D33"/>
-    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="C162:C165"/>
+    <mergeCell ref="D162:D169"/>
+    <mergeCell ref="E162:E177"/>
+    <mergeCell ref="C218:C221"/>
+    <mergeCell ref="D218:D225"/>
+    <mergeCell ref="C222:C225"/>
+    <mergeCell ref="C226:C229"/>
+    <mergeCell ref="D226:D233"/>
+    <mergeCell ref="E226:E241"/>
+    <mergeCell ref="F194:F225"/>
+    <mergeCell ref="G194:G257"/>
+    <mergeCell ref="C198:C201"/>
+    <mergeCell ref="C202:C205"/>
+    <mergeCell ref="D202:D209"/>
+    <mergeCell ref="C206:C209"/>
+    <mergeCell ref="C210:C213"/>
+    <mergeCell ref="D210:D217"/>
+    <mergeCell ref="E210:E225"/>
+    <mergeCell ref="C214:C217"/>
+    <mergeCell ref="D250:D257"/>
+    <mergeCell ref="C254:C257"/>
+    <mergeCell ref="F226:F257"/>
+    <mergeCell ref="C230:C233"/>
+    <mergeCell ref="C234:C237"/>
+    <mergeCell ref="D234:D241"/>
+    <mergeCell ref="C238:C241"/>
+    <mergeCell ref="C242:C245"/>
+    <mergeCell ref="D242:D249"/>
+    <mergeCell ref="E242:E257"/>
+    <mergeCell ref="C246:C249"/>
+    <mergeCell ref="C250:C253"/>
+    <mergeCell ref="E194:E209"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
DNS javítása, Switchek ip cím osztása
</commit_message>
<xml_diff>
--- a/Kisvállalat létszám.xlsx
+++ b/Kisvállalat létszám.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\projekt\fluffy-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176F997A-8999-4DC7-B97D-C8E28220A6FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCAC3EC-1F5D-4942-B5F9-C84EC402FFD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alap" sheetId="1" r:id="rId1"/>
@@ -882,22 +882,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -918,46 +942,22 @@
     <xf numFmtId="0" fontId="7" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -1348,8 +1348,8 @@
   <dimension ref="A1:I257"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A231" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E242" sqref="E242:E257"/>
+      <pane ySplit="1" topLeftCell="A213" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A235" sqref="A235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1388,7 +1388,7 @@
       <c r="C2" s="55"/>
       <c r="D2" s="55"/>
       <c r="E2" s="55"/>
-      <c r="F2" s="81" t="s">
+      <c r="F2" s="56" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="55"/>
@@ -1407,7 +1407,7 @@
       <c r="C3" s="55"/>
       <c r="D3" s="55"/>
       <c r="E3" s="55"/>
-      <c r="F3" s="81"/>
+      <c r="F3" s="56"/>
       <c r="G3" s="55"/>
       <c r="H3" s="55"/>
       <c r="I3" s="43"/>
@@ -1422,7 +1422,7 @@
       <c r="C4" s="55"/>
       <c r="D4" s="55"/>
       <c r="E4" s="55"/>
-      <c r="F4" s="81"/>
+      <c r="F4" s="56"/>
       <c r="G4" s="55"/>
       <c r="H4" s="55"/>
       <c r="I4" s="43"/>
@@ -1437,7 +1437,7 @@
       <c r="C5" s="55"/>
       <c r="D5" s="55"/>
       <c r="E5" s="55"/>
-      <c r="F5" s="81"/>
+      <c r="F5" s="56"/>
       <c r="G5" s="55"/>
       <c r="H5" s="55"/>
       <c r="I5" s="43"/>
@@ -1452,7 +1452,7 @@
       <c r="C6" s="55"/>
       <c r="D6" s="55"/>
       <c r="E6" s="55"/>
-      <c r="F6" s="81"/>
+      <c r="F6" s="56"/>
       <c r="G6" s="55"/>
       <c r="H6" s="55"/>
       <c r="I6" s="43"/>
@@ -1467,7 +1467,7 @@
       <c r="C7" s="55"/>
       <c r="D7" s="55"/>
       <c r="E7" s="55"/>
-      <c r="F7" s="81"/>
+      <c r="F7" s="56"/>
       <c r="G7" s="55"/>
       <c r="H7" s="55"/>
       <c r="I7" s="43"/>
@@ -1482,7 +1482,7 @@
       <c r="C8" s="55"/>
       <c r="D8" s="55"/>
       <c r="E8" s="55"/>
-      <c r="F8" s="81"/>
+      <c r="F8" s="56"/>
       <c r="G8" s="55"/>
       <c r="H8" s="55"/>
       <c r="I8" s="43"/>
@@ -1497,7 +1497,7 @@
       <c r="C9" s="55"/>
       <c r="D9" s="55"/>
       <c r="E9" s="55"/>
-      <c r="F9" s="81"/>
+      <c r="F9" s="56"/>
       <c r="G9" s="55"/>
       <c r="H9" s="55"/>
       <c r="I9" s="43"/>
@@ -1512,7 +1512,7 @@
       <c r="C10" s="55"/>
       <c r="D10" s="55"/>
       <c r="E10" s="55"/>
-      <c r="F10" s="81"/>
+      <c r="F10" s="56"/>
       <c r="G10" s="55"/>
       <c r="H10" s="55"/>
       <c r="I10" s="43"/>
@@ -1527,7 +1527,7 @@
       <c r="C11" s="55"/>
       <c r="D11" s="55"/>
       <c r="E11" s="55"/>
-      <c r="F11" s="81"/>
+      <c r="F11" s="56"/>
       <c r="G11" s="55"/>
       <c r="H11" s="55"/>
       <c r="I11" s="54"/>
@@ -1542,7 +1542,7 @@
       <c r="C12" s="55"/>
       <c r="D12" s="55"/>
       <c r="E12" s="55"/>
-      <c r="F12" s="81"/>
+      <c r="F12" s="56"/>
       <c r="G12" s="55"/>
       <c r="H12" s="55"/>
       <c r="I12" s="43"/>
@@ -1557,7 +1557,7 @@
       <c r="C13" s="55"/>
       <c r="D13" s="55"/>
       <c r="E13" s="55"/>
-      <c r="F13" s="81"/>
+      <c r="F13" s="56"/>
       <c r="G13" s="55"/>
       <c r="H13" s="55"/>
       <c r="I13" s="43"/>
@@ -1572,7 +1572,7 @@
       <c r="C14" s="55"/>
       <c r="D14" s="55"/>
       <c r="E14" s="55"/>
-      <c r="F14" s="81"/>
+      <c r="F14" s="56"/>
       <c r="G14" s="55"/>
       <c r="H14" s="55"/>
       <c r="I14" s="43"/>
@@ -1587,7 +1587,7 @@
       <c r="C15" s="55"/>
       <c r="D15" s="55"/>
       <c r="E15" s="55"/>
-      <c r="F15" s="81"/>
+      <c r="F15" s="56"/>
       <c r="G15" s="55"/>
       <c r="H15" s="55"/>
       <c r="I15" s="43"/>
@@ -1602,7 +1602,7 @@
       <c r="C16" s="55"/>
       <c r="D16" s="55"/>
       <c r="E16" s="55"/>
-      <c r="F16" s="81"/>
+      <c r="F16" s="56"/>
       <c r="G16" s="55"/>
       <c r="H16" s="55"/>
       <c r="I16" s="43"/>
@@ -1617,7 +1617,7 @@
       <c r="C17" s="55"/>
       <c r="D17" s="55"/>
       <c r="E17" s="55"/>
-      <c r="F17" s="81"/>
+      <c r="F17" s="56"/>
       <c r="G17" s="55"/>
       <c r="H17" s="55"/>
       <c r="I17" s="43"/>
@@ -1632,7 +1632,7 @@
       <c r="C18" s="55"/>
       <c r="D18" s="55"/>
       <c r="E18" s="55"/>
-      <c r="F18" s="81"/>
+      <c r="F18" s="56"/>
       <c r="G18" s="55"/>
       <c r="H18" s="55"/>
       <c r="I18" s="43"/>
@@ -1647,7 +1647,7 @@
       <c r="C19" s="55"/>
       <c r="D19" s="55"/>
       <c r="E19" s="55"/>
-      <c r="F19" s="81"/>
+      <c r="F19" s="56"/>
       <c r="G19" s="55"/>
       <c r="H19" s="55"/>
       <c r="I19" s="43"/>
@@ -1662,7 +1662,7 @@
       <c r="C20" s="55"/>
       <c r="D20" s="55"/>
       <c r="E20" s="55"/>
-      <c r="F20" s="81"/>
+      <c r="F20" s="56"/>
       <c r="G20" s="55"/>
       <c r="H20" s="55"/>
       <c r="I20" s="54"/>
@@ -1677,7 +1677,7 @@
       <c r="C21" s="55"/>
       <c r="D21" s="55"/>
       <c r="E21" s="55"/>
-      <c r="F21" s="81"/>
+      <c r="F21" s="56"/>
       <c r="G21" s="55"/>
       <c r="H21" s="55"/>
       <c r="I21" s="43"/>
@@ -1692,7 +1692,7 @@
       <c r="C22" s="55"/>
       <c r="D22" s="55"/>
       <c r="E22" s="55"/>
-      <c r="F22" s="81"/>
+      <c r="F22" s="56"/>
       <c r="G22" s="55"/>
       <c r="H22" s="55"/>
       <c r="I22" s="43"/>
@@ -1707,7 +1707,7 @@
       <c r="C23" s="55"/>
       <c r="D23" s="55"/>
       <c r="E23" s="55"/>
-      <c r="F23" s="81"/>
+      <c r="F23" s="56"/>
       <c r="G23" s="55"/>
       <c r="H23" s="55"/>
       <c r="I23" s="43"/>
@@ -1722,7 +1722,7 @@
       <c r="C24" s="55"/>
       <c r="D24" s="55"/>
       <c r="E24" s="55"/>
-      <c r="F24" s="81"/>
+      <c r="F24" s="56"/>
       <c r="G24" s="55"/>
       <c r="H24" s="55"/>
       <c r="I24" s="43"/>
@@ -1737,7 +1737,7 @@
       <c r="C25" s="55"/>
       <c r="D25" s="55"/>
       <c r="E25" s="55"/>
-      <c r="F25" s="81"/>
+      <c r="F25" s="56"/>
       <c r="G25" s="55"/>
       <c r="H25" s="55"/>
       <c r="I25" s="43"/>
@@ -1752,7 +1752,7 @@
       <c r="C26" s="55"/>
       <c r="D26" s="55"/>
       <c r="E26" s="55"/>
-      <c r="F26" s="81"/>
+      <c r="F26" s="56"/>
       <c r="G26" s="55"/>
       <c r="H26" s="55"/>
       <c r="I26" s="43"/>
@@ -1767,7 +1767,7 @@
       <c r="C27" s="55"/>
       <c r="D27" s="55"/>
       <c r="E27" s="55"/>
-      <c r="F27" s="81"/>
+      <c r="F27" s="56"/>
       <c r="G27" s="55"/>
       <c r="H27" s="55"/>
       <c r="I27" s="43"/>
@@ -1782,7 +1782,7 @@
       <c r="C28" s="55"/>
       <c r="D28" s="55"/>
       <c r="E28" s="55"/>
-      <c r="F28" s="81"/>
+      <c r="F28" s="56"/>
       <c r="G28" s="55"/>
       <c r="H28" s="55"/>
       <c r="I28" s="43"/>
@@ -1797,7 +1797,7 @@
       <c r="C29" s="55"/>
       <c r="D29" s="55"/>
       <c r="E29" s="55"/>
-      <c r="F29" s="81"/>
+      <c r="F29" s="56"/>
       <c r="G29" s="55"/>
       <c r="H29" s="55"/>
       <c r="I29" s="54" t="s">
@@ -1814,7 +1814,7 @@
       <c r="C30" s="55"/>
       <c r="D30" s="55"/>
       <c r="E30" s="55"/>
-      <c r="F30" s="81"/>
+      <c r="F30" s="56"/>
       <c r="G30" s="55"/>
       <c r="H30" s="55"/>
       <c r="I30" s="43" t="s">
@@ -1831,7 +1831,7 @@
       <c r="C31" s="55"/>
       <c r="D31" s="55"/>
       <c r="E31" s="55"/>
-      <c r="F31" s="81"/>
+      <c r="F31" s="56"/>
       <c r="G31" s="55"/>
       <c r="H31" s="55"/>
       <c r="I31" s="43" t="s">
@@ -1848,7 +1848,7 @@
       <c r="C32" s="55"/>
       <c r="D32" s="55"/>
       <c r="E32" s="55"/>
-      <c r="F32" s="81"/>
+      <c r="F32" s="56"/>
       <c r="G32" s="55"/>
       <c r="H32" s="55"/>
       <c r="I32" s="43" t="s">
@@ -1865,7 +1865,7 @@
       <c r="C33" s="55"/>
       <c r="D33" s="55"/>
       <c r="E33" s="55"/>
-      <c r="F33" s="81"/>
+      <c r="F33" s="56"/>
       <c r="G33" s="55"/>
       <c r="H33" s="55"/>
       <c r="I33" s="43" t="s">
@@ -1881,7 +1881,7 @@
       </c>
       <c r="C34" s="55"/>
       <c r="D34" s="55"/>
-      <c r="E34" s="80" t="s">
+      <c r="E34" s="59" t="s">
         <v>16</v>
       </c>
       <c r="F34" s="55"/>
@@ -1900,7 +1900,7 @@
       </c>
       <c r="C35" s="55"/>
       <c r="D35" s="55"/>
-      <c r="E35" s="80"/>
+      <c r="E35" s="59"/>
       <c r="F35" s="55"/>
       <c r="G35" s="55"/>
       <c r="H35" s="55"/>
@@ -1915,7 +1915,7 @@
       </c>
       <c r="C36" s="55"/>
       <c r="D36" s="55"/>
-      <c r="E36" s="80"/>
+      <c r="E36" s="59"/>
       <c r="F36" s="55"/>
       <c r="G36" s="55"/>
       <c r="H36" s="55"/>
@@ -1930,7 +1930,7 @@
       </c>
       <c r="C37" s="55"/>
       <c r="D37" s="55"/>
-      <c r="E37" s="80"/>
+      <c r="E37" s="59"/>
       <c r="F37" s="55"/>
       <c r="G37" s="55"/>
       <c r="H37" s="55"/>
@@ -1945,7 +1945,7 @@
       </c>
       <c r="C38" s="55"/>
       <c r="D38" s="55"/>
-      <c r="E38" s="80"/>
+      <c r="E38" s="59"/>
       <c r="F38" s="55"/>
       <c r="G38" s="55"/>
       <c r="H38" s="55"/>
@@ -1960,7 +1960,7 @@
       </c>
       <c r="C39" s="55"/>
       <c r="D39" s="55"/>
-      <c r="E39" s="80"/>
+      <c r="E39" s="59"/>
       <c r="F39" s="55"/>
       <c r="G39" s="55"/>
       <c r="H39" s="55"/>
@@ -1975,7 +1975,7 @@
       </c>
       <c r="C40" s="55"/>
       <c r="D40" s="55"/>
-      <c r="E40" s="80"/>
+      <c r="E40" s="59"/>
       <c r="F40" s="55"/>
       <c r="G40" s="55"/>
       <c r="H40" s="55"/>
@@ -1990,7 +1990,7 @@
       </c>
       <c r="C41" s="55"/>
       <c r="D41" s="55"/>
-      <c r="E41" s="80"/>
+      <c r="E41" s="59"/>
       <c r="F41" s="55"/>
       <c r="G41" s="55"/>
       <c r="H41" s="55"/>
@@ -2005,7 +2005,7 @@
       </c>
       <c r="C42" s="55"/>
       <c r="D42" s="55"/>
-      <c r="E42" s="80"/>
+      <c r="E42" s="59"/>
       <c r="F42" s="55"/>
       <c r="G42" s="55"/>
       <c r="H42" s="55"/>
@@ -2020,7 +2020,7 @@
       </c>
       <c r="C43" s="55"/>
       <c r="D43" s="55"/>
-      <c r="E43" s="80"/>
+      <c r="E43" s="59"/>
       <c r="F43" s="55"/>
       <c r="G43" s="55"/>
       <c r="H43" s="55"/>
@@ -2035,7 +2035,7 @@
       </c>
       <c r="C44" s="55"/>
       <c r="D44" s="55"/>
-      <c r="E44" s="80"/>
+      <c r="E44" s="59"/>
       <c r="F44" s="55"/>
       <c r="G44" s="55"/>
       <c r="H44" s="55"/>
@@ -2050,7 +2050,7 @@
       </c>
       <c r="C45" s="55"/>
       <c r="D45" s="55"/>
-      <c r="E45" s="80"/>
+      <c r="E45" s="59"/>
       <c r="F45" s="55"/>
       <c r="G45" s="55"/>
       <c r="H45" s="55"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="C46" s="55"/>
       <c r="D46" s="55"/>
-      <c r="E46" s="80"/>
+      <c r="E46" s="59"/>
       <c r="F46" s="55"/>
       <c r="G46" s="55"/>
       <c r="H46" s="55"/>
@@ -2080,7 +2080,7 @@
       </c>
       <c r="C47" s="55"/>
       <c r="D47" s="55"/>
-      <c r="E47" s="80"/>
+      <c r="E47" s="59"/>
       <c r="F47" s="55"/>
       <c r="G47" s="55"/>
       <c r="H47" s="55"/>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="C48" s="55"/>
       <c r="D48" s="55"/>
-      <c r="E48" s="80"/>
+      <c r="E48" s="59"/>
       <c r="F48" s="55"/>
       <c r="G48" s="55"/>
       <c r="H48" s="55"/>
@@ -2112,7 +2112,7 @@
       </c>
       <c r="C49" s="55"/>
       <c r="D49" s="55"/>
-      <c r="E49" s="80"/>
+      <c r="E49" s="59"/>
       <c r="F49" s="55"/>
       <c r="G49" s="55"/>
       <c r="H49" s="55"/>
@@ -2129,7 +2129,7 @@
       </c>
       <c r="C50" s="55"/>
       <c r="D50" s="55"/>
-      <c r="E50" s="78" t="s">
+      <c r="E50" s="57" t="s">
         <v>17</v>
       </c>
       <c r="F50" s="55"/>
@@ -2148,7 +2148,7 @@
       </c>
       <c r="C51" s="55"/>
       <c r="D51" s="55"/>
-      <c r="E51" s="78"/>
+      <c r="E51" s="57"/>
       <c r="F51" s="55"/>
       <c r="G51" s="55"/>
       <c r="H51" s="55"/>
@@ -2163,7 +2163,7 @@
       </c>
       <c r="C52" s="55"/>
       <c r="D52" s="55"/>
-      <c r="E52" s="78"/>
+      <c r="E52" s="57"/>
       <c r="F52" s="55"/>
       <c r="G52" s="55"/>
       <c r="H52" s="55"/>
@@ -2178,7 +2178,7 @@
       </c>
       <c r="C53" s="55"/>
       <c r="D53" s="55"/>
-      <c r="E53" s="78"/>
+      <c r="E53" s="57"/>
       <c r="F53" s="55"/>
       <c r="G53" s="55"/>
       <c r="H53" s="55"/>
@@ -2193,7 +2193,7 @@
       </c>
       <c r="C54" s="55"/>
       <c r="D54" s="55"/>
-      <c r="E54" s="78"/>
+      <c r="E54" s="57"/>
       <c r="F54" s="55"/>
       <c r="G54" s="55"/>
       <c r="H54" s="55"/>
@@ -2208,7 +2208,7 @@
       </c>
       <c r="C55" s="55"/>
       <c r="D55" s="55"/>
-      <c r="E55" s="78"/>
+      <c r="E55" s="57"/>
       <c r="F55" s="55"/>
       <c r="G55" s="55"/>
       <c r="H55" s="55"/>
@@ -2223,7 +2223,7 @@
       </c>
       <c r="C56" s="55"/>
       <c r="D56" s="55"/>
-      <c r="E56" s="78"/>
+      <c r="E56" s="57"/>
       <c r="F56" s="55"/>
       <c r="G56" s="55"/>
       <c r="H56" s="55"/>
@@ -2238,7 +2238,7 @@
       </c>
       <c r="C57" s="55"/>
       <c r="D57" s="55"/>
-      <c r="E57" s="78"/>
+      <c r="E57" s="57"/>
       <c r="F57" s="55"/>
       <c r="G57" s="55"/>
       <c r="H57" s="55"/>
@@ -2253,7 +2253,7 @@
       </c>
       <c r="C58" s="55"/>
       <c r="D58" s="55"/>
-      <c r="E58" s="78"/>
+      <c r="E58" s="57"/>
       <c r="F58" s="55"/>
       <c r="G58" s="55"/>
       <c r="H58" s="55"/>
@@ -2268,7 +2268,7 @@
       </c>
       <c r="C59" s="55"/>
       <c r="D59" s="55"/>
-      <c r="E59" s="78"/>
+      <c r="E59" s="57"/>
       <c r="F59" s="55"/>
       <c r="G59" s="55"/>
       <c r="H59" s="55"/>
@@ -2283,7 +2283,7 @@
       </c>
       <c r="C60" s="55"/>
       <c r="D60" s="55"/>
-      <c r="E60" s="78"/>
+      <c r="E60" s="57"/>
       <c r="F60" s="55"/>
       <c r="G60" s="55"/>
       <c r="H60" s="55"/>
@@ -2298,7 +2298,7 @@
       </c>
       <c r="C61" s="55"/>
       <c r="D61" s="55"/>
-      <c r="E61" s="78"/>
+      <c r="E61" s="57"/>
       <c r="F61" s="55"/>
       <c r="G61" s="55"/>
       <c r="H61" s="55"/>
@@ -2313,7 +2313,7 @@
       </c>
       <c r="C62" s="55"/>
       <c r="D62" s="55"/>
-      <c r="E62" s="78"/>
+      <c r="E62" s="57"/>
       <c r="F62" s="55"/>
       <c r="G62" s="55"/>
       <c r="H62" s="55"/>
@@ -2328,7 +2328,7 @@
       </c>
       <c r="C63" s="55"/>
       <c r="D63" s="55"/>
-      <c r="E63" s="78"/>
+      <c r="E63" s="57"/>
       <c r="F63" s="55"/>
       <c r="G63" s="55"/>
       <c r="H63" s="55"/>
@@ -2343,7 +2343,7 @@
       </c>
       <c r="C64" s="55"/>
       <c r="D64" s="55"/>
-      <c r="E64" s="78"/>
+      <c r="E64" s="57"/>
       <c r="F64" s="55"/>
       <c r="G64" s="55"/>
       <c r="H64" s="55"/>
@@ -2360,7 +2360,7 @@
       </c>
       <c r="C65" s="55"/>
       <c r="D65" s="55"/>
-      <c r="E65" s="78"/>
+      <c r="E65" s="57"/>
       <c r="F65" s="55"/>
       <c r="G65" s="55"/>
       <c r="H65" s="55"/>
@@ -2377,7 +2377,7 @@
       </c>
       <c r="C66" s="55"/>
       <c r="D66" s="55"/>
-      <c r="E66" s="79" t="s">
+      <c r="E66" s="58" t="s">
         <v>18</v>
       </c>
       <c r="F66" s="55"/>
@@ -2396,7 +2396,7 @@
       </c>
       <c r="C67" s="55"/>
       <c r="D67" s="55"/>
-      <c r="E67" s="79"/>
+      <c r="E67" s="58"/>
       <c r="F67" s="55"/>
       <c r="G67" s="55"/>
       <c r="H67" s="55"/>
@@ -2411,7 +2411,7 @@
       </c>
       <c r="C68" s="55"/>
       <c r="D68" s="55"/>
-      <c r="E68" s="79"/>
+      <c r="E68" s="58"/>
       <c r="F68" s="55"/>
       <c r="G68" s="55"/>
       <c r="H68" s="55"/>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="C69" s="55"/>
       <c r="D69" s="55"/>
-      <c r="E69" s="79"/>
+      <c r="E69" s="58"/>
       <c r="F69" s="55"/>
       <c r="G69" s="55"/>
       <c r="H69" s="55"/>
@@ -2441,7 +2441,7 @@
       </c>
       <c r="C70" s="55"/>
       <c r="D70" s="55"/>
-      <c r="E70" s="79"/>
+      <c r="E70" s="58"/>
       <c r="F70" s="55"/>
       <c r="G70" s="55"/>
       <c r="H70" s="55"/>
@@ -2456,7 +2456,7 @@
       </c>
       <c r="C71" s="55"/>
       <c r="D71" s="55"/>
-      <c r="E71" s="79"/>
+      <c r="E71" s="58"/>
       <c r="F71" s="55"/>
       <c r="G71" s="55"/>
       <c r="H71" s="55"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="C72" s="55"/>
       <c r="D72" s="55"/>
-      <c r="E72" s="79"/>
+      <c r="E72" s="58"/>
       <c r="F72" s="55"/>
       <c r="G72" s="55"/>
       <c r="H72" s="55"/>
@@ -2486,7 +2486,7 @@
       </c>
       <c r="C73" s="55"/>
       <c r="D73" s="55"/>
-      <c r="E73" s="79"/>
+      <c r="E73" s="58"/>
       <c r="F73" s="55"/>
       <c r="G73" s="55"/>
       <c r="H73" s="55"/>
@@ -2501,7 +2501,7 @@
       </c>
       <c r="C74" s="55"/>
       <c r="D74" s="55"/>
-      <c r="E74" s="79"/>
+      <c r="E74" s="58"/>
       <c r="F74" s="55"/>
       <c r="G74" s="55"/>
       <c r="H74" s="55"/>
@@ -2516,7 +2516,7 @@
       </c>
       <c r="C75" s="55"/>
       <c r="D75" s="55"/>
-      <c r="E75" s="79"/>
+      <c r="E75" s="58"/>
       <c r="F75" s="55"/>
       <c r="G75" s="55"/>
       <c r="H75" s="55"/>
@@ -2531,7 +2531,7 @@
       </c>
       <c r="C76" s="55"/>
       <c r="D76" s="55"/>
-      <c r="E76" s="79"/>
+      <c r="E76" s="58"/>
       <c r="F76" s="55"/>
       <c r="G76" s="55"/>
       <c r="H76" s="55"/>
@@ -2546,7 +2546,7 @@
       </c>
       <c r="C77" s="55"/>
       <c r="D77" s="55"/>
-      <c r="E77" s="79"/>
+      <c r="E77" s="58"/>
       <c r="F77" s="55"/>
       <c r="G77" s="55"/>
       <c r="H77" s="55"/>
@@ -2561,7 +2561,7 @@
       </c>
       <c r="C78" s="55"/>
       <c r="D78" s="55"/>
-      <c r="E78" s="79"/>
+      <c r="E78" s="58"/>
       <c r="F78" s="55"/>
       <c r="G78" s="55"/>
       <c r="H78" s="55"/>
@@ -2576,7 +2576,7 @@
       </c>
       <c r="C79" s="55"/>
       <c r="D79" s="55"/>
-      <c r="E79" s="79"/>
+      <c r="E79" s="58"/>
       <c r="F79" s="55"/>
       <c r="G79" s="55"/>
       <c r="H79" s="55"/>
@@ -2591,7 +2591,7 @@
       </c>
       <c r="C80" s="55"/>
       <c r="D80" s="55"/>
-      <c r="E80" s="79"/>
+      <c r="E80" s="58"/>
       <c r="F80" s="55"/>
       <c r="G80" s="55"/>
       <c r="H80" s="55"/>
@@ -2608,7 +2608,7 @@
       </c>
       <c r="C81" s="55"/>
       <c r="D81" s="55"/>
-      <c r="E81" s="79"/>
+      <c r="E81" s="58"/>
       <c r="F81" s="55"/>
       <c r="G81" s="55"/>
       <c r="H81" s="55"/>
@@ -2625,7 +2625,7 @@
       </c>
       <c r="C82" s="55"/>
       <c r="D82" s="55"/>
-      <c r="E82" s="77" t="s">
+      <c r="E82" s="61" t="s">
         <v>19</v>
       </c>
       <c r="F82" s="55"/>
@@ -2644,7 +2644,7 @@
       </c>
       <c r="C83" s="55"/>
       <c r="D83" s="55"/>
-      <c r="E83" s="77"/>
+      <c r="E83" s="61"/>
       <c r="F83" s="55"/>
       <c r="G83" s="55"/>
       <c r="H83" s="55"/>
@@ -2659,7 +2659,7 @@
       </c>
       <c r="C84" s="55"/>
       <c r="D84" s="55"/>
-      <c r="E84" s="77"/>
+      <c r="E84" s="61"/>
       <c r="F84" s="55"/>
       <c r="G84" s="55"/>
       <c r="H84" s="55"/>
@@ -2674,7 +2674,7 @@
       </c>
       <c r="C85" s="55"/>
       <c r="D85" s="55"/>
-      <c r="E85" s="77"/>
+      <c r="E85" s="61"/>
       <c r="F85" s="55"/>
       <c r="G85" s="55"/>
       <c r="H85" s="55"/>
@@ -2689,7 +2689,7 @@
       </c>
       <c r="C86" s="55"/>
       <c r="D86" s="55"/>
-      <c r="E86" s="77"/>
+      <c r="E86" s="61"/>
       <c r="F86" s="55"/>
       <c r="G86" s="55"/>
       <c r="H86" s="55"/>
@@ -2704,7 +2704,7 @@
       </c>
       <c r="C87" s="55"/>
       <c r="D87" s="55"/>
-      <c r="E87" s="77"/>
+      <c r="E87" s="61"/>
       <c r="F87" s="55"/>
       <c r="G87" s="55"/>
       <c r="H87" s="55"/>
@@ -2719,7 +2719,7 @@
       </c>
       <c r="C88" s="55"/>
       <c r="D88" s="55"/>
-      <c r="E88" s="77"/>
+      <c r="E88" s="61"/>
       <c r="F88" s="55"/>
       <c r="G88" s="55"/>
       <c r="H88" s="55"/>
@@ -2734,7 +2734,7 @@
       </c>
       <c r="C89" s="55"/>
       <c r="D89" s="55"/>
-      <c r="E89" s="77"/>
+      <c r="E89" s="61"/>
       <c r="F89" s="55"/>
       <c r="G89" s="55"/>
       <c r="H89" s="55"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="C90" s="55"/>
       <c r="D90" s="55"/>
-      <c r="E90" s="77"/>
+      <c r="E90" s="61"/>
       <c r="F90" s="55"/>
       <c r="G90" s="55"/>
       <c r="H90" s="55"/>
@@ -2764,7 +2764,7 @@
       </c>
       <c r="C91" s="55"/>
       <c r="D91" s="55"/>
-      <c r="E91" s="77"/>
+      <c r="E91" s="61"/>
       <c r="F91" s="55"/>
       <c r="G91" s="55"/>
       <c r="H91" s="55"/>
@@ -2779,7 +2779,7 @@
       </c>
       <c r="C92" s="55"/>
       <c r="D92" s="55"/>
-      <c r="E92" s="77"/>
+      <c r="E92" s="61"/>
       <c r="F92" s="55"/>
       <c r="G92" s="55"/>
       <c r="H92" s="55"/>
@@ -2794,7 +2794,7 @@
       </c>
       <c r="C93" s="55"/>
       <c r="D93" s="55"/>
-      <c r="E93" s="77"/>
+      <c r="E93" s="61"/>
       <c r="F93" s="55"/>
       <c r="G93" s="55"/>
       <c r="H93" s="55"/>
@@ -2809,7 +2809,7 @@
       </c>
       <c r="C94" s="55"/>
       <c r="D94" s="55"/>
-      <c r="E94" s="77"/>
+      <c r="E94" s="61"/>
       <c r="F94" s="55"/>
       <c r="G94" s="55"/>
       <c r="H94" s="55"/>
@@ -2824,7 +2824,7 @@
       </c>
       <c r="C95" s="55"/>
       <c r="D95" s="55"/>
-      <c r="E95" s="77"/>
+      <c r="E95" s="61"/>
       <c r="F95" s="55"/>
       <c r="G95" s="55"/>
       <c r="H95" s="55"/>
@@ -2839,7 +2839,7 @@
       </c>
       <c r="C96" s="55"/>
       <c r="D96" s="55"/>
-      <c r="E96" s="77"/>
+      <c r="E96" s="61"/>
       <c r="F96" s="55"/>
       <c r="G96" s="55"/>
       <c r="H96" s="55"/>
@@ -2856,7 +2856,7 @@
       </c>
       <c r="C97" s="55"/>
       <c r="D97" s="55"/>
-      <c r="E97" s="77"/>
+      <c r="E97" s="61"/>
       <c r="F97" s="55"/>
       <c r="G97" s="55"/>
       <c r="H97" s="55"/>
@@ -2873,7 +2873,7 @@
       </c>
       <c r="C98" s="55"/>
       <c r="D98" s="55"/>
-      <c r="E98" s="76" t="s">
+      <c r="E98" s="60" t="s">
         <v>20</v>
       </c>
       <c r="F98" s="55"/>
@@ -2892,7 +2892,7 @@
       </c>
       <c r="C99" s="55"/>
       <c r="D99" s="55"/>
-      <c r="E99" s="76"/>
+      <c r="E99" s="60"/>
       <c r="F99" s="55"/>
       <c r="G99" s="55"/>
       <c r="H99" s="55"/>
@@ -2907,7 +2907,7 @@
       </c>
       <c r="C100" s="55"/>
       <c r="D100" s="55"/>
-      <c r="E100" s="76"/>
+      <c r="E100" s="60"/>
       <c r="F100" s="55"/>
       <c r="G100" s="55"/>
       <c r="H100" s="55"/>
@@ -2922,7 +2922,7 @@
       </c>
       <c r="C101" s="55"/>
       <c r="D101" s="55"/>
-      <c r="E101" s="76"/>
+      <c r="E101" s="60"/>
       <c r="F101" s="55"/>
       <c r="G101" s="55"/>
       <c r="H101" s="55"/>
@@ -2937,7 +2937,7 @@
       </c>
       <c r="C102" s="55"/>
       <c r="D102" s="55"/>
-      <c r="E102" s="76"/>
+      <c r="E102" s="60"/>
       <c r="F102" s="55"/>
       <c r="G102" s="55"/>
       <c r="H102" s="55"/>
@@ -2952,7 +2952,7 @@
       </c>
       <c r="C103" s="55"/>
       <c r="D103" s="55"/>
-      <c r="E103" s="76"/>
+      <c r="E103" s="60"/>
       <c r="F103" s="55"/>
       <c r="G103" s="55"/>
       <c r="H103" s="55"/>
@@ -2967,7 +2967,7 @@
       </c>
       <c r="C104" s="55"/>
       <c r="D104" s="55"/>
-      <c r="E104" s="76"/>
+      <c r="E104" s="60"/>
       <c r="F104" s="55"/>
       <c r="G104" s="55"/>
       <c r="H104" s="55"/>
@@ -2982,7 +2982,7 @@
       </c>
       <c r="C105" s="55"/>
       <c r="D105" s="55"/>
-      <c r="E105" s="76"/>
+      <c r="E105" s="60"/>
       <c r="F105" s="55"/>
       <c r="G105" s="55"/>
       <c r="H105" s="55"/>
@@ -2997,7 +2997,7 @@
       </c>
       <c r="C106" s="55"/>
       <c r="D106" s="55"/>
-      <c r="E106" s="76"/>
+      <c r="E106" s="60"/>
       <c r="F106" s="55"/>
       <c r="G106" s="55"/>
       <c r="H106" s="55"/>
@@ -3012,7 +3012,7 @@
       </c>
       <c r="C107" s="55"/>
       <c r="D107" s="55"/>
-      <c r="E107" s="76"/>
+      <c r="E107" s="60"/>
       <c r="F107" s="55"/>
       <c r="G107" s="55"/>
       <c r="H107" s="55"/>
@@ -3027,7 +3027,7 @@
       </c>
       <c r="C108" s="55"/>
       <c r="D108" s="55"/>
-      <c r="E108" s="76"/>
+      <c r="E108" s="60"/>
       <c r="F108" s="55"/>
       <c r="G108" s="55"/>
       <c r="H108" s="55"/>
@@ -3042,7 +3042,7 @@
       </c>
       <c r="C109" s="55"/>
       <c r="D109" s="55"/>
-      <c r="E109" s="76"/>
+      <c r="E109" s="60"/>
       <c r="F109" s="55"/>
       <c r="G109" s="55"/>
       <c r="H109" s="55"/>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="C110" s="55"/>
       <c r="D110" s="55"/>
-      <c r="E110" s="76"/>
+      <c r="E110" s="60"/>
       <c r="F110" s="55"/>
       <c r="G110" s="55"/>
       <c r="H110" s="55"/>
@@ -3072,7 +3072,7 @@
       </c>
       <c r="C111" s="55"/>
       <c r="D111" s="55"/>
-      <c r="E111" s="76"/>
+      <c r="E111" s="60"/>
       <c r="F111" s="55"/>
       <c r="G111" s="55"/>
       <c r="H111" s="55"/>
@@ -3087,7 +3087,7 @@
       </c>
       <c r="C112" s="55"/>
       <c r="D112" s="55"/>
-      <c r="E112" s="76"/>
+      <c r="E112" s="60"/>
       <c r="F112" s="55"/>
       <c r="G112" s="55"/>
       <c r="H112" s="55"/>
@@ -3104,7 +3104,7 @@
       </c>
       <c r="C113" s="55"/>
       <c r="D113" s="55"/>
-      <c r="E113" s="76"/>
+      <c r="E113" s="60"/>
       <c r="F113" s="55"/>
       <c r="G113" s="55"/>
       <c r="H113" s="55"/>
@@ -3121,7 +3121,7 @@
       </c>
       <c r="C114" s="55"/>
       <c r="D114" s="55"/>
-      <c r="E114" s="75" t="s">
+      <c r="E114" s="65" t="s">
         <v>21</v>
       </c>
       <c r="F114" s="55"/>
@@ -3140,7 +3140,7 @@
       </c>
       <c r="C115" s="55"/>
       <c r="D115" s="55"/>
-      <c r="E115" s="75"/>
+      <c r="E115" s="65"/>
       <c r="F115" s="55"/>
       <c r="G115" s="55"/>
       <c r="H115" s="55"/>
@@ -3155,7 +3155,7 @@
       </c>
       <c r="C116" s="55"/>
       <c r="D116" s="55"/>
-      <c r="E116" s="75"/>
+      <c r="E116" s="65"/>
       <c r="F116" s="55"/>
       <c r="G116" s="55"/>
       <c r="H116" s="55"/>
@@ -3170,7 +3170,7 @@
       </c>
       <c r="C117" s="55"/>
       <c r="D117" s="55"/>
-      <c r="E117" s="75"/>
+      <c r="E117" s="65"/>
       <c r="F117" s="55"/>
       <c r="G117" s="55"/>
       <c r="H117" s="55"/>
@@ -3185,7 +3185,7 @@
       </c>
       <c r="C118" s="55"/>
       <c r="D118" s="55"/>
-      <c r="E118" s="75"/>
+      <c r="E118" s="65"/>
       <c r="F118" s="55"/>
       <c r="G118" s="55"/>
       <c r="H118" s="55"/>
@@ -3200,7 +3200,7 @@
       </c>
       <c r="C119" s="55"/>
       <c r="D119" s="55"/>
-      <c r="E119" s="75"/>
+      <c r="E119" s="65"/>
       <c r="F119" s="55"/>
       <c r="G119" s="55"/>
       <c r="H119" s="55"/>
@@ -3215,7 +3215,7 @@
       </c>
       <c r="C120" s="55"/>
       <c r="D120" s="55"/>
-      <c r="E120" s="75"/>
+      <c r="E120" s="65"/>
       <c r="F120" s="55"/>
       <c r="G120" s="55"/>
       <c r="H120" s="55"/>
@@ -3230,7 +3230,7 @@
       </c>
       <c r="C121" s="55"/>
       <c r="D121" s="55"/>
-      <c r="E121" s="75"/>
+      <c r="E121" s="65"/>
       <c r="F121" s="55"/>
       <c r="G121" s="55"/>
       <c r="H121" s="55"/>
@@ -3245,7 +3245,7 @@
       </c>
       <c r="C122" s="55"/>
       <c r="D122" s="55"/>
-      <c r="E122" s="75"/>
+      <c r="E122" s="65"/>
       <c r="F122" s="55"/>
       <c r="G122" s="55"/>
       <c r="H122" s="55"/>
@@ -3260,7 +3260,7 @@
       </c>
       <c r="C123" s="55"/>
       <c r="D123" s="55"/>
-      <c r="E123" s="75"/>
+      <c r="E123" s="65"/>
       <c r="F123" s="55"/>
       <c r="G123" s="55"/>
       <c r="H123" s="55"/>
@@ -3275,7 +3275,7 @@
       </c>
       <c r="C124" s="55"/>
       <c r="D124" s="55"/>
-      <c r="E124" s="75"/>
+      <c r="E124" s="65"/>
       <c r="F124" s="55"/>
       <c r="G124" s="55"/>
       <c r="H124" s="55"/>
@@ -3290,7 +3290,7 @@
       </c>
       <c r="C125" s="55"/>
       <c r="D125" s="55"/>
-      <c r="E125" s="75"/>
+      <c r="E125" s="65"/>
       <c r="F125" s="55"/>
       <c r="G125" s="55"/>
       <c r="H125" s="55"/>
@@ -3305,7 +3305,7 @@
       </c>
       <c r="C126" s="55"/>
       <c r="D126" s="55"/>
-      <c r="E126" s="75"/>
+      <c r="E126" s="65"/>
       <c r="F126" s="55"/>
       <c r="G126" s="55"/>
       <c r="H126" s="55"/>
@@ -3320,7 +3320,7 @@
       </c>
       <c r="C127" s="55"/>
       <c r="D127" s="55"/>
-      <c r="E127" s="75"/>
+      <c r="E127" s="65"/>
       <c r="F127" s="55"/>
       <c r="G127" s="55"/>
       <c r="H127" s="55"/>
@@ -3335,7 +3335,7 @@
       </c>
       <c r="C128" s="55"/>
       <c r="D128" s="55"/>
-      <c r="E128" s="75"/>
+      <c r="E128" s="65"/>
       <c r="F128" s="55"/>
       <c r="G128" s="55"/>
       <c r="H128" s="55"/>
@@ -3352,7 +3352,7 @@
       </c>
       <c r="C129" s="55"/>
       <c r="D129" s="55"/>
-      <c r="E129" s="75"/>
+      <c r="E129" s="65"/>
       <c r="F129" s="55"/>
       <c r="G129" s="55"/>
       <c r="H129" s="55"/>
@@ -3369,7 +3369,7 @@
       </c>
       <c r="C130" s="55"/>
       <c r="D130" s="55"/>
-      <c r="E130" s="68" t="s">
+      <c r="E130" s="62" t="s">
         <v>22</v>
       </c>
       <c r="F130" s="55"/>
@@ -3388,7 +3388,7 @@
       </c>
       <c r="C131" s="55"/>
       <c r="D131" s="55"/>
-      <c r="E131" s="69"/>
+      <c r="E131" s="63"/>
       <c r="F131" s="55"/>
       <c r="G131" s="55"/>
       <c r="H131" s="55"/>
@@ -3403,7 +3403,7 @@
       </c>
       <c r="C132" s="55"/>
       <c r="D132" s="55"/>
-      <c r="E132" s="69"/>
+      <c r="E132" s="63"/>
       <c r="F132" s="55"/>
       <c r="G132" s="55"/>
       <c r="H132" s="55"/>
@@ -3418,7 +3418,7 @@
       </c>
       <c r="C133" s="55"/>
       <c r="D133" s="55"/>
-      <c r="E133" s="69"/>
+      <c r="E133" s="63"/>
       <c r="F133" s="55"/>
       <c r="G133" s="55"/>
       <c r="H133" s="55"/>
@@ -3433,7 +3433,7 @@
       </c>
       <c r="C134" s="55"/>
       <c r="D134" s="55"/>
-      <c r="E134" s="69"/>
+      <c r="E134" s="63"/>
       <c r="F134" s="55"/>
       <c r="G134" s="55"/>
       <c r="H134" s="55"/>
@@ -3448,7 +3448,7 @@
       </c>
       <c r="C135" s="55"/>
       <c r="D135" s="55"/>
-      <c r="E135" s="69"/>
+      <c r="E135" s="63"/>
       <c r="F135" s="55"/>
       <c r="G135" s="55"/>
       <c r="H135" s="55"/>
@@ -3463,7 +3463,7 @@
       </c>
       <c r="C136" s="55"/>
       <c r="D136" s="55"/>
-      <c r="E136" s="69"/>
+      <c r="E136" s="63"/>
       <c r="F136" s="55"/>
       <c r="G136" s="55"/>
       <c r="H136" s="55"/>
@@ -3478,7 +3478,7 @@
       </c>
       <c r="C137" s="55"/>
       <c r="D137" s="55"/>
-      <c r="E137" s="69"/>
+      <c r="E137" s="63"/>
       <c r="F137" s="55"/>
       <c r="G137" s="55"/>
       <c r="H137" s="55"/>
@@ -3493,7 +3493,7 @@
       </c>
       <c r="C138" s="55"/>
       <c r="D138" s="55"/>
-      <c r="E138" s="69"/>
+      <c r="E138" s="63"/>
       <c r="F138" s="55"/>
       <c r="G138" s="55"/>
       <c r="H138" s="55"/>
@@ -3508,7 +3508,7 @@
       </c>
       <c r="C139" s="55"/>
       <c r="D139" s="55"/>
-      <c r="E139" s="69"/>
+      <c r="E139" s="63"/>
       <c r="F139" s="55"/>
       <c r="G139" s="55"/>
       <c r="H139" s="55"/>
@@ -3523,7 +3523,7 @@
       </c>
       <c r="C140" s="55"/>
       <c r="D140" s="55"/>
-      <c r="E140" s="69"/>
+      <c r="E140" s="63"/>
       <c r="F140" s="55"/>
       <c r="G140" s="55"/>
       <c r="H140" s="55"/>
@@ -3538,7 +3538,7 @@
       </c>
       <c r="C141" s="55"/>
       <c r="D141" s="55"/>
-      <c r="E141" s="69"/>
+      <c r="E141" s="63"/>
       <c r="F141" s="55"/>
       <c r="G141" s="55"/>
       <c r="H141" s="55"/>
@@ -3553,7 +3553,7 @@
       </c>
       <c r="C142" s="55"/>
       <c r="D142" s="55"/>
-      <c r="E142" s="69"/>
+      <c r="E142" s="63"/>
       <c r="F142" s="55"/>
       <c r="G142" s="55"/>
       <c r="H142" s="55"/>
@@ -3568,7 +3568,7 @@
       </c>
       <c r="C143" s="55"/>
       <c r="D143" s="55"/>
-      <c r="E143" s="69"/>
+      <c r="E143" s="63"/>
       <c r="F143" s="55"/>
       <c r="G143" s="55"/>
       <c r="H143" s="55"/>
@@ -3583,7 +3583,7 @@
       </c>
       <c r="C144" s="55"/>
       <c r="D144" s="55"/>
-      <c r="E144" s="69"/>
+      <c r="E144" s="63"/>
       <c r="F144" s="55"/>
       <c r="G144" s="55"/>
       <c r="H144" s="55"/>
@@ -3600,7 +3600,7 @@
       </c>
       <c r="C145" s="55"/>
       <c r="D145" s="55"/>
-      <c r="E145" s="70"/>
+      <c r="E145" s="64"/>
       <c r="F145" s="55"/>
       <c r="G145" s="55"/>
       <c r="H145" s="55"/>
@@ -3617,7 +3617,7 @@
       </c>
       <c r="C146" s="55"/>
       <c r="D146" s="55"/>
-      <c r="E146" s="68" t="s">
+      <c r="E146" s="62" t="s">
         <v>23</v>
       </c>
       <c r="F146" s="55"/>
@@ -3636,7 +3636,7 @@
       </c>
       <c r="C147" s="55"/>
       <c r="D147" s="55"/>
-      <c r="E147" s="69"/>
+      <c r="E147" s="63"/>
       <c r="F147" s="55"/>
       <c r="G147" s="55"/>
       <c r="H147" s="55"/>
@@ -3651,7 +3651,7 @@
       </c>
       <c r="C148" s="55"/>
       <c r="D148" s="55"/>
-      <c r="E148" s="69"/>
+      <c r="E148" s="63"/>
       <c r="F148" s="55"/>
       <c r="G148" s="55"/>
       <c r="H148" s="55"/>
@@ -3666,7 +3666,7 @@
       </c>
       <c r="C149" s="55"/>
       <c r="D149" s="55"/>
-      <c r="E149" s="69"/>
+      <c r="E149" s="63"/>
       <c r="F149" s="55"/>
       <c r="G149" s="55"/>
       <c r="H149" s="55"/>
@@ -3681,7 +3681,7 @@
       </c>
       <c r="C150" s="55"/>
       <c r="D150" s="55"/>
-      <c r="E150" s="69"/>
+      <c r="E150" s="63"/>
       <c r="F150" s="55"/>
       <c r="G150" s="55"/>
       <c r="H150" s="55"/>
@@ -3696,7 +3696,7 @@
       </c>
       <c r="C151" s="55"/>
       <c r="D151" s="55"/>
-      <c r="E151" s="69"/>
+      <c r="E151" s="63"/>
       <c r="F151" s="55"/>
       <c r="G151" s="55"/>
       <c r="H151" s="55"/>
@@ -3711,7 +3711,7 @@
       </c>
       <c r="C152" s="55"/>
       <c r="D152" s="55"/>
-      <c r="E152" s="69"/>
+      <c r="E152" s="63"/>
       <c r="F152" s="55"/>
       <c r="G152" s="55"/>
       <c r="H152" s="55"/>
@@ -3726,7 +3726,7 @@
       </c>
       <c r="C153" s="55"/>
       <c r="D153" s="55"/>
-      <c r="E153" s="69"/>
+      <c r="E153" s="63"/>
       <c r="F153" s="55"/>
       <c r="G153" s="55"/>
       <c r="H153" s="55"/>
@@ -3741,7 +3741,7 @@
       </c>
       <c r="C154" s="55"/>
       <c r="D154" s="55"/>
-      <c r="E154" s="69"/>
+      <c r="E154" s="63"/>
       <c r="F154" s="55"/>
       <c r="G154" s="55"/>
       <c r="H154" s="55"/>
@@ -3756,7 +3756,7 @@
       </c>
       <c r="C155" s="55"/>
       <c r="D155" s="55"/>
-      <c r="E155" s="69"/>
+      <c r="E155" s="63"/>
       <c r="F155" s="55"/>
       <c r="G155" s="55"/>
       <c r="H155" s="55"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="C156" s="55"/>
       <c r="D156" s="55"/>
-      <c r="E156" s="69"/>
+      <c r="E156" s="63"/>
       <c r="F156" s="55"/>
       <c r="G156" s="55"/>
       <c r="H156" s="55"/>
@@ -3786,7 +3786,7 @@
       </c>
       <c r="C157" s="55"/>
       <c r="D157" s="55"/>
-      <c r="E157" s="69"/>
+      <c r="E157" s="63"/>
       <c r="F157" s="55"/>
       <c r="G157" s="55"/>
       <c r="H157" s="55"/>
@@ -3801,7 +3801,7 @@
       </c>
       <c r="C158" s="55"/>
       <c r="D158" s="55"/>
-      <c r="E158" s="69"/>
+      <c r="E158" s="63"/>
       <c r="F158" s="55"/>
       <c r="G158" s="55"/>
       <c r="H158" s="55"/>
@@ -3816,7 +3816,7 @@
       </c>
       <c r="C159" s="55"/>
       <c r="D159" s="55"/>
-      <c r="E159" s="69"/>
+      <c r="E159" s="63"/>
       <c r="F159" s="55"/>
       <c r="G159" s="55"/>
       <c r="H159" s="55"/>
@@ -3831,7 +3831,7 @@
       </c>
       <c r="C160" s="55"/>
       <c r="D160" s="55"/>
-      <c r="E160" s="69"/>
+      <c r="E160" s="63"/>
       <c r="F160" s="55"/>
       <c r="G160" s="55"/>
       <c r="H160" s="55"/>
@@ -3848,7 +3848,7 @@
       </c>
       <c r="C161" s="55"/>
       <c r="D161" s="55"/>
-      <c r="E161" s="70"/>
+      <c r="E161" s="64"/>
       <c r="F161" s="55"/>
       <c r="G161" s="55"/>
       <c r="H161" s="55"/>
@@ -3865,7 +3865,7 @@
       </c>
       <c r="C162" s="55"/>
       <c r="D162" s="55"/>
-      <c r="E162" s="62" t="s">
+      <c r="E162" s="70" t="s">
         <v>26</v>
       </c>
       <c r="F162" s="55"/>
@@ -3884,7 +3884,7 @@
       </c>
       <c r="C163" s="55"/>
       <c r="D163" s="55"/>
-      <c r="E163" s="63"/>
+      <c r="E163" s="71"/>
       <c r="F163" s="55"/>
       <c r="G163" s="55"/>
       <c r="H163" s="55"/>
@@ -3899,7 +3899,7 @@
       </c>
       <c r="C164" s="55"/>
       <c r="D164" s="55"/>
-      <c r="E164" s="63"/>
+      <c r="E164" s="71"/>
       <c r="F164" s="55"/>
       <c r="G164" s="55"/>
       <c r="H164" s="55"/>
@@ -3914,7 +3914,7 @@
       </c>
       <c r="C165" s="55"/>
       <c r="D165" s="55"/>
-      <c r="E165" s="63"/>
+      <c r="E165" s="71"/>
       <c r="F165" s="55"/>
       <c r="G165" s="55"/>
       <c r="H165" s="55"/>
@@ -3929,7 +3929,7 @@
       </c>
       <c r="C166" s="55"/>
       <c r="D166" s="55"/>
-      <c r="E166" s="63"/>
+      <c r="E166" s="71"/>
       <c r="F166" s="55"/>
       <c r="G166" s="55"/>
       <c r="H166" s="55"/>
@@ -3944,7 +3944,7 @@
       </c>
       <c r="C167" s="55"/>
       <c r="D167" s="55"/>
-      <c r="E167" s="63"/>
+      <c r="E167" s="71"/>
       <c r="F167" s="55"/>
       <c r="G167" s="55"/>
       <c r="H167" s="55"/>
@@ -3959,7 +3959,7 @@
       </c>
       <c r="C168" s="55"/>
       <c r="D168" s="55"/>
-      <c r="E168" s="63"/>
+      <c r="E168" s="71"/>
       <c r="F168" s="55"/>
       <c r="G168" s="55"/>
       <c r="H168" s="55"/>
@@ -3974,7 +3974,7 @@
       </c>
       <c r="C169" s="55"/>
       <c r="D169" s="55"/>
-      <c r="E169" s="63"/>
+      <c r="E169" s="71"/>
       <c r="F169" s="55"/>
       <c r="G169" s="55"/>
       <c r="H169" s="55"/>
@@ -3989,7 +3989,7 @@
       </c>
       <c r="C170" s="55"/>
       <c r="D170" s="55"/>
-      <c r="E170" s="63"/>
+      <c r="E170" s="71"/>
       <c r="F170" s="55"/>
       <c r="G170" s="55"/>
       <c r="H170" s="55"/>
@@ -4004,7 +4004,7 @@
       </c>
       <c r="C171" s="55"/>
       <c r="D171" s="55"/>
-      <c r="E171" s="63"/>
+      <c r="E171" s="71"/>
       <c r="F171" s="55"/>
       <c r="G171" s="55"/>
       <c r="H171" s="55"/>
@@ -4019,7 +4019,7 @@
       </c>
       <c r="C172" s="55"/>
       <c r="D172" s="55"/>
-      <c r="E172" s="63"/>
+      <c r="E172" s="71"/>
       <c r="F172" s="55"/>
       <c r="G172" s="55"/>
       <c r="H172" s="55"/>
@@ -4034,7 +4034,7 @@
       </c>
       <c r="C173" s="55"/>
       <c r="D173" s="55"/>
-      <c r="E173" s="63"/>
+      <c r="E173" s="71"/>
       <c r="F173" s="55"/>
       <c r="G173" s="55"/>
       <c r="H173" s="55"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="C174" s="55"/>
       <c r="D174" s="55"/>
-      <c r="E174" s="63"/>
+      <c r="E174" s="71"/>
       <c r="F174" s="55"/>
       <c r="G174" s="55"/>
       <c r="H174" s="55"/>
@@ -4064,7 +4064,7 @@
       </c>
       <c r="C175" s="55"/>
       <c r="D175" s="55"/>
-      <c r="E175" s="63"/>
+      <c r="E175" s="71"/>
       <c r="F175" s="55"/>
       <c r="G175" s="55"/>
       <c r="H175" s="55"/>
@@ -4079,7 +4079,7 @@
       </c>
       <c r="C176" s="55"/>
       <c r="D176" s="55"/>
-      <c r="E176" s="63"/>
+      <c r="E176" s="71"/>
       <c r="F176" s="55"/>
       <c r="G176" s="55"/>
       <c r="H176" s="55"/>
@@ -4096,7 +4096,7 @@
       </c>
       <c r="C177" s="55"/>
       <c r="D177" s="55"/>
-      <c r="E177" s="64"/>
+      <c r="E177" s="72"/>
       <c r="F177" s="55"/>
       <c r="G177" s="55"/>
       <c r="H177" s="55"/>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="C178" s="55"/>
       <c r="D178" s="55"/>
-      <c r="E178" s="71" t="s">
+      <c r="E178" s="66" t="s">
         <v>27</v>
       </c>
       <c r="F178" s="55"/>
@@ -4132,7 +4132,7 @@
       </c>
       <c r="C179" s="55"/>
       <c r="D179" s="55"/>
-      <c r="E179" s="71"/>
+      <c r="E179" s="66"/>
       <c r="F179" s="55"/>
       <c r="G179" s="55"/>
       <c r="H179" s="55"/>
@@ -4147,7 +4147,7 @@
       </c>
       <c r="C180" s="55"/>
       <c r="D180" s="55"/>
-      <c r="E180" s="71"/>
+      <c r="E180" s="66"/>
       <c r="F180" s="55"/>
       <c r="G180" s="55"/>
       <c r="H180" s="55"/>
@@ -4162,7 +4162,7 @@
       </c>
       <c r="C181" s="55"/>
       <c r="D181" s="55"/>
-      <c r="E181" s="71"/>
+      <c r="E181" s="66"/>
       <c r="F181" s="55"/>
       <c r="G181" s="55"/>
       <c r="H181" s="55"/>
@@ -4177,7 +4177,7 @@
       </c>
       <c r="C182" s="55"/>
       <c r="D182" s="55"/>
-      <c r="E182" s="71"/>
+      <c r="E182" s="66"/>
       <c r="F182" s="55"/>
       <c r="G182" s="55"/>
       <c r="H182" s="55"/>
@@ -4192,7 +4192,7 @@
       </c>
       <c r="C183" s="55"/>
       <c r="D183" s="55"/>
-      <c r="E183" s="71"/>
+      <c r="E183" s="66"/>
       <c r="F183" s="55"/>
       <c r="G183" s="55"/>
       <c r="H183" s="55"/>
@@ -4207,7 +4207,7 @@
       </c>
       <c r="C184" s="55"/>
       <c r="D184" s="55"/>
-      <c r="E184" s="71"/>
+      <c r="E184" s="66"/>
       <c r="F184" s="55"/>
       <c r="G184" s="55"/>
       <c r="H184" s="55"/>
@@ -4222,7 +4222,7 @@
       </c>
       <c r="C185" s="55"/>
       <c r="D185" s="55"/>
-      <c r="E185" s="71"/>
+      <c r="E185" s="66"/>
       <c r="F185" s="55"/>
       <c r="G185" s="55"/>
       <c r="H185" s="55"/>
@@ -4237,7 +4237,7 @@
       </c>
       <c r="C186" s="55"/>
       <c r="D186" s="55"/>
-      <c r="E186" s="71"/>
+      <c r="E186" s="66"/>
       <c r="F186" s="55"/>
       <c r="G186" s="55"/>
       <c r="H186" s="55"/>
@@ -4252,7 +4252,7 @@
       </c>
       <c r="C187" s="55"/>
       <c r="D187" s="55"/>
-      <c r="E187" s="71"/>
+      <c r="E187" s="66"/>
       <c r="F187" s="55"/>
       <c r="G187" s="55"/>
       <c r="H187" s="55"/>
@@ -4267,7 +4267,7 @@
       </c>
       <c r="C188" s="55"/>
       <c r="D188" s="55"/>
-      <c r="E188" s="71"/>
+      <c r="E188" s="66"/>
       <c r="F188" s="55"/>
       <c r="G188" s="55"/>
       <c r="H188" s="55"/>
@@ -4282,7 +4282,7 @@
       </c>
       <c r="C189" s="55"/>
       <c r="D189" s="55"/>
-      <c r="E189" s="71"/>
+      <c r="E189" s="66"/>
       <c r="F189" s="55"/>
       <c r="G189" s="55"/>
       <c r="H189" s="55"/>
@@ -4297,7 +4297,7 @@
       </c>
       <c r="C190" s="55"/>
       <c r="D190" s="55"/>
-      <c r="E190" s="71"/>
+      <c r="E190" s="66"/>
       <c r="F190" s="55"/>
       <c r="G190" s="55"/>
       <c r="H190" s="55"/>
@@ -4312,7 +4312,7 @@
       </c>
       <c r="C191" s="55"/>
       <c r="D191" s="55"/>
-      <c r="E191" s="71"/>
+      <c r="E191" s="66"/>
       <c r="F191" s="55"/>
       <c r="G191" s="55"/>
       <c r="H191" s="55"/>
@@ -4327,7 +4327,7 @@
       </c>
       <c r="C192" s="55"/>
       <c r="D192" s="55"/>
-      <c r="E192" s="71"/>
+      <c r="E192" s="66"/>
       <c r="F192" s="55"/>
       <c r="G192" s="55"/>
       <c r="H192" s="55"/>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="C193" s="55"/>
       <c r="D193" s="55"/>
-      <c r="E193" s="71"/>
+      <c r="E193" s="66"/>
       <c r="F193" s="55"/>
       <c r="G193" s="55"/>
       <c r="H193" s="55"/>
@@ -4360,7 +4360,7 @@
         <v>192</v>
       </c>
       <c r="C194" s="55"/>
-      <c r="D194" s="72" t="s">
+      <c r="D194" s="67" t="s">
         <v>25</v>
       </c>
       <c r="E194" s="55"/>
@@ -4379,7 +4379,7 @@
         <v>193</v>
       </c>
       <c r="C195" s="55"/>
-      <c r="D195" s="73"/>
+      <c r="D195" s="68"/>
       <c r="E195" s="55"/>
       <c r="F195" s="55"/>
       <c r="G195" s="55"/>
@@ -4394,7 +4394,7 @@
         <v>194</v>
       </c>
       <c r="C196" s="55"/>
-      <c r="D196" s="73"/>
+      <c r="D196" s="68"/>
       <c r="E196" s="55"/>
       <c r="F196" s="55"/>
       <c r="G196" s="55"/>
@@ -4409,7 +4409,7 @@
         <v>195</v>
       </c>
       <c r="C197" s="55"/>
-      <c r="D197" s="73"/>
+      <c r="D197" s="68"/>
       <c r="E197" s="55"/>
       <c r="F197" s="55"/>
       <c r="G197" s="55"/>
@@ -4424,7 +4424,7 @@
         <v>196</v>
       </c>
       <c r="C198" s="55"/>
-      <c r="D198" s="73"/>
+      <c r="D198" s="68"/>
       <c r="E198" s="55"/>
       <c r="F198" s="55"/>
       <c r="G198" s="55"/>
@@ -4439,7 +4439,7 @@
         <v>197</v>
       </c>
       <c r="C199" s="55"/>
-      <c r="D199" s="73"/>
+      <c r="D199" s="68"/>
       <c r="E199" s="55"/>
       <c r="F199" s="55"/>
       <c r="G199" s="55"/>
@@ -4454,7 +4454,7 @@
         <v>198</v>
       </c>
       <c r="C200" s="55"/>
-      <c r="D200" s="73"/>
+      <c r="D200" s="68"/>
       <c r="E200" s="55"/>
       <c r="F200" s="55"/>
       <c r="G200" s="55"/>
@@ -4471,7 +4471,7 @@
         <v>199</v>
       </c>
       <c r="C201" s="55"/>
-      <c r="D201" s="74"/>
+      <c r="D201" s="69"/>
       <c r="E201" s="55"/>
       <c r="F201" s="55"/>
       <c r="G201" s="55"/>
@@ -4488,7 +4488,7 @@
         <v>200</v>
       </c>
       <c r="C202" s="55"/>
-      <c r="D202" s="56" t="s">
+      <c r="D202" s="76" t="s">
         <v>24</v>
       </c>
       <c r="E202" s="55"/>
@@ -4507,7 +4507,7 @@
         <v>201</v>
       </c>
       <c r="C203" s="55"/>
-      <c r="D203" s="56"/>
+      <c r="D203" s="76"/>
       <c r="E203" s="55"/>
       <c r="F203" s="55"/>
       <c r="G203" s="55"/>
@@ -4522,7 +4522,7 @@
         <v>202</v>
       </c>
       <c r="C204" s="55"/>
-      <c r="D204" s="56"/>
+      <c r="D204" s="76"/>
       <c r="E204" s="55"/>
       <c r="F204" s="55"/>
       <c r="G204" s="55"/>
@@ -4537,7 +4537,7 @@
         <v>203</v>
       </c>
       <c r="C205" s="55"/>
-      <c r="D205" s="56"/>
+      <c r="D205" s="76"/>
       <c r="E205" s="55"/>
       <c r="F205" s="55"/>
       <c r="G205" s="55"/>
@@ -4552,7 +4552,7 @@
         <v>204</v>
       </c>
       <c r="C206" s="55"/>
-      <c r="D206" s="56"/>
+      <c r="D206" s="76"/>
       <c r="E206" s="55"/>
       <c r="F206" s="55"/>
       <c r="G206" s="55"/>
@@ -4567,7 +4567,7 @@
         <v>205</v>
       </c>
       <c r="C207" s="55"/>
-      <c r="D207" s="56"/>
+      <c r="D207" s="76"/>
       <c r="E207" s="55"/>
       <c r="F207" s="55"/>
       <c r="G207" s="55"/>
@@ -4582,7 +4582,7 @@
         <v>206</v>
       </c>
       <c r="C208" s="55"/>
-      <c r="D208" s="56"/>
+      <c r="D208" s="76"/>
       <c r="E208" s="55"/>
       <c r="F208" s="55"/>
       <c r="G208" s="55"/>
@@ -4599,7 +4599,7 @@
         <v>207</v>
       </c>
       <c r="C209" s="55"/>
-      <c r="D209" s="56"/>
+      <c r="D209" s="76"/>
       <c r="E209" s="55"/>
       <c r="F209" s="55"/>
       <c r="G209" s="55"/>
@@ -4615,9 +4615,9 @@
       <c r="B210" s="32">
         <v>208</v>
       </c>
-      <c r="C210" s="57"/>
-      <c r="D210" s="58"/>
-      <c r="E210" s="59" t="s">
+      <c r="C210" s="77"/>
+      <c r="D210" s="78"/>
+      <c r="E210" s="79" t="s">
         <v>34</v>
       </c>
       <c r="F210" s="55"/>
@@ -4634,9 +4634,9 @@
       <c r="B211" s="32">
         <v>209</v>
       </c>
-      <c r="C211" s="57"/>
-      <c r="D211" s="58"/>
-      <c r="E211" s="59"/>
+      <c r="C211" s="77"/>
+      <c r="D211" s="78"/>
+      <c r="E211" s="79"/>
       <c r="F211" s="55"/>
       <c r="G211" s="55"/>
       <c r="H211" s="55"/>
@@ -4651,9 +4651,9 @@
       <c r="B212" s="32">
         <v>210</v>
       </c>
-      <c r="C212" s="57"/>
-      <c r="D212" s="58"/>
-      <c r="E212" s="59"/>
+      <c r="C212" s="77"/>
+      <c r="D212" s="78"/>
+      <c r="E212" s="79"/>
       <c r="F212" s="55"/>
       <c r="G212" s="55"/>
       <c r="H212" s="55"/>
@@ -4668,9 +4668,9 @@
       <c r="B213" s="32">
         <v>211</v>
       </c>
-      <c r="C213" s="57"/>
-      <c r="D213" s="58"/>
-      <c r="E213" s="59"/>
+      <c r="C213" s="77"/>
+      <c r="D213" s="78"/>
+      <c r="E213" s="79"/>
       <c r="F213" s="55"/>
       <c r="G213" s="55"/>
       <c r="H213" s="55"/>
@@ -4685,9 +4685,9 @@
       <c r="B214" s="32">
         <v>212</v>
       </c>
-      <c r="C214" s="57"/>
-      <c r="D214" s="58"/>
-      <c r="E214" s="59"/>
+      <c r="C214" s="77"/>
+      <c r="D214" s="78"/>
+      <c r="E214" s="79"/>
       <c r="F214" s="55"/>
       <c r="G214" s="55"/>
       <c r="H214" s="55"/>
@@ -4700,9 +4700,9 @@
       <c r="B215" s="32">
         <v>213</v>
       </c>
-      <c r="C215" s="57"/>
-      <c r="D215" s="58"/>
-      <c r="E215" s="59"/>
+      <c r="C215" s="77"/>
+      <c r="D215" s="78"/>
+      <c r="E215" s="79"/>
       <c r="F215" s="55"/>
       <c r="G215" s="55"/>
       <c r="H215" s="55"/>
@@ -4715,9 +4715,9 @@
       <c r="B216" s="32">
         <v>214</v>
       </c>
-      <c r="C216" s="57"/>
-      <c r="D216" s="58"/>
-      <c r="E216" s="59"/>
+      <c r="C216" s="77"/>
+      <c r="D216" s="78"/>
+      <c r="E216" s="79"/>
       <c r="F216" s="55"/>
       <c r="G216" s="55"/>
       <c r="H216" s="55"/>
@@ -4730,9 +4730,9 @@
       <c r="B217" s="32">
         <v>215</v>
       </c>
-      <c r="C217" s="57"/>
-      <c r="D217" s="58"/>
-      <c r="E217" s="59"/>
+      <c r="C217" s="77"/>
+      <c r="D217" s="78"/>
+      <c r="E217" s="79"/>
       <c r="F217" s="55"/>
       <c r="G217" s="55"/>
       <c r="H217" s="55"/>
@@ -4746,8 +4746,8 @@
         <v>216</v>
       </c>
       <c r="C218" s="55"/>
-      <c r="D218" s="65"/>
-      <c r="E218" s="59"/>
+      <c r="D218" s="73"/>
+      <c r="E218" s="79"/>
       <c r="F218" s="55"/>
       <c r="G218" s="55"/>
       <c r="H218" s="55"/>
@@ -4761,8 +4761,8 @@
         <v>217</v>
       </c>
       <c r="C219" s="55"/>
-      <c r="D219" s="65"/>
-      <c r="E219" s="59"/>
+      <c r="D219" s="73"/>
+      <c r="E219" s="79"/>
       <c r="F219" s="55"/>
       <c r="G219" s="55"/>
       <c r="H219" s="55"/>
@@ -4776,8 +4776,8 @@
         <v>218</v>
       </c>
       <c r="C220" s="55"/>
-      <c r="D220" s="65"/>
-      <c r="E220" s="59"/>
+      <c r="D220" s="73"/>
+      <c r="E220" s="79"/>
       <c r="F220" s="55"/>
       <c r="G220" s="55"/>
       <c r="H220" s="55"/>
@@ -4791,8 +4791,8 @@
         <v>219</v>
       </c>
       <c r="C221" s="55"/>
-      <c r="D221" s="65"/>
-      <c r="E221" s="59"/>
+      <c r="D221" s="73"/>
+      <c r="E221" s="79"/>
       <c r="F221" s="55"/>
       <c r="G221" s="55"/>
       <c r="H221" s="55"/>
@@ -4806,8 +4806,8 @@
         <v>220</v>
       </c>
       <c r="C222" s="55"/>
-      <c r="D222" s="65"/>
-      <c r="E222" s="59"/>
+      <c r="D222" s="73"/>
+      <c r="E222" s="79"/>
       <c r="F222" s="55"/>
       <c r="G222" s="55"/>
       <c r="H222" s="55"/>
@@ -4821,8 +4821,8 @@
         <v>221</v>
       </c>
       <c r="C223" s="55"/>
-      <c r="D223" s="65"/>
-      <c r="E223" s="59"/>
+      <c r="D223" s="73"/>
+      <c r="E223" s="79"/>
       <c r="F223" s="55"/>
       <c r="G223" s="55"/>
       <c r="H223" s="55"/>
@@ -4836,8 +4836,8 @@
         <v>222</v>
       </c>
       <c r="C224" s="55"/>
-      <c r="D224" s="65"/>
-      <c r="E224" s="59"/>
+      <c r="D224" s="73"/>
+      <c r="E224" s="79"/>
       <c r="F224" s="55"/>
       <c r="G224" s="55"/>
       <c r="H224" s="55"/>
@@ -4851,8 +4851,8 @@
         <v>223</v>
       </c>
       <c r="C225" s="55"/>
-      <c r="D225" s="65"/>
-      <c r="E225" s="59"/>
+      <c r="D225" s="73"/>
+      <c r="E225" s="79"/>
       <c r="F225" s="55"/>
       <c r="G225" s="55"/>
       <c r="H225" s="55"/>
@@ -4867,8 +4867,8 @@
       <c r="B226" s="51">
         <v>224</v>
       </c>
-      <c r="C226" s="66"/>
-      <c r="D226" s="67" t="s">
+      <c r="C226" s="74"/>
+      <c r="D226" s="75" t="s">
         <v>29</v>
       </c>
       <c r="E226" s="55"/>
@@ -4886,8 +4886,8 @@
       <c r="B227" s="51">
         <v>225</v>
       </c>
-      <c r="C227" s="66"/>
-      <c r="D227" s="67"/>
+      <c r="C227" s="74"/>
+      <c r="D227" s="75"/>
       <c r="E227" s="55"/>
       <c r="F227" s="55"/>
       <c r="G227" s="55"/>
@@ -4901,8 +4901,8 @@
       <c r="B228" s="51">
         <v>226</v>
       </c>
-      <c r="C228" s="66"/>
-      <c r="D228" s="67"/>
+      <c r="C228" s="74"/>
+      <c r="D228" s="75"/>
       <c r="E228" s="55"/>
       <c r="F228" s="55"/>
       <c r="G228" s="55"/>
@@ -4916,8 +4916,8 @@
       <c r="B229" s="51">
         <v>227</v>
       </c>
-      <c r="C229" s="66"/>
-      <c r="D229" s="67"/>
+      <c r="C229" s="74"/>
+      <c r="D229" s="75"/>
       <c r="E229" s="55"/>
       <c r="F229" s="55"/>
       <c r="G229" s="55"/>
@@ -4931,8 +4931,8 @@
       <c r="B230" s="51">
         <v>228</v>
       </c>
-      <c r="C230" s="60"/>
-      <c r="D230" s="67"/>
+      <c r="C230" s="80"/>
+      <c r="D230" s="75"/>
       <c r="E230" s="55"/>
       <c r="F230" s="55"/>
       <c r="G230" s="55"/>
@@ -4946,8 +4946,8 @@
       <c r="B231" s="51">
         <v>229</v>
       </c>
-      <c r="C231" s="60"/>
-      <c r="D231" s="67"/>
+      <c r="C231" s="80"/>
+      <c r="D231" s="75"/>
       <c r="E231" s="55"/>
       <c r="F231" s="55"/>
       <c r="G231" s="55"/>
@@ -4961,8 +4961,8 @@
       <c r="B232" s="51">
         <v>230</v>
       </c>
-      <c r="C232" s="60"/>
-      <c r="D232" s="67"/>
+      <c r="C232" s="80"/>
+      <c r="D232" s="75"/>
       <c r="E232" s="55"/>
       <c r="F232" s="55"/>
       <c r="G232" s="55"/>
@@ -4976,8 +4976,8 @@
       <c r="B233" s="51">
         <v>231</v>
       </c>
-      <c r="C233" s="60"/>
-      <c r="D233" s="67"/>
+      <c r="C233" s="80"/>
+      <c r="D233" s="75"/>
       <c r="E233" s="55"/>
       <c r="F233" s="55"/>
       <c r="G233" s="55"/>
@@ -4993,7 +4993,7 @@
       <c r="B234" s="47">
         <v>232</v>
       </c>
-      <c r="C234" s="61" t="s">
+      <c r="C234" s="81" t="s">
         <v>30</v>
       </c>
       <c r="D234" s="55"/>
@@ -5012,7 +5012,7 @@
       <c r="B235" s="47">
         <v>233</v>
       </c>
-      <c r="C235" s="61"/>
+      <c r="C235" s="81"/>
       <c r="D235" s="55"/>
       <c r="E235" s="55"/>
       <c r="F235" s="55"/>
@@ -5029,7 +5029,7 @@
       <c r="B236" s="47">
         <v>234</v>
       </c>
-      <c r="C236" s="61"/>
+      <c r="C236" s="81"/>
       <c r="D236" s="55"/>
       <c r="E236" s="55"/>
       <c r="F236" s="55"/>
@@ -5046,7 +5046,7 @@
       <c r="B237" s="47">
         <v>235</v>
       </c>
-      <c r="C237" s="61"/>
+      <c r="C237" s="81"/>
       <c r="D237" s="55"/>
       <c r="E237" s="55"/>
       <c r="F237" s="55"/>
@@ -5358,6 +5358,108 @@
     </row>
   </sheetData>
   <mergeCells count="126">
+    <mergeCell ref="F194:F225"/>
+    <mergeCell ref="G194:G257"/>
+    <mergeCell ref="C198:C201"/>
+    <mergeCell ref="C202:C205"/>
+    <mergeCell ref="D202:D209"/>
+    <mergeCell ref="C206:C209"/>
+    <mergeCell ref="C210:C213"/>
+    <mergeCell ref="D210:D217"/>
+    <mergeCell ref="E210:E225"/>
+    <mergeCell ref="C214:C217"/>
+    <mergeCell ref="D250:D257"/>
+    <mergeCell ref="C254:C257"/>
+    <mergeCell ref="F226:F257"/>
+    <mergeCell ref="C230:C233"/>
+    <mergeCell ref="C234:C237"/>
+    <mergeCell ref="D234:D241"/>
+    <mergeCell ref="C238:C241"/>
+    <mergeCell ref="C242:C245"/>
+    <mergeCell ref="D242:D249"/>
+    <mergeCell ref="E242:E257"/>
+    <mergeCell ref="C246:C249"/>
+    <mergeCell ref="C250:C253"/>
+    <mergeCell ref="E194:E209"/>
+    <mergeCell ref="C162:C165"/>
+    <mergeCell ref="D162:D169"/>
+    <mergeCell ref="E162:E177"/>
+    <mergeCell ref="C218:C221"/>
+    <mergeCell ref="D218:D225"/>
+    <mergeCell ref="C222:C225"/>
+    <mergeCell ref="C226:C229"/>
+    <mergeCell ref="D226:D233"/>
+    <mergeCell ref="E226:E241"/>
+    <mergeCell ref="F162:F193"/>
+    <mergeCell ref="C166:C169"/>
+    <mergeCell ref="C170:C173"/>
+    <mergeCell ref="D170:D177"/>
+    <mergeCell ref="C174:C177"/>
+    <mergeCell ref="C178:C181"/>
+    <mergeCell ref="D178:D185"/>
+    <mergeCell ref="G130:G193"/>
+    <mergeCell ref="H130:H257"/>
+    <mergeCell ref="C134:C137"/>
+    <mergeCell ref="C138:C141"/>
+    <mergeCell ref="D138:D145"/>
+    <mergeCell ref="C142:C145"/>
+    <mergeCell ref="C146:C149"/>
+    <mergeCell ref="D146:D153"/>
+    <mergeCell ref="E146:E161"/>
+    <mergeCell ref="C150:C153"/>
+    <mergeCell ref="E178:E193"/>
+    <mergeCell ref="C182:C185"/>
+    <mergeCell ref="C186:C189"/>
+    <mergeCell ref="D186:D193"/>
+    <mergeCell ref="C190:C193"/>
+    <mergeCell ref="C194:C197"/>
+    <mergeCell ref="D194:D201"/>
+    <mergeCell ref="C130:C133"/>
+    <mergeCell ref="D130:D137"/>
+    <mergeCell ref="E130:E145"/>
+    <mergeCell ref="F130:F161"/>
+    <mergeCell ref="C154:C157"/>
+    <mergeCell ref="D154:D161"/>
+    <mergeCell ref="C158:C161"/>
+    <mergeCell ref="F98:F129"/>
+    <mergeCell ref="C102:C105"/>
+    <mergeCell ref="C106:C109"/>
+    <mergeCell ref="D106:D113"/>
+    <mergeCell ref="C110:C113"/>
+    <mergeCell ref="C114:C117"/>
+    <mergeCell ref="D114:D121"/>
+    <mergeCell ref="E114:E129"/>
+    <mergeCell ref="C118:C121"/>
+    <mergeCell ref="C122:C125"/>
+    <mergeCell ref="C90:C93"/>
+    <mergeCell ref="D90:D97"/>
+    <mergeCell ref="C94:C97"/>
+    <mergeCell ref="C98:C101"/>
+    <mergeCell ref="D98:D105"/>
+    <mergeCell ref="E98:E113"/>
+    <mergeCell ref="F66:F97"/>
+    <mergeCell ref="G66:G129"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="C74:C77"/>
+    <mergeCell ref="D74:D81"/>
+    <mergeCell ref="C78:C81"/>
+    <mergeCell ref="C82:C85"/>
+    <mergeCell ref="D82:D89"/>
+    <mergeCell ref="E82:E97"/>
+    <mergeCell ref="C86:C89"/>
+    <mergeCell ref="D122:D129"/>
+    <mergeCell ref="C126:C129"/>
+    <mergeCell ref="E50:E65"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="D58:D65"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="D66:D73"/>
+    <mergeCell ref="E66:E81"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="D34:D41"/>
+    <mergeCell ref="E34:E49"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="D2:D9"/>
     <mergeCell ref="E2:E17"/>
@@ -5382,108 +5484,6 @@
     <mergeCell ref="C26:C29"/>
     <mergeCell ref="D26:D33"/>
     <mergeCell ref="C30:C33"/>
-    <mergeCell ref="E50:E65"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="D58:D65"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="C66:C69"/>
-    <mergeCell ref="D66:D73"/>
-    <mergeCell ref="E66:E81"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="D34:D41"/>
-    <mergeCell ref="E34:E49"/>
-    <mergeCell ref="C90:C93"/>
-    <mergeCell ref="D90:D97"/>
-    <mergeCell ref="C94:C97"/>
-    <mergeCell ref="C98:C101"/>
-    <mergeCell ref="D98:D105"/>
-    <mergeCell ref="E98:E113"/>
-    <mergeCell ref="F66:F97"/>
-    <mergeCell ref="G66:G129"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="C74:C77"/>
-    <mergeCell ref="D74:D81"/>
-    <mergeCell ref="C78:C81"/>
-    <mergeCell ref="C82:C85"/>
-    <mergeCell ref="D82:D89"/>
-    <mergeCell ref="E82:E97"/>
-    <mergeCell ref="C86:C89"/>
-    <mergeCell ref="D122:D129"/>
-    <mergeCell ref="C126:C129"/>
-    <mergeCell ref="C130:C133"/>
-    <mergeCell ref="D130:D137"/>
-    <mergeCell ref="E130:E145"/>
-    <mergeCell ref="F130:F161"/>
-    <mergeCell ref="C154:C157"/>
-    <mergeCell ref="D154:D161"/>
-    <mergeCell ref="C158:C161"/>
-    <mergeCell ref="F98:F129"/>
-    <mergeCell ref="C102:C105"/>
-    <mergeCell ref="C106:C109"/>
-    <mergeCell ref="D106:D113"/>
-    <mergeCell ref="C110:C113"/>
-    <mergeCell ref="C114:C117"/>
-    <mergeCell ref="D114:D121"/>
-    <mergeCell ref="E114:E129"/>
-    <mergeCell ref="C118:C121"/>
-    <mergeCell ref="C122:C125"/>
-    <mergeCell ref="F162:F193"/>
-    <mergeCell ref="C166:C169"/>
-    <mergeCell ref="C170:C173"/>
-    <mergeCell ref="D170:D177"/>
-    <mergeCell ref="C174:C177"/>
-    <mergeCell ref="C178:C181"/>
-    <mergeCell ref="D178:D185"/>
-    <mergeCell ref="G130:G193"/>
-    <mergeCell ref="H130:H257"/>
-    <mergeCell ref="C134:C137"/>
-    <mergeCell ref="C138:C141"/>
-    <mergeCell ref="D138:D145"/>
-    <mergeCell ref="C142:C145"/>
-    <mergeCell ref="C146:C149"/>
-    <mergeCell ref="D146:D153"/>
-    <mergeCell ref="E146:E161"/>
-    <mergeCell ref="C150:C153"/>
-    <mergeCell ref="E178:E193"/>
-    <mergeCell ref="C182:C185"/>
-    <mergeCell ref="C186:C189"/>
-    <mergeCell ref="D186:D193"/>
-    <mergeCell ref="C190:C193"/>
-    <mergeCell ref="C194:C197"/>
-    <mergeCell ref="D194:D201"/>
-    <mergeCell ref="C162:C165"/>
-    <mergeCell ref="D162:D169"/>
-    <mergeCell ref="E162:E177"/>
-    <mergeCell ref="C218:C221"/>
-    <mergeCell ref="D218:D225"/>
-    <mergeCell ref="C222:C225"/>
-    <mergeCell ref="C226:C229"/>
-    <mergeCell ref="D226:D233"/>
-    <mergeCell ref="E226:E241"/>
-    <mergeCell ref="F194:F225"/>
-    <mergeCell ref="G194:G257"/>
-    <mergeCell ref="C198:C201"/>
-    <mergeCell ref="C202:C205"/>
-    <mergeCell ref="D202:D209"/>
-    <mergeCell ref="C206:C209"/>
-    <mergeCell ref="C210:C213"/>
-    <mergeCell ref="D210:D217"/>
-    <mergeCell ref="E210:E225"/>
-    <mergeCell ref="C214:C217"/>
-    <mergeCell ref="D250:D257"/>
-    <mergeCell ref="C254:C257"/>
-    <mergeCell ref="F226:F257"/>
-    <mergeCell ref="C230:C233"/>
-    <mergeCell ref="C234:C237"/>
-    <mergeCell ref="D234:D241"/>
-    <mergeCell ref="C238:C241"/>
-    <mergeCell ref="C242:C245"/>
-    <mergeCell ref="D242:D249"/>
-    <mergeCell ref="E242:E257"/>
-    <mergeCell ref="C246:C249"/>
-    <mergeCell ref="C250:C253"/>
-    <mergeCell ref="E194:E209"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Test plan finished, added DHCP table to \Kisvállalat létszám.xlsx
</commit_message>
<xml_diff>
--- a/Kisvállalat létszám.xlsx
+++ b/Kisvállalat létszám.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\projekt\fluffy-system\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\School\11.o\Hálózat\projekt\fluffy-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCAC3EC-1F5D-4942-B5F9-C84EC402FFD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACE4CBB-EDAE-4896-B22D-B8E816D0116A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13755" windowHeight="10665" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alap" sheetId="1" r:id="rId1"/>
     <sheet name="VLSM" sheetId="4" r:id="rId2"/>
     <sheet name="VLAN" sheetId="5" r:id="rId3"/>
+    <sheet name="DHCP" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="98">
   <si>
     <t>I.em</t>
   </si>
@@ -210,6 +211,117 @@
   </si>
   <si>
     <t>S2</t>
+  </si>
+  <si>
+    <t>Szervezeti egység</t>
+  </si>
+  <si>
+    <t>Alhálózat címe</t>
+  </si>
+  <si>
+    <t>Átjáró címe</t>
+  </si>
+  <si>
+    <t>DNS</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>Net engeneer</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>WiFi</t>
+  </si>
+  <si>
+    <t>192.168.1.233</t>
+  </si>
+  <si>
+    <t>192.168.1.200 /29</t>
+  </si>
+  <si>
+    <t>192.168.1.64 / 28</t>
+  </si>
+  <si>
+    <t>192.168.1.32 /28</t>
+  </si>
+  <si>
+    <t>192.168.1.160 /28</t>
+  </si>
+  <si>
+    <t>192.168.1.96 /28</t>
+  </si>
+  <si>
+    <t>192.168.1.128 /28</t>
+  </si>
+  <si>
+    <t>192.168.1.0 /27</t>
+  </si>
+  <si>
+    <t>192.168.1.206</t>
+  </si>
+  <si>
+    <t>192.168.1.78</t>
+  </si>
+  <si>
+    <t>192.168.1.46</t>
+  </si>
+  <si>
+    <t>192.168.1.174</t>
+  </si>
+  <si>
+    <t>192.168.1.110</t>
+  </si>
+  <si>
+    <t>192.168.1.142</t>
+  </si>
+  <si>
+    <t>192.168.1.30</t>
+  </si>
+  <si>
+    <t>192.168.1.192</t>
+  </si>
+  <si>
+    <t>192.168.1.80</t>
+  </si>
+  <si>
+    <t>192.168.1.48</t>
+  </si>
+  <si>
+    <t>192.168.1.176</t>
+  </si>
+  <si>
+    <t>192.168.1.112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">192.168.1.144 </t>
+  </si>
+  <si>
+    <t>192.168.1.198</t>
+  </si>
+  <si>
+    <t>192.168.1.94</t>
+  </si>
+  <si>
+    <t>192.168.1.62</t>
+  </si>
+  <si>
+    <t>192.168.1.190</t>
+  </si>
+  <si>
+    <t>192.168.1.126</t>
+  </si>
+  <si>
+    <t>192.168.1.158</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>Telefon</t>
   </si>
 </sst>
 </file>
@@ -483,7 +595,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -771,11 +883,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -960,6 +1081,14 @@
     <xf numFmtId="0" fontId="7" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -1256,8 +1385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,9 +1476,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12CB4148-414F-422C-94F5-AFDA695DCD79}">
   <dimension ref="A1:I257"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A213" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A235" sqref="A235"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J238" sqref="J238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5642,4 +5771,229 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D8CF1E-1520-40BE-96A0-0CF16ECCE840}">
+  <dimension ref="B1:E19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="82" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="82" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="82" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="82" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="82" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="83"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="84" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="84" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="84" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="85"/>
+      <c r="C19" s="85"/>
+      <c r="D19" s="85"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Major updates: Remade full configs so it matches real life deivces; Added PRINTER dhcp pool, since we forgot that;Fixed cableing because it wasn't effective, now cables go from switches to IP phones then to PCs ;Updated 8.2.1 so it matches 8.1.1; I didn't yet updated the documents (Switchek, Dokumentáció, Prezentáció, Kisvállalat létszám)
</commit_message>
<xml_diff>
--- a/Kisvállalat létszám.xlsx
+++ b/Kisvállalat létszám.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20396"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\School\11.o\Hálózat\projekt\fluffy-system\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Izumi\Documents\github-repos\fluffy-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E0D563-C0FA-432D-8B5F-CC282EB1DF32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D93F74-8D73-4CF5-9661-30A6BD3DCC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13410" windowHeight="10665" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32775" yWindow="375" windowWidth="14520" windowHeight="14205" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alap" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="115">
   <si>
     <t>I.em</t>
   </si>
@@ -949,7 +949,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1056,7 +1056,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
@@ -1064,46 +1064,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1124,25 +1100,48 @@
     <xf numFmtId="0" fontId="7" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -1530,9 +1529,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12CB4148-414F-422C-94F5-AFDA695DCD79}">
   <dimension ref="A1:I257"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A197" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I234" activeCellId="1" sqref="A234:C237 I234:I237"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K223" sqref="K223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1571,7 +1570,7 @@
       <c r="C2" s="59"/>
       <c r="D2" s="59"/>
       <c r="E2" s="59"/>
-      <c r="F2" s="60" t="s">
+      <c r="F2" s="85" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="59"/>
@@ -1590,7 +1589,7 @@
       <c r="C3" s="59"/>
       <c r="D3" s="59"/>
       <c r="E3" s="59"/>
-      <c r="F3" s="60"/>
+      <c r="F3" s="85"/>
       <c r="G3" s="59"/>
       <c r="H3" s="59"/>
       <c r="I3" s="43"/>
@@ -1605,7 +1604,7 @@
       <c r="C4" s="59"/>
       <c r="D4" s="59"/>
       <c r="E4" s="59"/>
-      <c r="F4" s="60"/>
+      <c r="F4" s="85"/>
       <c r="G4" s="59"/>
       <c r="H4" s="59"/>
       <c r="I4" s="43"/>
@@ -1620,7 +1619,7 @@
       <c r="C5" s="59"/>
       <c r="D5" s="59"/>
       <c r="E5" s="59"/>
-      <c r="F5" s="60"/>
+      <c r="F5" s="85"/>
       <c r="G5" s="59"/>
       <c r="H5" s="59"/>
       <c r="I5" s="43"/>
@@ -1635,7 +1634,7 @@
       <c r="C6" s="59"/>
       <c r="D6" s="59"/>
       <c r="E6" s="59"/>
-      <c r="F6" s="60"/>
+      <c r="F6" s="85"/>
       <c r="G6" s="59"/>
       <c r="H6" s="59"/>
       <c r="I6" s="43"/>
@@ -1650,7 +1649,7 @@
       <c r="C7" s="59"/>
       <c r="D7" s="59"/>
       <c r="E7" s="59"/>
-      <c r="F7" s="60"/>
+      <c r="F7" s="85"/>
       <c r="G7" s="59"/>
       <c r="H7" s="59"/>
       <c r="I7" s="43"/>
@@ -1665,7 +1664,7 @@
       <c r="C8" s="59"/>
       <c r="D8" s="59"/>
       <c r="E8" s="59"/>
-      <c r="F8" s="60"/>
+      <c r="F8" s="85"/>
       <c r="G8" s="59"/>
       <c r="H8" s="59"/>
       <c r="I8" s="43"/>
@@ -1680,7 +1679,7 @@
       <c r="C9" s="59"/>
       <c r="D9" s="59"/>
       <c r="E9" s="59"/>
-      <c r="F9" s="60"/>
+      <c r="F9" s="85"/>
       <c r="G9" s="59"/>
       <c r="H9" s="59"/>
       <c r="I9" s="43"/>
@@ -1695,7 +1694,7 @@
       <c r="C10" s="59"/>
       <c r="D10" s="59"/>
       <c r="E10" s="59"/>
-      <c r="F10" s="60"/>
+      <c r="F10" s="85"/>
       <c r="G10" s="59"/>
       <c r="H10" s="59"/>
       <c r="I10" s="43"/>
@@ -1710,7 +1709,7 @@
       <c r="C11" s="59"/>
       <c r="D11" s="59"/>
       <c r="E11" s="59"/>
-      <c r="F11" s="60"/>
+      <c r="F11" s="85"/>
       <c r="G11" s="59"/>
       <c r="H11" s="59"/>
       <c r="I11" s="54"/>
@@ -1725,7 +1724,7 @@
       <c r="C12" s="59"/>
       <c r="D12" s="59"/>
       <c r="E12" s="59"/>
-      <c r="F12" s="60"/>
+      <c r="F12" s="85"/>
       <c r="G12" s="59"/>
       <c r="H12" s="59"/>
       <c r="I12" s="43"/>
@@ -1740,7 +1739,7 @@
       <c r="C13" s="59"/>
       <c r="D13" s="59"/>
       <c r="E13" s="59"/>
-      <c r="F13" s="60"/>
+      <c r="F13" s="85"/>
       <c r="G13" s="59"/>
       <c r="H13" s="59"/>
       <c r="I13" s="43"/>
@@ -1755,7 +1754,7 @@
       <c r="C14" s="59"/>
       <c r="D14" s="59"/>
       <c r="E14" s="59"/>
-      <c r="F14" s="60"/>
+      <c r="F14" s="85"/>
       <c r="G14" s="59"/>
       <c r="H14" s="59"/>
       <c r="I14" s="43"/>
@@ -1770,7 +1769,7 @@
       <c r="C15" s="59"/>
       <c r="D15" s="59"/>
       <c r="E15" s="59"/>
-      <c r="F15" s="60"/>
+      <c r="F15" s="85"/>
       <c r="G15" s="59"/>
       <c r="H15" s="59"/>
       <c r="I15" s="43"/>
@@ -1785,7 +1784,7 @@
       <c r="C16" s="59"/>
       <c r="D16" s="59"/>
       <c r="E16" s="59"/>
-      <c r="F16" s="60"/>
+      <c r="F16" s="85"/>
       <c r="G16" s="59"/>
       <c r="H16" s="59"/>
       <c r="I16" s="43"/>
@@ -1800,7 +1799,7 @@
       <c r="C17" s="59"/>
       <c r="D17" s="59"/>
       <c r="E17" s="59"/>
-      <c r="F17" s="60"/>
+      <c r="F17" s="85"/>
       <c r="G17" s="59"/>
       <c r="H17" s="59"/>
       <c r="I17" s="43"/>
@@ -1815,7 +1814,7 @@
       <c r="C18" s="59"/>
       <c r="D18" s="59"/>
       <c r="E18" s="59"/>
-      <c r="F18" s="60"/>
+      <c r="F18" s="85"/>
       <c r="G18" s="59"/>
       <c r="H18" s="59"/>
       <c r="I18" s="43"/>
@@ -1830,7 +1829,7 @@
       <c r="C19" s="59"/>
       <c r="D19" s="59"/>
       <c r="E19" s="59"/>
-      <c r="F19" s="60"/>
+      <c r="F19" s="85"/>
       <c r="G19" s="59"/>
       <c r="H19" s="59"/>
       <c r="I19" s="43"/>
@@ -1845,7 +1844,7 @@
       <c r="C20" s="59"/>
       <c r="D20" s="59"/>
       <c r="E20" s="59"/>
-      <c r="F20" s="60"/>
+      <c r="F20" s="85"/>
       <c r="G20" s="59"/>
       <c r="H20" s="59"/>
       <c r="I20" s="54"/>
@@ -1860,7 +1859,7 @@
       <c r="C21" s="59"/>
       <c r="D21" s="59"/>
       <c r="E21" s="59"/>
-      <c r="F21" s="60"/>
+      <c r="F21" s="85"/>
       <c r="G21" s="59"/>
       <c r="H21" s="59"/>
       <c r="I21" s="43"/>
@@ -1875,7 +1874,7 @@
       <c r="C22" s="59"/>
       <c r="D22" s="59"/>
       <c r="E22" s="59"/>
-      <c r="F22" s="60"/>
+      <c r="F22" s="85"/>
       <c r="G22" s="59"/>
       <c r="H22" s="59"/>
       <c r="I22" s="43"/>
@@ -1890,7 +1889,7 @@
       <c r="C23" s="59"/>
       <c r="D23" s="59"/>
       <c r="E23" s="59"/>
-      <c r="F23" s="60"/>
+      <c r="F23" s="85"/>
       <c r="G23" s="59"/>
       <c r="H23" s="59"/>
       <c r="I23" s="43"/>
@@ -1905,7 +1904,7 @@
       <c r="C24" s="59"/>
       <c r="D24" s="59"/>
       <c r="E24" s="59"/>
-      <c r="F24" s="60"/>
+      <c r="F24" s="85"/>
       <c r="G24" s="59"/>
       <c r="H24" s="59"/>
       <c r="I24" s="43"/>
@@ -1920,7 +1919,7 @@
       <c r="C25" s="59"/>
       <c r="D25" s="59"/>
       <c r="E25" s="59"/>
-      <c r="F25" s="60"/>
+      <c r="F25" s="85"/>
       <c r="G25" s="59"/>
       <c r="H25" s="59"/>
       <c r="I25" s="43"/>
@@ -1935,7 +1934,7 @@
       <c r="C26" s="59"/>
       <c r="D26" s="59"/>
       <c r="E26" s="59"/>
-      <c r="F26" s="60"/>
+      <c r="F26" s="85"/>
       <c r="G26" s="59"/>
       <c r="H26" s="59"/>
       <c r="I26" s="43"/>
@@ -1950,7 +1949,7 @@
       <c r="C27" s="59"/>
       <c r="D27" s="59"/>
       <c r="E27" s="59"/>
-      <c r="F27" s="60"/>
+      <c r="F27" s="85"/>
       <c r="G27" s="59"/>
       <c r="H27" s="59"/>
       <c r="I27" s="43"/>
@@ -1965,7 +1964,7 @@
       <c r="C28" s="59"/>
       <c r="D28" s="59"/>
       <c r="E28" s="59"/>
-      <c r="F28" s="60"/>
+      <c r="F28" s="85"/>
       <c r="G28" s="59"/>
       <c r="H28" s="59"/>
       <c r="I28" s="43"/>
@@ -1980,7 +1979,7 @@
       <c r="C29" s="59"/>
       <c r="D29" s="59"/>
       <c r="E29" s="59"/>
-      <c r="F29" s="60"/>
+      <c r="F29" s="85"/>
       <c r="G29" s="59"/>
       <c r="H29" s="59"/>
       <c r="I29" s="54" t="s">
@@ -1997,7 +1996,7 @@
       <c r="C30" s="59"/>
       <c r="D30" s="59"/>
       <c r="E30" s="59"/>
-      <c r="F30" s="60"/>
+      <c r="F30" s="85"/>
       <c r="G30" s="59"/>
       <c r="H30" s="59"/>
       <c r="I30" s="43" t="s">
@@ -2014,7 +2013,7 @@
       <c r="C31" s="59"/>
       <c r="D31" s="59"/>
       <c r="E31" s="59"/>
-      <c r="F31" s="60"/>
+      <c r="F31" s="85"/>
       <c r="G31" s="59"/>
       <c r="H31" s="59"/>
       <c r="I31" s="43" t="s">
@@ -2031,7 +2030,7 @@
       <c r="C32" s="59"/>
       <c r="D32" s="59"/>
       <c r="E32" s="59"/>
-      <c r="F32" s="60"/>
+      <c r="F32" s="85"/>
       <c r="G32" s="59"/>
       <c r="H32" s="59"/>
       <c r="I32" s="43" t="s">
@@ -2048,7 +2047,7 @@
       <c r="C33" s="59"/>
       <c r="D33" s="59"/>
       <c r="E33" s="59"/>
-      <c r="F33" s="60"/>
+      <c r="F33" s="85"/>
       <c r="G33" s="59"/>
       <c r="H33" s="59"/>
       <c r="I33" s="43" t="s">
@@ -2064,7 +2063,7 @@
       </c>
       <c r="C34" s="59"/>
       <c r="D34" s="59"/>
-      <c r="E34" s="63" t="s">
+      <c r="E34" s="84" t="s">
         <v>16</v>
       </c>
       <c r="F34" s="59"/>
@@ -2083,7 +2082,7 @@
       </c>
       <c r="C35" s="59"/>
       <c r="D35" s="59"/>
-      <c r="E35" s="63"/>
+      <c r="E35" s="84"/>
       <c r="F35" s="59"/>
       <c r="G35" s="59"/>
       <c r="H35" s="59"/>
@@ -2098,7 +2097,7 @@
       </c>
       <c r="C36" s="59"/>
       <c r="D36" s="59"/>
-      <c r="E36" s="63"/>
+      <c r="E36" s="84"/>
       <c r="F36" s="59"/>
       <c r="G36" s="59"/>
       <c r="H36" s="59"/>
@@ -2113,7 +2112,7 @@
       </c>
       <c r="C37" s="59"/>
       <c r="D37" s="59"/>
-      <c r="E37" s="63"/>
+      <c r="E37" s="84"/>
       <c r="F37" s="59"/>
       <c r="G37" s="59"/>
       <c r="H37" s="59"/>
@@ -2128,7 +2127,7 @@
       </c>
       <c r="C38" s="59"/>
       <c r="D38" s="59"/>
-      <c r="E38" s="63"/>
+      <c r="E38" s="84"/>
       <c r="F38" s="59"/>
       <c r="G38" s="59"/>
       <c r="H38" s="59"/>
@@ -2143,7 +2142,7 @@
       </c>
       <c r="C39" s="59"/>
       <c r="D39" s="59"/>
-      <c r="E39" s="63"/>
+      <c r="E39" s="84"/>
       <c r="F39" s="59"/>
       <c r="G39" s="59"/>
       <c r="H39" s="59"/>
@@ -2158,7 +2157,7 @@
       </c>
       <c r="C40" s="59"/>
       <c r="D40" s="59"/>
-      <c r="E40" s="63"/>
+      <c r="E40" s="84"/>
       <c r="F40" s="59"/>
       <c r="G40" s="59"/>
       <c r="H40" s="59"/>
@@ -2173,7 +2172,7 @@
       </c>
       <c r="C41" s="59"/>
       <c r="D41" s="59"/>
-      <c r="E41" s="63"/>
+      <c r="E41" s="84"/>
       <c r="F41" s="59"/>
       <c r="G41" s="59"/>
       <c r="H41" s="59"/>
@@ -2188,7 +2187,7 @@
       </c>
       <c r="C42" s="59"/>
       <c r="D42" s="59"/>
-      <c r="E42" s="63"/>
+      <c r="E42" s="84"/>
       <c r="F42" s="59"/>
       <c r="G42" s="59"/>
       <c r="H42" s="59"/>
@@ -2203,7 +2202,7 @@
       </c>
       <c r="C43" s="59"/>
       <c r="D43" s="59"/>
-      <c r="E43" s="63"/>
+      <c r="E43" s="84"/>
       <c r="F43" s="59"/>
       <c r="G43" s="59"/>
       <c r="H43" s="59"/>
@@ -2218,7 +2217,7 @@
       </c>
       <c r="C44" s="59"/>
       <c r="D44" s="59"/>
-      <c r="E44" s="63"/>
+      <c r="E44" s="84"/>
       <c r="F44" s="59"/>
       <c r="G44" s="59"/>
       <c r="H44" s="59"/>
@@ -2233,7 +2232,7 @@
       </c>
       <c r="C45" s="59"/>
       <c r="D45" s="59"/>
-      <c r="E45" s="63"/>
+      <c r="E45" s="84"/>
       <c r="F45" s="59"/>
       <c r="G45" s="59"/>
       <c r="H45" s="59"/>
@@ -2248,7 +2247,7 @@
       </c>
       <c r="C46" s="59"/>
       <c r="D46" s="59"/>
-      <c r="E46" s="63"/>
+      <c r="E46" s="84"/>
       <c r="F46" s="59"/>
       <c r="G46" s="59"/>
       <c r="H46" s="59"/>
@@ -2263,7 +2262,7 @@
       </c>
       <c r="C47" s="59"/>
       <c r="D47" s="59"/>
-      <c r="E47" s="63"/>
+      <c r="E47" s="84"/>
       <c r="F47" s="59"/>
       <c r="G47" s="59"/>
       <c r="H47" s="59"/>
@@ -2278,7 +2277,7 @@
       </c>
       <c r="C48" s="59"/>
       <c r="D48" s="59"/>
-      <c r="E48" s="63"/>
+      <c r="E48" s="84"/>
       <c r="F48" s="59"/>
       <c r="G48" s="59"/>
       <c r="H48" s="59"/>
@@ -2295,7 +2294,7 @@
       </c>
       <c r="C49" s="59"/>
       <c r="D49" s="59"/>
-      <c r="E49" s="63"/>
+      <c r="E49" s="84"/>
       <c r="F49" s="59"/>
       <c r="G49" s="59"/>
       <c r="H49" s="59"/>
@@ -2312,7 +2311,7 @@
       </c>
       <c r="C50" s="59"/>
       <c r="D50" s="59"/>
-      <c r="E50" s="61" t="s">
+      <c r="E50" s="82" t="s">
         <v>17</v>
       </c>
       <c r="F50" s="59"/>
@@ -2331,7 +2330,7 @@
       </c>
       <c r="C51" s="59"/>
       <c r="D51" s="59"/>
-      <c r="E51" s="61"/>
+      <c r="E51" s="82"/>
       <c r="F51" s="59"/>
       <c r="G51" s="59"/>
       <c r="H51" s="59"/>
@@ -2346,7 +2345,7 @@
       </c>
       <c r="C52" s="59"/>
       <c r="D52" s="59"/>
-      <c r="E52" s="61"/>
+      <c r="E52" s="82"/>
       <c r="F52" s="59"/>
       <c r="G52" s="59"/>
       <c r="H52" s="59"/>
@@ -2361,7 +2360,7 @@
       </c>
       <c r="C53" s="59"/>
       <c r="D53" s="59"/>
-      <c r="E53" s="61"/>
+      <c r="E53" s="82"/>
       <c r="F53" s="59"/>
       <c r="G53" s="59"/>
       <c r="H53" s="59"/>
@@ -2376,7 +2375,7 @@
       </c>
       <c r="C54" s="59"/>
       <c r="D54" s="59"/>
-      <c r="E54" s="61"/>
+      <c r="E54" s="82"/>
       <c r="F54" s="59"/>
       <c r="G54" s="59"/>
       <c r="H54" s="59"/>
@@ -2391,7 +2390,7 @@
       </c>
       <c r="C55" s="59"/>
       <c r="D55" s="59"/>
-      <c r="E55" s="61"/>
+      <c r="E55" s="82"/>
       <c r="F55" s="59"/>
       <c r="G55" s="59"/>
       <c r="H55" s="59"/>
@@ -2406,7 +2405,7 @@
       </c>
       <c r="C56" s="59"/>
       <c r="D56" s="59"/>
-      <c r="E56" s="61"/>
+      <c r="E56" s="82"/>
       <c r="F56" s="59"/>
       <c r="G56" s="59"/>
       <c r="H56" s="59"/>
@@ -2421,7 +2420,7 @@
       </c>
       <c r="C57" s="59"/>
       <c r="D57" s="59"/>
-      <c r="E57" s="61"/>
+      <c r="E57" s="82"/>
       <c r="F57" s="59"/>
       <c r="G57" s="59"/>
       <c r="H57" s="59"/>
@@ -2436,7 +2435,7 @@
       </c>
       <c r="C58" s="59"/>
       <c r="D58" s="59"/>
-      <c r="E58" s="61"/>
+      <c r="E58" s="82"/>
       <c r="F58" s="59"/>
       <c r="G58" s="59"/>
       <c r="H58" s="59"/>
@@ -2451,7 +2450,7 @@
       </c>
       <c r="C59" s="59"/>
       <c r="D59" s="59"/>
-      <c r="E59" s="61"/>
+      <c r="E59" s="82"/>
       <c r="F59" s="59"/>
       <c r="G59" s="59"/>
       <c r="H59" s="59"/>
@@ -2466,7 +2465,7 @@
       </c>
       <c r="C60" s="59"/>
       <c r="D60" s="59"/>
-      <c r="E60" s="61"/>
+      <c r="E60" s="82"/>
       <c r="F60" s="59"/>
       <c r="G60" s="59"/>
       <c r="H60" s="59"/>
@@ -2481,7 +2480,7 @@
       </c>
       <c r="C61" s="59"/>
       <c r="D61" s="59"/>
-      <c r="E61" s="61"/>
+      <c r="E61" s="82"/>
       <c r="F61" s="59"/>
       <c r="G61" s="59"/>
       <c r="H61" s="59"/>
@@ -2496,7 +2495,7 @@
       </c>
       <c r="C62" s="59"/>
       <c r="D62" s="59"/>
-      <c r="E62" s="61"/>
+      <c r="E62" s="82"/>
       <c r="F62" s="59"/>
       <c r="G62" s="59"/>
       <c r="H62" s="59"/>
@@ -2511,7 +2510,7 @@
       </c>
       <c r="C63" s="59"/>
       <c r="D63" s="59"/>
-      <c r="E63" s="61"/>
+      <c r="E63" s="82"/>
       <c r="F63" s="59"/>
       <c r="G63" s="59"/>
       <c r="H63" s="59"/>
@@ -2526,7 +2525,7 @@
       </c>
       <c r="C64" s="59"/>
       <c r="D64" s="59"/>
-      <c r="E64" s="61"/>
+      <c r="E64" s="82"/>
       <c r="F64" s="59"/>
       <c r="G64" s="59"/>
       <c r="H64" s="59"/>
@@ -2543,7 +2542,7 @@
       </c>
       <c r="C65" s="59"/>
       <c r="D65" s="59"/>
-      <c r="E65" s="61"/>
+      <c r="E65" s="82"/>
       <c r="F65" s="59"/>
       <c r="G65" s="59"/>
       <c r="H65" s="59"/>
@@ -2560,7 +2559,7 @@
       </c>
       <c r="C66" s="59"/>
       <c r="D66" s="59"/>
-      <c r="E66" s="62" t="s">
+      <c r="E66" s="83" t="s">
         <v>18</v>
       </c>
       <c r="F66" s="59"/>
@@ -2579,7 +2578,7 @@
       </c>
       <c r="C67" s="59"/>
       <c r="D67" s="59"/>
-      <c r="E67" s="62"/>
+      <c r="E67" s="83"/>
       <c r="F67" s="59"/>
       <c r="G67" s="59"/>
       <c r="H67" s="59"/>
@@ -2594,7 +2593,7 @@
       </c>
       <c r="C68" s="59"/>
       <c r="D68" s="59"/>
-      <c r="E68" s="62"/>
+      <c r="E68" s="83"/>
       <c r="F68" s="59"/>
       <c r="G68" s="59"/>
       <c r="H68" s="59"/>
@@ -2609,7 +2608,7 @@
       </c>
       <c r="C69" s="59"/>
       <c r="D69" s="59"/>
-      <c r="E69" s="62"/>
+      <c r="E69" s="83"/>
       <c r="F69" s="59"/>
       <c r="G69" s="59"/>
       <c r="H69" s="59"/>
@@ -2624,7 +2623,7 @@
       </c>
       <c r="C70" s="59"/>
       <c r="D70" s="59"/>
-      <c r="E70" s="62"/>
+      <c r="E70" s="83"/>
       <c r="F70" s="59"/>
       <c r="G70" s="59"/>
       <c r="H70" s="59"/>
@@ -2639,7 +2638,7 @@
       </c>
       <c r="C71" s="59"/>
       <c r="D71" s="59"/>
-      <c r="E71" s="62"/>
+      <c r="E71" s="83"/>
       <c r="F71" s="59"/>
       <c r="G71" s="59"/>
       <c r="H71" s="59"/>
@@ -2654,7 +2653,7 @@
       </c>
       <c r="C72" s="59"/>
       <c r="D72" s="59"/>
-      <c r="E72" s="62"/>
+      <c r="E72" s="83"/>
       <c r="F72" s="59"/>
       <c r="G72" s="59"/>
       <c r="H72" s="59"/>
@@ -2669,7 +2668,7 @@
       </c>
       <c r="C73" s="59"/>
       <c r="D73" s="59"/>
-      <c r="E73" s="62"/>
+      <c r="E73" s="83"/>
       <c r="F73" s="59"/>
       <c r="G73" s="59"/>
       <c r="H73" s="59"/>
@@ -2684,7 +2683,7 @@
       </c>
       <c r="C74" s="59"/>
       <c r="D74" s="59"/>
-      <c r="E74" s="62"/>
+      <c r="E74" s="83"/>
       <c r="F74" s="59"/>
       <c r="G74" s="59"/>
       <c r="H74" s="59"/>
@@ -2699,7 +2698,7 @@
       </c>
       <c r="C75" s="59"/>
       <c r="D75" s="59"/>
-      <c r="E75" s="62"/>
+      <c r="E75" s="83"/>
       <c r="F75" s="59"/>
       <c r="G75" s="59"/>
       <c r="H75" s="59"/>
@@ -2714,7 +2713,7 @@
       </c>
       <c r="C76" s="59"/>
       <c r="D76" s="59"/>
-      <c r="E76" s="62"/>
+      <c r="E76" s="83"/>
       <c r="F76" s="59"/>
       <c r="G76" s="59"/>
       <c r="H76" s="59"/>
@@ -2729,7 +2728,7 @@
       </c>
       <c r="C77" s="59"/>
       <c r="D77" s="59"/>
-      <c r="E77" s="62"/>
+      <c r="E77" s="83"/>
       <c r="F77" s="59"/>
       <c r="G77" s="59"/>
       <c r="H77" s="59"/>
@@ -2744,7 +2743,7 @@
       </c>
       <c r="C78" s="59"/>
       <c r="D78" s="59"/>
-      <c r="E78" s="62"/>
+      <c r="E78" s="83"/>
       <c r="F78" s="59"/>
       <c r="G78" s="59"/>
       <c r="H78" s="59"/>
@@ -2759,7 +2758,7 @@
       </c>
       <c r="C79" s="59"/>
       <c r="D79" s="59"/>
-      <c r="E79" s="62"/>
+      <c r="E79" s="83"/>
       <c r="F79" s="59"/>
       <c r="G79" s="59"/>
       <c r="H79" s="59"/>
@@ -2774,7 +2773,7 @@
       </c>
       <c r="C80" s="59"/>
       <c r="D80" s="59"/>
-      <c r="E80" s="62"/>
+      <c r="E80" s="83"/>
       <c r="F80" s="59"/>
       <c r="G80" s="59"/>
       <c r="H80" s="59"/>
@@ -2791,7 +2790,7 @@
       </c>
       <c r="C81" s="59"/>
       <c r="D81" s="59"/>
-      <c r="E81" s="62"/>
+      <c r="E81" s="83"/>
       <c r="F81" s="59"/>
       <c r="G81" s="59"/>
       <c r="H81" s="59"/>
@@ -2808,7 +2807,7 @@
       </c>
       <c r="C82" s="59"/>
       <c r="D82" s="59"/>
-      <c r="E82" s="65" t="s">
+      <c r="E82" s="81" t="s">
         <v>19</v>
       </c>
       <c r="F82" s="59"/>
@@ -2827,7 +2826,7 @@
       </c>
       <c r="C83" s="59"/>
       <c r="D83" s="59"/>
-      <c r="E83" s="65"/>
+      <c r="E83" s="81"/>
       <c r="F83" s="59"/>
       <c r="G83" s="59"/>
       <c r="H83" s="59"/>
@@ -2842,7 +2841,7 @@
       </c>
       <c r="C84" s="59"/>
       <c r="D84" s="59"/>
-      <c r="E84" s="65"/>
+      <c r="E84" s="81"/>
       <c r="F84" s="59"/>
       <c r="G84" s="59"/>
       <c r="H84" s="59"/>
@@ -2857,7 +2856,7 @@
       </c>
       <c r="C85" s="59"/>
       <c r="D85" s="59"/>
-      <c r="E85" s="65"/>
+      <c r="E85" s="81"/>
       <c r="F85" s="59"/>
       <c r="G85" s="59"/>
       <c r="H85" s="59"/>
@@ -2872,7 +2871,7 @@
       </c>
       <c r="C86" s="59"/>
       <c r="D86" s="59"/>
-      <c r="E86" s="65"/>
+      <c r="E86" s="81"/>
       <c r="F86" s="59"/>
       <c r="G86" s="59"/>
       <c r="H86" s="59"/>
@@ -2887,7 +2886,7 @@
       </c>
       <c r="C87" s="59"/>
       <c r="D87" s="59"/>
-      <c r="E87" s="65"/>
+      <c r="E87" s="81"/>
       <c r="F87" s="59"/>
       <c r="G87" s="59"/>
       <c r="H87" s="59"/>
@@ -2902,7 +2901,7 @@
       </c>
       <c r="C88" s="59"/>
       <c r="D88" s="59"/>
-      <c r="E88" s="65"/>
+      <c r="E88" s="81"/>
       <c r="F88" s="59"/>
       <c r="G88" s="59"/>
       <c r="H88" s="59"/>
@@ -2917,7 +2916,7 @@
       </c>
       <c r="C89" s="59"/>
       <c r="D89" s="59"/>
-      <c r="E89" s="65"/>
+      <c r="E89" s="81"/>
       <c r="F89" s="59"/>
       <c r="G89" s="59"/>
       <c r="H89" s="59"/>
@@ -2932,7 +2931,7 @@
       </c>
       <c r="C90" s="59"/>
       <c r="D90" s="59"/>
-      <c r="E90" s="65"/>
+      <c r="E90" s="81"/>
       <c r="F90" s="59"/>
       <c r="G90" s="59"/>
       <c r="H90" s="59"/>
@@ -2947,7 +2946,7 @@
       </c>
       <c r="C91" s="59"/>
       <c r="D91" s="59"/>
-      <c r="E91" s="65"/>
+      <c r="E91" s="81"/>
       <c r="F91" s="59"/>
       <c r="G91" s="59"/>
       <c r="H91" s="59"/>
@@ -2962,7 +2961,7 @@
       </c>
       <c r="C92" s="59"/>
       <c r="D92" s="59"/>
-      <c r="E92" s="65"/>
+      <c r="E92" s="81"/>
       <c r="F92" s="59"/>
       <c r="G92" s="59"/>
       <c r="H92" s="59"/>
@@ -2977,7 +2976,7 @@
       </c>
       <c r="C93" s="59"/>
       <c r="D93" s="59"/>
-      <c r="E93" s="65"/>
+      <c r="E93" s="81"/>
       <c r="F93" s="59"/>
       <c r="G93" s="59"/>
       <c r="H93" s="59"/>
@@ -2992,7 +2991,7 @@
       </c>
       <c r="C94" s="59"/>
       <c r="D94" s="59"/>
-      <c r="E94" s="65"/>
+      <c r="E94" s="81"/>
       <c r="F94" s="59"/>
       <c r="G94" s="59"/>
       <c r="H94" s="59"/>
@@ -3007,7 +3006,7 @@
       </c>
       <c r="C95" s="59"/>
       <c r="D95" s="59"/>
-      <c r="E95" s="65"/>
+      <c r="E95" s="81"/>
       <c r="F95" s="59"/>
       <c r="G95" s="59"/>
       <c r="H95" s="59"/>
@@ -3022,7 +3021,7 @@
       </c>
       <c r="C96" s="59"/>
       <c r="D96" s="59"/>
-      <c r="E96" s="65"/>
+      <c r="E96" s="81"/>
       <c r="F96" s="59"/>
       <c r="G96" s="59"/>
       <c r="H96" s="59"/>
@@ -3039,7 +3038,7 @@
       </c>
       <c r="C97" s="59"/>
       <c r="D97" s="59"/>
-      <c r="E97" s="65"/>
+      <c r="E97" s="81"/>
       <c r="F97" s="59"/>
       <c r="G97" s="59"/>
       <c r="H97" s="59"/>
@@ -3056,7 +3055,7 @@
       </c>
       <c r="C98" s="59"/>
       <c r="D98" s="59"/>
-      <c r="E98" s="64" t="s">
+      <c r="E98" s="80" t="s">
         <v>20</v>
       </c>
       <c r="F98" s="59"/>
@@ -3075,7 +3074,7 @@
       </c>
       <c r="C99" s="59"/>
       <c r="D99" s="59"/>
-      <c r="E99" s="64"/>
+      <c r="E99" s="80"/>
       <c r="F99" s="59"/>
       <c r="G99" s="59"/>
       <c r="H99" s="59"/>
@@ -3090,7 +3089,7 @@
       </c>
       <c r="C100" s="59"/>
       <c r="D100" s="59"/>
-      <c r="E100" s="64"/>
+      <c r="E100" s="80"/>
       <c r="F100" s="59"/>
       <c r="G100" s="59"/>
       <c r="H100" s="59"/>
@@ -3105,7 +3104,7 @@
       </c>
       <c r="C101" s="59"/>
       <c r="D101" s="59"/>
-      <c r="E101" s="64"/>
+      <c r="E101" s="80"/>
       <c r="F101" s="59"/>
       <c r="G101" s="59"/>
       <c r="H101" s="59"/>
@@ -3120,7 +3119,7 @@
       </c>
       <c r="C102" s="59"/>
       <c r="D102" s="59"/>
-      <c r="E102" s="64"/>
+      <c r="E102" s="80"/>
       <c r="F102" s="59"/>
       <c r="G102" s="59"/>
       <c r="H102" s="59"/>
@@ -3135,7 +3134,7 @@
       </c>
       <c r="C103" s="59"/>
       <c r="D103" s="59"/>
-      <c r="E103" s="64"/>
+      <c r="E103" s="80"/>
       <c r="F103" s="59"/>
       <c r="G103" s="59"/>
       <c r="H103" s="59"/>
@@ -3150,7 +3149,7 @@
       </c>
       <c r="C104" s="59"/>
       <c r="D104" s="59"/>
-      <c r="E104" s="64"/>
+      <c r="E104" s="80"/>
       <c r="F104" s="59"/>
       <c r="G104" s="59"/>
       <c r="H104" s="59"/>
@@ -3165,7 +3164,7 @@
       </c>
       <c r="C105" s="59"/>
       <c r="D105" s="59"/>
-      <c r="E105" s="64"/>
+      <c r="E105" s="80"/>
       <c r="F105" s="59"/>
       <c r="G105" s="59"/>
       <c r="H105" s="59"/>
@@ -3180,7 +3179,7 @@
       </c>
       <c r="C106" s="59"/>
       <c r="D106" s="59"/>
-      <c r="E106" s="64"/>
+      <c r="E106" s="80"/>
       <c r="F106" s="59"/>
       <c r="G106" s="59"/>
       <c r="H106" s="59"/>
@@ -3195,7 +3194,7 @@
       </c>
       <c r="C107" s="59"/>
       <c r="D107" s="59"/>
-      <c r="E107" s="64"/>
+      <c r="E107" s="80"/>
       <c r="F107" s="59"/>
       <c r="G107" s="59"/>
       <c r="H107" s="59"/>
@@ -3210,7 +3209,7 @@
       </c>
       <c r="C108" s="59"/>
       <c r="D108" s="59"/>
-      <c r="E108" s="64"/>
+      <c r="E108" s="80"/>
       <c r="F108" s="59"/>
       <c r="G108" s="59"/>
       <c r="H108" s="59"/>
@@ -3225,7 +3224,7 @@
       </c>
       <c r="C109" s="59"/>
       <c r="D109" s="59"/>
-      <c r="E109" s="64"/>
+      <c r="E109" s="80"/>
       <c r="F109" s="59"/>
       <c r="G109" s="59"/>
       <c r="H109" s="59"/>
@@ -3240,7 +3239,7 @@
       </c>
       <c r="C110" s="59"/>
       <c r="D110" s="59"/>
-      <c r="E110" s="64"/>
+      <c r="E110" s="80"/>
       <c r="F110" s="59"/>
       <c r="G110" s="59"/>
       <c r="H110" s="59"/>
@@ -3255,7 +3254,7 @@
       </c>
       <c r="C111" s="59"/>
       <c r="D111" s="59"/>
-      <c r="E111" s="64"/>
+      <c r="E111" s="80"/>
       <c r="F111" s="59"/>
       <c r="G111" s="59"/>
       <c r="H111" s="59"/>
@@ -3270,7 +3269,7 @@
       </c>
       <c r="C112" s="59"/>
       <c r="D112" s="59"/>
-      <c r="E112" s="64"/>
+      <c r="E112" s="80"/>
       <c r="F112" s="59"/>
       <c r="G112" s="59"/>
       <c r="H112" s="59"/>
@@ -3287,7 +3286,7 @@
       </c>
       <c r="C113" s="59"/>
       <c r="D113" s="59"/>
-      <c r="E113" s="64"/>
+      <c r="E113" s="80"/>
       <c r="F113" s="59"/>
       <c r="G113" s="59"/>
       <c r="H113" s="59"/>
@@ -3304,7 +3303,7 @@
       </c>
       <c r="C114" s="59"/>
       <c r="D114" s="59"/>
-      <c r="E114" s="69" t="s">
+      <c r="E114" s="79" t="s">
         <v>21</v>
       </c>
       <c r="F114" s="59"/>
@@ -3323,7 +3322,7 @@
       </c>
       <c r="C115" s="59"/>
       <c r="D115" s="59"/>
-      <c r="E115" s="69"/>
+      <c r="E115" s="79"/>
       <c r="F115" s="59"/>
       <c r="G115" s="59"/>
       <c r="H115" s="59"/>
@@ -3338,7 +3337,7 @@
       </c>
       <c r="C116" s="59"/>
       <c r="D116" s="59"/>
-      <c r="E116" s="69"/>
+      <c r="E116" s="79"/>
       <c r="F116" s="59"/>
       <c r="G116" s="59"/>
       <c r="H116" s="59"/>
@@ -3353,7 +3352,7 @@
       </c>
       <c r="C117" s="59"/>
       <c r="D117" s="59"/>
-      <c r="E117" s="69"/>
+      <c r="E117" s="79"/>
       <c r="F117" s="59"/>
       <c r="G117" s="59"/>
       <c r="H117" s="59"/>
@@ -3368,7 +3367,7 @@
       </c>
       <c r="C118" s="59"/>
       <c r="D118" s="59"/>
-      <c r="E118" s="69"/>
+      <c r="E118" s="79"/>
       <c r="F118" s="59"/>
       <c r="G118" s="59"/>
       <c r="H118" s="59"/>
@@ -3383,7 +3382,7 @@
       </c>
       <c r="C119" s="59"/>
       <c r="D119" s="59"/>
-      <c r="E119" s="69"/>
+      <c r="E119" s="79"/>
       <c r="F119" s="59"/>
       <c r="G119" s="59"/>
       <c r="H119" s="59"/>
@@ -3398,7 +3397,7 @@
       </c>
       <c r="C120" s="59"/>
       <c r="D120" s="59"/>
-      <c r="E120" s="69"/>
+      <c r="E120" s="79"/>
       <c r="F120" s="59"/>
       <c r="G120" s="59"/>
       <c r="H120" s="59"/>
@@ -3413,7 +3412,7 @@
       </c>
       <c r="C121" s="59"/>
       <c r="D121" s="59"/>
-      <c r="E121" s="69"/>
+      <c r="E121" s="79"/>
       <c r="F121" s="59"/>
       <c r="G121" s="59"/>
       <c r="H121" s="59"/>
@@ -3428,7 +3427,7 @@
       </c>
       <c r="C122" s="59"/>
       <c r="D122" s="59"/>
-      <c r="E122" s="69"/>
+      <c r="E122" s="79"/>
       <c r="F122" s="59"/>
       <c r="G122" s="59"/>
       <c r="H122" s="59"/>
@@ -3443,7 +3442,7 @@
       </c>
       <c r="C123" s="59"/>
       <c r="D123" s="59"/>
-      <c r="E123" s="69"/>
+      <c r="E123" s="79"/>
       <c r="F123" s="59"/>
       <c r="G123" s="59"/>
       <c r="H123" s="59"/>
@@ -3458,7 +3457,7 @@
       </c>
       <c r="C124" s="59"/>
       <c r="D124" s="59"/>
-      <c r="E124" s="69"/>
+      <c r="E124" s="79"/>
       <c r="F124" s="59"/>
       <c r="G124" s="59"/>
       <c r="H124" s="59"/>
@@ -3473,7 +3472,7 @@
       </c>
       <c r="C125" s="59"/>
       <c r="D125" s="59"/>
-      <c r="E125" s="69"/>
+      <c r="E125" s="79"/>
       <c r="F125" s="59"/>
       <c r="G125" s="59"/>
       <c r="H125" s="59"/>
@@ -3488,7 +3487,7 @@
       </c>
       <c r="C126" s="59"/>
       <c r="D126" s="59"/>
-      <c r="E126" s="69"/>
+      <c r="E126" s="79"/>
       <c r="F126" s="59"/>
       <c r="G126" s="59"/>
       <c r="H126" s="59"/>
@@ -3503,7 +3502,7 @@
       </c>
       <c r="C127" s="59"/>
       <c r="D127" s="59"/>
-      <c r="E127" s="69"/>
+      <c r="E127" s="79"/>
       <c r="F127" s="59"/>
       <c r="G127" s="59"/>
       <c r="H127" s="59"/>
@@ -3518,7 +3517,7 @@
       </c>
       <c r="C128" s="59"/>
       <c r="D128" s="59"/>
-      <c r="E128" s="69"/>
+      <c r="E128" s="79"/>
       <c r="F128" s="59"/>
       <c r="G128" s="59"/>
       <c r="H128" s="59"/>
@@ -3535,7 +3534,7 @@
       </c>
       <c r="C129" s="59"/>
       <c r="D129" s="59"/>
-      <c r="E129" s="69"/>
+      <c r="E129" s="79"/>
       <c r="F129" s="59"/>
       <c r="G129" s="59"/>
       <c r="H129" s="59"/>
@@ -3552,7 +3551,7 @@
       </c>
       <c r="C130" s="59"/>
       <c r="D130" s="59"/>
-      <c r="E130" s="66" t="s">
+      <c r="E130" s="72" t="s">
         <v>22</v>
       </c>
       <c r="F130" s="59"/>
@@ -3571,7 +3570,7 @@
       </c>
       <c r="C131" s="59"/>
       <c r="D131" s="59"/>
-      <c r="E131" s="67"/>
+      <c r="E131" s="73"/>
       <c r="F131" s="59"/>
       <c r="G131" s="59"/>
       <c r="H131" s="59"/>
@@ -3586,7 +3585,7 @@
       </c>
       <c r="C132" s="59"/>
       <c r="D132" s="59"/>
-      <c r="E132" s="67"/>
+      <c r="E132" s="73"/>
       <c r="F132" s="59"/>
       <c r="G132" s="59"/>
       <c r="H132" s="59"/>
@@ -3601,7 +3600,7 @@
       </c>
       <c r="C133" s="59"/>
       <c r="D133" s="59"/>
-      <c r="E133" s="67"/>
+      <c r="E133" s="73"/>
       <c r="F133" s="59"/>
       <c r="G133" s="59"/>
       <c r="H133" s="59"/>
@@ -3616,7 +3615,7 @@
       </c>
       <c r="C134" s="59"/>
       <c r="D134" s="59"/>
-      <c r="E134" s="67"/>
+      <c r="E134" s="73"/>
       <c r="F134" s="59"/>
       <c r="G134" s="59"/>
       <c r="H134" s="59"/>
@@ -3631,7 +3630,7 @@
       </c>
       <c r="C135" s="59"/>
       <c r="D135" s="59"/>
-      <c r="E135" s="67"/>
+      <c r="E135" s="73"/>
       <c r="F135" s="59"/>
       <c r="G135" s="59"/>
       <c r="H135" s="59"/>
@@ -3646,7 +3645,7 @@
       </c>
       <c r="C136" s="59"/>
       <c r="D136" s="59"/>
-      <c r="E136" s="67"/>
+      <c r="E136" s="73"/>
       <c r="F136" s="59"/>
       <c r="G136" s="59"/>
       <c r="H136" s="59"/>
@@ -3661,7 +3660,7 @@
       </c>
       <c r="C137" s="59"/>
       <c r="D137" s="59"/>
-      <c r="E137" s="67"/>
+      <c r="E137" s="73"/>
       <c r="F137" s="59"/>
       <c r="G137" s="59"/>
       <c r="H137" s="59"/>
@@ -3676,7 +3675,7 @@
       </c>
       <c r="C138" s="59"/>
       <c r="D138" s="59"/>
-      <c r="E138" s="67"/>
+      <c r="E138" s="73"/>
       <c r="F138" s="59"/>
       <c r="G138" s="59"/>
       <c r="H138" s="59"/>
@@ -3691,7 +3690,7 @@
       </c>
       <c r="C139" s="59"/>
       <c r="D139" s="59"/>
-      <c r="E139" s="67"/>
+      <c r="E139" s="73"/>
       <c r="F139" s="59"/>
       <c r="G139" s="59"/>
       <c r="H139" s="59"/>
@@ -3706,7 +3705,7 @@
       </c>
       <c r="C140" s="59"/>
       <c r="D140" s="59"/>
-      <c r="E140" s="67"/>
+      <c r="E140" s="73"/>
       <c r="F140" s="59"/>
       <c r="G140" s="59"/>
       <c r="H140" s="59"/>
@@ -3721,7 +3720,7 @@
       </c>
       <c r="C141" s="59"/>
       <c r="D141" s="59"/>
-      <c r="E141" s="67"/>
+      <c r="E141" s="73"/>
       <c r="F141" s="59"/>
       <c r="G141" s="59"/>
       <c r="H141" s="59"/>
@@ -3736,7 +3735,7 @@
       </c>
       <c r="C142" s="59"/>
       <c r="D142" s="59"/>
-      <c r="E142" s="67"/>
+      <c r="E142" s="73"/>
       <c r="F142" s="59"/>
       <c r="G142" s="59"/>
       <c r="H142" s="59"/>
@@ -3751,7 +3750,7 @@
       </c>
       <c r="C143" s="59"/>
       <c r="D143" s="59"/>
-      <c r="E143" s="67"/>
+      <c r="E143" s="73"/>
       <c r="F143" s="59"/>
       <c r="G143" s="59"/>
       <c r="H143" s="59"/>
@@ -3766,7 +3765,7 @@
       </c>
       <c r="C144" s="59"/>
       <c r="D144" s="59"/>
-      <c r="E144" s="67"/>
+      <c r="E144" s="73"/>
       <c r="F144" s="59"/>
       <c r="G144" s="59"/>
       <c r="H144" s="59"/>
@@ -3783,7 +3782,7 @@
       </c>
       <c r="C145" s="59"/>
       <c r="D145" s="59"/>
-      <c r="E145" s="68"/>
+      <c r="E145" s="74"/>
       <c r="F145" s="59"/>
       <c r="G145" s="59"/>
       <c r="H145" s="59"/>
@@ -3800,7 +3799,7 @@
       </c>
       <c r="C146" s="59"/>
       <c r="D146" s="59"/>
-      <c r="E146" s="66" t="s">
+      <c r="E146" s="72" t="s">
         <v>23</v>
       </c>
       <c r="F146" s="59"/>
@@ -3819,7 +3818,7 @@
       </c>
       <c r="C147" s="59"/>
       <c r="D147" s="59"/>
-      <c r="E147" s="67"/>
+      <c r="E147" s="73"/>
       <c r="F147" s="59"/>
       <c r="G147" s="59"/>
       <c r="H147" s="59"/>
@@ -3834,7 +3833,7 @@
       </c>
       <c r="C148" s="59"/>
       <c r="D148" s="59"/>
-      <c r="E148" s="67"/>
+      <c r="E148" s="73"/>
       <c r="F148" s="59"/>
       <c r="G148" s="59"/>
       <c r="H148" s="59"/>
@@ -3849,7 +3848,7 @@
       </c>
       <c r="C149" s="59"/>
       <c r="D149" s="59"/>
-      <c r="E149" s="67"/>
+      <c r="E149" s="73"/>
       <c r="F149" s="59"/>
       <c r="G149" s="59"/>
       <c r="H149" s="59"/>
@@ -3864,7 +3863,7 @@
       </c>
       <c r="C150" s="59"/>
       <c r="D150" s="59"/>
-      <c r="E150" s="67"/>
+      <c r="E150" s="73"/>
       <c r="F150" s="59"/>
       <c r="G150" s="59"/>
       <c r="H150" s="59"/>
@@ -3879,7 +3878,7 @@
       </c>
       <c r="C151" s="59"/>
       <c r="D151" s="59"/>
-      <c r="E151" s="67"/>
+      <c r="E151" s="73"/>
       <c r="F151" s="59"/>
       <c r="G151" s="59"/>
       <c r="H151" s="59"/>
@@ -3894,7 +3893,7 @@
       </c>
       <c r="C152" s="59"/>
       <c r="D152" s="59"/>
-      <c r="E152" s="67"/>
+      <c r="E152" s="73"/>
       <c r="F152" s="59"/>
       <c r="G152" s="59"/>
       <c r="H152" s="59"/>
@@ -3909,7 +3908,7 @@
       </c>
       <c r="C153" s="59"/>
       <c r="D153" s="59"/>
-      <c r="E153" s="67"/>
+      <c r="E153" s="73"/>
       <c r="F153" s="59"/>
       <c r="G153" s="59"/>
       <c r="H153" s="59"/>
@@ -3924,7 +3923,7 @@
       </c>
       <c r="C154" s="59"/>
       <c r="D154" s="59"/>
-      <c r="E154" s="67"/>
+      <c r="E154" s="73"/>
       <c r="F154" s="59"/>
       <c r="G154" s="59"/>
       <c r="H154" s="59"/>
@@ -3939,7 +3938,7 @@
       </c>
       <c r="C155" s="59"/>
       <c r="D155" s="59"/>
-      <c r="E155" s="67"/>
+      <c r="E155" s="73"/>
       <c r="F155" s="59"/>
       <c r="G155" s="59"/>
       <c r="H155" s="59"/>
@@ -3954,7 +3953,7 @@
       </c>
       <c r="C156" s="59"/>
       <c r="D156" s="59"/>
-      <c r="E156" s="67"/>
+      <c r="E156" s="73"/>
       <c r="F156" s="59"/>
       <c r="G156" s="59"/>
       <c r="H156" s="59"/>
@@ -3969,7 +3968,7 @@
       </c>
       <c r="C157" s="59"/>
       <c r="D157" s="59"/>
-      <c r="E157" s="67"/>
+      <c r="E157" s="73"/>
       <c r="F157" s="59"/>
       <c r="G157" s="59"/>
       <c r="H157" s="59"/>
@@ -3984,7 +3983,7 @@
       </c>
       <c r="C158" s="59"/>
       <c r="D158" s="59"/>
-      <c r="E158" s="67"/>
+      <c r="E158" s="73"/>
       <c r="F158" s="59"/>
       <c r="G158" s="59"/>
       <c r="H158" s="59"/>
@@ -3999,7 +3998,7 @@
       </c>
       <c r="C159" s="59"/>
       <c r="D159" s="59"/>
-      <c r="E159" s="67"/>
+      <c r="E159" s="73"/>
       <c r="F159" s="59"/>
       <c r="G159" s="59"/>
       <c r="H159" s="59"/>
@@ -4014,7 +4013,7 @@
       </c>
       <c r="C160" s="59"/>
       <c r="D160" s="59"/>
-      <c r="E160" s="67"/>
+      <c r="E160" s="73"/>
       <c r="F160" s="59"/>
       <c r="G160" s="59"/>
       <c r="H160" s="59"/>
@@ -4031,7 +4030,7 @@
       </c>
       <c r="C161" s="59"/>
       <c r="D161" s="59"/>
-      <c r="E161" s="68"/>
+      <c r="E161" s="74"/>
       <c r="F161" s="59"/>
       <c r="G161" s="59"/>
       <c r="H161" s="59"/>
@@ -4048,7 +4047,7 @@
       </c>
       <c r="C162" s="59"/>
       <c r="D162" s="59"/>
-      <c r="E162" s="74" t="s">
+      <c r="E162" s="66" t="s">
         <v>26</v>
       </c>
       <c r="F162" s="59"/>
@@ -4067,7 +4066,7 @@
       </c>
       <c r="C163" s="59"/>
       <c r="D163" s="59"/>
-      <c r="E163" s="75"/>
+      <c r="E163" s="67"/>
       <c r="F163" s="59"/>
       <c r="G163" s="59"/>
       <c r="H163" s="59"/>
@@ -4082,7 +4081,7 @@
       </c>
       <c r="C164" s="59"/>
       <c r="D164" s="59"/>
-      <c r="E164" s="75"/>
+      <c r="E164" s="67"/>
       <c r="F164" s="59"/>
       <c r="G164" s="59"/>
       <c r="H164" s="59"/>
@@ -4097,7 +4096,7 @@
       </c>
       <c r="C165" s="59"/>
       <c r="D165" s="59"/>
-      <c r="E165" s="75"/>
+      <c r="E165" s="67"/>
       <c r="F165" s="59"/>
       <c r="G165" s="59"/>
       <c r="H165" s="59"/>
@@ -4112,7 +4111,7 @@
       </c>
       <c r="C166" s="59"/>
       <c r="D166" s="59"/>
-      <c r="E166" s="75"/>
+      <c r="E166" s="67"/>
       <c r="F166" s="59"/>
       <c r="G166" s="59"/>
       <c r="H166" s="59"/>
@@ -4127,7 +4126,7 @@
       </c>
       <c r="C167" s="59"/>
       <c r="D167" s="59"/>
-      <c r="E167" s="75"/>
+      <c r="E167" s="67"/>
       <c r="F167" s="59"/>
       <c r="G167" s="59"/>
       <c r="H167" s="59"/>
@@ -4142,7 +4141,7 @@
       </c>
       <c r="C168" s="59"/>
       <c r="D168" s="59"/>
-      <c r="E168" s="75"/>
+      <c r="E168" s="67"/>
       <c r="F168" s="59"/>
       <c r="G168" s="59"/>
       <c r="H168" s="59"/>
@@ -4157,7 +4156,7 @@
       </c>
       <c r="C169" s="59"/>
       <c r="D169" s="59"/>
-      <c r="E169" s="75"/>
+      <c r="E169" s="67"/>
       <c r="F169" s="59"/>
       <c r="G169" s="59"/>
       <c r="H169" s="59"/>
@@ -4172,7 +4171,7 @@
       </c>
       <c r="C170" s="59"/>
       <c r="D170" s="59"/>
-      <c r="E170" s="75"/>
+      <c r="E170" s="67"/>
       <c r="F170" s="59"/>
       <c r="G170" s="59"/>
       <c r="H170" s="59"/>
@@ -4187,7 +4186,7 @@
       </c>
       <c r="C171" s="59"/>
       <c r="D171" s="59"/>
-      <c r="E171" s="75"/>
+      <c r="E171" s="67"/>
       <c r="F171" s="59"/>
       <c r="G171" s="59"/>
       <c r="H171" s="59"/>
@@ -4202,7 +4201,7 @@
       </c>
       <c r="C172" s="59"/>
       <c r="D172" s="59"/>
-      <c r="E172" s="75"/>
+      <c r="E172" s="67"/>
       <c r="F172" s="59"/>
       <c r="G172" s="59"/>
       <c r="H172" s="59"/>
@@ -4217,7 +4216,7 @@
       </c>
       <c r="C173" s="59"/>
       <c r="D173" s="59"/>
-      <c r="E173" s="75"/>
+      <c r="E173" s="67"/>
       <c r="F173" s="59"/>
       <c r="G173" s="59"/>
       <c r="H173" s="59"/>
@@ -4232,7 +4231,7 @@
       </c>
       <c r="C174" s="59"/>
       <c r="D174" s="59"/>
-      <c r="E174" s="75"/>
+      <c r="E174" s="67"/>
       <c r="F174" s="59"/>
       <c r="G174" s="59"/>
       <c r="H174" s="59"/>
@@ -4247,7 +4246,7 @@
       </c>
       <c r="C175" s="59"/>
       <c r="D175" s="59"/>
-      <c r="E175" s="75"/>
+      <c r="E175" s="67"/>
       <c r="F175" s="59"/>
       <c r="G175" s="59"/>
       <c r="H175" s="59"/>
@@ -4262,7 +4261,7 @@
       </c>
       <c r="C176" s="59"/>
       <c r="D176" s="59"/>
-      <c r="E176" s="75"/>
+      <c r="E176" s="67"/>
       <c r="F176" s="59"/>
       <c r="G176" s="59"/>
       <c r="H176" s="59"/>
@@ -4279,7 +4278,7 @@
       </c>
       <c r="C177" s="59"/>
       <c r="D177" s="59"/>
-      <c r="E177" s="76"/>
+      <c r="E177" s="68"/>
       <c r="F177" s="59"/>
       <c r="G177" s="59"/>
       <c r="H177" s="59"/>
@@ -4296,7 +4295,7 @@
       </c>
       <c r="C178" s="59"/>
       <c r="D178" s="59"/>
-      <c r="E178" s="70" t="s">
+      <c r="E178" s="75" t="s">
         <v>27</v>
       </c>
       <c r="F178" s="59"/>
@@ -4315,7 +4314,7 @@
       </c>
       <c r="C179" s="59"/>
       <c r="D179" s="59"/>
-      <c r="E179" s="70"/>
+      <c r="E179" s="75"/>
       <c r="F179" s="59"/>
       <c r="G179" s="59"/>
       <c r="H179" s="59"/>
@@ -4330,7 +4329,7 @@
       </c>
       <c r="C180" s="59"/>
       <c r="D180" s="59"/>
-      <c r="E180" s="70"/>
+      <c r="E180" s="75"/>
       <c r="F180" s="59"/>
       <c r="G180" s="59"/>
       <c r="H180" s="59"/>
@@ -4345,7 +4344,7 @@
       </c>
       <c r="C181" s="59"/>
       <c r="D181" s="59"/>
-      <c r="E181" s="70"/>
+      <c r="E181" s="75"/>
       <c r="F181" s="59"/>
       <c r="G181" s="59"/>
       <c r="H181" s="59"/>
@@ -4360,7 +4359,7 @@
       </c>
       <c r="C182" s="59"/>
       <c r="D182" s="59"/>
-      <c r="E182" s="70"/>
+      <c r="E182" s="75"/>
       <c r="F182" s="59"/>
       <c r="G182" s="59"/>
       <c r="H182" s="59"/>
@@ -4375,7 +4374,7 @@
       </c>
       <c r="C183" s="59"/>
       <c r="D183" s="59"/>
-      <c r="E183" s="70"/>
+      <c r="E183" s="75"/>
       <c r="F183" s="59"/>
       <c r="G183" s="59"/>
       <c r="H183" s="59"/>
@@ -4390,7 +4389,7 @@
       </c>
       <c r="C184" s="59"/>
       <c r="D184" s="59"/>
-      <c r="E184" s="70"/>
+      <c r="E184" s="75"/>
       <c r="F184" s="59"/>
       <c r="G184" s="59"/>
       <c r="H184" s="59"/>
@@ -4405,7 +4404,7 @@
       </c>
       <c r="C185" s="59"/>
       <c r="D185" s="59"/>
-      <c r="E185" s="70"/>
+      <c r="E185" s="75"/>
       <c r="F185" s="59"/>
       <c r="G185" s="59"/>
       <c r="H185" s="59"/>
@@ -4420,7 +4419,7 @@
       </c>
       <c r="C186" s="59"/>
       <c r="D186" s="59"/>
-      <c r="E186" s="70"/>
+      <c r="E186" s="75"/>
       <c r="F186" s="59"/>
       <c r="G186" s="59"/>
       <c r="H186" s="59"/>
@@ -4435,7 +4434,7 @@
       </c>
       <c r="C187" s="59"/>
       <c r="D187" s="59"/>
-      <c r="E187" s="70"/>
+      <c r="E187" s="75"/>
       <c r="F187" s="59"/>
       <c r="G187" s="59"/>
       <c r="H187" s="59"/>
@@ -4450,7 +4449,7 @@
       </c>
       <c r="C188" s="59"/>
       <c r="D188" s="59"/>
-      <c r="E188" s="70"/>
+      <c r="E188" s="75"/>
       <c r="F188" s="59"/>
       <c r="G188" s="59"/>
       <c r="H188" s="59"/>
@@ -4465,7 +4464,7 @@
       </c>
       <c r="C189" s="59"/>
       <c r="D189" s="59"/>
-      <c r="E189" s="70"/>
+      <c r="E189" s="75"/>
       <c r="F189" s="59"/>
       <c r="G189" s="59"/>
       <c r="H189" s="59"/>
@@ -4480,7 +4479,7 @@
       </c>
       <c r="C190" s="59"/>
       <c r="D190" s="59"/>
-      <c r="E190" s="70"/>
+      <c r="E190" s="75"/>
       <c r="F190" s="59"/>
       <c r="G190" s="59"/>
       <c r="H190" s="59"/>
@@ -4495,7 +4494,7 @@
       </c>
       <c r="C191" s="59"/>
       <c r="D191" s="59"/>
-      <c r="E191" s="70"/>
+      <c r="E191" s="75"/>
       <c r="F191" s="59"/>
       <c r="G191" s="59"/>
       <c r="H191" s="59"/>
@@ -4510,7 +4509,7 @@
       </c>
       <c r="C192" s="59"/>
       <c r="D192" s="59"/>
-      <c r="E192" s="70"/>
+      <c r="E192" s="75"/>
       <c r="F192" s="59"/>
       <c r="G192" s="59"/>
       <c r="H192" s="59"/>
@@ -4527,7 +4526,7 @@
       </c>
       <c r="C193" s="59"/>
       <c r="D193" s="59"/>
-      <c r="E193" s="70"/>
+      <c r="E193" s="75"/>
       <c r="F193" s="59"/>
       <c r="G193" s="59"/>
       <c r="H193" s="59"/>
@@ -4543,7 +4542,7 @@
         <v>192</v>
       </c>
       <c r="C194" s="59"/>
-      <c r="D194" s="71" t="s">
+      <c r="D194" s="76" t="s">
         <v>25</v>
       </c>
       <c r="E194" s="59"/>
@@ -4562,7 +4561,7 @@
         <v>193</v>
       </c>
       <c r="C195" s="59"/>
-      <c r="D195" s="72"/>
+      <c r="D195" s="77"/>
       <c r="E195" s="59"/>
       <c r="F195" s="59"/>
       <c r="G195" s="59"/>
@@ -4577,7 +4576,7 @@
         <v>194</v>
       </c>
       <c r="C196" s="59"/>
-      <c r="D196" s="72"/>
+      <c r="D196" s="77"/>
       <c r="E196" s="59"/>
       <c r="F196" s="59"/>
       <c r="G196" s="59"/>
@@ -4592,7 +4591,7 @@
         <v>195</v>
       </c>
       <c r="C197" s="59"/>
-      <c r="D197" s="72"/>
+      <c r="D197" s="77"/>
       <c r="E197" s="59"/>
       <c r="F197" s="59"/>
       <c r="G197" s="59"/>
@@ -4607,7 +4606,7 @@
         <v>196</v>
       </c>
       <c r="C198" s="59"/>
-      <c r="D198" s="72"/>
+      <c r="D198" s="77"/>
       <c r="E198" s="59"/>
       <c r="F198" s="59"/>
       <c r="G198" s="59"/>
@@ -4622,7 +4621,7 @@
         <v>197</v>
       </c>
       <c r="C199" s="59"/>
-      <c r="D199" s="72"/>
+      <c r="D199" s="77"/>
       <c r="E199" s="59"/>
       <c r="F199" s="59"/>
       <c r="G199" s="59"/>
@@ -4637,7 +4636,7 @@
         <v>198</v>
       </c>
       <c r="C200" s="59"/>
-      <c r="D200" s="72"/>
+      <c r="D200" s="77"/>
       <c r="E200" s="59"/>
       <c r="F200" s="59"/>
       <c r="G200" s="59"/>
@@ -4654,7 +4653,7 @@
         <v>199</v>
       </c>
       <c r="C201" s="59"/>
-      <c r="D201" s="73"/>
+      <c r="D201" s="78"/>
       <c r="E201" s="59"/>
       <c r="F201" s="59"/>
       <c r="G201" s="59"/>
@@ -4671,7 +4670,7 @@
         <v>200</v>
       </c>
       <c r="C202" s="59"/>
-      <c r="D202" s="80" t="s">
+      <c r="D202" s="60" t="s">
         <v>24</v>
       </c>
       <c r="E202" s="59"/>
@@ -4690,7 +4689,7 @@
         <v>201</v>
       </c>
       <c r="C203" s="59"/>
-      <c r="D203" s="80"/>
+      <c r="D203" s="60"/>
       <c r="E203" s="59"/>
       <c r="F203" s="59"/>
       <c r="G203" s="59"/>
@@ -4705,7 +4704,7 @@
         <v>202</v>
       </c>
       <c r="C204" s="59"/>
-      <c r="D204" s="80"/>
+      <c r="D204" s="60"/>
       <c r="E204" s="59"/>
       <c r="F204" s="59"/>
       <c r="G204" s="59"/>
@@ -4720,7 +4719,7 @@
         <v>203</v>
       </c>
       <c r="C205" s="59"/>
-      <c r="D205" s="80"/>
+      <c r="D205" s="60"/>
       <c r="E205" s="59"/>
       <c r="F205" s="59"/>
       <c r="G205" s="59"/>
@@ -4735,7 +4734,7 @@
         <v>204</v>
       </c>
       <c r="C206" s="59"/>
-      <c r="D206" s="80"/>
+      <c r="D206" s="60"/>
       <c r="E206" s="59"/>
       <c r="F206" s="59"/>
       <c r="G206" s="59"/>
@@ -4750,7 +4749,7 @@
         <v>205</v>
       </c>
       <c r="C207" s="59"/>
-      <c r="D207" s="80"/>
+      <c r="D207" s="60"/>
       <c r="E207" s="59"/>
       <c r="F207" s="59"/>
       <c r="G207" s="59"/>
@@ -4765,7 +4764,7 @@
         <v>206</v>
       </c>
       <c r="C208" s="59"/>
-      <c r="D208" s="80"/>
+      <c r="D208" s="60"/>
       <c r="E208" s="59"/>
       <c r="F208" s="59"/>
       <c r="G208" s="59"/>
@@ -4782,7 +4781,7 @@
         <v>207</v>
       </c>
       <c r="C209" s="59"/>
-      <c r="D209" s="80"/>
+      <c r="D209" s="60"/>
       <c r="E209" s="59"/>
       <c r="F209" s="59"/>
       <c r="G209" s="59"/>
@@ -4798,9 +4797,9 @@
       <c r="B210" s="32">
         <v>208</v>
       </c>
-      <c r="C210" s="81"/>
-      <c r="D210" s="82"/>
-      <c r="E210" s="83" t="s">
+      <c r="C210" s="61"/>
+      <c r="D210" s="62"/>
+      <c r="E210" s="63" t="s">
         <v>34</v>
       </c>
       <c r="F210" s="59"/>
@@ -4817,9 +4816,9 @@
       <c r="B211" s="32">
         <v>209</v>
       </c>
-      <c r="C211" s="81"/>
-      <c r="D211" s="82"/>
-      <c r="E211" s="83"/>
+      <c r="C211" s="61"/>
+      <c r="D211" s="62"/>
+      <c r="E211" s="63"/>
       <c r="F211" s="59"/>
       <c r="G211" s="59"/>
       <c r="H211" s="59"/>
@@ -4834,9 +4833,9 @@
       <c r="B212" s="32">
         <v>210</v>
       </c>
-      <c r="C212" s="81"/>
-      <c r="D212" s="82"/>
-      <c r="E212" s="83"/>
+      <c r="C212" s="61"/>
+      <c r="D212" s="62"/>
+      <c r="E212" s="63"/>
       <c r="F212" s="59"/>
       <c r="G212" s="59"/>
       <c r="H212" s="59"/>
@@ -4851,9 +4850,9 @@
       <c r="B213" s="32">
         <v>211</v>
       </c>
-      <c r="C213" s="81"/>
-      <c r="D213" s="82"/>
-      <c r="E213" s="83"/>
+      <c r="C213" s="61"/>
+      <c r="D213" s="62"/>
+      <c r="E213" s="63"/>
       <c r="F213" s="59"/>
       <c r="G213" s="59"/>
       <c r="H213" s="59"/>
@@ -4868,9 +4867,9 @@
       <c r="B214" s="32">
         <v>212</v>
       </c>
-      <c r="C214" s="81"/>
-      <c r="D214" s="82"/>
-      <c r="E214" s="83"/>
+      <c r="C214" s="61"/>
+      <c r="D214" s="62"/>
+      <c r="E214" s="63"/>
       <c r="F214" s="59"/>
       <c r="G214" s="59"/>
       <c r="H214" s="59"/>
@@ -4883,9 +4882,9 @@
       <c r="B215" s="32">
         <v>213</v>
       </c>
-      <c r="C215" s="81"/>
-      <c r="D215" s="82"/>
-      <c r="E215" s="83"/>
+      <c r="C215" s="61"/>
+      <c r="D215" s="62"/>
+      <c r="E215" s="63"/>
       <c r="F215" s="59"/>
       <c r="G215" s="59"/>
       <c r="H215" s="59"/>
@@ -4898,9 +4897,9 @@
       <c r="B216" s="32">
         <v>214</v>
       </c>
-      <c r="C216" s="81"/>
-      <c r="D216" s="82"/>
-      <c r="E216" s="83"/>
+      <c r="C216" s="61"/>
+      <c r="D216" s="62"/>
+      <c r="E216" s="63"/>
       <c r="F216" s="59"/>
       <c r="G216" s="59"/>
       <c r="H216" s="59"/>
@@ -4913,9 +4912,9 @@
       <c r="B217" s="32">
         <v>215</v>
       </c>
-      <c r="C217" s="81"/>
-      <c r="D217" s="82"/>
-      <c r="E217" s="83"/>
+      <c r="C217" s="61"/>
+      <c r="D217" s="62"/>
+      <c r="E217" s="63"/>
       <c r="F217" s="59"/>
       <c r="G217" s="59"/>
       <c r="H217" s="59"/>
@@ -4929,8 +4928,8 @@
         <v>216</v>
       </c>
       <c r="C218" s="59"/>
-      <c r="D218" s="77"/>
-      <c r="E218" s="83"/>
+      <c r="D218" s="69"/>
+      <c r="E218" s="63"/>
       <c r="F218" s="59"/>
       <c r="G218" s="59"/>
       <c r="H218" s="59"/>
@@ -4944,8 +4943,8 @@
         <v>217</v>
       </c>
       <c r="C219" s="59"/>
-      <c r="D219" s="77"/>
-      <c r="E219" s="83"/>
+      <c r="D219" s="69"/>
+      <c r="E219" s="63"/>
       <c r="F219" s="59"/>
       <c r="G219" s="59"/>
       <c r="H219" s="59"/>
@@ -4959,8 +4958,8 @@
         <v>218</v>
       </c>
       <c r="C220" s="59"/>
-      <c r="D220" s="77"/>
-      <c r="E220" s="83"/>
+      <c r="D220" s="69"/>
+      <c r="E220" s="63"/>
       <c r="F220" s="59"/>
       <c r="G220" s="59"/>
       <c r="H220" s="59"/>
@@ -4974,8 +4973,8 @@
         <v>219</v>
       </c>
       <c r="C221" s="59"/>
-      <c r="D221" s="77"/>
-      <c r="E221" s="83"/>
+      <c r="D221" s="69"/>
+      <c r="E221" s="63"/>
       <c r="F221" s="59"/>
       <c r="G221" s="59"/>
       <c r="H221" s="59"/>
@@ -4989,8 +4988,8 @@
         <v>220</v>
       </c>
       <c r="C222" s="59"/>
-      <c r="D222" s="77"/>
-      <c r="E222" s="83"/>
+      <c r="D222" s="69"/>
+      <c r="E222" s="63"/>
       <c r="F222" s="59"/>
       <c r="G222" s="59"/>
       <c r="H222" s="59"/>
@@ -5004,8 +5003,8 @@
         <v>221</v>
       </c>
       <c r="C223" s="59"/>
-      <c r="D223" s="77"/>
-      <c r="E223" s="83"/>
+      <c r="D223" s="69"/>
+      <c r="E223" s="63"/>
       <c r="F223" s="59"/>
       <c r="G223" s="59"/>
       <c r="H223" s="59"/>
@@ -5019,8 +5018,8 @@
         <v>222</v>
       </c>
       <c r="C224" s="59"/>
-      <c r="D224" s="77"/>
-      <c r="E224" s="83"/>
+      <c r="D224" s="69"/>
+      <c r="E224" s="63"/>
       <c r="F224" s="59"/>
       <c r="G224" s="59"/>
       <c r="H224" s="59"/>
@@ -5034,8 +5033,8 @@
         <v>223</v>
       </c>
       <c r="C225" s="59"/>
-      <c r="D225" s="77"/>
-      <c r="E225" s="83"/>
+      <c r="D225" s="69"/>
+      <c r="E225" s="63"/>
       <c r="F225" s="59"/>
       <c r="G225" s="59"/>
       <c r="H225" s="59"/>
@@ -5050,8 +5049,8 @@
       <c r="B226" s="51">
         <v>224</v>
       </c>
-      <c r="C226" s="78"/>
-      <c r="D226" s="79" t="s">
+      <c r="C226" s="70"/>
+      <c r="D226" s="71" t="s">
         <v>29</v>
       </c>
       <c r="E226" s="59"/>
@@ -5069,8 +5068,8 @@
       <c r="B227" s="51">
         <v>225</v>
       </c>
-      <c r="C227" s="78"/>
-      <c r="D227" s="79"/>
+      <c r="C227" s="70"/>
+      <c r="D227" s="71"/>
       <c r="E227" s="59"/>
       <c r="F227" s="59"/>
       <c r="G227" s="59"/>
@@ -5084,8 +5083,8 @@
       <c r="B228" s="51">
         <v>226</v>
       </c>
-      <c r="C228" s="78"/>
-      <c r="D228" s="79"/>
+      <c r="C228" s="70"/>
+      <c r="D228" s="71"/>
       <c r="E228" s="59"/>
       <c r="F228" s="59"/>
       <c r="G228" s="59"/>
@@ -5099,8 +5098,8 @@
       <c r="B229" s="51">
         <v>227</v>
       </c>
-      <c r="C229" s="78"/>
-      <c r="D229" s="79"/>
+      <c r="C229" s="70"/>
+      <c r="D229" s="71"/>
       <c r="E229" s="59"/>
       <c r="F229" s="59"/>
       <c r="G229" s="59"/>
@@ -5114,8 +5113,8 @@
       <c r="B230" s="51">
         <v>228</v>
       </c>
-      <c r="C230" s="84"/>
-      <c r="D230" s="79"/>
+      <c r="C230" s="64"/>
+      <c r="D230" s="71"/>
       <c r="E230" s="59"/>
       <c r="F230" s="59"/>
       <c r="G230" s="59"/>
@@ -5129,8 +5128,8 @@
       <c r="B231" s="51">
         <v>229</v>
       </c>
-      <c r="C231" s="84"/>
-      <c r="D231" s="79"/>
+      <c r="C231" s="64"/>
+      <c r="D231" s="71"/>
       <c r="E231" s="59"/>
       <c r="F231" s="59"/>
       <c r="G231" s="59"/>
@@ -5144,13 +5143,15 @@
       <c r="B232" s="51">
         <v>230</v>
       </c>
-      <c r="C232" s="84"/>
-      <c r="D232" s="79"/>
+      <c r="C232" s="64"/>
+      <c r="D232" s="71"/>
       <c r="E232" s="59"/>
       <c r="F232" s="59"/>
       <c r="G232" s="59"/>
       <c r="H232" s="59"/>
-      <c r="I232" s="48"/>
+      <c r="I232" s="48" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" s="50" t="s">
@@ -5159,8 +5160,8 @@
       <c r="B233" s="51">
         <v>231</v>
       </c>
-      <c r="C233" s="84"/>
-      <c r="D233" s="79"/>
+      <c r="C233" s="64"/>
+      <c r="D233" s="71"/>
       <c r="E233" s="59"/>
       <c r="F233" s="59"/>
       <c r="G233" s="59"/>
@@ -5176,7 +5177,7 @@
       <c r="B234" s="47">
         <v>232</v>
       </c>
-      <c r="C234" s="85" t="s">
+      <c r="C234" s="65" t="s">
         <v>30</v>
       </c>
       <c r="D234" s="59"/>
@@ -5195,7 +5196,7 @@
       <c r="B235" s="47">
         <v>233</v>
       </c>
-      <c r="C235" s="85"/>
+      <c r="C235" s="65"/>
       <c r="D235" s="59"/>
       <c r="E235" s="59"/>
       <c r="F235" s="59"/>
@@ -5212,7 +5213,7 @@
       <c r="B236" s="47">
         <v>234</v>
       </c>
-      <c r="C236" s="85"/>
+      <c r="C236" s="65"/>
       <c r="D236" s="59"/>
       <c r="E236" s="59"/>
       <c r="F236" s="59"/>
@@ -5229,7 +5230,7 @@
       <c r="B237" s="47">
         <v>235</v>
       </c>
-      <c r="C237" s="85"/>
+      <c r="C237" s="65"/>
       <c r="D237" s="59"/>
       <c r="E237" s="59"/>
       <c r="F237" s="59"/>
@@ -5541,38 +5542,76 @@
     </row>
   </sheetData>
   <mergeCells count="126">
-    <mergeCell ref="F194:F225"/>
-    <mergeCell ref="G194:G257"/>
-    <mergeCell ref="C198:C201"/>
-    <mergeCell ref="C202:C205"/>
-    <mergeCell ref="D202:D209"/>
-    <mergeCell ref="C206:C209"/>
-    <mergeCell ref="C210:C213"/>
-    <mergeCell ref="D210:D217"/>
-    <mergeCell ref="E210:E225"/>
-    <mergeCell ref="C214:C217"/>
-    <mergeCell ref="D250:D257"/>
-    <mergeCell ref="C254:C257"/>
-    <mergeCell ref="F226:F257"/>
-    <mergeCell ref="C230:C233"/>
-    <mergeCell ref="C234:C237"/>
-    <mergeCell ref="D234:D241"/>
-    <mergeCell ref="C238:C241"/>
-    <mergeCell ref="C242:C245"/>
-    <mergeCell ref="D242:D249"/>
-    <mergeCell ref="E242:E257"/>
-    <mergeCell ref="C246:C249"/>
-    <mergeCell ref="C250:C253"/>
-    <mergeCell ref="E194:E209"/>
-    <mergeCell ref="C162:C165"/>
-    <mergeCell ref="D162:D169"/>
-    <mergeCell ref="E162:E177"/>
-    <mergeCell ref="C218:C221"/>
-    <mergeCell ref="D218:D225"/>
-    <mergeCell ref="C222:C225"/>
-    <mergeCell ref="C226:C229"/>
-    <mergeCell ref="D226:D233"/>
-    <mergeCell ref="E226:E241"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D9"/>
+    <mergeCell ref="E2:E17"/>
+    <mergeCell ref="F2:F33"/>
+    <mergeCell ref="G2:G65"/>
+    <mergeCell ref="H2:H129"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="F34:F65"/>
+    <mergeCell ref="C38:C41"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="D42:D49"/>
+    <mergeCell ref="C46:C49"/>
+    <mergeCell ref="C50:C53"/>
+    <mergeCell ref="D50:D57"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D25"/>
+    <mergeCell ref="E18:E33"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D26:D33"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="E50:E65"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="D58:D65"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="D66:D73"/>
+    <mergeCell ref="E66:E81"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="D34:D41"/>
+    <mergeCell ref="E34:E49"/>
+    <mergeCell ref="C90:C93"/>
+    <mergeCell ref="D90:D97"/>
+    <mergeCell ref="C94:C97"/>
+    <mergeCell ref="C98:C101"/>
+    <mergeCell ref="D98:D105"/>
+    <mergeCell ref="E98:E113"/>
+    <mergeCell ref="F66:F97"/>
+    <mergeCell ref="G66:G129"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="C74:C77"/>
+    <mergeCell ref="D74:D81"/>
+    <mergeCell ref="C78:C81"/>
+    <mergeCell ref="C82:C85"/>
+    <mergeCell ref="D82:D89"/>
+    <mergeCell ref="E82:E97"/>
+    <mergeCell ref="C86:C89"/>
+    <mergeCell ref="D122:D129"/>
+    <mergeCell ref="C126:C129"/>
+    <mergeCell ref="C130:C133"/>
+    <mergeCell ref="D130:D137"/>
+    <mergeCell ref="E130:E145"/>
+    <mergeCell ref="F130:F161"/>
+    <mergeCell ref="C154:C157"/>
+    <mergeCell ref="D154:D161"/>
+    <mergeCell ref="C158:C161"/>
+    <mergeCell ref="F98:F129"/>
+    <mergeCell ref="C102:C105"/>
+    <mergeCell ref="C106:C109"/>
+    <mergeCell ref="D106:D113"/>
+    <mergeCell ref="C110:C113"/>
+    <mergeCell ref="C114:C117"/>
+    <mergeCell ref="D114:D121"/>
+    <mergeCell ref="E114:E129"/>
+    <mergeCell ref="C118:C121"/>
+    <mergeCell ref="C122:C125"/>
     <mergeCell ref="F162:F193"/>
     <mergeCell ref="C166:C169"/>
     <mergeCell ref="C170:C173"/>
@@ -5597,76 +5636,38 @@
     <mergeCell ref="C190:C193"/>
     <mergeCell ref="C194:C197"/>
     <mergeCell ref="D194:D201"/>
-    <mergeCell ref="C130:C133"/>
-    <mergeCell ref="D130:D137"/>
-    <mergeCell ref="E130:E145"/>
-    <mergeCell ref="F130:F161"/>
-    <mergeCell ref="C154:C157"/>
-    <mergeCell ref="D154:D161"/>
-    <mergeCell ref="C158:C161"/>
-    <mergeCell ref="F98:F129"/>
-    <mergeCell ref="C102:C105"/>
-    <mergeCell ref="C106:C109"/>
-    <mergeCell ref="D106:D113"/>
-    <mergeCell ref="C110:C113"/>
-    <mergeCell ref="C114:C117"/>
-    <mergeCell ref="D114:D121"/>
-    <mergeCell ref="E114:E129"/>
-    <mergeCell ref="C118:C121"/>
-    <mergeCell ref="C122:C125"/>
-    <mergeCell ref="C90:C93"/>
-    <mergeCell ref="D90:D97"/>
-    <mergeCell ref="C94:C97"/>
-    <mergeCell ref="C98:C101"/>
-    <mergeCell ref="D98:D105"/>
-    <mergeCell ref="E98:E113"/>
-    <mergeCell ref="F66:F97"/>
-    <mergeCell ref="G66:G129"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="C74:C77"/>
-    <mergeCell ref="D74:D81"/>
-    <mergeCell ref="C78:C81"/>
-    <mergeCell ref="C82:C85"/>
-    <mergeCell ref="D82:D89"/>
-    <mergeCell ref="E82:E97"/>
-    <mergeCell ref="C86:C89"/>
-    <mergeCell ref="D122:D129"/>
-    <mergeCell ref="C126:C129"/>
-    <mergeCell ref="E50:E65"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="D58:D65"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="C66:C69"/>
-    <mergeCell ref="D66:D73"/>
-    <mergeCell ref="E66:E81"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="D34:D41"/>
-    <mergeCell ref="E34:E49"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="D2:D9"/>
-    <mergeCell ref="E2:E17"/>
-    <mergeCell ref="F2:F33"/>
-    <mergeCell ref="G2:G65"/>
-    <mergeCell ref="H2:H129"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="D10:D17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="F34:F65"/>
-    <mergeCell ref="C38:C41"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="D42:D49"/>
-    <mergeCell ref="C46:C49"/>
-    <mergeCell ref="C50:C53"/>
-    <mergeCell ref="D50:D57"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D25"/>
-    <mergeCell ref="E18:E33"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="D26:D33"/>
-    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="C162:C165"/>
+    <mergeCell ref="D162:D169"/>
+    <mergeCell ref="E162:E177"/>
+    <mergeCell ref="C218:C221"/>
+    <mergeCell ref="D218:D225"/>
+    <mergeCell ref="C222:C225"/>
+    <mergeCell ref="C226:C229"/>
+    <mergeCell ref="D226:D233"/>
+    <mergeCell ref="E226:E241"/>
+    <mergeCell ref="F194:F225"/>
+    <mergeCell ref="G194:G257"/>
+    <mergeCell ref="C198:C201"/>
+    <mergeCell ref="C202:C205"/>
+    <mergeCell ref="D202:D209"/>
+    <mergeCell ref="C206:C209"/>
+    <mergeCell ref="C210:C213"/>
+    <mergeCell ref="D210:D217"/>
+    <mergeCell ref="E210:E225"/>
+    <mergeCell ref="C214:C217"/>
+    <mergeCell ref="D250:D257"/>
+    <mergeCell ref="C254:C257"/>
+    <mergeCell ref="F226:F257"/>
+    <mergeCell ref="C230:C233"/>
+    <mergeCell ref="C234:C237"/>
+    <mergeCell ref="D234:D241"/>
+    <mergeCell ref="C238:C241"/>
+    <mergeCell ref="C242:C245"/>
+    <mergeCell ref="D242:D249"/>
+    <mergeCell ref="E242:E257"/>
+    <mergeCell ref="C246:C249"/>
+    <mergeCell ref="C250:C253"/>
+    <mergeCell ref="E194:E209"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5851,7 +5852,7 @@
       <c r="B1" s="33">
         <v>0</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="85" t="s">
         <v>15</v>
       </c>
       <c r="D1" s="43" t="s">
@@ -5863,7 +5864,7 @@
       <c r="G1" s="40">
         <v>32</v>
       </c>
-      <c r="H1" s="63" t="s">
+      <c r="H1" s="84" t="s">
         <v>16</v>
       </c>
       <c r="I1" s="44" t="s">
@@ -5875,7 +5876,7 @@
       <c r="L1" s="41">
         <v>64</v>
       </c>
-      <c r="M1" s="62" t="s">
+      <c r="M1" s="83" t="s">
         <v>18</v>
       </c>
       <c r="N1" s="45" t="s">
@@ -5887,7 +5888,7 @@
       <c r="Q1" s="42">
         <v>96</v>
       </c>
-      <c r="R1" s="64" t="s">
+      <c r="R1" s="80" t="s">
         <v>20</v>
       </c>
       <c r="S1" s="46" t="s">
@@ -5899,7 +5900,7 @@
       <c r="V1" s="39">
         <v>128</v>
       </c>
-      <c r="W1" s="66" t="s">
+      <c r="W1" s="72" t="s">
         <v>22</v>
       </c>
       <c r="X1" s="38" t="s">
@@ -5913,7 +5914,7 @@
       <c r="B2" s="33">
         <v>1</v>
       </c>
-      <c r="C2" s="60"/>
+      <c r="C2" s="85"/>
       <c r="D2" s="43"/>
       <c r="F2" s="40" t="s">
         <v>38</v>
@@ -5921,7 +5922,7 @@
       <c r="G2" s="40">
         <v>33</v>
       </c>
-      <c r="H2" s="63"/>
+      <c r="H2" s="84"/>
       <c r="I2" s="44"/>
       <c r="K2" s="41" t="s">
         <v>38</v>
@@ -5929,7 +5930,7 @@
       <c r="L2" s="41">
         <v>65</v>
       </c>
-      <c r="M2" s="62"/>
+      <c r="M2" s="83"/>
       <c r="N2" s="45"/>
       <c r="P2" s="42" t="s">
         <v>38</v>
@@ -5937,7 +5938,7 @@
       <c r="Q2" s="42">
         <v>97</v>
       </c>
-      <c r="R2" s="64"/>
+      <c r="R2" s="80"/>
       <c r="S2" s="46"/>
       <c r="U2" s="39" t="s">
         <v>38</v>
@@ -5945,7 +5946,7 @@
       <c r="V2" s="39">
         <v>129</v>
       </c>
-      <c r="W2" s="67"/>
+      <c r="W2" s="73"/>
       <c r="X2" s="38"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
@@ -5955,7 +5956,7 @@
       <c r="B3" s="33">
         <v>2</v>
       </c>
-      <c r="C3" s="60"/>
+      <c r="C3" s="85"/>
       <c r="D3" s="43"/>
       <c r="F3" s="40" t="s">
         <v>38</v>
@@ -5963,7 +5964,7 @@
       <c r="G3" s="40">
         <v>34</v>
       </c>
-      <c r="H3" s="63"/>
+      <c r="H3" s="84"/>
       <c r="I3" s="44"/>
       <c r="K3" s="41" t="s">
         <v>38</v>
@@ -5971,7 +5972,7 @@
       <c r="L3" s="41">
         <v>66</v>
       </c>
-      <c r="M3" s="62"/>
+      <c r="M3" s="83"/>
       <c r="N3" s="45"/>
       <c r="P3" s="42" t="s">
         <v>38</v>
@@ -5979,7 +5980,7 @@
       <c r="Q3" s="42">
         <v>98</v>
       </c>
-      <c r="R3" s="64"/>
+      <c r="R3" s="80"/>
       <c r="S3" s="46"/>
       <c r="U3" s="39" t="s">
         <v>38</v>
@@ -5987,7 +5988,7 @@
       <c r="V3" s="39">
         <v>130</v>
       </c>
-      <c r="W3" s="67"/>
+      <c r="W3" s="73"/>
       <c r="X3" s="38"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -5997,7 +5998,7 @@
       <c r="B4" s="33">
         <v>3</v>
       </c>
-      <c r="C4" s="60"/>
+      <c r="C4" s="85"/>
       <c r="D4" s="43"/>
       <c r="F4" s="40" t="s">
         <v>38</v>
@@ -6005,7 +6006,7 @@
       <c r="G4" s="40">
         <v>35</v>
       </c>
-      <c r="H4" s="63"/>
+      <c r="H4" s="84"/>
       <c r="I4" s="44"/>
       <c r="K4" s="41" t="s">
         <v>38</v>
@@ -6013,7 +6014,7 @@
       <c r="L4" s="41">
         <v>67</v>
       </c>
-      <c r="M4" s="62"/>
+      <c r="M4" s="83"/>
       <c r="N4" s="45"/>
       <c r="P4" s="42" t="s">
         <v>38</v>
@@ -6021,7 +6022,7 @@
       <c r="Q4" s="42">
         <v>99</v>
       </c>
-      <c r="R4" s="64"/>
+      <c r="R4" s="80"/>
       <c r="S4" s="46"/>
       <c r="U4" s="39" t="s">
         <v>38</v>
@@ -6029,7 +6030,7 @@
       <c r="V4" s="39">
         <v>131</v>
       </c>
-      <c r="W4" s="67"/>
+      <c r="W4" s="73"/>
       <c r="X4" s="38"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -6039,7 +6040,7 @@
       <c r="B5" s="33">
         <v>4</v>
       </c>
-      <c r="C5" s="60"/>
+      <c r="C5" s="85"/>
       <c r="D5" s="43"/>
       <c r="F5" s="40" t="s">
         <v>38</v>
@@ -6047,7 +6048,7 @@
       <c r="G5" s="40">
         <v>36</v>
       </c>
-      <c r="H5" s="63"/>
+      <c r="H5" s="84"/>
       <c r="I5" s="44"/>
       <c r="K5" s="41" t="s">
         <v>38</v>
@@ -6055,7 +6056,7 @@
       <c r="L5" s="41">
         <v>68</v>
       </c>
-      <c r="M5" s="62"/>
+      <c r="M5" s="83"/>
       <c r="N5" s="45"/>
       <c r="P5" s="42" t="s">
         <v>38</v>
@@ -6063,7 +6064,7 @@
       <c r="Q5" s="42">
         <v>100</v>
       </c>
-      <c r="R5" s="64"/>
+      <c r="R5" s="80"/>
       <c r="S5" s="46"/>
       <c r="U5" s="39" t="s">
         <v>38</v>
@@ -6071,7 +6072,7 @@
       <c r="V5" s="39">
         <v>132</v>
       </c>
-      <c r="W5" s="67"/>
+      <c r="W5" s="73"/>
       <c r="X5" s="38"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -6081,7 +6082,7 @@
       <c r="B6" s="33">
         <v>5</v>
       </c>
-      <c r="C6" s="60"/>
+      <c r="C6" s="85"/>
       <c r="D6" s="43"/>
       <c r="F6" s="40" t="s">
         <v>38</v>
@@ -6089,7 +6090,7 @@
       <c r="G6" s="40">
         <v>37</v>
       </c>
-      <c r="H6" s="63"/>
+      <c r="H6" s="84"/>
       <c r="I6" s="44"/>
       <c r="K6" s="41" t="s">
         <v>38</v>
@@ -6097,7 +6098,7 @@
       <c r="L6" s="41">
         <v>69</v>
       </c>
-      <c r="M6" s="62"/>
+      <c r="M6" s="83"/>
       <c r="N6" s="45"/>
       <c r="P6" s="42" t="s">
         <v>38</v>
@@ -6105,7 +6106,7 @@
       <c r="Q6" s="42">
         <v>101</v>
       </c>
-      <c r="R6" s="64"/>
+      <c r="R6" s="80"/>
       <c r="S6" s="46"/>
       <c r="U6" s="39" t="s">
         <v>38</v>
@@ -6113,7 +6114,7 @@
       <c r="V6" s="39">
         <v>133</v>
       </c>
-      <c r="W6" s="67"/>
+      <c r="W6" s="73"/>
       <c r="X6" s="38"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -6123,7 +6124,7 @@
       <c r="B7" s="33">
         <v>6</v>
       </c>
-      <c r="C7" s="60"/>
+      <c r="C7" s="85"/>
       <c r="D7" s="43"/>
       <c r="F7" s="40" t="s">
         <v>38</v>
@@ -6131,7 +6132,7 @@
       <c r="G7" s="40">
         <v>38</v>
       </c>
-      <c r="H7" s="63"/>
+      <c r="H7" s="84"/>
       <c r="I7" s="44"/>
       <c r="K7" s="41" t="s">
         <v>38</v>
@@ -6139,7 +6140,7 @@
       <c r="L7" s="41">
         <v>70</v>
       </c>
-      <c r="M7" s="62"/>
+      <c r="M7" s="83"/>
       <c r="N7" s="45"/>
       <c r="P7" s="42" t="s">
         <v>38</v>
@@ -6147,7 +6148,7 @@
       <c r="Q7" s="42">
         <v>102</v>
       </c>
-      <c r="R7" s="64"/>
+      <c r="R7" s="80"/>
       <c r="S7" s="46"/>
       <c r="U7" s="39" t="s">
         <v>38</v>
@@ -6155,7 +6156,7 @@
       <c r="V7" s="39">
         <v>134</v>
       </c>
-      <c r="W7" s="67"/>
+      <c r="W7" s="73"/>
       <c r="X7" s="38"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -6165,7 +6166,7 @@
       <c r="B8" s="33">
         <v>7</v>
       </c>
-      <c r="C8" s="60"/>
+      <c r="C8" s="85"/>
       <c r="D8" s="43"/>
       <c r="F8" s="40" t="s">
         <v>38</v>
@@ -6173,7 +6174,7 @@
       <c r="G8" s="40">
         <v>39</v>
       </c>
-      <c r="H8" s="63"/>
+      <c r="H8" s="84"/>
       <c r="I8" s="44"/>
       <c r="K8" s="41" t="s">
         <v>38</v>
@@ -6181,7 +6182,7 @@
       <c r="L8" s="41">
         <v>71</v>
       </c>
-      <c r="M8" s="62"/>
+      <c r="M8" s="83"/>
       <c r="N8" s="45"/>
       <c r="P8" s="42" t="s">
         <v>38</v>
@@ -6189,7 +6190,7 @@
       <c r="Q8" s="42">
         <v>103</v>
       </c>
-      <c r="R8" s="64"/>
+      <c r="R8" s="80"/>
       <c r="S8" s="46"/>
       <c r="U8" s="39" t="s">
         <v>38</v>
@@ -6197,7 +6198,7 @@
       <c r="V8" s="39">
         <v>135</v>
       </c>
-      <c r="W8" s="67"/>
+      <c r="W8" s="73"/>
       <c r="X8" s="38"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
@@ -6207,7 +6208,7 @@
       <c r="B9" s="33">
         <v>8</v>
       </c>
-      <c r="C9" s="60"/>
+      <c r="C9" s="85"/>
       <c r="D9" s="43"/>
       <c r="F9" s="40" t="s">
         <v>38</v>
@@ -6215,7 +6216,7 @@
       <c r="G9" s="40">
         <v>40</v>
       </c>
-      <c r="H9" s="63"/>
+      <c r="H9" s="84"/>
       <c r="I9" s="44"/>
       <c r="K9" s="41" t="s">
         <v>38</v>
@@ -6223,7 +6224,7 @@
       <c r="L9" s="41">
         <v>72</v>
       </c>
-      <c r="M9" s="62"/>
+      <c r="M9" s="83"/>
       <c r="N9" s="45"/>
       <c r="P9" s="42" t="s">
         <v>38</v>
@@ -6231,7 +6232,7 @@
       <c r="Q9" s="42">
         <v>104</v>
       </c>
-      <c r="R9" s="64"/>
+      <c r="R9" s="80"/>
       <c r="S9" s="46"/>
       <c r="U9" s="39" t="s">
         <v>38</v>
@@ -6239,7 +6240,7 @@
       <c r="V9" s="39">
         <v>136</v>
       </c>
-      <c r="W9" s="67"/>
+      <c r="W9" s="73"/>
       <c r="X9" s="38"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -6249,7 +6250,7 @@
       <c r="B10" s="33">
         <v>9</v>
       </c>
-      <c r="C10" s="60"/>
+      <c r="C10" s="85"/>
       <c r="D10" s="54"/>
       <c r="F10" s="40" t="s">
         <v>38</v>
@@ -6257,7 +6258,7 @@
       <c r="G10" s="40">
         <v>41</v>
       </c>
-      <c r="H10" s="63"/>
+      <c r="H10" s="84"/>
       <c r="I10" s="44"/>
       <c r="K10" s="41" t="s">
         <v>38</v>
@@ -6265,7 +6266,7 @@
       <c r="L10" s="41">
         <v>73</v>
       </c>
-      <c r="M10" s="62"/>
+      <c r="M10" s="83"/>
       <c r="N10" s="45"/>
       <c r="P10" s="42" t="s">
         <v>38</v>
@@ -6273,7 +6274,7 @@
       <c r="Q10" s="42">
         <v>105</v>
       </c>
-      <c r="R10" s="64"/>
+      <c r="R10" s="80"/>
       <c r="S10" s="46"/>
       <c r="U10" s="39" t="s">
         <v>38</v>
@@ -6281,7 +6282,7 @@
       <c r="V10" s="39">
         <v>137</v>
       </c>
-      <c r="W10" s="67"/>
+      <c r="W10" s="73"/>
       <c r="X10" s="38"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
@@ -6291,7 +6292,7 @@
       <c r="B11" s="33">
         <v>10</v>
       </c>
-      <c r="C11" s="60"/>
+      <c r="C11" s="85"/>
       <c r="D11" s="43"/>
       <c r="F11" s="40" t="s">
         <v>38</v>
@@ -6299,7 +6300,7 @@
       <c r="G11" s="40">
         <v>42</v>
       </c>
-      <c r="H11" s="63"/>
+      <c r="H11" s="84"/>
       <c r="I11" s="44"/>
       <c r="K11" s="41" t="s">
         <v>38</v>
@@ -6307,7 +6308,7 @@
       <c r="L11" s="41">
         <v>74</v>
       </c>
-      <c r="M11" s="62"/>
+      <c r="M11" s="83"/>
       <c r="N11" s="45"/>
       <c r="P11" s="42" t="s">
         <v>38</v>
@@ -6315,7 +6316,7 @@
       <c r="Q11" s="42">
         <v>106</v>
       </c>
-      <c r="R11" s="64"/>
+      <c r="R11" s="80"/>
       <c r="S11" s="46"/>
       <c r="U11" s="39" t="s">
         <v>38</v>
@@ -6323,7 +6324,7 @@
       <c r="V11" s="39">
         <v>138</v>
       </c>
-      <c r="W11" s="67"/>
+      <c r="W11" s="73"/>
       <c r="X11" s="38"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
@@ -6333,7 +6334,7 @@
       <c r="B12" s="33">
         <v>11</v>
       </c>
-      <c r="C12" s="60"/>
+      <c r="C12" s="85"/>
       <c r="D12" s="43"/>
       <c r="F12" s="40" t="s">
         <v>38</v>
@@ -6341,7 +6342,7 @@
       <c r="G12" s="40">
         <v>43</v>
       </c>
-      <c r="H12" s="63"/>
+      <c r="H12" s="84"/>
       <c r="I12" s="44"/>
       <c r="K12" s="41" t="s">
         <v>38</v>
@@ -6349,7 +6350,7 @@
       <c r="L12" s="41">
         <v>75</v>
       </c>
-      <c r="M12" s="62"/>
+      <c r="M12" s="83"/>
       <c r="N12" s="45"/>
       <c r="P12" s="42" t="s">
         <v>38</v>
@@ -6357,7 +6358,7 @@
       <c r="Q12" s="42">
         <v>107</v>
       </c>
-      <c r="R12" s="64"/>
+      <c r="R12" s="80"/>
       <c r="S12" s="46"/>
       <c r="U12" s="39" t="s">
         <v>38</v>
@@ -6365,7 +6366,7 @@
       <c r="V12" s="39">
         <v>139</v>
       </c>
-      <c r="W12" s="67"/>
+      <c r="W12" s="73"/>
       <c r="X12" s="38"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
@@ -6375,7 +6376,7 @@
       <c r="B13" s="33">
         <v>12</v>
       </c>
-      <c r="C13" s="60"/>
+      <c r="C13" s="85"/>
       <c r="D13" s="43"/>
       <c r="F13" s="40" t="s">
         <v>38</v>
@@ -6383,7 +6384,7 @@
       <c r="G13" s="40">
         <v>44</v>
       </c>
-      <c r="H13" s="63"/>
+      <c r="H13" s="84"/>
       <c r="I13" s="44"/>
       <c r="K13" s="41" t="s">
         <v>38</v>
@@ -6391,7 +6392,7 @@
       <c r="L13" s="41">
         <v>76</v>
       </c>
-      <c r="M13" s="62"/>
+      <c r="M13" s="83"/>
       <c r="N13" s="45"/>
       <c r="P13" s="42" t="s">
         <v>38</v>
@@ -6399,7 +6400,7 @@
       <c r="Q13" s="42">
         <v>108</v>
       </c>
-      <c r="R13" s="64"/>
+      <c r="R13" s="80"/>
       <c r="S13" s="46"/>
       <c r="U13" s="39" t="s">
         <v>38</v>
@@ -6407,7 +6408,7 @@
       <c r="V13" s="39">
         <v>140</v>
       </c>
-      <c r="W13" s="67"/>
+      <c r="W13" s="73"/>
       <c r="X13" s="38"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
@@ -6417,7 +6418,7 @@
       <c r="B14" s="33">
         <v>13</v>
       </c>
-      <c r="C14" s="60"/>
+      <c r="C14" s="85"/>
       <c r="D14" s="43"/>
       <c r="F14" s="40" t="s">
         <v>38</v>
@@ -6425,7 +6426,7 @@
       <c r="G14" s="40">
         <v>45</v>
       </c>
-      <c r="H14" s="63"/>
+      <c r="H14" s="84"/>
       <c r="I14" s="44"/>
       <c r="K14" s="41" t="s">
         <v>38</v>
@@ -6433,7 +6434,7 @@
       <c r="L14" s="41">
         <v>77</v>
       </c>
-      <c r="M14" s="62"/>
+      <c r="M14" s="83"/>
       <c r="N14" s="45"/>
       <c r="P14" s="42" t="s">
         <v>38</v>
@@ -6441,7 +6442,7 @@
       <c r="Q14" s="42">
         <v>109</v>
       </c>
-      <c r="R14" s="64"/>
+      <c r="R14" s="80"/>
       <c r="S14" s="46"/>
       <c r="U14" s="39" t="s">
         <v>38</v>
@@ -6449,7 +6450,7 @@
       <c r="V14" s="39">
         <v>141</v>
       </c>
-      <c r="W14" s="67"/>
+      <c r="W14" s="73"/>
       <c r="X14" s="38"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
@@ -6459,7 +6460,7 @@
       <c r="B15" s="33">
         <v>14</v>
       </c>
-      <c r="C15" s="60"/>
+      <c r="C15" s="85"/>
       <c r="D15" s="43"/>
       <c r="F15" s="40" t="s">
         <v>38</v>
@@ -6467,7 +6468,7 @@
       <c r="G15" s="40">
         <v>46</v>
       </c>
-      <c r="H15" s="63"/>
+      <c r="H15" s="84"/>
       <c r="I15" s="44" t="s">
         <v>33</v>
       </c>
@@ -6477,7 +6478,7 @@
       <c r="L15" s="41">
         <v>78</v>
       </c>
-      <c r="M15" s="62"/>
+      <c r="M15" s="83"/>
       <c r="N15" s="45" t="s">
         <v>33</v>
       </c>
@@ -6487,7 +6488,7 @@
       <c r="Q15" s="42">
         <v>110</v>
       </c>
-      <c r="R15" s="64"/>
+      <c r="R15" s="80"/>
       <c r="S15" s="46" t="s">
         <v>33</v>
       </c>
@@ -6497,7 +6498,7 @@
       <c r="V15" s="39">
         <v>142</v>
       </c>
-      <c r="W15" s="67"/>
+      <c r="W15" s="73"/>
       <c r="X15" s="38" t="s">
         <v>33</v>
       </c>
@@ -6509,7 +6510,7 @@
       <c r="B16" s="33">
         <v>15</v>
       </c>
-      <c r="C16" s="60"/>
+      <c r="C16" s="85"/>
       <c r="D16" s="43"/>
       <c r="F16" s="40" t="s">
         <v>38</v>
@@ -6517,7 +6518,7 @@
       <c r="G16" s="40">
         <v>47</v>
       </c>
-      <c r="H16" s="63"/>
+      <c r="H16" s="84"/>
       <c r="I16" s="44" t="s">
         <v>32</v>
       </c>
@@ -6527,7 +6528,7 @@
       <c r="L16" s="41">
         <v>79</v>
       </c>
-      <c r="M16" s="62"/>
+      <c r="M16" s="83"/>
       <c r="N16" s="45" t="s">
         <v>32</v>
       </c>
@@ -6537,7 +6538,7 @@
       <c r="Q16" s="42">
         <v>111</v>
       </c>
-      <c r="R16" s="64"/>
+      <c r="R16" s="80"/>
       <c r="S16" s="46" t="s">
         <v>32</v>
       </c>
@@ -6547,7 +6548,7 @@
       <c r="V16" s="39">
         <v>143</v>
       </c>
-      <c r="W16" s="68"/>
+      <c r="W16" s="74"/>
       <c r="X16" s="38" t="s">
         <v>32</v>
       </c>
@@ -6559,7 +6560,7 @@
       <c r="B17" s="33">
         <v>16</v>
       </c>
-      <c r="C17" s="60"/>
+      <c r="C17" s="85"/>
       <c r="D17" s="43"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
@@ -6569,7 +6570,7 @@
       <c r="B18" s="33">
         <v>17</v>
       </c>
-      <c r="C18" s="60"/>
+      <c r="C18" s="85"/>
       <c r="D18" s="43"/>
       <c r="F18" s="40" t="s">
         <v>38</v>
@@ -6577,7 +6578,7 @@
       <c r="G18" s="40">
         <v>48</v>
       </c>
-      <c r="H18" s="61" t="s">
+      <c r="H18" s="82" t="s">
         <v>17</v>
       </c>
       <c r="I18" s="44" t="s">
@@ -6589,7 +6590,7 @@
       <c r="L18" s="41">
         <v>80</v>
       </c>
-      <c r="M18" s="65" t="s">
+      <c r="M18" s="81" t="s">
         <v>19</v>
       </c>
       <c r="N18" s="45" t="s">
@@ -6601,7 +6602,7 @@
       <c r="Q18" s="42">
         <v>112</v>
       </c>
-      <c r="R18" s="69" t="s">
+      <c r="R18" s="79" t="s">
         <v>21</v>
       </c>
       <c r="S18" s="46" t="s">
@@ -6613,7 +6614,7 @@
       <c r="V18" s="39">
         <v>144</v>
       </c>
-      <c r="W18" s="66" t="s">
+      <c r="W18" s="72" t="s">
         <v>23</v>
       </c>
       <c r="X18" s="38" t="s">
@@ -6627,7 +6628,7 @@
       <c r="B19" s="33">
         <v>18</v>
       </c>
-      <c r="C19" s="60"/>
+      <c r="C19" s="85"/>
       <c r="D19" s="54"/>
       <c r="F19" s="40" t="s">
         <v>38</v>
@@ -6635,7 +6636,7 @@
       <c r="G19" s="40">
         <v>49</v>
       </c>
-      <c r="H19" s="61"/>
+      <c r="H19" s="82"/>
       <c r="I19" s="44"/>
       <c r="K19" s="41" t="s">
         <v>38</v>
@@ -6643,7 +6644,7 @@
       <c r="L19" s="41">
         <v>81</v>
       </c>
-      <c r="M19" s="65"/>
+      <c r="M19" s="81"/>
       <c r="N19" s="45"/>
       <c r="P19" s="42" t="s">
         <v>38</v>
@@ -6651,7 +6652,7 @@
       <c r="Q19" s="42">
         <v>113</v>
       </c>
-      <c r="R19" s="69"/>
+      <c r="R19" s="79"/>
       <c r="S19" s="46"/>
       <c r="U19" s="39" t="s">
         <v>38</v>
@@ -6659,7 +6660,7 @@
       <c r="V19" s="39">
         <v>145</v>
       </c>
-      <c r="W19" s="67"/>
+      <c r="W19" s="73"/>
       <c r="X19" s="38"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
@@ -6669,7 +6670,7 @@
       <c r="B20" s="33">
         <v>19</v>
       </c>
-      <c r="C20" s="60"/>
+      <c r="C20" s="85"/>
       <c r="D20" s="43"/>
       <c r="F20" s="40" t="s">
         <v>38</v>
@@ -6677,7 +6678,7 @@
       <c r="G20" s="40">
         <v>50</v>
       </c>
-      <c r="H20" s="61"/>
+      <c r="H20" s="82"/>
       <c r="I20" s="44"/>
       <c r="K20" s="41" t="s">
         <v>38</v>
@@ -6685,7 +6686,7 @@
       <c r="L20" s="41">
         <v>82</v>
       </c>
-      <c r="M20" s="65"/>
+      <c r="M20" s="81"/>
       <c r="N20" s="45"/>
       <c r="P20" s="42" t="s">
         <v>38</v>
@@ -6693,7 +6694,7 @@
       <c r="Q20" s="42">
         <v>114</v>
       </c>
-      <c r="R20" s="69"/>
+      <c r="R20" s="79"/>
       <c r="S20" s="46"/>
       <c r="U20" s="39" t="s">
         <v>38</v>
@@ -6701,7 +6702,7 @@
       <c r="V20" s="39">
         <v>146</v>
       </c>
-      <c r="W20" s="67"/>
+      <c r="W20" s="73"/>
       <c r="X20" s="38"/>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
@@ -6711,7 +6712,7 @@
       <c r="B21" s="33">
         <v>20</v>
       </c>
-      <c r="C21" s="60"/>
+      <c r="C21" s="85"/>
       <c r="D21" s="43"/>
       <c r="F21" s="40" t="s">
         <v>38</v>
@@ -6719,7 +6720,7 @@
       <c r="G21" s="40">
         <v>51</v>
       </c>
-      <c r="H21" s="61"/>
+      <c r="H21" s="82"/>
       <c r="I21" s="44"/>
       <c r="K21" s="41" t="s">
         <v>38</v>
@@ -6727,7 +6728,7 @@
       <c r="L21" s="41">
         <v>83</v>
       </c>
-      <c r="M21" s="65"/>
+      <c r="M21" s="81"/>
       <c r="N21" s="45"/>
       <c r="P21" s="42" t="s">
         <v>38</v>
@@ -6735,7 +6736,7 @@
       <c r="Q21" s="42">
         <v>115</v>
       </c>
-      <c r="R21" s="69"/>
+      <c r="R21" s="79"/>
       <c r="S21" s="46"/>
       <c r="U21" s="39" t="s">
         <v>38</v>
@@ -6743,7 +6744,7 @@
       <c r="V21" s="39">
         <v>147</v>
       </c>
-      <c r="W21" s="67"/>
+      <c r="W21" s="73"/>
       <c r="X21" s="38"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
@@ -6753,7 +6754,7 @@
       <c r="B22" s="33">
         <v>21</v>
       </c>
-      <c r="C22" s="60"/>
+      <c r="C22" s="85"/>
       <c r="D22" s="43"/>
       <c r="F22" s="40" t="s">
         <v>38</v>
@@ -6761,7 +6762,7 @@
       <c r="G22" s="40">
         <v>52</v>
       </c>
-      <c r="H22" s="61"/>
+      <c r="H22" s="82"/>
       <c r="I22" s="44"/>
       <c r="K22" s="41" t="s">
         <v>38</v>
@@ -6769,7 +6770,7 @@
       <c r="L22" s="41">
         <v>84</v>
       </c>
-      <c r="M22" s="65"/>
+      <c r="M22" s="81"/>
       <c r="N22" s="45"/>
       <c r="P22" s="42" t="s">
         <v>38</v>
@@ -6777,7 +6778,7 @@
       <c r="Q22" s="42">
         <v>116</v>
       </c>
-      <c r="R22" s="69"/>
+      <c r="R22" s="79"/>
       <c r="S22" s="46"/>
       <c r="U22" s="39" t="s">
         <v>38</v>
@@ -6785,7 +6786,7 @@
       <c r="V22" s="39">
         <v>148</v>
       </c>
-      <c r="W22" s="67"/>
+      <c r="W22" s="73"/>
       <c r="X22" s="38"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
@@ -6795,7 +6796,7 @@
       <c r="B23" s="33">
         <v>22</v>
       </c>
-      <c r="C23" s="60"/>
+      <c r="C23" s="85"/>
       <c r="D23" s="43"/>
       <c r="F23" s="40" t="s">
         <v>38</v>
@@ -6803,7 +6804,7 @@
       <c r="G23" s="40">
         <v>53</v>
       </c>
-      <c r="H23" s="61"/>
+      <c r="H23" s="82"/>
       <c r="I23" s="44"/>
       <c r="K23" s="41" t="s">
         <v>38</v>
@@ -6811,7 +6812,7 @@
       <c r="L23" s="41">
         <v>85</v>
       </c>
-      <c r="M23" s="65"/>
+      <c r="M23" s="81"/>
       <c r="N23" s="45"/>
       <c r="P23" s="42" t="s">
         <v>38</v>
@@ -6819,7 +6820,7 @@
       <c r="Q23" s="42">
         <v>117</v>
       </c>
-      <c r="R23" s="69"/>
+      <c r="R23" s="79"/>
       <c r="S23" s="46"/>
       <c r="U23" s="39" t="s">
         <v>38</v>
@@ -6827,7 +6828,7 @@
       <c r="V23" s="39">
         <v>149</v>
       </c>
-      <c r="W23" s="67"/>
+      <c r="W23" s="73"/>
       <c r="X23" s="38"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
@@ -6837,7 +6838,7 @@
       <c r="B24" s="33">
         <v>23</v>
       </c>
-      <c r="C24" s="60"/>
+      <c r="C24" s="85"/>
       <c r="D24" s="43"/>
       <c r="F24" s="40" t="s">
         <v>38</v>
@@ -6845,7 +6846,7 @@
       <c r="G24" s="40">
         <v>54</v>
       </c>
-      <c r="H24" s="61"/>
+      <c r="H24" s="82"/>
       <c r="I24" s="44"/>
       <c r="K24" s="41" t="s">
         <v>38</v>
@@ -6853,7 +6854,7 @@
       <c r="L24" s="41">
         <v>86</v>
       </c>
-      <c r="M24" s="65"/>
+      <c r="M24" s="81"/>
       <c r="N24" s="45"/>
       <c r="P24" s="42" t="s">
         <v>38</v>
@@ -6861,7 +6862,7 @@
       <c r="Q24" s="42">
         <v>118</v>
       </c>
-      <c r="R24" s="69"/>
+      <c r="R24" s="79"/>
       <c r="S24" s="46"/>
       <c r="U24" s="39" t="s">
         <v>38</v>
@@ -6869,7 +6870,7 @@
       <c r="V24" s="39">
         <v>150</v>
       </c>
-      <c r="W24" s="67"/>
+      <c r="W24" s="73"/>
       <c r="X24" s="38"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
@@ -6879,7 +6880,7 @@
       <c r="B25" s="33">
         <v>24</v>
       </c>
-      <c r="C25" s="60"/>
+      <c r="C25" s="85"/>
       <c r="D25" s="43"/>
       <c r="F25" s="40" t="s">
         <v>38</v>
@@ -6887,7 +6888,7 @@
       <c r="G25" s="40">
         <v>55</v>
       </c>
-      <c r="H25" s="61"/>
+      <c r="H25" s="82"/>
       <c r="I25" s="44"/>
       <c r="K25" s="41" t="s">
         <v>38</v>
@@ -6895,7 +6896,7 @@
       <c r="L25" s="41">
         <v>87</v>
       </c>
-      <c r="M25" s="65"/>
+      <c r="M25" s="81"/>
       <c r="N25" s="45"/>
       <c r="P25" s="42" t="s">
         <v>38</v>
@@ -6903,7 +6904,7 @@
       <c r="Q25" s="42">
         <v>119</v>
       </c>
-      <c r="R25" s="69"/>
+      <c r="R25" s="79"/>
       <c r="S25" s="46"/>
       <c r="U25" s="39" t="s">
         <v>38</v>
@@ -6911,7 +6912,7 @@
       <c r="V25" s="39">
         <v>151</v>
       </c>
-      <c r="W25" s="67"/>
+      <c r="W25" s="73"/>
       <c r="X25" s="38"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
@@ -6921,7 +6922,7 @@
       <c r="B26" s="33">
         <v>25</v>
       </c>
-      <c r="C26" s="60"/>
+      <c r="C26" s="85"/>
       <c r="D26" s="43"/>
       <c r="F26" s="40" t="s">
         <v>38</v>
@@ -6929,7 +6930,7 @@
       <c r="G26" s="40">
         <v>56</v>
       </c>
-      <c r="H26" s="61"/>
+      <c r="H26" s="82"/>
       <c r="I26" s="44"/>
       <c r="K26" s="41" t="s">
         <v>38</v>
@@ -6937,7 +6938,7 @@
       <c r="L26" s="41">
         <v>88</v>
       </c>
-      <c r="M26" s="65"/>
+      <c r="M26" s="81"/>
       <c r="N26" s="45"/>
       <c r="P26" s="42" t="s">
         <v>38</v>
@@ -6945,7 +6946,7 @@
       <c r="Q26" s="42">
         <v>120</v>
       </c>
-      <c r="R26" s="69"/>
+      <c r="R26" s="79"/>
       <c r="S26" s="46"/>
       <c r="U26" s="39" t="s">
         <v>38</v>
@@ -6953,7 +6954,7 @@
       <c r="V26" s="39">
         <v>152</v>
       </c>
-      <c r="W26" s="67"/>
+      <c r="W26" s="73"/>
       <c r="X26" s="38"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
@@ -6963,7 +6964,7 @@
       <c r="B27" s="33">
         <v>26</v>
       </c>
-      <c r="C27" s="60"/>
+      <c r="C27" s="85"/>
       <c r="D27" s="43"/>
       <c r="F27" s="40" t="s">
         <v>38</v>
@@ -6971,7 +6972,7 @@
       <c r="G27" s="40">
         <v>57</v>
       </c>
-      <c r="H27" s="61"/>
+      <c r="H27" s="82"/>
       <c r="I27" s="44"/>
       <c r="K27" s="41" t="s">
         <v>38</v>
@@ -6979,7 +6980,7 @@
       <c r="L27" s="41">
         <v>89</v>
       </c>
-      <c r="M27" s="65"/>
+      <c r="M27" s="81"/>
       <c r="N27" s="45"/>
       <c r="P27" s="42" t="s">
         <v>38</v>
@@ -6987,7 +6988,7 @@
       <c r="Q27" s="42">
         <v>121</v>
       </c>
-      <c r="R27" s="69"/>
+      <c r="R27" s="79"/>
       <c r="S27" s="46"/>
       <c r="U27" s="39" t="s">
         <v>38</v>
@@ -6995,7 +6996,7 @@
       <c r="V27" s="39">
         <v>153</v>
       </c>
-      <c r="W27" s="67"/>
+      <c r="W27" s="73"/>
       <c r="X27" s="38"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
@@ -7005,7 +7006,7 @@
       <c r="B28" s="33">
         <v>27</v>
       </c>
-      <c r="C28" s="60"/>
+      <c r="C28" s="85"/>
       <c r="D28" s="54" t="s">
         <v>35</v>
       </c>
@@ -7015,7 +7016,7 @@
       <c r="G28" s="40">
         <v>58</v>
       </c>
-      <c r="H28" s="61"/>
+      <c r="H28" s="82"/>
       <c r="I28" s="44"/>
       <c r="K28" s="41" t="s">
         <v>38</v>
@@ -7023,7 +7024,7 @@
       <c r="L28" s="41">
         <v>90</v>
       </c>
-      <c r="M28" s="65"/>
+      <c r="M28" s="81"/>
       <c r="N28" s="45"/>
       <c r="P28" s="42" t="s">
         <v>38</v>
@@ -7031,7 +7032,7 @@
       <c r="Q28" s="42">
         <v>122</v>
       </c>
-      <c r="R28" s="69"/>
+      <c r="R28" s="79"/>
       <c r="S28" s="46"/>
       <c r="U28" s="39" t="s">
         <v>38</v>
@@ -7039,7 +7040,7 @@
       <c r="V28" s="39">
         <v>154</v>
       </c>
-      <c r="W28" s="67"/>
+      <c r="W28" s="73"/>
       <c r="X28" s="38"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
@@ -7049,7 +7050,7 @@
       <c r="B29" s="33">
         <v>28</v>
       </c>
-      <c r="C29" s="60"/>
+      <c r="C29" s="85"/>
       <c r="D29" s="43" t="s">
         <v>36</v>
       </c>
@@ -7059,7 +7060,7 @@
       <c r="G29" s="40">
         <v>59</v>
       </c>
-      <c r="H29" s="61"/>
+      <c r="H29" s="82"/>
       <c r="I29" s="44"/>
       <c r="K29" s="41" t="s">
         <v>38</v>
@@ -7067,7 +7068,7 @@
       <c r="L29" s="41">
         <v>91</v>
       </c>
-      <c r="M29" s="65"/>
+      <c r="M29" s="81"/>
       <c r="N29" s="45"/>
       <c r="P29" s="42" t="s">
         <v>38</v>
@@ -7075,7 +7076,7 @@
       <c r="Q29" s="42">
         <v>123</v>
       </c>
-      <c r="R29" s="69"/>
+      <c r="R29" s="79"/>
       <c r="S29" s="46"/>
       <c r="U29" s="39" t="s">
         <v>38</v>
@@ -7083,7 +7084,7 @@
       <c r="V29" s="39">
         <v>155</v>
       </c>
-      <c r="W29" s="67"/>
+      <c r="W29" s="73"/>
       <c r="X29" s="38"/>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
@@ -7093,7 +7094,7 @@
       <c r="B30" s="33">
         <v>29</v>
       </c>
-      <c r="C30" s="60"/>
+      <c r="C30" s="85"/>
       <c r="D30" s="43" t="s">
         <v>37</v>
       </c>
@@ -7103,7 +7104,7 @@
       <c r="G30" s="40">
         <v>60</v>
       </c>
-      <c r="H30" s="61"/>
+      <c r="H30" s="82"/>
       <c r="I30" s="44"/>
       <c r="K30" s="41" t="s">
         <v>38</v>
@@ -7111,7 +7112,7 @@
       <c r="L30" s="41">
         <v>92</v>
       </c>
-      <c r="M30" s="65"/>
+      <c r="M30" s="81"/>
       <c r="N30" s="45"/>
       <c r="P30" s="42" t="s">
         <v>38</v>
@@ -7119,7 +7120,7 @@
       <c r="Q30" s="42">
         <v>124</v>
       </c>
-      <c r="R30" s="69"/>
+      <c r="R30" s="79"/>
       <c r="S30" s="46"/>
       <c r="U30" s="39" t="s">
         <v>38</v>
@@ -7127,7 +7128,7 @@
       <c r="V30" s="39">
         <v>156</v>
       </c>
-      <c r="W30" s="67"/>
+      <c r="W30" s="73"/>
       <c r="X30" s="38"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
@@ -7137,7 +7138,7 @@
       <c r="B31" s="33">
         <v>30</v>
       </c>
-      <c r="C31" s="60"/>
+      <c r="C31" s="85"/>
       <c r="D31" s="43" t="s">
         <v>33</v>
       </c>
@@ -7147,7 +7148,7 @@
       <c r="G31" s="40">
         <v>61</v>
       </c>
-      <c r="H31" s="61"/>
+      <c r="H31" s="82"/>
       <c r="I31" s="44"/>
       <c r="K31" s="41" t="s">
         <v>38</v>
@@ -7155,7 +7156,7 @@
       <c r="L31" s="41">
         <v>93</v>
       </c>
-      <c r="M31" s="65"/>
+      <c r="M31" s="81"/>
       <c r="N31" s="45"/>
       <c r="P31" s="42" t="s">
         <v>38</v>
@@ -7163,7 +7164,7 @@
       <c r="Q31" s="42">
         <v>125</v>
       </c>
-      <c r="R31" s="69"/>
+      <c r="R31" s="79"/>
       <c r="S31" s="46"/>
       <c r="U31" s="39" t="s">
         <v>38</v>
@@ -7171,7 +7172,7 @@
       <c r="V31" s="39">
         <v>157</v>
       </c>
-      <c r="W31" s="67"/>
+      <c r="W31" s="73"/>
       <c r="X31" s="38"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
@@ -7181,7 +7182,7 @@
       <c r="B32" s="33">
         <v>31</v>
       </c>
-      <c r="C32" s="60"/>
+      <c r="C32" s="85"/>
       <c r="D32" s="43" t="s">
         <v>32</v>
       </c>
@@ -7191,7 +7192,7 @@
       <c r="G32" s="40">
         <v>62</v>
       </c>
-      <c r="H32" s="61"/>
+      <c r="H32" s="82"/>
       <c r="I32" s="44" t="s">
         <v>33</v>
       </c>
@@ -7201,7 +7202,7 @@
       <c r="L32" s="41">
         <v>94</v>
       </c>
-      <c r="M32" s="65"/>
+      <c r="M32" s="81"/>
       <c r="N32" s="45" t="s">
         <v>33</v>
       </c>
@@ -7211,7 +7212,7 @@
       <c r="Q32" s="42">
         <v>126</v>
       </c>
-      <c r="R32" s="69"/>
+      <c r="R32" s="79"/>
       <c r="S32" s="46" t="s">
         <v>33</v>
       </c>
@@ -7221,7 +7222,7 @@
       <c r="V32" s="39">
         <v>158</v>
       </c>
-      <c r="W32" s="67"/>
+      <c r="W32" s="73"/>
       <c r="X32" s="38" t="s">
         <v>33</v>
       </c>
@@ -7233,7 +7234,7 @@
       <c r="G33" s="40">
         <v>63</v>
       </c>
-      <c r="H33" s="61"/>
+      <c r="H33" s="82"/>
       <c r="I33" s="44" t="s">
         <v>32</v>
       </c>
@@ -7243,7 +7244,7 @@
       <c r="L33" s="41">
         <v>95</v>
       </c>
-      <c r="M33" s="65"/>
+      <c r="M33" s="81"/>
       <c r="N33" s="45" t="s">
         <v>32</v>
       </c>
@@ -7253,7 +7254,7 @@
       <c r="Q33" s="42">
         <v>127</v>
       </c>
-      <c r="R33" s="69"/>
+      <c r="R33" s="79"/>
       <c r="S33" s="46" t="s">
         <v>32</v>
       </c>
@@ -7263,7 +7264,7 @@
       <c r="V33" s="39">
         <v>159</v>
       </c>
-      <c r="W33" s="68"/>
+      <c r="W33" s="74"/>
       <c r="X33" s="38" t="s">
         <v>32</v>
       </c>
@@ -7275,7 +7276,7 @@
       <c r="B35" s="37">
         <v>160</v>
       </c>
-      <c r="C35" s="74" t="s">
+      <c r="C35" s="66" t="s">
         <v>26</v>
       </c>
       <c r="D35" s="34" t="s">
@@ -7287,7 +7288,7 @@
       <c r="G35" s="37">
         <v>176</v>
       </c>
-      <c r="H35" s="70" t="s">
+      <c r="H35" s="75" t="s">
         <v>27</v>
       </c>
       <c r="I35" s="34" t="s">
@@ -7299,7 +7300,7 @@
       <c r="L35" s="35">
         <v>192</v>
       </c>
-      <c r="M35" s="71" t="s">
+      <c r="M35" s="76" t="s">
         <v>25</v>
       </c>
       <c r="N35" s="36" t="s">
@@ -7311,7 +7312,7 @@
       <c r="Q35" s="32">
         <v>208</v>
       </c>
-      <c r="R35" s="83" t="s">
+      <c r="R35" s="63" t="s">
         <v>34</v>
       </c>
       <c r="S35" s="31" t="s">
@@ -7323,7 +7324,7 @@
       <c r="V35" s="51">
         <v>224</v>
       </c>
-      <c r="W35" s="79" t="s">
+      <c r="W35" s="71" t="s">
         <v>29</v>
       </c>
       <c r="X35" s="48" t="s">
@@ -7337,7 +7338,7 @@
       <c r="B36" s="37">
         <v>161</v>
       </c>
-      <c r="C36" s="75"/>
+      <c r="C36" s="67"/>
       <c r="D36" s="34"/>
       <c r="F36" s="37" t="s">
         <v>38</v>
@@ -7345,7 +7346,7 @@
       <c r="G36" s="37">
         <v>177</v>
       </c>
-      <c r="H36" s="70"/>
+      <c r="H36" s="75"/>
       <c r="I36" s="34"/>
       <c r="K36" s="35" t="s">
         <v>38</v>
@@ -7353,7 +7354,7 @@
       <c r="L36" s="35">
         <v>193</v>
       </c>
-      <c r="M36" s="72"/>
+      <c r="M36" s="77"/>
       <c r="N36" s="36"/>
       <c r="P36" s="32" t="s">
         <v>38</v>
@@ -7361,7 +7362,7 @@
       <c r="Q36" s="32">
         <v>209</v>
       </c>
-      <c r="R36" s="83"/>
+      <c r="R36" s="63"/>
       <c r="S36" s="31" t="s">
         <v>58</v>
       </c>
@@ -7371,7 +7372,7 @@
       <c r="V36" s="51">
         <v>225</v>
       </c>
-      <c r="W36" s="79"/>
+      <c r="W36" s="71"/>
       <c r="X36" s="48"/>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
@@ -7381,7 +7382,7 @@
       <c r="B37" s="37">
         <v>162</v>
       </c>
-      <c r="C37" s="75"/>
+      <c r="C37" s="67"/>
       <c r="D37" s="34"/>
       <c r="F37" s="37" t="s">
         <v>38</v>
@@ -7389,7 +7390,7 @@
       <c r="G37" s="37">
         <v>178</v>
       </c>
-      <c r="H37" s="70"/>
+      <c r="H37" s="75"/>
       <c r="I37" s="34"/>
       <c r="K37" s="35" t="s">
         <v>38</v>
@@ -7397,7 +7398,7 @@
       <c r="L37" s="35">
         <v>194</v>
       </c>
-      <c r="M37" s="72"/>
+      <c r="M37" s="77"/>
       <c r="N37" s="36"/>
       <c r="P37" s="32" t="s">
         <v>38</v>
@@ -7405,7 +7406,7 @@
       <c r="Q37" s="32">
         <v>210</v>
       </c>
-      <c r="R37" s="83"/>
+      <c r="R37" s="63"/>
       <c r="S37" s="31" t="s">
         <v>59</v>
       </c>
@@ -7415,7 +7416,7 @@
       <c r="V37" s="51">
         <v>226</v>
       </c>
-      <c r="W37" s="79"/>
+      <c r="W37" s="71"/>
       <c r="X37" s="48"/>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
@@ -7425,7 +7426,7 @@
       <c r="B38" s="37">
         <v>163</v>
       </c>
-      <c r="C38" s="75"/>
+      <c r="C38" s="67"/>
       <c r="D38" s="34"/>
       <c r="F38" s="37" t="s">
         <v>38</v>
@@ -7433,7 +7434,7 @@
       <c r="G38" s="37">
         <v>179</v>
       </c>
-      <c r="H38" s="70"/>
+      <c r="H38" s="75"/>
       <c r="I38" s="34"/>
       <c r="K38" s="35" t="s">
         <v>38</v>
@@ -7441,7 +7442,7 @@
       <c r="L38" s="35">
         <v>195</v>
       </c>
-      <c r="M38" s="72"/>
+      <c r="M38" s="77"/>
       <c r="N38" s="36"/>
       <c r="P38" s="32" t="s">
         <v>38</v>
@@ -7449,7 +7450,7 @@
       <c r="Q38" s="32">
         <v>211</v>
       </c>
-      <c r="R38" s="83"/>
+      <c r="R38" s="63"/>
       <c r="S38" s="31" t="s">
         <v>60</v>
       </c>
@@ -7459,7 +7460,7 @@
       <c r="V38" s="51">
         <v>227</v>
       </c>
-      <c r="W38" s="79"/>
+      <c r="W38" s="71"/>
       <c r="X38" s="48"/>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
@@ -7469,7 +7470,7 @@
       <c r="B39" s="37">
         <v>164</v>
       </c>
-      <c r="C39" s="75"/>
+      <c r="C39" s="67"/>
       <c r="D39" s="34"/>
       <c r="F39" s="37" t="s">
         <v>38</v>
@@ -7477,7 +7478,7 @@
       <c r="G39" s="37">
         <v>180</v>
       </c>
-      <c r="H39" s="70"/>
+      <c r="H39" s="75"/>
       <c r="I39" s="34"/>
       <c r="K39" s="35" t="s">
         <v>38</v>
@@ -7485,7 +7486,7 @@
       <c r="L39" s="35">
         <v>196</v>
       </c>
-      <c r="M39" s="72"/>
+      <c r="M39" s="77"/>
       <c r="N39" s="36"/>
       <c r="P39" s="32" t="s">
         <v>38</v>
@@ -7493,7 +7494,7 @@
       <c r="Q39" s="32">
         <v>212</v>
       </c>
-      <c r="R39" s="83"/>
+      <c r="R39" s="63"/>
       <c r="S39" s="31"/>
       <c r="U39" s="50" t="s">
         <v>38</v>
@@ -7501,7 +7502,7 @@
       <c r="V39" s="51">
         <v>228</v>
       </c>
-      <c r="W39" s="79"/>
+      <c r="W39" s="71"/>
       <c r="X39" s="48"/>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
@@ -7511,7 +7512,7 @@
       <c r="B40" s="37">
         <v>165</v>
       </c>
-      <c r="C40" s="75"/>
+      <c r="C40" s="67"/>
       <c r="D40" s="34"/>
       <c r="F40" s="37" t="s">
         <v>38</v>
@@ -7519,7 +7520,7 @@
       <c r="G40" s="37">
         <v>181</v>
       </c>
-      <c r="H40" s="70"/>
+      <c r="H40" s="75"/>
       <c r="I40" s="34"/>
       <c r="K40" s="35" t="s">
         <v>38</v>
@@ -7527,7 +7528,7 @@
       <c r="L40" s="35">
         <v>197</v>
       </c>
-      <c r="M40" s="72"/>
+      <c r="M40" s="77"/>
       <c r="N40" s="36"/>
       <c r="P40" s="32" t="s">
         <v>38</v>
@@ -7535,7 +7536,7 @@
       <c r="Q40" s="32">
         <v>213</v>
       </c>
-      <c r="R40" s="83"/>
+      <c r="R40" s="63"/>
       <c r="S40" s="31"/>
       <c r="U40" s="50" t="s">
         <v>38</v>
@@ -7543,7 +7544,7 @@
       <c r="V40" s="51">
         <v>229</v>
       </c>
-      <c r="W40" s="79"/>
+      <c r="W40" s="71"/>
       <c r="X40" s="48"/>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
@@ -7553,7 +7554,7 @@
       <c r="B41" s="37">
         <v>166</v>
       </c>
-      <c r="C41" s="75"/>
+      <c r="C41" s="67"/>
       <c r="D41" s="34"/>
       <c r="F41" s="37" t="s">
         <v>38</v>
@@ -7561,7 +7562,7 @@
       <c r="G41" s="37">
         <v>182</v>
       </c>
-      <c r="H41" s="70"/>
+      <c r="H41" s="75"/>
       <c r="I41" s="34"/>
       <c r="K41" s="35" t="s">
         <v>38</v>
@@ -7569,7 +7570,7 @@
       <c r="L41" s="35">
         <v>198</v>
       </c>
-      <c r="M41" s="72"/>
+      <c r="M41" s="77"/>
       <c r="N41" s="36" t="s">
         <v>33</v>
       </c>
@@ -7579,7 +7580,7 @@
       <c r="Q41" s="32">
         <v>214</v>
       </c>
-      <c r="R41" s="83"/>
+      <c r="R41" s="63"/>
       <c r="S41" s="31"/>
       <c r="U41" s="50" t="s">
         <v>38</v>
@@ -7587,7 +7588,7 @@
       <c r="V41" s="51">
         <v>230</v>
       </c>
-      <c r="W41" s="79"/>
+      <c r="W41" s="71"/>
       <c r="X41" s="48"/>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
@@ -7597,7 +7598,7 @@
       <c r="B42" s="37">
         <v>167</v>
       </c>
-      <c r="C42" s="75"/>
+      <c r="C42" s="67"/>
       <c r="D42" s="34"/>
       <c r="F42" s="37" t="s">
         <v>38</v>
@@ -7605,7 +7606,7 @@
       <c r="G42" s="37">
         <v>183</v>
       </c>
-      <c r="H42" s="70"/>
+      <c r="H42" s="75"/>
       <c r="I42" s="34"/>
       <c r="K42" s="35" t="s">
         <v>38</v>
@@ -7613,7 +7614,7 @@
       <c r="L42" s="35">
         <v>199</v>
       </c>
-      <c r="M42" s="73"/>
+      <c r="M42" s="78"/>
       <c r="N42" s="36" t="s">
         <v>32</v>
       </c>
@@ -7623,7 +7624,7 @@
       <c r="Q42" s="32">
         <v>215</v>
       </c>
-      <c r="R42" s="83"/>
+      <c r="R42" s="63"/>
       <c r="S42" s="31"/>
       <c r="U42" s="50" t="s">
         <v>38</v>
@@ -7631,7 +7632,7 @@
       <c r="V42" s="51">
         <v>231</v>
       </c>
-      <c r="W42" s="79"/>
+      <c r="W42" s="71"/>
       <c r="X42" s="48" t="s">
         <v>32</v>
       </c>
@@ -7643,7 +7644,7 @@
       <c r="B43" s="37">
         <v>168</v>
       </c>
-      <c r="C43" s="75"/>
+      <c r="C43" s="67"/>
       <c r="D43" s="34"/>
       <c r="F43" s="37" t="s">
         <v>38</v>
@@ -7651,7 +7652,7 @@
       <c r="G43" s="37">
         <v>184</v>
       </c>
-      <c r="H43" s="70"/>
+      <c r="H43" s="75"/>
       <c r="I43" s="34"/>
       <c r="P43" s="32" t="s">
         <v>38</v>
@@ -7659,7 +7660,7 @@
       <c r="Q43" s="32">
         <v>216</v>
       </c>
-      <c r="R43" s="83"/>
+      <c r="R43" s="63"/>
       <c r="S43" s="31"/>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
@@ -7669,7 +7670,7 @@
       <c r="B44" s="37">
         <v>169</v>
       </c>
-      <c r="C44" s="75"/>
+      <c r="C44" s="67"/>
       <c r="D44" s="34"/>
       <c r="F44" s="37" t="s">
         <v>38</v>
@@ -7677,7 +7678,7 @@
       <c r="G44" s="37">
         <v>185</v>
       </c>
-      <c r="H44" s="70"/>
+      <c r="H44" s="75"/>
       <c r="I44" s="34"/>
       <c r="K44" s="35" t="s">
         <v>38</v>
@@ -7685,7 +7686,7 @@
       <c r="L44" s="35">
         <v>200</v>
       </c>
-      <c r="M44" s="80" t="s">
+      <c r="M44" s="60" t="s">
         <v>24</v>
       </c>
       <c r="N44" s="36" t="s">
@@ -7697,7 +7698,7 @@
       <c r="Q44" s="32">
         <v>217</v>
       </c>
-      <c r="R44" s="83"/>
+      <c r="R44" s="63"/>
       <c r="S44" s="31"/>
       <c r="U44" s="47" t="s">
         <v>38</v>
@@ -7705,7 +7706,7 @@
       <c r="V44" s="47">
         <v>232</v>
       </c>
-      <c r="W44" s="85" t="s">
+      <c r="W44" s="65" t="s">
         <v>30</v>
       </c>
       <c r="X44" s="49" t="s">
@@ -7719,7 +7720,7 @@
       <c r="B45" s="37">
         <v>170</v>
       </c>
-      <c r="C45" s="75"/>
+      <c r="C45" s="67"/>
       <c r="D45" s="34"/>
       <c r="F45" s="37" t="s">
         <v>38</v>
@@ -7727,7 +7728,7 @@
       <c r="G45" s="37">
         <v>186</v>
       </c>
-      <c r="H45" s="70"/>
+      <c r="H45" s="75"/>
       <c r="I45" s="34"/>
       <c r="K45" s="35" t="s">
         <v>38</v>
@@ -7735,7 +7736,7 @@
       <c r="L45" s="35">
         <v>201</v>
       </c>
-      <c r="M45" s="80"/>
+      <c r="M45" s="60"/>
       <c r="N45" s="36"/>
       <c r="P45" s="32" t="s">
         <v>38</v>
@@ -7743,7 +7744,7 @@
       <c r="Q45" s="32">
         <v>218</v>
       </c>
-      <c r="R45" s="83"/>
+      <c r="R45" s="63"/>
       <c r="S45" s="31"/>
       <c r="U45" s="47" t="s">
         <v>38</v>
@@ -7751,7 +7752,7 @@
       <c r="V45" s="47">
         <v>233</v>
       </c>
-      <c r="W45" s="85"/>
+      <c r="W45" s="65"/>
       <c r="X45" s="49" t="s">
         <v>57</v>
       </c>
@@ -7763,7 +7764,7 @@
       <c r="B46" s="37">
         <v>171</v>
       </c>
-      <c r="C46" s="75"/>
+      <c r="C46" s="67"/>
       <c r="D46" s="34"/>
       <c r="F46" s="37" t="s">
         <v>38</v>
@@ -7771,7 +7772,7 @@
       <c r="G46" s="37">
         <v>187</v>
       </c>
-      <c r="H46" s="70"/>
+      <c r="H46" s="75"/>
       <c r="I46" s="34"/>
       <c r="K46" s="35" t="s">
         <v>38</v>
@@ -7779,7 +7780,7 @@
       <c r="L46" s="35">
         <v>202</v>
       </c>
-      <c r="M46" s="80"/>
+      <c r="M46" s="60"/>
       <c r="N46" s="36"/>
       <c r="P46" s="32" t="s">
         <v>38</v>
@@ -7787,7 +7788,7 @@
       <c r="Q46" s="32">
         <v>219</v>
       </c>
-      <c r="R46" s="83"/>
+      <c r="R46" s="63"/>
       <c r="S46" s="31"/>
       <c r="U46" s="47" t="s">
         <v>38</v>
@@ -7795,7 +7796,7 @@
       <c r="V46" s="47">
         <v>234</v>
       </c>
-      <c r="W46" s="85"/>
+      <c r="W46" s="65"/>
       <c r="X46" s="49" t="s">
         <v>33</v>
       </c>
@@ -7807,7 +7808,7 @@
       <c r="B47" s="37">
         <v>172</v>
       </c>
-      <c r="C47" s="75"/>
+      <c r="C47" s="67"/>
       <c r="D47" s="34"/>
       <c r="F47" s="37" t="s">
         <v>38</v>
@@ -7815,7 +7816,7 @@
       <c r="G47" s="37">
         <v>188</v>
       </c>
-      <c r="H47" s="70"/>
+      <c r="H47" s="75"/>
       <c r="I47" s="34"/>
       <c r="K47" s="35" t="s">
         <v>38</v>
@@ -7823,7 +7824,7 @@
       <c r="L47" s="35">
         <v>203</v>
       </c>
-      <c r="M47" s="80"/>
+      <c r="M47" s="60"/>
       <c r="N47" s="36"/>
       <c r="P47" s="32" t="s">
         <v>38</v>
@@ -7831,7 +7832,7 @@
       <c r="Q47" s="32">
         <v>220</v>
       </c>
-      <c r="R47" s="83"/>
+      <c r="R47" s="63"/>
       <c r="S47" s="31"/>
       <c r="U47" s="47" t="s">
         <v>38</v>
@@ -7839,7 +7840,7 @@
       <c r="V47" s="47">
         <v>235</v>
       </c>
-      <c r="W47" s="85"/>
+      <c r="W47" s="65"/>
       <c r="X47" s="49" t="s">
         <v>32</v>
       </c>
@@ -7851,7 +7852,7 @@
       <c r="B48" s="37">
         <v>173</v>
       </c>
-      <c r="C48" s="75"/>
+      <c r="C48" s="67"/>
       <c r="D48" s="34"/>
       <c r="F48" s="37" t="s">
         <v>38</v>
@@ -7859,7 +7860,7 @@
       <c r="G48" s="37">
         <v>189</v>
       </c>
-      <c r="H48" s="70"/>
+      <c r="H48" s="75"/>
       <c r="I48" s="34"/>
       <c r="K48" s="35" t="s">
         <v>38</v>
@@ -7867,7 +7868,7 @@
       <c r="L48" s="35">
         <v>204</v>
       </c>
-      <c r="M48" s="80"/>
+      <c r="M48" s="60"/>
       <c r="N48" s="36"/>
       <c r="P48" s="32" t="s">
         <v>38</v>
@@ -7875,7 +7876,7 @@
       <c r="Q48" s="32">
         <v>221</v>
       </c>
-      <c r="R48" s="83"/>
+      <c r="R48" s="63"/>
       <c r="S48" s="31"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
@@ -7885,7 +7886,7 @@
       <c r="B49" s="37">
         <v>174</v>
       </c>
-      <c r="C49" s="75"/>
+      <c r="C49" s="67"/>
       <c r="D49" s="34" t="s">
         <v>33</v>
       </c>
@@ -7895,7 +7896,7 @@
       <c r="G49" s="37">
         <v>190</v>
       </c>
-      <c r="H49" s="70"/>
+      <c r="H49" s="75"/>
       <c r="I49" s="34" t="s">
         <v>33</v>
       </c>
@@ -7905,7 +7906,7 @@
       <c r="L49" s="35">
         <v>205</v>
       </c>
-      <c r="M49" s="80"/>
+      <c r="M49" s="60"/>
       <c r="N49" s="36"/>
       <c r="P49" s="32" t="s">
         <v>38</v>
@@ -7913,7 +7914,7 @@
       <c r="Q49" s="32">
         <v>222</v>
       </c>
-      <c r="R49" s="83"/>
+      <c r="R49" s="63"/>
       <c r="S49" s="31"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
@@ -7923,7 +7924,7 @@
       <c r="B50" s="37">
         <v>175</v>
       </c>
-      <c r="C50" s="76"/>
+      <c r="C50" s="68"/>
       <c r="D50" s="34" t="s">
         <v>32</v>
       </c>
@@ -7933,7 +7934,7 @@
       <c r="G50" s="37">
         <v>191</v>
       </c>
-      <c r="H50" s="70"/>
+      <c r="H50" s="75"/>
       <c r="I50" s="34" t="s">
         <v>32</v>
       </c>
@@ -7943,7 +7944,7 @@
       <c r="L50" s="35">
         <v>206</v>
       </c>
-      <c r="M50" s="80"/>
+      <c r="M50" s="60"/>
       <c r="N50" s="36" t="s">
         <v>33</v>
       </c>
@@ -7953,7 +7954,7 @@
       <c r="Q50" s="32">
         <v>223</v>
       </c>
-      <c r="R50" s="83"/>
+      <c r="R50" s="63"/>
       <c r="S50" s="31" t="s">
         <v>32</v>
       </c>
@@ -7965,7 +7966,7 @@
       <c r="L51" s="35">
         <v>207</v>
       </c>
-      <c r="M51" s="80"/>
+      <c r="M51" s="60"/>
       <c r="N51" s="36" t="s">
         <v>32</v>
       </c>
@@ -8222,7 +8223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{094E0344-2B81-4E6D-AD84-5D175246353F}">
   <dimension ref="B2:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -8251,7 +8252,7 @@
       <c r="F2" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="G2" s="86" t="s">
+      <c r="G2" s="29" t="s">
         <v>101</v>
       </c>
       <c r="H2" s="29" t="s">
@@ -8274,7 +8275,7 @@
       <c r="F3" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="G3" s="86" t="s">
+      <c r="G3" s="29" t="s">
         <v>114</v>
       </c>
       <c r="H3" s="29">
@@ -8297,7 +8298,7 @@
       <c r="F4" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="G4" s="86" t="s">
+      <c r="G4" s="29" t="s">
         <v>114</v>
       </c>
       <c r="H4" s="29">
@@ -8320,7 +8321,7 @@
       <c r="F5" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="G5" s="86" t="s">
+      <c r="G5" s="29" t="s">
         <v>114</v>
       </c>
       <c r="H5" s="29">

</xml_diff>

<commit_message>
Generated keys for ssh and documented it
</commit_message>
<xml_diff>
--- a/Kisvállalat létszám.xlsx
+++ b/Kisvállalat létszám.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\projekt\fluffy-system\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\School\11.o\Hálózat\projekt\fluffy-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1966E98-77FC-47ED-8294-91C0C5A54DC1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989A0D1D-64D0-4341-9E9C-27B89B8F32F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alap" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="122">
   <si>
     <t>I.em</t>
   </si>
@@ -384,6 +384,18 @@
   </si>
   <si>
     <t>192.168.1.230</t>
+  </si>
+  <si>
+    <t>S0 Vlan 1</t>
+  </si>
+  <si>
+    <t>S1 Vlan 1</t>
+  </si>
+  <si>
+    <t>S2 Vlan 1</t>
+  </si>
+  <si>
+    <t>R1 Vlan 1</t>
   </si>
 </sst>
 </file>
@@ -1073,46 +1085,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1133,22 +1121,46 @@
     <xf numFmtId="0" fontId="7" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -1538,9 +1550,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12CB4148-414F-422C-94F5-AFDA695DCD79}">
   <dimension ref="A1:I257"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A197" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I226" sqref="I226"/>
+      <selection pane="bottomLeft" activeCell="I214" sqref="I214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1579,7 +1591,7 @@
       <c r="C2" s="59"/>
       <c r="D2" s="59"/>
       <c r="E2" s="59"/>
-      <c r="F2" s="60" t="s">
+      <c r="F2" s="85" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="59"/>
@@ -1598,7 +1610,7 @@
       <c r="C3" s="59"/>
       <c r="D3" s="59"/>
       <c r="E3" s="59"/>
-      <c r="F3" s="60"/>
+      <c r="F3" s="85"/>
       <c r="G3" s="59"/>
       <c r="H3" s="59"/>
       <c r="I3" s="43"/>
@@ -1613,7 +1625,7 @@
       <c r="C4" s="59"/>
       <c r="D4" s="59"/>
       <c r="E4" s="59"/>
-      <c r="F4" s="60"/>
+      <c r="F4" s="85"/>
       <c r="G4" s="59"/>
       <c r="H4" s="59"/>
       <c r="I4" s="43"/>
@@ -1628,7 +1640,7 @@
       <c r="C5" s="59"/>
       <c r="D5" s="59"/>
       <c r="E5" s="59"/>
-      <c r="F5" s="60"/>
+      <c r="F5" s="85"/>
       <c r="G5" s="59"/>
       <c r="H5" s="59"/>
       <c r="I5" s="43"/>
@@ -1643,7 +1655,7 @@
       <c r="C6" s="59"/>
       <c r="D6" s="59"/>
       <c r="E6" s="59"/>
-      <c r="F6" s="60"/>
+      <c r="F6" s="85"/>
       <c r="G6" s="59"/>
       <c r="H6" s="59"/>
       <c r="I6" s="43"/>
@@ -1658,7 +1670,7 @@
       <c r="C7" s="59"/>
       <c r="D7" s="59"/>
       <c r="E7" s="59"/>
-      <c r="F7" s="60"/>
+      <c r="F7" s="85"/>
       <c r="G7" s="59"/>
       <c r="H7" s="59"/>
       <c r="I7" s="43"/>
@@ -1673,7 +1685,7 @@
       <c r="C8" s="59"/>
       <c r="D8" s="59"/>
       <c r="E8" s="59"/>
-      <c r="F8" s="60"/>
+      <c r="F8" s="85"/>
       <c r="G8" s="59"/>
       <c r="H8" s="59"/>
       <c r="I8" s="43"/>
@@ -1688,7 +1700,7 @@
       <c r="C9" s="59"/>
       <c r="D9" s="59"/>
       <c r="E9" s="59"/>
-      <c r="F9" s="60"/>
+      <c r="F9" s="85"/>
       <c r="G9" s="59"/>
       <c r="H9" s="59"/>
       <c r="I9" s="43"/>
@@ -1703,7 +1715,7 @@
       <c r="C10" s="59"/>
       <c r="D10" s="59"/>
       <c r="E10" s="59"/>
-      <c r="F10" s="60"/>
+      <c r="F10" s="85"/>
       <c r="G10" s="59"/>
       <c r="H10" s="59"/>
       <c r="I10" s="43"/>
@@ -1718,7 +1730,7 @@
       <c r="C11" s="59"/>
       <c r="D11" s="59"/>
       <c r="E11" s="59"/>
-      <c r="F11" s="60"/>
+      <c r="F11" s="85"/>
       <c r="G11" s="59"/>
       <c r="H11" s="59"/>
       <c r="I11" s="54"/>
@@ -1733,7 +1745,7 @@
       <c r="C12" s="59"/>
       <c r="D12" s="59"/>
       <c r="E12" s="59"/>
-      <c r="F12" s="60"/>
+      <c r="F12" s="85"/>
       <c r="G12" s="59"/>
       <c r="H12" s="59"/>
       <c r="I12" s="43"/>
@@ -1748,7 +1760,7 @@
       <c r="C13" s="59"/>
       <c r="D13" s="59"/>
       <c r="E13" s="59"/>
-      <c r="F13" s="60"/>
+      <c r="F13" s="85"/>
       <c r="G13" s="59"/>
       <c r="H13" s="59"/>
       <c r="I13" s="43"/>
@@ -1763,7 +1775,7 @@
       <c r="C14" s="59"/>
       <c r="D14" s="59"/>
       <c r="E14" s="59"/>
-      <c r="F14" s="60"/>
+      <c r="F14" s="85"/>
       <c r="G14" s="59"/>
       <c r="H14" s="59"/>
       <c r="I14" s="43"/>
@@ -1778,7 +1790,7 @@
       <c r="C15" s="59"/>
       <c r="D15" s="59"/>
       <c r="E15" s="59"/>
-      <c r="F15" s="60"/>
+      <c r="F15" s="85"/>
       <c r="G15" s="59"/>
       <c r="H15" s="59"/>
       <c r="I15" s="43"/>
@@ -1793,7 +1805,7 @@
       <c r="C16" s="59"/>
       <c r="D16" s="59"/>
       <c r="E16" s="59"/>
-      <c r="F16" s="60"/>
+      <c r="F16" s="85"/>
       <c r="G16" s="59"/>
       <c r="H16" s="59"/>
       <c r="I16" s="43"/>
@@ -1808,7 +1820,7 @@
       <c r="C17" s="59"/>
       <c r="D17" s="59"/>
       <c r="E17" s="59"/>
-      <c r="F17" s="60"/>
+      <c r="F17" s="85"/>
       <c r="G17" s="59"/>
       <c r="H17" s="59"/>
       <c r="I17" s="43"/>
@@ -1823,7 +1835,7 @@
       <c r="C18" s="59"/>
       <c r="D18" s="59"/>
       <c r="E18" s="59"/>
-      <c r="F18" s="60"/>
+      <c r="F18" s="85"/>
       <c r="G18" s="59"/>
       <c r="H18" s="59"/>
       <c r="I18" s="43"/>
@@ -1838,7 +1850,7 @@
       <c r="C19" s="59"/>
       <c r="D19" s="59"/>
       <c r="E19" s="59"/>
-      <c r="F19" s="60"/>
+      <c r="F19" s="85"/>
       <c r="G19" s="59"/>
       <c r="H19" s="59"/>
       <c r="I19" s="43"/>
@@ -1853,7 +1865,7 @@
       <c r="C20" s="59"/>
       <c r="D20" s="59"/>
       <c r="E20" s="59"/>
-      <c r="F20" s="60"/>
+      <c r="F20" s="85"/>
       <c r="G20" s="59"/>
       <c r="H20" s="59"/>
       <c r="I20" s="54"/>
@@ -1868,7 +1880,7 @@
       <c r="C21" s="59"/>
       <c r="D21" s="59"/>
       <c r="E21" s="59"/>
-      <c r="F21" s="60"/>
+      <c r="F21" s="85"/>
       <c r="G21" s="59"/>
       <c r="H21" s="59"/>
       <c r="I21" s="43"/>
@@ -1883,7 +1895,7 @@
       <c r="C22" s="59"/>
       <c r="D22" s="59"/>
       <c r="E22" s="59"/>
-      <c r="F22" s="60"/>
+      <c r="F22" s="85"/>
       <c r="G22" s="59"/>
       <c r="H22" s="59"/>
       <c r="I22" s="43"/>
@@ -1898,7 +1910,7 @@
       <c r="C23" s="59"/>
       <c r="D23" s="59"/>
       <c r="E23" s="59"/>
-      <c r="F23" s="60"/>
+      <c r="F23" s="85"/>
       <c r="G23" s="59"/>
       <c r="H23" s="59"/>
       <c r="I23" s="43"/>
@@ -1913,7 +1925,7 @@
       <c r="C24" s="59"/>
       <c r="D24" s="59"/>
       <c r="E24" s="59"/>
-      <c r="F24" s="60"/>
+      <c r="F24" s="85"/>
       <c r="G24" s="59"/>
       <c r="H24" s="59"/>
       <c r="I24" s="43"/>
@@ -1928,7 +1940,7 @@
       <c r="C25" s="59"/>
       <c r="D25" s="59"/>
       <c r="E25" s="59"/>
-      <c r="F25" s="60"/>
+      <c r="F25" s="85"/>
       <c r="G25" s="59"/>
       <c r="H25" s="59"/>
       <c r="I25" s="43"/>
@@ -1943,7 +1955,7 @@
       <c r="C26" s="59"/>
       <c r="D26" s="59"/>
       <c r="E26" s="59"/>
-      <c r="F26" s="60"/>
+      <c r="F26" s="85"/>
       <c r="G26" s="59"/>
       <c r="H26" s="59"/>
       <c r="I26" s="43"/>
@@ -1958,7 +1970,7 @@
       <c r="C27" s="59"/>
       <c r="D27" s="59"/>
       <c r="E27" s="59"/>
-      <c r="F27" s="60"/>
+      <c r="F27" s="85"/>
       <c r="G27" s="59"/>
       <c r="H27" s="59"/>
       <c r="I27" s="43"/>
@@ -1973,7 +1985,7 @@
       <c r="C28" s="59"/>
       <c r="D28" s="59"/>
       <c r="E28" s="59"/>
-      <c r="F28" s="60"/>
+      <c r="F28" s="85"/>
       <c r="G28" s="59"/>
       <c r="H28" s="59"/>
       <c r="I28" s="43"/>
@@ -1988,7 +2000,7 @@
       <c r="C29" s="59"/>
       <c r="D29" s="59"/>
       <c r="E29" s="59"/>
-      <c r="F29" s="60"/>
+      <c r="F29" s="85"/>
       <c r="G29" s="59"/>
       <c r="H29" s="59"/>
       <c r="I29" s="54" t="s">
@@ -2005,7 +2017,7 @@
       <c r="C30" s="59"/>
       <c r="D30" s="59"/>
       <c r="E30" s="59"/>
-      <c r="F30" s="60"/>
+      <c r="F30" s="85"/>
       <c r="G30" s="59"/>
       <c r="H30" s="59"/>
       <c r="I30" s="43" t="s">
@@ -2022,7 +2034,7 @@
       <c r="C31" s="59"/>
       <c r="D31" s="59"/>
       <c r="E31" s="59"/>
-      <c r="F31" s="60"/>
+      <c r="F31" s="85"/>
       <c r="G31" s="59"/>
       <c r="H31" s="59"/>
       <c r="I31" s="43" t="s">
@@ -2039,7 +2051,7 @@
       <c r="C32" s="59"/>
       <c r="D32" s="59"/>
       <c r="E32" s="59"/>
-      <c r="F32" s="60"/>
+      <c r="F32" s="85"/>
       <c r="G32" s="59"/>
       <c r="H32" s="59"/>
       <c r="I32" s="43" t="s">
@@ -2056,7 +2068,7 @@
       <c r="C33" s="59"/>
       <c r="D33" s="59"/>
       <c r="E33" s="59"/>
-      <c r="F33" s="60"/>
+      <c r="F33" s="85"/>
       <c r="G33" s="59"/>
       <c r="H33" s="59"/>
       <c r="I33" s="43" t="s">
@@ -2072,7 +2084,7 @@
       </c>
       <c r="C34" s="59"/>
       <c r="D34" s="59"/>
-      <c r="E34" s="63" t="s">
+      <c r="E34" s="84" t="s">
         <v>16</v>
       </c>
       <c r="F34" s="59"/>
@@ -2091,7 +2103,7 @@
       </c>
       <c r="C35" s="59"/>
       <c r="D35" s="59"/>
-      <c r="E35" s="63"/>
+      <c r="E35" s="84"/>
       <c r="F35" s="59"/>
       <c r="G35" s="59"/>
       <c r="H35" s="59"/>
@@ -2106,7 +2118,7 @@
       </c>
       <c r="C36" s="59"/>
       <c r="D36" s="59"/>
-      <c r="E36" s="63"/>
+      <c r="E36" s="84"/>
       <c r="F36" s="59"/>
       <c r="G36" s="59"/>
       <c r="H36" s="59"/>
@@ -2121,7 +2133,7 @@
       </c>
       <c r="C37" s="59"/>
       <c r="D37" s="59"/>
-      <c r="E37" s="63"/>
+      <c r="E37" s="84"/>
       <c r="F37" s="59"/>
       <c r="G37" s="59"/>
       <c r="H37" s="59"/>
@@ -2136,7 +2148,7 @@
       </c>
       <c r="C38" s="59"/>
       <c r="D38" s="59"/>
-      <c r="E38" s="63"/>
+      <c r="E38" s="84"/>
       <c r="F38" s="59"/>
       <c r="G38" s="59"/>
       <c r="H38" s="59"/>
@@ -2151,7 +2163,7 @@
       </c>
       <c r="C39" s="59"/>
       <c r="D39" s="59"/>
-      <c r="E39" s="63"/>
+      <c r="E39" s="84"/>
       <c r="F39" s="59"/>
       <c r="G39" s="59"/>
       <c r="H39" s="59"/>
@@ -2166,7 +2178,7 @@
       </c>
       <c r="C40" s="59"/>
       <c r="D40" s="59"/>
-      <c r="E40" s="63"/>
+      <c r="E40" s="84"/>
       <c r="F40" s="59"/>
       <c r="G40" s="59"/>
       <c r="H40" s="59"/>
@@ -2181,7 +2193,7 @@
       </c>
       <c r="C41" s="59"/>
       <c r="D41" s="59"/>
-      <c r="E41" s="63"/>
+      <c r="E41" s="84"/>
       <c r="F41" s="59"/>
       <c r="G41" s="59"/>
       <c r="H41" s="59"/>
@@ -2196,7 +2208,7 @@
       </c>
       <c r="C42" s="59"/>
       <c r="D42" s="59"/>
-      <c r="E42" s="63"/>
+      <c r="E42" s="84"/>
       <c r="F42" s="59"/>
       <c r="G42" s="59"/>
       <c r="H42" s="59"/>
@@ -2211,7 +2223,7 @@
       </c>
       <c r="C43" s="59"/>
       <c r="D43" s="59"/>
-      <c r="E43" s="63"/>
+      <c r="E43" s="84"/>
       <c r="F43" s="59"/>
       <c r="G43" s="59"/>
       <c r="H43" s="59"/>
@@ -2226,7 +2238,7 @@
       </c>
       <c r="C44" s="59"/>
       <c r="D44" s="59"/>
-      <c r="E44" s="63"/>
+      <c r="E44" s="84"/>
       <c r="F44" s="59"/>
       <c r="G44" s="59"/>
       <c r="H44" s="59"/>
@@ -2241,7 +2253,7 @@
       </c>
       <c r="C45" s="59"/>
       <c r="D45" s="59"/>
-      <c r="E45" s="63"/>
+      <c r="E45" s="84"/>
       <c r="F45" s="59"/>
       <c r="G45" s="59"/>
       <c r="H45" s="59"/>
@@ -2256,7 +2268,7 @@
       </c>
       <c r="C46" s="59"/>
       <c r="D46" s="59"/>
-      <c r="E46" s="63"/>
+      <c r="E46" s="84"/>
       <c r="F46" s="59"/>
       <c r="G46" s="59"/>
       <c r="H46" s="59"/>
@@ -2271,7 +2283,7 @@
       </c>
       <c r="C47" s="59"/>
       <c r="D47" s="59"/>
-      <c r="E47" s="63"/>
+      <c r="E47" s="84"/>
       <c r="F47" s="59"/>
       <c r="G47" s="59"/>
       <c r="H47" s="59"/>
@@ -2286,7 +2298,7 @@
       </c>
       <c r="C48" s="59"/>
       <c r="D48" s="59"/>
-      <c r="E48" s="63"/>
+      <c r="E48" s="84"/>
       <c r="F48" s="59"/>
       <c r="G48" s="59"/>
       <c r="H48" s="59"/>
@@ -2303,7 +2315,7 @@
       </c>
       <c r="C49" s="59"/>
       <c r="D49" s="59"/>
-      <c r="E49" s="63"/>
+      <c r="E49" s="84"/>
       <c r="F49" s="59"/>
       <c r="G49" s="59"/>
       <c r="H49" s="59"/>
@@ -2320,7 +2332,7 @@
       </c>
       <c r="C50" s="59"/>
       <c r="D50" s="59"/>
-      <c r="E50" s="61" t="s">
+      <c r="E50" s="82" t="s">
         <v>17</v>
       </c>
       <c r="F50" s="59"/>
@@ -2339,7 +2351,7 @@
       </c>
       <c r="C51" s="59"/>
       <c r="D51" s="59"/>
-      <c r="E51" s="61"/>
+      <c r="E51" s="82"/>
       <c r="F51" s="59"/>
       <c r="G51" s="59"/>
       <c r="H51" s="59"/>
@@ -2354,7 +2366,7 @@
       </c>
       <c r="C52" s="59"/>
       <c r="D52" s="59"/>
-      <c r="E52" s="61"/>
+      <c r="E52" s="82"/>
       <c r="F52" s="59"/>
       <c r="G52" s="59"/>
       <c r="H52" s="59"/>
@@ -2369,7 +2381,7 @@
       </c>
       <c r="C53" s="59"/>
       <c r="D53" s="59"/>
-      <c r="E53" s="61"/>
+      <c r="E53" s="82"/>
       <c r="F53" s="59"/>
       <c r="G53" s="59"/>
       <c r="H53" s="59"/>
@@ -2384,7 +2396,7 @@
       </c>
       <c r="C54" s="59"/>
       <c r="D54" s="59"/>
-      <c r="E54" s="61"/>
+      <c r="E54" s="82"/>
       <c r="F54" s="59"/>
       <c r="G54" s="59"/>
       <c r="H54" s="59"/>
@@ -2399,7 +2411,7 @@
       </c>
       <c r="C55" s="59"/>
       <c r="D55" s="59"/>
-      <c r="E55" s="61"/>
+      <c r="E55" s="82"/>
       <c r="F55" s="59"/>
       <c r="G55" s="59"/>
       <c r="H55" s="59"/>
@@ -2414,7 +2426,7 @@
       </c>
       <c r="C56" s="59"/>
       <c r="D56" s="59"/>
-      <c r="E56" s="61"/>
+      <c r="E56" s="82"/>
       <c r="F56" s="59"/>
       <c r="G56" s="59"/>
       <c r="H56" s="59"/>
@@ -2429,7 +2441,7 @@
       </c>
       <c r="C57" s="59"/>
       <c r="D57" s="59"/>
-      <c r="E57" s="61"/>
+      <c r="E57" s="82"/>
       <c r="F57" s="59"/>
       <c r="G57" s="59"/>
       <c r="H57" s="59"/>
@@ -2444,7 +2456,7 @@
       </c>
       <c r="C58" s="59"/>
       <c r="D58" s="59"/>
-      <c r="E58" s="61"/>
+      <c r="E58" s="82"/>
       <c r="F58" s="59"/>
       <c r="G58" s="59"/>
       <c r="H58" s="59"/>
@@ -2459,7 +2471,7 @@
       </c>
       <c r="C59" s="59"/>
       <c r="D59" s="59"/>
-      <c r="E59" s="61"/>
+      <c r="E59" s="82"/>
       <c r="F59" s="59"/>
       <c r="G59" s="59"/>
       <c r="H59" s="59"/>
@@ -2474,7 +2486,7 @@
       </c>
       <c r="C60" s="59"/>
       <c r="D60" s="59"/>
-      <c r="E60" s="61"/>
+      <c r="E60" s="82"/>
       <c r="F60" s="59"/>
       <c r="G60" s="59"/>
       <c r="H60" s="59"/>
@@ -2489,7 +2501,7 @@
       </c>
       <c r="C61" s="59"/>
       <c r="D61" s="59"/>
-      <c r="E61" s="61"/>
+      <c r="E61" s="82"/>
       <c r="F61" s="59"/>
       <c r="G61" s="59"/>
       <c r="H61" s="59"/>
@@ -2504,7 +2516,7 @@
       </c>
       <c r="C62" s="59"/>
       <c r="D62" s="59"/>
-      <c r="E62" s="61"/>
+      <c r="E62" s="82"/>
       <c r="F62" s="59"/>
       <c r="G62" s="59"/>
       <c r="H62" s="59"/>
@@ -2519,7 +2531,7 @@
       </c>
       <c r="C63" s="59"/>
       <c r="D63" s="59"/>
-      <c r="E63" s="61"/>
+      <c r="E63" s="82"/>
       <c r="F63" s="59"/>
       <c r="G63" s="59"/>
       <c r="H63" s="59"/>
@@ -2534,7 +2546,7 @@
       </c>
       <c r="C64" s="59"/>
       <c r="D64" s="59"/>
-      <c r="E64" s="61"/>
+      <c r="E64" s="82"/>
       <c r="F64" s="59"/>
       <c r="G64" s="59"/>
       <c r="H64" s="59"/>
@@ -2551,7 +2563,7 @@
       </c>
       <c r="C65" s="59"/>
       <c r="D65" s="59"/>
-      <c r="E65" s="61"/>
+      <c r="E65" s="82"/>
       <c r="F65" s="59"/>
       <c r="G65" s="59"/>
       <c r="H65" s="59"/>
@@ -2568,7 +2580,7 @@
       </c>
       <c r="C66" s="59"/>
       <c r="D66" s="59"/>
-      <c r="E66" s="62" t="s">
+      <c r="E66" s="83" t="s">
         <v>18</v>
       </c>
       <c r="F66" s="59"/>
@@ -2587,7 +2599,7 @@
       </c>
       <c r="C67" s="59"/>
       <c r="D67" s="59"/>
-      <c r="E67" s="62"/>
+      <c r="E67" s="83"/>
       <c r="F67" s="59"/>
       <c r="G67" s="59"/>
       <c r="H67" s="59"/>
@@ -2602,7 +2614,7 @@
       </c>
       <c r="C68" s="59"/>
       <c r="D68" s="59"/>
-      <c r="E68" s="62"/>
+      <c r="E68" s="83"/>
       <c r="F68" s="59"/>
       <c r="G68" s="59"/>
       <c r="H68" s="59"/>
@@ -2617,7 +2629,7 @@
       </c>
       <c r="C69" s="59"/>
       <c r="D69" s="59"/>
-      <c r="E69" s="62"/>
+      <c r="E69" s="83"/>
       <c r="F69" s="59"/>
       <c r="G69" s="59"/>
       <c r="H69" s="59"/>
@@ -2632,7 +2644,7 @@
       </c>
       <c r="C70" s="59"/>
       <c r="D70" s="59"/>
-      <c r="E70" s="62"/>
+      <c r="E70" s="83"/>
       <c r="F70" s="59"/>
       <c r="G70" s="59"/>
       <c r="H70" s="59"/>
@@ -2647,7 +2659,7 @@
       </c>
       <c r="C71" s="59"/>
       <c r="D71" s="59"/>
-      <c r="E71" s="62"/>
+      <c r="E71" s="83"/>
       <c r="F71" s="59"/>
       <c r="G71" s="59"/>
       <c r="H71" s="59"/>
@@ -2662,7 +2674,7 @@
       </c>
       <c r="C72" s="59"/>
       <c r="D72" s="59"/>
-      <c r="E72" s="62"/>
+      <c r="E72" s="83"/>
       <c r="F72" s="59"/>
       <c r="G72" s="59"/>
       <c r="H72" s="59"/>
@@ -2677,7 +2689,7 @@
       </c>
       <c r="C73" s="59"/>
       <c r="D73" s="59"/>
-      <c r="E73" s="62"/>
+      <c r="E73" s="83"/>
       <c r="F73" s="59"/>
       <c r="G73" s="59"/>
       <c r="H73" s="59"/>
@@ -2692,7 +2704,7 @@
       </c>
       <c r="C74" s="59"/>
       <c r="D74" s="59"/>
-      <c r="E74" s="62"/>
+      <c r="E74" s="83"/>
       <c r="F74" s="59"/>
       <c r="G74" s="59"/>
       <c r="H74" s="59"/>
@@ -2707,7 +2719,7 @@
       </c>
       <c r="C75" s="59"/>
       <c r="D75" s="59"/>
-      <c r="E75" s="62"/>
+      <c r="E75" s="83"/>
       <c r="F75" s="59"/>
       <c r="G75" s="59"/>
       <c r="H75" s="59"/>
@@ -2722,7 +2734,7 @@
       </c>
       <c r="C76" s="59"/>
       <c r="D76" s="59"/>
-      <c r="E76" s="62"/>
+      <c r="E76" s="83"/>
       <c r="F76" s="59"/>
       <c r="G76" s="59"/>
       <c r="H76" s="59"/>
@@ -2737,7 +2749,7 @@
       </c>
       <c r="C77" s="59"/>
       <c r="D77" s="59"/>
-      <c r="E77" s="62"/>
+      <c r="E77" s="83"/>
       <c r="F77" s="59"/>
       <c r="G77" s="59"/>
       <c r="H77" s="59"/>
@@ -2752,7 +2764,7 @@
       </c>
       <c r="C78" s="59"/>
       <c r="D78" s="59"/>
-      <c r="E78" s="62"/>
+      <c r="E78" s="83"/>
       <c r="F78" s="59"/>
       <c r="G78" s="59"/>
       <c r="H78" s="59"/>
@@ -2767,7 +2779,7 @@
       </c>
       <c r="C79" s="59"/>
       <c r="D79" s="59"/>
-      <c r="E79" s="62"/>
+      <c r="E79" s="83"/>
       <c r="F79" s="59"/>
       <c r="G79" s="59"/>
       <c r="H79" s="59"/>
@@ -2782,7 +2794,7 @@
       </c>
       <c r="C80" s="59"/>
       <c r="D80" s="59"/>
-      <c r="E80" s="62"/>
+      <c r="E80" s="83"/>
       <c r="F80" s="59"/>
       <c r="G80" s="59"/>
       <c r="H80" s="59"/>
@@ -2799,7 +2811,7 @@
       </c>
       <c r="C81" s="59"/>
       <c r="D81" s="59"/>
-      <c r="E81" s="62"/>
+      <c r="E81" s="83"/>
       <c r="F81" s="59"/>
       <c r="G81" s="59"/>
       <c r="H81" s="59"/>
@@ -2816,7 +2828,7 @@
       </c>
       <c r="C82" s="59"/>
       <c r="D82" s="59"/>
-      <c r="E82" s="65" t="s">
+      <c r="E82" s="81" t="s">
         <v>19</v>
       </c>
       <c r="F82" s="59"/>
@@ -2835,7 +2847,7 @@
       </c>
       <c r="C83" s="59"/>
       <c r="D83" s="59"/>
-      <c r="E83" s="65"/>
+      <c r="E83" s="81"/>
       <c r="F83" s="59"/>
       <c r="G83" s="59"/>
       <c r="H83" s="59"/>
@@ -2850,7 +2862,7 @@
       </c>
       <c r="C84" s="59"/>
       <c r="D84" s="59"/>
-      <c r="E84" s="65"/>
+      <c r="E84" s="81"/>
       <c r="F84" s="59"/>
       <c r="G84" s="59"/>
       <c r="H84" s="59"/>
@@ -2865,7 +2877,7 @@
       </c>
       <c r="C85" s="59"/>
       <c r="D85" s="59"/>
-      <c r="E85" s="65"/>
+      <c r="E85" s="81"/>
       <c r="F85" s="59"/>
       <c r="G85" s="59"/>
       <c r="H85" s="59"/>
@@ -2880,7 +2892,7 @@
       </c>
       <c r="C86" s="59"/>
       <c r="D86" s="59"/>
-      <c r="E86" s="65"/>
+      <c r="E86" s="81"/>
       <c r="F86" s="59"/>
       <c r="G86" s="59"/>
       <c r="H86" s="59"/>
@@ -2895,7 +2907,7 @@
       </c>
       <c r="C87" s="59"/>
       <c r="D87" s="59"/>
-      <c r="E87" s="65"/>
+      <c r="E87" s="81"/>
       <c r="F87" s="59"/>
       <c r="G87" s="59"/>
       <c r="H87" s="59"/>
@@ -2910,7 +2922,7 @@
       </c>
       <c r="C88" s="59"/>
       <c r="D88" s="59"/>
-      <c r="E88" s="65"/>
+      <c r="E88" s="81"/>
       <c r="F88" s="59"/>
       <c r="G88" s="59"/>
       <c r="H88" s="59"/>
@@ -2925,7 +2937,7 @@
       </c>
       <c r="C89" s="59"/>
       <c r="D89" s="59"/>
-      <c r="E89" s="65"/>
+      <c r="E89" s="81"/>
       <c r="F89" s="59"/>
       <c r="G89" s="59"/>
       <c r="H89" s="59"/>
@@ -2940,7 +2952,7 @@
       </c>
       <c r="C90" s="59"/>
       <c r="D90" s="59"/>
-      <c r="E90" s="65"/>
+      <c r="E90" s="81"/>
       <c r="F90" s="59"/>
       <c r="G90" s="59"/>
       <c r="H90" s="59"/>
@@ -2955,7 +2967,7 @@
       </c>
       <c r="C91" s="59"/>
       <c r="D91" s="59"/>
-      <c r="E91" s="65"/>
+      <c r="E91" s="81"/>
       <c r="F91" s="59"/>
       <c r="G91" s="59"/>
       <c r="H91" s="59"/>
@@ -2970,7 +2982,7 @@
       </c>
       <c r="C92" s="59"/>
       <c r="D92" s="59"/>
-      <c r="E92" s="65"/>
+      <c r="E92" s="81"/>
       <c r="F92" s="59"/>
       <c r="G92" s="59"/>
       <c r="H92" s="59"/>
@@ -2985,7 +2997,7 @@
       </c>
       <c r="C93" s="59"/>
       <c r="D93" s="59"/>
-      <c r="E93" s="65"/>
+      <c r="E93" s="81"/>
       <c r="F93" s="59"/>
       <c r="G93" s="59"/>
       <c r="H93" s="59"/>
@@ -3000,7 +3012,7 @@
       </c>
       <c r="C94" s="59"/>
       <c r="D94" s="59"/>
-      <c r="E94" s="65"/>
+      <c r="E94" s="81"/>
       <c r="F94" s="59"/>
       <c r="G94" s="59"/>
       <c r="H94" s="59"/>
@@ -3015,7 +3027,7 @@
       </c>
       <c r="C95" s="59"/>
       <c r="D95" s="59"/>
-      <c r="E95" s="65"/>
+      <c r="E95" s="81"/>
       <c r="F95" s="59"/>
       <c r="G95" s="59"/>
       <c r="H95" s="59"/>
@@ -3030,7 +3042,7 @@
       </c>
       <c r="C96" s="59"/>
       <c r="D96" s="59"/>
-      <c r="E96" s="65"/>
+      <c r="E96" s="81"/>
       <c r="F96" s="59"/>
       <c r="G96" s="59"/>
       <c r="H96" s="59"/>
@@ -3047,7 +3059,7 @@
       </c>
       <c r="C97" s="59"/>
       <c r="D97" s="59"/>
-      <c r="E97" s="65"/>
+      <c r="E97" s="81"/>
       <c r="F97" s="59"/>
       <c r="G97" s="59"/>
       <c r="H97" s="59"/>
@@ -3064,7 +3076,7 @@
       </c>
       <c r="C98" s="59"/>
       <c r="D98" s="59"/>
-      <c r="E98" s="64" t="s">
+      <c r="E98" s="80" t="s">
         <v>20</v>
       </c>
       <c r="F98" s="59"/>
@@ -3083,7 +3095,7 @@
       </c>
       <c r="C99" s="59"/>
       <c r="D99" s="59"/>
-      <c r="E99" s="64"/>
+      <c r="E99" s="80"/>
       <c r="F99" s="59"/>
       <c r="G99" s="59"/>
       <c r="H99" s="59"/>
@@ -3098,7 +3110,7 @@
       </c>
       <c r="C100" s="59"/>
       <c r="D100" s="59"/>
-      <c r="E100" s="64"/>
+      <c r="E100" s="80"/>
       <c r="F100" s="59"/>
       <c r="G100" s="59"/>
       <c r="H100" s="59"/>
@@ -3113,7 +3125,7 @@
       </c>
       <c r="C101" s="59"/>
       <c r="D101" s="59"/>
-      <c r="E101" s="64"/>
+      <c r="E101" s="80"/>
       <c r="F101" s="59"/>
       <c r="G101" s="59"/>
       <c r="H101" s="59"/>
@@ -3128,7 +3140,7 @@
       </c>
       <c r="C102" s="59"/>
       <c r="D102" s="59"/>
-      <c r="E102" s="64"/>
+      <c r="E102" s="80"/>
       <c r="F102" s="59"/>
       <c r="G102" s="59"/>
       <c r="H102" s="59"/>
@@ -3143,7 +3155,7 @@
       </c>
       <c r="C103" s="59"/>
       <c r="D103" s="59"/>
-      <c r="E103" s="64"/>
+      <c r="E103" s="80"/>
       <c r="F103" s="59"/>
       <c r="G103" s="59"/>
       <c r="H103" s="59"/>
@@ -3158,7 +3170,7 @@
       </c>
       <c r="C104" s="59"/>
       <c r="D104" s="59"/>
-      <c r="E104" s="64"/>
+      <c r="E104" s="80"/>
       <c r="F104" s="59"/>
       <c r="G104" s="59"/>
       <c r="H104" s="59"/>
@@ -3173,7 +3185,7 @@
       </c>
       <c r="C105" s="59"/>
       <c r="D105" s="59"/>
-      <c r="E105" s="64"/>
+      <c r="E105" s="80"/>
       <c r="F105" s="59"/>
       <c r="G105" s="59"/>
       <c r="H105" s="59"/>
@@ -3188,7 +3200,7 @@
       </c>
       <c r="C106" s="59"/>
       <c r="D106" s="59"/>
-      <c r="E106" s="64"/>
+      <c r="E106" s="80"/>
       <c r="F106" s="59"/>
       <c r="G106" s="59"/>
       <c r="H106" s="59"/>
@@ -3203,7 +3215,7 @@
       </c>
       <c r="C107" s="59"/>
       <c r="D107" s="59"/>
-      <c r="E107" s="64"/>
+      <c r="E107" s="80"/>
       <c r="F107" s="59"/>
       <c r="G107" s="59"/>
       <c r="H107" s="59"/>
@@ -3218,7 +3230,7 @@
       </c>
       <c r="C108" s="59"/>
       <c r="D108" s="59"/>
-      <c r="E108" s="64"/>
+      <c r="E108" s="80"/>
       <c r="F108" s="59"/>
       <c r="G108" s="59"/>
       <c r="H108" s="59"/>
@@ -3233,7 +3245,7 @@
       </c>
       <c r="C109" s="59"/>
       <c r="D109" s="59"/>
-      <c r="E109" s="64"/>
+      <c r="E109" s="80"/>
       <c r="F109" s="59"/>
       <c r="G109" s="59"/>
       <c r="H109" s="59"/>
@@ -3248,7 +3260,7 @@
       </c>
       <c r="C110" s="59"/>
       <c r="D110" s="59"/>
-      <c r="E110" s="64"/>
+      <c r="E110" s="80"/>
       <c r="F110" s="59"/>
       <c r="G110" s="59"/>
       <c r="H110" s="59"/>
@@ -3263,7 +3275,7 @@
       </c>
       <c r="C111" s="59"/>
       <c r="D111" s="59"/>
-      <c r="E111" s="64"/>
+      <c r="E111" s="80"/>
       <c r="F111" s="59"/>
       <c r="G111" s="59"/>
       <c r="H111" s="59"/>
@@ -3278,7 +3290,7 @@
       </c>
       <c r="C112" s="59"/>
       <c r="D112" s="59"/>
-      <c r="E112" s="64"/>
+      <c r="E112" s="80"/>
       <c r="F112" s="59"/>
       <c r="G112" s="59"/>
       <c r="H112" s="59"/>
@@ -3295,7 +3307,7 @@
       </c>
       <c r="C113" s="59"/>
       <c r="D113" s="59"/>
-      <c r="E113" s="64"/>
+      <c r="E113" s="80"/>
       <c r="F113" s="59"/>
       <c r="G113" s="59"/>
       <c r="H113" s="59"/>
@@ -3312,7 +3324,7 @@
       </c>
       <c r="C114" s="59"/>
       <c r="D114" s="59"/>
-      <c r="E114" s="69" t="s">
+      <c r="E114" s="79" t="s">
         <v>21</v>
       </c>
       <c r="F114" s="59"/>
@@ -3331,7 +3343,7 @@
       </c>
       <c r="C115" s="59"/>
       <c r="D115" s="59"/>
-      <c r="E115" s="69"/>
+      <c r="E115" s="79"/>
       <c r="F115" s="59"/>
       <c r="G115" s="59"/>
       <c r="H115" s="59"/>
@@ -3346,7 +3358,7 @@
       </c>
       <c r="C116" s="59"/>
       <c r="D116" s="59"/>
-      <c r="E116" s="69"/>
+      <c r="E116" s="79"/>
       <c r="F116" s="59"/>
       <c r="G116" s="59"/>
       <c r="H116" s="59"/>
@@ -3361,7 +3373,7 @@
       </c>
       <c r="C117" s="59"/>
       <c r="D117" s="59"/>
-      <c r="E117" s="69"/>
+      <c r="E117" s="79"/>
       <c r="F117" s="59"/>
       <c r="G117" s="59"/>
       <c r="H117" s="59"/>
@@ -3376,7 +3388,7 @@
       </c>
       <c r="C118" s="59"/>
       <c r="D118" s="59"/>
-      <c r="E118" s="69"/>
+      <c r="E118" s="79"/>
       <c r="F118" s="59"/>
       <c r="G118" s="59"/>
       <c r="H118" s="59"/>
@@ -3391,7 +3403,7 @@
       </c>
       <c r="C119" s="59"/>
       <c r="D119" s="59"/>
-      <c r="E119" s="69"/>
+      <c r="E119" s="79"/>
       <c r="F119" s="59"/>
       <c r="G119" s="59"/>
       <c r="H119" s="59"/>
@@ -3406,7 +3418,7 @@
       </c>
       <c r="C120" s="59"/>
       <c r="D120" s="59"/>
-      <c r="E120" s="69"/>
+      <c r="E120" s="79"/>
       <c r="F120" s="59"/>
       <c r="G120" s="59"/>
       <c r="H120" s="59"/>
@@ -3421,7 +3433,7 @@
       </c>
       <c r="C121" s="59"/>
       <c r="D121" s="59"/>
-      <c r="E121" s="69"/>
+      <c r="E121" s="79"/>
       <c r="F121" s="59"/>
       <c r="G121" s="59"/>
       <c r="H121" s="59"/>
@@ -3436,7 +3448,7 @@
       </c>
       <c r="C122" s="59"/>
       <c r="D122" s="59"/>
-      <c r="E122" s="69"/>
+      <c r="E122" s="79"/>
       <c r="F122" s="59"/>
       <c r="G122" s="59"/>
       <c r="H122" s="59"/>
@@ -3451,7 +3463,7 @@
       </c>
       <c r="C123" s="59"/>
       <c r="D123" s="59"/>
-      <c r="E123" s="69"/>
+      <c r="E123" s="79"/>
       <c r="F123" s="59"/>
       <c r="G123" s="59"/>
       <c r="H123" s="59"/>
@@ -3466,7 +3478,7 @@
       </c>
       <c r="C124" s="59"/>
       <c r="D124" s="59"/>
-      <c r="E124" s="69"/>
+      <c r="E124" s="79"/>
       <c r="F124" s="59"/>
       <c r="G124" s="59"/>
       <c r="H124" s="59"/>
@@ -3481,7 +3493,7 @@
       </c>
       <c r="C125" s="59"/>
       <c r="D125" s="59"/>
-      <c r="E125" s="69"/>
+      <c r="E125" s="79"/>
       <c r="F125" s="59"/>
       <c r="G125" s="59"/>
       <c r="H125" s="59"/>
@@ -3496,7 +3508,7 @@
       </c>
       <c r="C126" s="59"/>
       <c r="D126" s="59"/>
-      <c r="E126" s="69"/>
+      <c r="E126" s="79"/>
       <c r="F126" s="59"/>
       <c r="G126" s="59"/>
       <c r="H126" s="59"/>
@@ -3511,7 +3523,7 @@
       </c>
       <c r="C127" s="59"/>
       <c r="D127" s="59"/>
-      <c r="E127" s="69"/>
+      <c r="E127" s="79"/>
       <c r="F127" s="59"/>
       <c r="G127" s="59"/>
       <c r="H127" s="59"/>
@@ -3526,7 +3538,7 @@
       </c>
       <c r="C128" s="59"/>
       <c r="D128" s="59"/>
-      <c r="E128" s="69"/>
+      <c r="E128" s="79"/>
       <c r="F128" s="59"/>
       <c r="G128" s="59"/>
       <c r="H128" s="59"/>
@@ -3543,7 +3555,7 @@
       </c>
       <c r="C129" s="59"/>
       <c r="D129" s="59"/>
-      <c r="E129" s="69"/>
+      <c r="E129" s="79"/>
       <c r="F129" s="59"/>
       <c r="G129" s="59"/>
       <c r="H129" s="59"/>
@@ -3560,7 +3572,7 @@
       </c>
       <c r="C130" s="59"/>
       <c r="D130" s="59"/>
-      <c r="E130" s="66" t="s">
+      <c r="E130" s="72" t="s">
         <v>22</v>
       </c>
       <c r="F130" s="59"/>
@@ -3579,7 +3591,7 @@
       </c>
       <c r="C131" s="59"/>
       <c r="D131" s="59"/>
-      <c r="E131" s="67"/>
+      <c r="E131" s="73"/>
       <c r="F131" s="59"/>
       <c r="G131" s="59"/>
       <c r="H131" s="59"/>
@@ -3594,7 +3606,7 @@
       </c>
       <c r="C132" s="59"/>
       <c r="D132" s="59"/>
-      <c r="E132" s="67"/>
+      <c r="E132" s="73"/>
       <c r="F132" s="59"/>
       <c r="G132" s="59"/>
       <c r="H132" s="59"/>
@@ -3609,7 +3621,7 @@
       </c>
       <c r="C133" s="59"/>
       <c r="D133" s="59"/>
-      <c r="E133" s="67"/>
+      <c r="E133" s="73"/>
       <c r="F133" s="59"/>
       <c r="G133" s="59"/>
       <c r="H133" s="59"/>
@@ -3624,7 +3636,7 @@
       </c>
       <c r="C134" s="59"/>
       <c r="D134" s="59"/>
-      <c r="E134" s="67"/>
+      <c r="E134" s="73"/>
       <c r="F134" s="59"/>
       <c r="G134" s="59"/>
       <c r="H134" s="59"/>
@@ -3639,7 +3651,7 @@
       </c>
       <c r="C135" s="59"/>
       <c r="D135" s="59"/>
-      <c r="E135" s="67"/>
+      <c r="E135" s="73"/>
       <c r="F135" s="59"/>
       <c r="G135" s="59"/>
       <c r="H135" s="59"/>
@@ -3654,7 +3666,7 @@
       </c>
       <c r="C136" s="59"/>
       <c r="D136" s="59"/>
-      <c r="E136" s="67"/>
+      <c r="E136" s="73"/>
       <c r="F136" s="59"/>
       <c r="G136" s="59"/>
       <c r="H136" s="59"/>
@@ -3669,7 +3681,7 @@
       </c>
       <c r="C137" s="59"/>
       <c r="D137" s="59"/>
-      <c r="E137" s="67"/>
+      <c r="E137" s="73"/>
       <c r="F137" s="59"/>
       <c r="G137" s="59"/>
       <c r="H137" s="59"/>
@@ -3684,7 +3696,7 @@
       </c>
       <c r="C138" s="59"/>
       <c r="D138" s="59"/>
-      <c r="E138" s="67"/>
+      <c r="E138" s="73"/>
       <c r="F138" s="59"/>
       <c r="G138" s="59"/>
       <c r="H138" s="59"/>
@@ -3699,7 +3711,7 @@
       </c>
       <c r="C139" s="59"/>
       <c r="D139" s="59"/>
-      <c r="E139" s="67"/>
+      <c r="E139" s="73"/>
       <c r="F139" s="59"/>
       <c r="G139" s="59"/>
       <c r="H139" s="59"/>
@@ -3714,7 +3726,7 @@
       </c>
       <c r="C140" s="59"/>
       <c r="D140" s="59"/>
-      <c r="E140" s="67"/>
+      <c r="E140" s="73"/>
       <c r="F140" s="59"/>
       <c r="G140" s="59"/>
       <c r="H140" s="59"/>
@@ -3729,7 +3741,7 @@
       </c>
       <c r="C141" s="59"/>
       <c r="D141" s="59"/>
-      <c r="E141" s="67"/>
+      <c r="E141" s="73"/>
       <c r="F141" s="59"/>
       <c r="G141" s="59"/>
       <c r="H141" s="59"/>
@@ -3744,7 +3756,7 @@
       </c>
       <c r="C142" s="59"/>
       <c r="D142" s="59"/>
-      <c r="E142" s="67"/>
+      <c r="E142" s="73"/>
       <c r="F142" s="59"/>
       <c r="G142" s="59"/>
       <c r="H142" s="59"/>
@@ -3759,7 +3771,7 @@
       </c>
       <c r="C143" s="59"/>
       <c r="D143" s="59"/>
-      <c r="E143" s="67"/>
+      <c r="E143" s="73"/>
       <c r="F143" s="59"/>
       <c r="G143" s="59"/>
       <c r="H143" s="59"/>
@@ -3774,7 +3786,7 @@
       </c>
       <c r="C144" s="59"/>
       <c r="D144" s="59"/>
-      <c r="E144" s="67"/>
+      <c r="E144" s="73"/>
       <c r="F144" s="59"/>
       <c r="G144" s="59"/>
       <c r="H144" s="59"/>
@@ -3791,7 +3803,7 @@
       </c>
       <c r="C145" s="59"/>
       <c r="D145" s="59"/>
-      <c r="E145" s="68"/>
+      <c r="E145" s="74"/>
       <c r="F145" s="59"/>
       <c r="G145" s="59"/>
       <c r="H145" s="59"/>
@@ -3808,7 +3820,7 @@
       </c>
       <c r="C146" s="59"/>
       <c r="D146" s="59"/>
-      <c r="E146" s="66" t="s">
+      <c r="E146" s="72" t="s">
         <v>23</v>
       </c>
       <c r="F146" s="59"/>
@@ -3827,7 +3839,7 @@
       </c>
       <c r="C147" s="59"/>
       <c r="D147" s="59"/>
-      <c r="E147" s="67"/>
+      <c r="E147" s="73"/>
       <c r="F147" s="59"/>
       <c r="G147" s="59"/>
       <c r="H147" s="59"/>
@@ -3842,7 +3854,7 @@
       </c>
       <c r="C148" s="59"/>
       <c r="D148" s="59"/>
-      <c r="E148" s="67"/>
+      <c r="E148" s="73"/>
       <c r="F148" s="59"/>
       <c r="G148" s="59"/>
       <c r="H148" s="59"/>
@@ -3857,7 +3869,7 @@
       </c>
       <c r="C149" s="59"/>
       <c r="D149" s="59"/>
-      <c r="E149" s="67"/>
+      <c r="E149" s="73"/>
       <c r="F149" s="59"/>
       <c r="G149" s="59"/>
       <c r="H149" s="59"/>
@@ -3872,7 +3884,7 @@
       </c>
       <c r="C150" s="59"/>
       <c r="D150" s="59"/>
-      <c r="E150" s="67"/>
+      <c r="E150" s="73"/>
       <c r="F150" s="59"/>
       <c r="G150" s="59"/>
       <c r="H150" s="59"/>
@@ -3887,7 +3899,7 @@
       </c>
       <c r="C151" s="59"/>
       <c r="D151" s="59"/>
-      <c r="E151" s="67"/>
+      <c r="E151" s="73"/>
       <c r="F151" s="59"/>
       <c r="G151" s="59"/>
       <c r="H151" s="59"/>
@@ -3902,7 +3914,7 @@
       </c>
       <c r="C152" s="59"/>
       <c r="D152" s="59"/>
-      <c r="E152" s="67"/>
+      <c r="E152" s="73"/>
       <c r="F152" s="59"/>
       <c r="G152" s="59"/>
       <c r="H152" s="59"/>
@@ -3917,7 +3929,7 @@
       </c>
       <c r="C153" s="59"/>
       <c r="D153" s="59"/>
-      <c r="E153" s="67"/>
+      <c r="E153" s="73"/>
       <c r="F153" s="59"/>
       <c r="G153" s="59"/>
       <c r="H153" s="59"/>
@@ -3932,7 +3944,7 @@
       </c>
       <c r="C154" s="59"/>
       <c r="D154" s="59"/>
-      <c r="E154" s="67"/>
+      <c r="E154" s="73"/>
       <c r="F154" s="59"/>
       <c r="G154" s="59"/>
       <c r="H154" s="59"/>
@@ -3947,7 +3959,7 @@
       </c>
       <c r="C155" s="59"/>
       <c r="D155" s="59"/>
-      <c r="E155" s="67"/>
+      <c r="E155" s="73"/>
       <c r="F155" s="59"/>
       <c r="G155" s="59"/>
       <c r="H155" s="59"/>
@@ -3962,7 +3974,7 @@
       </c>
       <c r="C156" s="59"/>
       <c r="D156" s="59"/>
-      <c r="E156" s="67"/>
+      <c r="E156" s="73"/>
       <c r="F156" s="59"/>
       <c r="G156" s="59"/>
       <c r="H156" s="59"/>
@@ -3977,7 +3989,7 @@
       </c>
       <c r="C157" s="59"/>
       <c r="D157" s="59"/>
-      <c r="E157" s="67"/>
+      <c r="E157" s="73"/>
       <c r="F157" s="59"/>
       <c r="G157" s="59"/>
       <c r="H157" s="59"/>
@@ -3992,7 +4004,7 @@
       </c>
       <c r="C158" s="59"/>
       <c r="D158" s="59"/>
-      <c r="E158" s="67"/>
+      <c r="E158" s="73"/>
       <c r="F158" s="59"/>
       <c r="G158" s="59"/>
       <c r="H158" s="59"/>
@@ -4007,7 +4019,7 @@
       </c>
       <c r="C159" s="59"/>
       <c r="D159" s="59"/>
-      <c r="E159" s="67"/>
+      <c r="E159" s="73"/>
       <c r="F159" s="59"/>
       <c r="G159" s="59"/>
       <c r="H159" s="59"/>
@@ -4022,7 +4034,7 @@
       </c>
       <c r="C160" s="59"/>
       <c r="D160" s="59"/>
-      <c r="E160" s="67"/>
+      <c r="E160" s="73"/>
       <c r="F160" s="59"/>
       <c r="G160" s="59"/>
       <c r="H160" s="59"/>
@@ -4039,7 +4051,7 @@
       </c>
       <c r="C161" s="59"/>
       <c r="D161" s="59"/>
-      <c r="E161" s="68"/>
+      <c r="E161" s="74"/>
       <c r="F161" s="59"/>
       <c r="G161" s="59"/>
       <c r="H161" s="59"/>
@@ -4056,7 +4068,7 @@
       </c>
       <c r="C162" s="59"/>
       <c r="D162" s="59"/>
-      <c r="E162" s="74" t="s">
+      <c r="E162" s="66" t="s">
         <v>26</v>
       </c>
       <c r="F162" s="59"/>
@@ -4075,7 +4087,7 @@
       </c>
       <c r="C163" s="59"/>
       <c r="D163" s="59"/>
-      <c r="E163" s="75"/>
+      <c r="E163" s="67"/>
       <c r="F163" s="59"/>
       <c r="G163" s="59"/>
       <c r="H163" s="59"/>
@@ -4090,7 +4102,7 @@
       </c>
       <c r="C164" s="59"/>
       <c r="D164" s="59"/>
-      <c r="E164" s="75"/>
+      <c r="E164" s="67"/>
       <c r="F164" s="59"/>
       <c r="G164" s="59"/>
       <c r="H164" s="59"/>
@@ -4105,7 +4117,7 @@
       </c>
       <c r="C165" s="59"/>
       <c r="D165" s="59"/>
-      <c r="E165" s="75"/>
+      <c r="E165" s="67"/>
       <c r="F165" s="59"/>
       <c r="G165" s="59"/>
       <c r="H165" s="59"/>
@@ -4120,7 +4132,7 @@
       </c>
       <c r="C166" s="59"/>
       <c r="D166" s="59"/>
-      <c r="E166" s="75"/>
+      <c r="E166" s="67"/>
       <c r="F166" s="59"/>
       <c r="G166" s="59"/>
       <c r="H166" s="59"/>
@@ -4135,7 +4147,7 @@
       </c>
       <c r="C167" s="59"/>
       <c r="D167" s="59"/>
-      <c r="E167" s="75"/>
+      <c r="E167" s="67"/>
       <c r="F167" s="59"/>
       <c r="G167" s="59"/>
       <c r="H167" s="59"/>
@@ -4150,7 +4162,7 @@
       </c>
       <c r="C168" s="59"/>
       <c r="D168" s="59"/>
-      <c r="E168" s="75"/>
+      <c r="E168" s="67"/>
       <c r="F168" s="59"/>
       <c r="G168" s="59"/>
       <c r="H168" s="59"/>
@@ -4165,7 +4177,7 @@
       </c>
       <c r="C169" s="59"/>
       <c r="D169" s="59"/>
-      <c r="E169" s="75"/>
+      <c r="E169" s="67"/>
       <c r="F169" s="59"/>
       <c r="G169" s="59"/>
       <c r="H169" s="59"/>
@@ -4180,7 +4192,7 @@
       </c>
       <c r="C170" s="59"/>
       <c r="D170" s="59"/>
-      <c r="E170" s="75"/>
+      <c r="E170" s="67"/>
       <c r="F170" s="59"/>
       <c r="G170" s="59"/>
       <c r="H170" s="59"/>
@@ -4195,7 +4207,7 @@
       </c>
       <c r="C171" s="59"/>
       <c r="D171" s="59"/>
-      <c r="E171" s="75"/>
+      <c r="E171" s="67"/>
       <c r="F171" s="59"/>
       <c r="G171" s="59"/>
       <c r="H171" s="59"/>
@@ -4210,7 +4222,7 @@
       </c>
       <c r="C172" s="59"/>
       <c r="D172" s="59"/>
-      <c r="E172" s="75"/>
+      <c r="E172" s="67"/>
       <c r="F172" s="59"/>
       <c r="G172" s="59"/>
       <c r="H172" s="59"/>
@@ -4225,7 +4237,7 @@
       </c>
       <c r="C173" s="59"/>
       <c r="D173" s="59"/>
-      <c r="E173" s="75"/>
+      <c r="E173" s="67"/>
       <c r="F173" s="59"/>
       <c r="G173" s="59"/>
       <c r="H173" s="59"/>
@@ -4240,7 +4252,7 @@
       </c>
       <c r="C174" s="59"/>
       <c r="D174" s="59"/>
-      <c r="E174" s="75"/>
+      <c r="E174" s="67"/>
       <c r="F174" s="59"/>
       <c r="G174" s="59"/>
       <c r="H174" s="59"/>
@@ -4255,7 +4267,7 @@
       </c>
       <c r="C175" s="59"/>
       <c r="D175" s="59"/>
-      <c r="E175" s="75"/>
+      <c r="E175" s="67"/>
       <c r="F175" s="59"/>
       <c r="G175" s="59"/>
       <c r="H175" s="59"/>
@@ -4270,7 +4282,7 @@
       </c>
       <c r="C176" s="59"/>
       <c r="D176" s="59"/>
-      <c r="E176" s="75"/>
+      <c r="E176" s="67"/>
       <c r="F176" s="59"/>
       <c r="G176" s="59"/>
       <c r="H176" s="59"/>
@@ -4287,7 +4299,7 @@
       </c>
       <c r="C177" s="59"/>
       <c r="D177" s="59"/>
-      <c r="E177" s="76"/>
+      <c r="E177" s="68"/>
       <c r="F177" s="59"/>
       <c r="G177" s="59"/>
       <c r="H177" s="59"/>
@@ -4304,7 +4316,7 @@
       </c>
       <c r="C178" s="59"/>
       <c r="D178" s="59"/>
-      <c r="E178" s="70" t="s">
+      <c r="E178" s="75" t="s">
         <v>27</v>
       </c>
       <c r="F178" s="59"/>
@@ -4323,7 +4335,7 @@
       </c>
       <c r="C179" s="59"/>
       <c r="D179" s="59"/>
-      <c r="E179" s="70"/>
+      <c r="E179" s="75"/>
       <c r="F179" s="59"/>
       <c r="G179" s="59"/>
       <c r="H179" s="59"/>
@@ -4338,7 +4350,7 @@
       </c>
       <c r="C180" s="59"/>
       <c r="D180" s="59"/>
-      <c r="E180" s="70"/>
+      <c r="E180" s="75"/>
       <c r="F180" s="59"/>
       <c r="G180" s="59"/>
       <c r="H180" s="59"/>
@@ -4353,7 +4365,7 @@
       </c>
       <c r="C181" s="59"/>
       <c r="D181" s="59"/>
-      <c r="E181" s="70"/>
+      <c r="E181" s="75"/>
       <c r="F181" s="59"/>
       <c r="G181" s="59"/>
       <c r="H181" s="59"/>
@@ -4368,7 +4380,7 @@
       </c>
       <c r="C182" s="59"/>
       <c r="D182" s="59"/>
-      <c r="E182" s="70"/>
+      <c r="E182" s="75"/>
       <c r="F182" s="59"/>
       <c r="G182" s="59"/>
       <c r="H182" s="59"/>
@@ -4383,7 +4395,7 @@
       </c>
       <c r="C183" s="59"/>
       <c r="D183" s="59"/>
-      <c r="E183" s="70"/>
+      <c r="E183" s="75"/>
       <c r="F183" s="59"/>
       <c r="G183" s="59"/>
       <c r="H183" s="59"/>
@@ -4398,7 +4410,7 @@
       </c>
       <c r="C184" s="59"/>
       <c r="D184" s="59"/>
-      <c r="E184" s="70"/>
+      <c r="E184" s="75"/>
       <c r="F184" s="59"/>
       <c r="G184" s="59"/>
       <c r="H184" s="59"/>
@@ -4413,7 +4425,7 @@
       </c>
       <c r="C185" s="59"/>
       <c r="D185" s="59"/>
-      <c r="E185" s="70"/>
+      <c r="E185" s="75"/>
       <c r="F185" s="59"/>
       <c r="G185" s="59"/>
       <c r="H185" s="59"/>
@@ -4428,7 +4440,7 @@
       </c>
       <c r="C186" s="59"/>
       <c r="D186" s="59"/>
-      <c r="E186" s="70"/>
+      <c r="E186" s="75"/>
       <c r="F186" s="59"/>
       <c r="G186" s="59"/>
       <c r="H186" s="59"/>
@@ -4443,7 +4455,7 @@
       </c>
       <c r="C187" s="59"/>
       <c r="D187" s="59"/>
-      <c r="E187" s="70"/>
+      <c r="E187" s="75"/>
       <c r="F187" s="59"/>
       <c r="G187" s="59"/>
       <c r="H187" s="59"/>
@@ -4458,7 +4470,7 @@
       </c>
       <c r="C188" s="59"/>
       <c r="D188" s="59"/>
-      <c r="E188" s="70"/>
+      <c r="E188" s="75"/>
       <c r="F188" s="59"/>
       <c r="G188" s="59"/>
       <c r="H188" s="59"/>
@@ -4473,7 +4485,7 @@
       </c>
       <c r="C189" s="59"/>
       <c r="D189" s="59"/>
-      <c r="E189" s="70"/>
+      <c r="E189" s="75"/>
       <c r="F189" s="59"/>
       <c r="G189" s="59"/>
       <c r="H189" s="59"/>
@@ -4488,7 +4500,7 @@
       </c>
       <c r="C190" s="59"/>
       <c r="D190" s="59"/>
-      <c r="E190" s="70"/>
+      <c r="E190" s="75"/>
       <c r="F190" s="59"/>
       <c r="G190" s="59"/>
       <c r="H190" s="59"/>
@@ -4503,7 +4515,7 @@
       </c>
       <c r="C191" s="59"/>
       <c r="D191" s="59"/>
-      <c r="E191" s="70"/>
+      <c r="E191" s="75"/>
       <c r="F191" s="59"/>
       <c r="G191" s="59"/>
       <c r="H191" s="59"/>
@@ -4518,7 +4530,7 @@
       </c>
       <c r="C192" s="59"/>
       <c r="D192" s="59"/>
-      <c r="E192" s="70"/>
+      <c r="E192" s="75"/>
       <c r="F192" s="59"/>
       <c r="G192" s="59"/>
       <c r="H192" s="59"/>
@@ -4535,7 +4547,7 @@
       </c>
       <c r="C193" s="59"/>
       <c r="D193" s="59"/>
-      <c r="E193" s="70"/>
+      <c r="E193" s="75"/>
       <c r="F193" s="59"/>
       <c r="G193" s="59"/>
       <c r="H193" s="59"/>
@@ -4551,7 +4563,7 @@
         <v>192</v>
       </c>
       <c r="C194" s="59"/>
-      <c r="D194" s="71" t="s">
+      <c r="D194" s="76" t="s">
         <v>25</v>
       </c>
       <c r="E194" s="59"/>
@@ -4570,7 +4582,7 @@
         <v>193</v>
       </c>
       <c r="C195" s="59"/>
-      <c r="D195" s="72"/>
+      <c r="D195" s="77"/>
       <c r="E195" s="59"/>
       <c r="F195" s="59"/>
       <c r="G195" s="59"/>
@@ -4585,7 +4597,7 @@
         <v>194</v>
       </c>
       <c r="C196" s="59"/>
-      <c r="D196" s="72"/>
+      <c r="D196" s="77"/>
       <c r="E196" s="59"/>
       <c r="F196" s="59"/>
       <c r="G196" s="59"/>
@@ -4600,7 +4612,7 @@
         <v>195</v>
       </c>
       <c r="C197" s="59"/>
-      <c r="D197" s="72"/>
+      <c r="D197" s="77"/>
       <c r="E197" s="59"/>
       <c r="F197" s="59"/>
       <c r="G197" s="59"/>
@@ -4615,7 +4627,7 @@
         <v>196</v>
       </c>
       <c r="C198" s="59"/>
-      <c r="D198" s="72"/>
+      <c r="D198" s="77"/>
       <c r="E198" s="59"/>
       <c r="F198" s="59"/>
       <c r="G198" s="59"/>
@@ -4630,7 +4642,7 @@
         <v>197</v>
       </c>
       <c r="C199" s="59"/>
-      <c r="D199" s="72"/>
+      <c r="D199" s="77"/>
       <c r="E199" s="59"/>
       <c r="F199" s="59"/>
       <c r="G199" s="59"/>
@@ -4645,7 +4657,7 @@
         <v>198</v>
       </c>
       <c r="C200" s="59"/>
-      <c r="D200" s="72"/>
+      <c r="D200" s="77"/>
       <c r="E200" s="59"/>
       <c r="F200" s="59"/>
       <c r="G200" s="59"/>
@@ -4662,7 +4674,7 @@
         <v>199</v>
       </c>
       <c r="C201" s="59"/>
-      <c r="D201" s="73"/>
+      <c r="D201" s="78"/>
       <c r="E201" s="59"/>
       <c r="F201" s="59"/>
       <c r="G201" s="59"/>
@@ -4679,7 +4691,7 @@
         <v>200</v>
       </c>
       <c r="C202" s="59"/>
-      <c r="D202" s="80" t="s">
+      <c r="D202" s="60" t="s">
         <v>24</v>
       </c>
       <c r="E202" s="59"/>
@@ -4698,7 +4710,7 @@
         <v>201</v>
       </c>
       <c r="C203" s="59"/>
-      <c r="D203" s="80"/>
+      <c r="D203" s="60"/>
       <c r="E203" s="59"/>
       <c r="F203" s="59"/>
       <c r="G203" s="59"/>
@@ -4713,7 +4725,7 @@
         <v>202</v>
       </c>
       <c r="C204" s="59"/>
-      <c r="D204" s="80"/>
+      <c r="D204" s="60"/>
       <c r="E204" s="59"/>
       <c r="F204" s="59"/>
       <c r="G204" s="59"/>
@@ -4728,7 +4740,7 @@
         <v>203</v>
       </c>
       <c r="C205" s="59"/>
-      <c r="D205" s="80"/>
+      <c r="D205" s="60"/>
       <c r="E205" s="59"/>
       <c r="F205" s="59"/>
       <c r="G205" s="59"/>
@@ -4743,7 +4755,7 @@
         <v>204</v>
       </c>
       <c r="C206" s="59"/>
-      <c r="D206" s="80"/>
+      <c r="D206" s="60"/>
       <c r="E206" s="59"/>
       <c r="F206" s="59"/>
       <c r="G206" s="59"/>
@@ -4758,7 +4770,7 @@
         <v>205</v>
       </c>
       <c r="C207" s="59"/>
-      <c r="D207" s="80"/>
+      <c r="D207" s="60"/>
       <c r="E207" s="59"/>
       <c r="F207" s="59"/>
       <c r="G207" s="59"/>
@@ -4773,7 +4785,7 @@
         <v>206</v>
       </c>
       <c r="C208" s="59"/>
-      <c r="D208" s="80"/>
+      <c r="D208" s="60"/>
       <c r="E208" s="59"/>
       <c r="F208" s="59"/>
       <c r="G208" s="59"/>
@@ -4790,7 +4802,7 @@
         <v>207</v>
       </c>
       <c r="C209" s="59"/>
-      <c r="D209" s="80"/>
+      <c r="D209" s="60"/>
       <c r="E209" s="59"/>
       <c r="F209" s="59"/>
       <c r="G209" s="59"/>
@@ -4806,9 +4818,9 @@
       <c r="B210" s="32">
         <v>208</v>
       </c>
-      <c r="C210" s="81"/>
-      <c r="D210" s="82"/>
-      <c r="E210" s="83" t="s">
+      <c r="C210" s="61"/>
+      <c r="D210" s="62"/>
+      <c r="E210" s="63" t="s">
         <v>34</v>
       </c>
       <c r="F210" s="59"/>
@@ -4825,14 +4837,14 @@
       <c r="B211" s="32">
         <v>209</v>
       </c>
-      <c r="C211" s="81"/>
-      <c r="D211" s="82"/>
-      <c r="E211" s="83"/>
+      <c r="C211" s="61"/>
+      <c r="D211" s="62"/>
+      <c r="E211" s="63"/>
       <c r="F211" s="59"/>
       <c r="G211" s="59"/>
       <c r="H211" s="59"/>
       <c r="I211" s="31" t="s">
-        <v>58</v>
+        <v>118</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
@@ -4842,14 +4854,14 @@
       <c r="B212" s="32">
         <v>210</v>
       </c>
-      <c r="C212" s="81"/>
-      <c r="D212" s="82"/>
-      <c r="E212" s="83"/>
+      <c r="C212" s="61"/>
+      <c r="D212" s="62"/>
+      <c r="E212" s="63"/>
       <c r="F212" s="59"/>
       <c r="G212" s="59"/>
       <c r="H212" s="59"/>
       <c r="I212" s="31" t="s">
-        <v>59</v>
+        <v>119</v>
       </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.25">
@@ -4859,14 +4871,14 @@
       <c r="B213" s="32">
         <v>211</v>
       </c>
-      <c r="C213" s="81"/>
-      <c r="D213" s="82"/>
-      <c r="E213" s="83"/>
+      <c r="C213" s="61"/>
+      <c r="D213" s="62"/>
+      <c r="E213" s="63"/>
       <c r="F213" s="59"/>
       <c r="G213" s="59"/>
       <c r="H213" s="59"/>
       <c r="I213" s="31" t="s">
-        <v>60</v>
+        <v>120</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
@@ -4876,13 +4888,15 @@
       <c r="B214" s="32">
         <v>212</v>
       </c>
-      <c r="C214" s="81"/>
-      <c r="D214" s="82"/>
-      <c r="E214" s="83"/>
+      <c r="C214" s="61"/>
+      <c r="D214" s="62"/>
+      <c r="E214" s="63"/>
       <c r="F214" s="59"/>
       <c r="G214" s="59"/>
       <c r="H214" s="59"/>
-      <c r="I214" s="31"/>
+      <c r="I214" s="31" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" s="32" t="s">
@@ -4891,9 +4905,9 @@
       <c r="B215" s="32">
         <v>213</v>
       </c>
-      <c r="C215" s="81"/>
-      <c r="D215" s="82"/>
-      <c r="E215" s="83"/>
+      <c r="C215" s="61"/>
+      <c r="D215" s="62"/>
+      <c r="E215" s="63"/>
       <c r="F215" s="59"/>
       <c r="G215" s="59"/>
       <c r="H215" s="59"/>
@@ -4906,9 +4920,9 @@
       <c r="B216" s="32">
         <v>214</v>
       </c>
-      <c r="C216" s="81"/>
-      <c r="D216" s="82"/>
-      <c r="E216" s="83"/>
+      <c r="C216" s="61"/>
+      <c r="D216" s="62"/>
+      <c r="E216" s="63"/>
       <c r="F216" s="59"/>
       <c r="G216" s="59"/>
       <c r="H216" s="59"/>
@@ -4921,9 +4935,9 @@
       <c r="B217" s="32">
         <v>215</v>
       </c>
-      <c r="C217" s="81"/>
-      <c r="D217" s="82"/>
-      <c r="E217" s="83"/>
+      <c r="C217" s="61"/>
+      <c r="D217" s="62"/>
+      <c r="E217" s="63"/>
       <c r="F217" s="59"/>
       <c r="G217" s="59"/>
       <c r="H217" s="59"/>
@@ -4937,8 +4951,8 @@
         <v>216</v>
       </c>
       <c r="C218" s="59"/>
-      <c r="D218" s="77"/>
-      <c r="E218" s="83"/>
+      <c r="D218" s="69"/>
+      <c r="E218" s="63"/>
       <c r="F218" s="59"/>
       <c r="G218" s="59"/>
       <c r="H218" s="59"/>
@@ -4952,8 +4966,8 @@
         <v>217</v>
       </c>
       <c r="C219" s="59"/>
-      <c r="D219" s="77"/>
-      <c r="E219" s="83"/>
+      <c r="D219" s="69"/>
+      <c r="E219" s="63"/>
       <c r="F219" s="59"/>
       <c r="G219" s="59"/>
       <c r="H219" s="59"/>
@@ -4967,8 +4981,8 @@
         <v>218</v>
       </c>
       <c r="C220" s="59"/>
-      <c r="D220" s="77"/>
-      <c r="E220" s="83"/>
+      <c r="D220" s="69"/>
+      <c r="E220" s="63"/>
       <c r="F220" s="59"/>
       <c r="G220" s="59"/>
       <c r="H220" s="59"/>
@@ -4982,8 +4996,8 @@
         <v>219</v>
       </c>
       <c r="C221" s="59"/>
-      <c r="D221" s="77"/>
-      <c r="E221" s="83"/>
+      <c r="D221" s="69"/>
+      <c r="E221" s="63"/>
       <c r="F221" s="59"/>
       <c r="G221" s="59"/>
       <c r="H221" s="59"/>
@@ -4997,8 +5011,8 @@
         <v>220</v>
       </c>
       <c r="C222" s="59"/>
-      <c r="D222" s="77"/>
-      <c r="E222" s="83"/>
+      <c r="D222" s="69"/>
+      <c r="E222" s="63"/>
       <c r="F222" s="59"/>
       <c r="G222" s="59"/>
       <c r="H222" s="59"/>
@@ -5012,8 +5026,8 @@
         <v>221</v>
       </c>
       <c r="C223" s="59"/>
-      <c r="D223" s="77"/>
-      <c r="E223" s="83"/>
+      <c r="D223" s="69"/>
+      <c r="E223" s="63"/>
       <c r="F223" s="59"/>
       <c r="G223" s="59"/>
       <c r="H223" s="59"/>
@@ -5027,8 +5041,8 @@
         <v>222</v>
       </c>
       <c r="C224" s="59"/>
-      <c r="D224" s="77"/>
-      <c r="E224" s="83"/>
+      <c r="D224" s="69"/>
+      <c r="E224" s="63"/>
       <c r="F224" s="59"/>
       <c r="G224" s="59"/>
       <c r="H224" s="59"/>
@@ -5042,8 +5056,8 @@
         <v>223</v>
       </c>
       <c r="C225" s="59"/>
-      <c r="D225" s="77"/>
-      <c r="E225" s="83"/>
+      <c r="D225" s="69"/>
+      <c r="E225" s="63"/>
       <c r="F225" s="59"/>
       <c r="G225" s="59"/>
       <c r="H225" s="59"/>
@@ -5058,8 +5072,8 @@
       <c r="B226" s="51">
         <v>224</v>
       </c>
-      <c r="C226" s="78"/>
-      <c r="D226" s="79" t="s">
+      <c r="C226" s="70"/>
+      <c r="D226" s="71" t="s">
         <v>29</v>
       </c>
       <c r="E226" s="59"/>
@@ -5077,8 +5091,8 @@
       <c r="B227" s="51">
         <v>225</v>
       </c>
-      <c r="C227" s="78"/>
-      <c r="D227" s="79"/>
+      <c r="C227" s="70"/>
+      <c r="D227" s="71"/>
       <c r="E227" s="59"/>
       <c r="F227" s="59"/>
       <c r="G227" s="59"/>
@@ -5092,8 +5106,8 @@
       <c r="B228" s="51">
         <v>226</v>
       </c>
-      <c r="C228" s="78"/>
-      <c r="D228" s="79"/>
+      <c r="C228" s="70"/>
+      <c r="D228" s="71"/>
       <c r="E228" s="59"/>
       <c r="F228" s="59"/>
       <c r="G228" s="59"/>
@@ -5107,8 +5121,8 @@
       <c r="B229" s="51">
         <v>227</v>
       </c>
-      <c r="C229" s="78"/>
-      <c r="D229" s="79"/>
+      <c r="C229" s="70"/>
+      <c r="D229" s="71"/>
       <c r="E229" s="59"/>
       <c r="F229" s="59"/>
       <c r="G229" s="59"/>
@@ -5122,8 +5136,8 @@
       <c r="B230" s="51">
         <v>228</v>
       </c>
-      <c r="C230" s="84"/>
-      <c r="D230" s="79"/>
+      <c r="C230" s="64"/>
+      <c r="D230" s="71"/>
       <c r="E230" s="59"/>
       <c r="F230" s="59"/>
       <c r="G230" s="59"/>
@@ -5137,8 +5151,8 @@
       <c r="B231" s="51">
         <v>229</v>
       </c>
-      <c r="C231" s="84"/>
-      <c r="D231" s="79"/>
+      <c r="C231" s="64"/>
+      <c r="D231" s="71"/>
       <c r="E231" s="59"/>
       <c r="F231" s="59"/>
       <c r="G231" s="59"/>
@@ -5152,8 +5166,8 @@
       <c r="B232" s="51">
         <v>230</v>
       </c>
-      <c r="C232" s="84"/>
-      <c r="D232" s="79"/>
+      <c r="C232" s="64"/>
+      <c r="D232" s="71"/>
       <c r="E232" s="59"/>
       <c r="F232" s="59"/>
       <c r="G232" s="59"/>
@@ -5169,8 +5183,8 @@
       <c r="B233" s="51">
         <v>231</v>
       </c>
-      <c r="C233" s="84"/>
-      <c r="D233" s="79"/>
+      <c r="C233" s="64"/>
+      <c r="D233" s="71"/>
       <c r="E233" s="59"/>
       <c r="F233" s="59"/>
       <c r="G233" s="59"/>
@@ -5186,7 +5200,7 @@
       <c r="B234" s="47">
         <v>232</v>
       </c>
-      <c r="C234" s="85" t="s">
+      <c r="C234" s="65" t="s">
         <v>30</v>
       </c>
       <c r="D234" s="59"/>
@@ -5205,7 +5219,7 @@
       <c r="B235" s="47">
         <v>233</v>
       </c>
-      <c r="C235" s="85"/>
+      <c r="C235" s="65"/>
       <c r="D235" s="59"/>
       <c r="E235" s="59"/>
       <c r="F235" s="59"/>
@@ -5222,7 +5236,7 @@
       <c r="B236" s="47">
         <v>234</v>
       </c>
-      <c r="C236" s="85"/>
+      <c r="C236" s="65"/>
       <c r="D236" s="59"/>
       <c r="E236" s="59"/>
       <c r="F236" s="59"/>
@@ -5239,7 +5253,7 @@
       <c r="B237" s="47">
         <v>235</v>
       </c>
-      <c r="C237" s="85"/>
+      <c r="C237" s="65"/>
       <c r="D237" s="59"/>
       <c r="E237" s="59"/>
       <c r="F237" s="59"/>
@@ -5551,38 +5565,76 @@
     </row>
   </sheetData>
   <mergeCells count="126">
-    <mergeCell ref="F194:F225"/>
-    <mergeCell ref="G194:G257"/>
-    <mergeCell ref="C198:C201"/>
-    <mergeCell ref="C202:C205"/>
-    <mergeCell ref="D202:D209"/>
-    <mergeCell ref="C206:C209"/>
-    <mergeCell ref="C210:C213"/>
-    <mergeCell ref="D210:D217"/>
-    <mergeCell ref="E210:E225"/>
-    <mergeCell ref="C214:C217"/>
-    <mergeCell ref="D250:D257"/>
-    <mergeCell ref="C254:C257"/>
-    <mergeCell ref="F226:F257"/>
-    <mergeCell ref="C230:C233"/>
-    <mergeCell ref="C234:C237"/>
-    <mergeCell ref="D234:D241"/>
-    <mergeCell ref="C238:C241"/>
-    <mergeCell ref="C242:C245"/>
-    <mergeCell ref="D242:D249"/>
-    <mergeCell ref="E242:E257"/>
-    <mergeCell ref="C246:C249"/>
-    <mergeCell ref="C250:C253"/>
-    <mergeCell ref="E194:E209"/>
-    <mergeCell ref="C162:C165"/>
-    <mergeCell ref="D162:D169"/>
-    <mergeCell ref="E162:E177"/>
-    <mergeCell ref="C218:C221"/>
-    <mergeCell ref="D218:D225"/>
-    <mergeCell ref="C222:C225"/>
-    <mergeCell ref="C226:C229"/>
-    <mergeCell ref="D226:D233"/>
-    <mergeCell ref="E226:E241"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D9"/>
+    <mergeCell ref="E2:E17"/>
+    <mergeCell ref="F2:F33"/>
+    <mergeCell ref="G2:G65"/>
+    <mergeCell ref="H2:H129"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="F34:F65"/>
+    <mergeCell ref="C38:C41"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="D42:D49"/>
+    <mergeCell ref="C46:C49"/>
+    <mergeCell ref="C50:C53"/>
+    <mergeCell ref="D50:D57"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D25"/>
+    <mergeCell ref="E18:E33"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D26:D33"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="E50:E65"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="D58:D65"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="D66:D73"/>
+    <mergeCell ref="E66:E81"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="D34:D41"/>
+    <mergeCell ref="E34:E49"/>
+    <mergeCell ref="C90:C93"/>
+    <mergeCell ref="D90:D97"/>
+    <mergeCell ref="C94:C97"/>
+    <mergeCell ref="C98:C101"/>
+    <mergeCell ref="D98:D105"/>
+    <mergeCell ref="E98:E113"/>
+    <mergeCell ref="F66:F97"/>
+    <mergeCell ref="G66:G129"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="C74:C77"/>
+    <mergeCell ref="D74:D81"/>
+    <mergeCell ref="C78:C81"/>
+    <mergeCell ref="C82:C85"/>
+    <mergeCell ref="D82:D89"/>
+    <mergeCell ref="E82:E97"/>
+    <mergeCell ref="C86:C89"/>
+    <mergeCell ref="D122:D129"/>
+    <mergeCell ref="C126:C129"/>
+    <mergeCell ref="C130:C133"/>
+    <mergeCell ref="D130:D137"/>
+    <mergeCell ref="E130:E145"/>
+    <mergeCell ref="F130:F161"/>
+    <mergeCell ref="C154:C157"/>
+    <mergeCell ref="D154:D161"/>
+    <mergeCell ref="C158:C161"/>
+    <mergeCell ref="F98:F129"/>
+    <mergeCell ref="C102:C105"/>
+    <mergeCell ref="C106:C109"/>
+    <mergeCell ref="D106:D113"/>
+    <mergeCell ref="C110:C113"/>
+    <mergeCell ref="C114:C117"/>
+    <mergeCell ref="D114:D121"/>
+    <mergeCell ref="E114:E129"/>
+    <mergeCell ref="C118:C121"/>
+    <mergeCell ref="C122:C125"/>
     <mergeCell ref="F162:F193"/>
     <mergeCell ref="C166:C169"/>
     <mergeCell ref="C170:C173"/>
@@ -5607,76 +5659,38 @@
     <mergeCell ref="C190:C193"/>
     <mergeCell ref="C194:C197"/>
     <mergeCell ref="D194:D201"/>
-    <mergeCell ref="C130:C133"/>
-    <mergeCell ref="D130:D137"/>
-    <mergeCell ref="E130:E145"/>
-    <mergeCell ref="F130:F161"/>
-    <mergeCell ref="C154:C157"/>
-    <mergeCell ref="D154:D161"/>
-    <mergeCell ref="C158:C161"/>
-    <mergeCell ref="F98:F129"/>
-    <mergeCell ref="C102:C105"/>
-    <mergeCell ref="C106:C109"/>
-    <mergeCell ref="D106:D113"/>
-    <mergeCell ref="C110:C113"/>
-    <mergeCell ref="C114:C117"/>
-    <mergeCell ref="D114:D121"/>
-    <mergeCell ref="E114:E129"/>
-    <mergeCell ref="C118:C121"/>
-    <mergeCell ref="C122:C125"/>
-    <mergeCell ref="C90:C93"/>
-    <mergeCell ref="D90:D97"/>
-    <mergeCell ref="C94:C97"/>
-    <mergeCell ref="C98:C101"/>
-    <mergeCell ref="D98:D105"/>
-    <mergeCell ref="E98:E113"/>
-    <mergeCell ref="F66:F97"/>
-    <mergeCell ref="G66:G129"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="C74:C77"/>
-    <mergeCell ref="D74:D81"/>
-    <mergeCell ref="C78:C81"/>
-    <mergeCell ref="C82:C85"/>
-    <mergeCell ref="D82:D89"/>
-    <mergeCell ref="E82:E97"/>
-    <mergeCell ref="C86:C89"/>
-    <mergeCell ref="D122:D129"/>
-    <mergeCell ref="C126:C129"/>
-    <mergeCell ref="E50:E65"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="D58:D65"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="C66:C69"/>
-    <mergeCell ref="D66:D73"/>
-    <mergeCell ref="E66:E81"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="D34:D41"/>
-    <mergeCell ref="E34:E49"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="D2:D9"/>
-    <mergeCell ref="E2:E17"/>
-    <mergeCell ref="F2:F33"/>
-    <mergeCell ref="G2:G65"/>
-    <mergeCell ref="H2:H129"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="D10:D17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="F34:F65"/>
-    <mergeCell ref="C38:C41"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="D42:D49"/>
-    <mergeCell ref="C46:C49"/>
-    <mergeCell ref="C50:C53"/>
-    <mergeCell ref="D50:D57"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D25"/>
-    <mergeCell ref="E18:E33"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="D26:D33"/>
-    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="C162:C165"/>
+    <mergeCell ref="D162:D169"/>
+    <mergeCell ref="E162:E177"/>
+    <mergeCell ref="C218:C221"/>
+    <mergeCell ref="D218:D225"/>
+    <mergeCell ref="C222:C225"/>
+    <mergeCell ref="C226:C229"/>
+    <mergeCell ref="D226:D233"/>
+    <mergeCell ref="E226:E241"/>
+    <mergeCell ref="F194:F225"/>
+    <mergeCell ref="G194:G257"/>
+    <mergeCell ref="C198:C201"/>
+    <mergeCell ref="C202:C205"/>
+    <mergeCell ref="D202:D209"/>
+    <mergeCell ref="C206:C209"/>
+    <mergeCell ref="C210:C213"/>
+    <mergeCell ref="D210:D217"/>
+    <mergeCell ref="E210:E225"/>
+    <mergeCell ref="C214:C217"/>
+    <mergeCell ref="D250:D257"/>
+    <mergeCell ref="C254:C257"/>
+    <mergeCell ref="F226:F257"/>
+    <mergeCell ref="C230:C233"/>
+    <mergeCell ref="C234:C237"/>
+    <mergeCell ref="D234:D241"/>
+    <mergeCell ref="C238:C241"/>
+    <mergeCell ref="C242:C245"/>
+    <mergeCell ref="D242:D249"/>
+    <mergeCell ref="E242:E257"/>
+    <mergeCell ref="C246:C249"/>
+    <mergeCell ref="C250:C253"/>
+    <mergeCell ref="E194:E209"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5861,7 +5875,7 @@
       <c r="B1" s="33">
         <v>0</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="85" t="s">
         <v>15</v>
       </c>
       <c r="D1" s="43" t="s">
@@ -5873,7 +5887,7 @@
       <c r="G1" s="40">
         <v>32</v>
       </c>
-      <c r="H1" s="63" t="s">
+      <c r="H1" s="84" t="s">
         <v>16</v>
       </c>
       <c r="I1" s="44" t="s">
@@ -5885,7 +5899,7 @@
       <c r="L1" s="41">
         <v>64</v>
       </c>
-      <c r="M1" s="62" t="s">
+      <c r="M1" s="83" t="s">
         <v>18</v>
       </c>
       <c r="N1" s="45" t="s">
@@ -5897,7 +5911,7 @@
       <c r="Q1" s="42">
         <v>96</v>
       </c>
-      <c r="R1" s="64" t="s">
+      <c r="R1" s="80" t="s">
         <v>20</v>
       </c>
       <c r="S1" s="46" t="s">
@@ -5909,7 +5923,7 @@
       <c r="V1" s="39">
         <v>128</v>
       </c>
-      <c r="W1" s="66" t="s">
+      <c r="W1" s="72" t="s">
         <v>22</v>
       </c>
       <c r="X1" s="38" t="s">
@@ -5923,7 +5937,7 @@
       <c r="B2" s="33">
         <v>1</v>
       </c>
-      <c r="C2" s="60"/>
+      <c r="C2" s="85"/>
       <c r="D2" s="43"/>
       <c r="F2" s="40" t="s">
         <v>38</v>
@@ -5931,7 +5945,7 @@
       <c r="G2" s="40">
         <v>33</v>
       </c>
-      <c r="H2" s="63"/>
+      <c r="H2" s="84"/>
       <c r="I2" s="44"/>
       <c r="K2" s="41" t="s">
         <v>38</v>
@@ -5939,7 +5953,7 @@
       <c r="L2" s="41">
         <v>65</v>
       </c>
-      <c r="M2" s="62"/>
+      <c r="M2" s="83"/>
       <c r="N2" s="45"/>
       <c r="P2" s="42" t="s">
         <v>38</v>
@@ -5947,7 +5961,7 @@
       <c r="Q2" s="42">
         <v>97</v>
       </c>
-      <c r="R2" s="64"/>
+      <c r="R2" s="80"/>
       <c r="S2" s="46"/>
       <c r="U2" s="39" t="s">
         <v>38</v>
@@ -5955,7 +5969,7 @@
       <c r="V2" s="39">
         <v>129</v>
       </c>
-      <c r="W2" s="67"/>
+      <c r="W2" s="73"/>
       <c r="X2" s="38"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
@@ -5965,7 +5979,7 @@
       <c r="B3" s="33">
         <v>2</v>
       </c>
-      <c r="C3" s="60"/>
+      <c r="C3" s="85"/>
       <c r="D3" s="43"/>
       <c r="F3" s="40" t="s">
         <v>38</v>
@@ -5973,7 +5987,7 @@
       <c r="G3" s="40">
         <v>34</v>
       </c>
-      <c r="H3" s="63"/>
+      <c r="H3" s="84"/>
       <c r="I3" s="44"/>
       <c r="K3" s="41" t="s">
         <v>38</v>
@@ -5981,7 +5995,7 @@
       <c r="L3" s="41">
         <v>66</v>
       </c>
-      <c r="M3" s="62"/>
+      <c r="M3" s="83"/>
       <c r="N3" s="45"/>
       <c r="P3" s="42" t="s">
         <v>38</v>
@@ -5989,7 +6003,7 @@
       <c r="Q3" s="42">
         <v>98</v>
       </c>
-      <c r="R3" s="64"/>
+      <c r="R3" s="80"/>
       <c r="S3" s="46"/>
       <c r="U3" s="39" t="s">
         <v>38</v>
@@ -5997,7 +6011,7 @@
       <c r="V3" s="39">
         <v>130</v>
       </c>
-      <c r="W3" s="67"/>
+      <c r="W3" s="73"/>
       <c r="X3" s="38"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -6007,7 +6021,7 @@
       <c r="B4" s="33">
         <v>3</v>
       </c>
-      <c r="C4" s="60"/>
+      <c r="C4" s="85"/>
       <c r="D4" s="43"/>
       <c r="F4" s="40" t="s">
         <v>38</v>
@@ -6015,7 +6029,7 @@
       <c r="G4" s="40">
         <v>35</v>
       </c>
-      <c r="H4" s="63"/>
+      <c r="H4" s="84"/>
       <c r="I4" s="44"/>
       <c r="K4" s="41" t="s">
         <v>38</v>
@@ -6023,7 +6037,7 @@
       <c r="L4" s="41">
         <v>67</v>
       </c>
-      <c r="M4" s="62"/>
+      <c r="M4" s="83"/>
       <c r="N4" s="45"/>
       <c r="P4" s="42" t="s">
         <v>38</v>
@@ -6031,7 +6045,7 @@
       <c r="Q4" s="42">
         <v>99</v>
       </c>
-      <c r="R4" s="64"/>
+      <c r="R4" s="80"/>
       <c r="S4" s="46"/>
       <c r="U4" s="39" t="s">
         <v>38</v>
@@ -6039,7 +6053,7 @@
       <c r="V4" s="39">
         <v>131</v>
       </c>
-      <c r="W4" s="67"/>
+      <c r="W4" s="73"/>
       <c r="X4" s="38"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -6049,7 +6063,7 @@
       <c r="B5" s="33">
         <v>4</v>
       </c>
-      <c r="C5" s="60"/>
+      <c r="C5" s="85"/>
       <c r="D5" s="43"/>
       <c r="F5" s="40" t="s">
         <v>38</v>
@@ -6057,7 +6071,7 @@
       <c r="G5" s="40">
         <v>36</v>
       </c>
-      <c r="H5" s="63"/>
+      <c r="H5" s="84"/>
       <c r="I5" s="44"/>
       <c r="K5" s="41" t="s">
         <v>38</v>
@@ -6065,7 +6079,7 @@
       <c r="L5" s="41">
         <v>68</v>
       </c>
-      <c r="M5" s="62"/>
+      <c r="M5" s="83"/>
       <c r="N5" s="45"/>
       <c r="P5" s="42" t="s">
         <v>38</v>
@@ -6073,7 +6087,7 @@
       <c r="Q5" s="42">
         <v>100</v>
       </c>
-      <c r="R5" s="64"/>
+      <c r="R5" s="80"/>
       <c r="S5" s="46"/>
       <c r="U5" s="39" t="s">
         <v>38</v>
@@ -6081,7 +6095,7 @@
       <c r="V5" s="39">
         <v>132</v>
       </c>
-      <c r="W5" s="67"/>
+      <c r="W5" s="73"/>
       <c r="X5" s="38"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -6091,7 +6105,7 @@
       <c r="B6" s="33">
         <v>5</v>
       </c>
-      <c r="C6" s="60"/>
+      <c r="C6" s="85"/>
       <c r="D6" s="43"/>
       <c r="F6" s="40" t="s">
         <v>38</v>
@@ -6099,7 +6113,7 @@
       <c r="G6" s="40">
         <v>37</v>
       </c>
-      <c r="H6" s="63"/>
+      <c r="H6" s="84"/>
       <c r="I6" s="44"/>
       <c r="K6" s="41" t="s">
         <v>38</v>
@@ -6107,7 +6121,7 @@
       <c r="L6" s="41">
         <v>69</v>
       </c>
-      <c r="M6" s="62"/>
+      <c r="M6" s="83"/>
       <c r="N6" s="45"/>
       <c r="P6" s="42" t="s">
         <v>38</v>
@@ -6115,7 +6129,7 @@
       <c r="Q6" s="42">
         <v>101</v>
       </c>
-      <c r="R6" s="64"/>
+      <c r="R6" s="80"/>
       <c r="S6" s="46"/>
       <c r="U6" s="39" t="s">
         <v>38</v>
@@ -6123,7 +6137,7 @@
       <c r="V6" s="39">
         <v>133</v>
       </c>
-      <c r="W6" s="67"/>
+      <c r="W6" s="73"/>
       <c r="X6" s="38"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -6133,7 +6147,7 @@
       <c r="B7" s="33">
         <v>6</v>
       </c>
-      <c r="C7" s="60"/>
+      <c r="C7" s="85"/>
       <c r="D7" s="43"/>
       <c r="F7" s="40" t="s">
         <v>38</v>
@@ -6141,7 +6155,7 @@
       <c r="G7" s="40">
         <v>38</v>
       </c>
-      <c r="H7" s="63"/>
+      <c r="H7" s="84"/>
       <c r="I7" s="44"/>
       <c r="K7" s="41" t="s">
         <v>38</v>
@@ -6149,7 +6163,7 @@
       <c r="L7" s="41">
         <v>70</v>
       </c>
-      <c r="M7" s="62"/>
+      <c r="M7" s="83"/>
       <c r="N7" s="45"/>
       <c r="P7" s="42" t="s">
         <v>38</v>
@@ -6157,7 +6171,7 @@
       <c r="Q7" s="42">
         <v>102</v>
       </c>
-      <c r="R7" s="64"/>
+      <c r="R7" s="80"/>
       <c r="S7" s="46"/>
       <c r="U7" s="39" t="s">
         <v>38</v>
@@ -6165,7 +6179,7 @@
       <c r="V7" s="39">
         <v>134</v>
       </c>
-      <c r="W7" s="67"/>
+      <c r="W7" s="73"/>
       <c r="X7" s="38"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -6175,7 +6189,7 @@
       <c r="B8" s="33">
         <v>7</v>
       </c>
-      <c r="C8" s="60"/>
+      <c r="C8" s="85"/>
       <c r="D8" s="43"/>
       <c r="F8" s="40" t="s">
         <v>38</v>
@@ -6183,7 +6197,7 @@
       <c r="G8" s="40">
         <v>39</v>
       </c>
-      <c r="H8" s="63"/>
+      <c r="H8" s="84"/>
       <c r="I8" s="44"/>
       <c r="K8" s="41" t="s">
         <v>38</v>
@@ -6191,7 +6205,7 @@
       <c r="L8" s="41">
         <v>71</v>
       </c>
-      <c r="M8" s="62"/>
+      <c r="M8" s="83"/>
       <c r="N8" s="45"/>
       <c r="P8" s="42" t="s">
         <v>38</v>
@@ -6199,7 +6213,7 @@
       <c r="Q8" s="42">
         <v>103</v>
       </c>
-      <c r="R8" s="64"/>
+      <c r="R8" s="80"/>
       <c r="S8" s="46"/>
       <c r="U8" s="39" t="s">
         <v>38</v>
@@ -6207,7 +6221,7 @@
       <c r="V8" s="39">
         <v>135</v>
       </c>
-      <c r="W8" s="67"/>
+      <c r="W8" s="73"/>
       <c r="X8" s="38"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
@@ -6217,7 +6231,7 @@
       <c r="B9" s="33">
         <v>8</v>
       </c>
-      <c r="C9" s="60"/>
+      <c r="C9" s="85"/>
       <c r="D9" s="43"/>
       <c r="F9" s="40" t="s">
         <v>38</v>
@@ -6225,7 +6239,7 @@
       <c r="G9" s="40">
         <v>40</v>
       </c>
-      <c r="H9" s="63"/>
+      <c r="H9" s="84"/>
       <c r="I9" s="44"/>
       <c r="K9" s="41" t="s">
         <v>38</v>
@@ -6233,7 +6247,7 @@
       <c r="L9" s="41">
         <v>72</v>
       </c>
-      <c r="M9" s="62"/>
+      <c r="M9" s="83"/>
       <c r="N9" s="45"/>
       <c r="P9" s="42" t="s">
         <v>38</v>
@@ -6241,7 +6255,7 @@
       <c r="Q9" s="42">
         <v>104</v>
       </c>
-      <c r="R9" s="64"/>
+      <c r="R9" s="80"/>
       <c r="S9" s="46"/>
       <c r="U9" s="39" t="s">
         <v>38</v>
@@ -6249,7 +6263,7 @@
       <c r="V9" s="39">
         <v>136</v>
       </c>
-      <c r="W9" s="67"/>
+      <c r="W9" s="73"/>
       <c r="X9" s="38"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -6259,7 +6273,7 @@
       <c r="B10" s="33">
         <v>9</v>
       </c>
-      <c r="C10" s="60"/>
+      <c r="C10" s="85"/>
       <c r="D10" s="54"/>
       <c r="F10" s="40" t="s">
         <v>38</v>
@@ -6267,7 +6281,7 @@
       <c r="G10" s="40">
         <v>41</v>
       </c>
-      <c r="H10" s="63"/>
+      <c r="H10" s="84"/>
       <c r="I10" s="44"/>
       <c r="K10" s="41" t="s">
         <v>38</v>
@@ -6275,7 +6289,7 @@
       <c r="L10" s="41">
         <v>73</v>
       </c>
-      <c r="M10" s="62"/>
+      <c r="M10" s="83"/>
       <c r="N10" s="45"/>
       <c r="P10" s="42" t="s">
         <v>38</v>
@@ -6283,7 +6297,7 @@
       <c r="Q10" s="42">
         <v>105</v>
       </c>
-      <c r="R10" s="64"/>
+      <c r="R10" s="80"/>
       <c r="S10" s="46"/>
       <c r="U10" s="39" t="s">
         <v>38</v>
@@ -6291,7 +6305,7 @@
       <c r="V10" s="39">
         <v>137</v>
       </c>
-      <c r="W10" s="67"/>
+      <c r="W10" s="73"/>
       <c r="X10" s="38"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
@@ -6301,7 +6315,7 @@
       <c r="B11" s="33">
         <v>10</v>
       </c>
-      <c r="C11" s="60"/>
+      <c r="C11" s="85"/>
       <c r="D11" s="43"/>
       <c r="F11" s="40" t="s">
         <v>38</v>
@@ -6309,7 +6323,7 @@
       <c r="G11" s="40">
         <v>42</v>
       </c>
-      <c r="H11" s="63"/>
+      <c r="H11" s="84"/>
       <c r="I11" s="44"/>
       <c r="K11" s="41" t="s">
         <v>38</v>
@@ -6317,7 +6331,7 @@
       <c r="L11" s="41">
         <v>74</v>
       </c>
-      <c r="M11" s="62"/>
+      <c r="M11" s="83"/>
       <c r="N11" s="45"/>
       <c r="P11" s="42" t="s">
         <v>38</v>
@@ -6325,7 +6339,7 @@
       <c r="Q11" s="42">
         <v>106</v>
       </c>
-      <c r="R11" s="64"/>
+      <c r="R11" s="80"/>
       <c r="S11" s="46"/>
       <c r="U11" s="39" t="s">
         <v>38</v>
@@ -6333,7 +6347,7 @@
       <c r="V11" s="39">
         <v>138</v>
       </c>
-      <c r="W11" s="67"/>
+      <c r="W11" s="73"/>
       <c r="X11" s="38"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
@@ -6343,7 +6357,7 @@
       <c r="B12" s="33">
         <v>11</v>
       </c>
-      <c r="C12" s="60"/>
+      <c r="C12" s="85"/>
       <c r="D12" s="43"/>
       <c r="F12" s="40" t="s">
         <v>38</v>
@@ -6351,7 +6365,7 @@
       <c r="G12" s="40">
         <v>43</v>
       </c>
-      <c r="H12" s="63"/>
+      <c r="H12" s="84"/>
       <c r="I12" s="44"/>
       <c r="K12" s="41" t="s">
         <v>38</v>
@@ -6359,7 +6373,7 @@
       <c r="L12" s="41">
         <v>75</v>
       </c>
-      <c r="M12" s="62"/>
+      <c r="M12" s="83"/>
       <c r="N12" s="45"/>
       <c r="P12" s="42" t="s">
         <v>38</v>
@@ -6367,7 +6381,7 @@
       <c r="Q12" s="42">
         <v>107</v>
       </c>
-      <c r="R12" s="64"/>
+      <c r="R12" s="80"/>
       <c r="S12" s="46"/>
       <c r="U12" s="39" t="s">
         <v>38</v>
@@ -6375,7 +6389,7 @@
       <c r="V12" s="39">
         <v>139</v>
       </c>
-      <c r="W12" s="67"/>
+      <c r="W12" s="73"/>
       <c r="X12" s="38"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
@@ -6385,7 +6399,7 @@
       <c r="B13" s="33">
         <v>12</v>
       </c>
-      <c r="C13" s="60"/>
+      <c r="C13" s="85"/>
       <c r="D13" s="43"/>
       <c r="F13" s="40" t="s">
         <v>38</v>
@@ -6393,7 +6407,7 @@
       <c r="G13" s="40">
         <v>44</v>
       </c>
-      <c r="H13" s="63"/>
+      <c r="H13" s="84"/>
       <c r="I13" s="44"/>
       <c r="K13" s="41" t="s">
         <v>38</v>
@@ -6401,7 +6415,7 @@
       <c r="L13" s="41">
         <v>76</v>
       </c>
-      <c r="M13" s="62"/>
+      <c r="M13" s="83"/>
       <c r="N13" s="45"/>
       <c r="P13" s="42" t="s">
         <v>38</v>
@@ -6409,7 +6423,7 @@
       <c r="Q13" s="42">
         <v>108</v>
       </c>
-      <c r="R13" s="64"/>
+      <c r="R13" s="80"/>
       <c r="S13" s="46"/>
       <c r="U13" s="39" t="s">
         <v>38</v>
@@ -6417,7 +6431,7 @@
       <c r="V13" s="39">
         <v>140</v>
       </c>
-      <c r="W13" s="67"/>
+      <c r="W13" s="73"/>
       <c r="X13" s="38"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
@@ -6427,7 +6441,7 @@
       <c r="B14" s="33">
         <v>13</v>
       </c>
-      <c r="C14" s="60"/>
+      <c r="C14" s="85"/>
       <c r="D14" s="43"/>
       <c r="F14" s="40" t="s">
         <v>38</v>
@@ -6435,7 +6449,7 @@
       <c r="G14" s="40">
         <v>45</v>
       </c>
-      <c r="H14" s="63"/>
+      <c r="H14" s="84"/>
       <c r="I14" s="44"/>
       <c r="K14" s="41" t="s">
         <v>38</v>
@@ -6443,7 +6457,7 @@
       <c r="L14" s="41">
         <v>77</v>
       </c>
-      <c r="M14" s="62"/>
+      <c r="M14" s="83"/>
       <c r="N14" s="45"/>
       <c r="P14" s="42" t="s">
         <v>38</v>
@@ -6451,7 +6465,7 @@
       <c r="Q14" s="42">
         <v>109</v>
       </c>
-      <c r="R14" s="64"/>
+      <c r="R14" s="80"/>
       <c r="S14" s="46"/>
       <c r="U14" s="39" t="s">
         <v>38</v>
@@ -6459,7 +6473,7 @@
       <c r="V14" s="39">
         <v>141</v>
       </c>
-      <c r="W14" s="67"/>
+      <c r="W14" s="73"/>
       <c r="X14" s="38"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
@@ -6469,7 +6483,7 @@
       <c r="B15" s="33">
         <v>14</v>
       </c>
-      <c r="C15" s="60"/>
+      <c r="C15" s="85"/>
       <c r="D15" s="43"/>
       <c r="F15" s="40" t="s">
         <v>38</v>
@@ -6477,7 +6491,7 @@
       <c r="G15" s="40">
         <v>46</v>
       </c>
-      <c r="H15" s="63"/>
+      <c r="H15" s="84"/>
       <c r="I15" s="44" t="s">
         <v>33</v>
       </c>
@@ -6487,7 +6501,7 @@
       <c r="L15" s="41">
         <v>78</v>
       </c>
-      <c r="M15" s="62"/>
+      <c r="M15" s="83"/>
       <c r="N15" s="45" t="s">
         <v>33</v>
       </c>
@@ -6497,7 +6511,7 @@
       <c r="Q15" s="42">
         <v>110</v>
       </c>
-      <c r="R15" s="64"/>
+      <c r="R15" s="80"/>
       <c r="S15" s="46" t="s">
         <v>33</v>
       </c>
@@ -6507,7 +6521,7 @@
       <c r="V15" s="39">
         <v>142</v>
       </c>
-      <c r="W15" s="67"/>
+      <c r="W15" s="73"/>
       <c r="X15" s="38" t="s">
         <v>33</v>
       </c>
@@ -6519,7 +6533,7 @@
       <c r="B16" s="33">
         <v>15</v>
       </c>
-      <c r="C16" s="60"/>
+      <c r="C16" s="85"/>
       <c r="D16" s="43"/>
       <c r="F16" s="40" t="s">
         <v>38</v>
@@ -6527,7 +6541,7 @@
       <c r="G16" s="40">
         <v>47</v>
       </c>
-      <c r="H16" s="63"/>
+      <c r="H16" s="84"/>
       <c r="I16" s="44" t="s">
         <v>32</v>
       </c>
@@ -6537,7 +6551,7 @@
       <c r="L16" s="41">
         <v>79</v>
       </c>
-      <c r="M16" s="62"/>
+      <c r="M16" s="83"/>
       <c r="N16" s="45" t="s">
         <v>32</v>
       </c>
@@ -6547,7 +6561,7 @@
       <c r="Q16" s="42">
         <v>111</v>
       </c>
-      <c r="R16" s="64"/>
+      <c r="R16" s="80"/>
       <c r="S16" s="46" t="s">
         <v>32</v>
       </c>
@@ -6557,7 +6571,7 @@
       <c r="V16" s="39">
         <v>143</v>
       </c>
-      <c r="W16" s="68"/>
+      <c r="W16" s="74"/>
       <c r="X16" s="38" t="s">
         <v>32</v>
       </c>
@@ -6569,7 +6583,7 @@
       <c r="B17" s="33">
         <v>16</v>
       </c>
-      <c r="C17" s="60"/>
+      <c r="C17" s="85"/>
       <c r="D17" s="43"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
@@ -6579,7 +6593,7 @@
       <c r="B18" s="33">
         <v>17</v>
       </c>
-      <c r="C18" s="60"/>
+      <c r="C18" s="85"/>
       <c r="D18" s="43"/>
       <c r="F18" s="40" t="s">
         <v>38</v>
@@ -6587,7 +6601,7 @@
       <c r="G18" s="40">
         <v>48</v>
       </c>
-      <c r="H18" s="61" t="s">
+      <c r="H18" s="82" t="s">
         <v>17</v>
       </c>
       <c r="I18" s="44" t="s">
@@ -6599,7 +6613,7 @@
       <c r="L18" s="41">
         <v>80</v>
       </c>
-      <c r="M18" s="65" t="s">
+      <c r="M18" s="81" t="s">
         <v>19</v>
       </c>
       <c r="N18" s="45" t="s">
@@ -6611,7 +6625,7 @@
       <c r="Q18" s="42">
         <v>112</v>
       </c>
-      <c r="R18" s="69" t="s">
+      <c r="R18" s="79" t="s">
         <v>21</v>
       </c>
       <c r="S18" s="46" t="s">
@@ -6623,7 +6637,7 @@
       <c r="V18" s="39">
         <v>144</v>
       </c>
-      <c r="W18" s="66" t="s">
+      <c r="W18" s="72" t="s">
         <v>23</v>
       </c>
       <c r="X18" s="38" t="s">
@@ -6637,7 +6651,7 @@
       <c r="B19" s="33">
         <v>18</v>
       </c>
-      <c r="C19" s="60"/>
+      <c r="C19" s="85"/>
       <c r="D19" s="54"/>
       <c r="F19" s="40" t="s">
         <v>38</v>
@@ -6645,7 +6659,7 @@
       <c r="G19" s="40">
         <v>49</v>
       </c>
-      <c r="H19" s="61"/>
+      <c r="H19" s="82"/>
       <c r="I19" s="44"/>
       <c r="K19" s="41" t="s">
         <v>38</v>
@@ -6653,7 +6667,7 @@
       <c r="L19" s="41">
         <v>81</v>
       </c>
-      <c r="M19" s="65"/>
+      <c r="M19" s="81"/>
       <c r="N19" s="45"/>
       <c r="P19" s="42" t="s">
         <v>38</v>
@@ -6661,7 +6675,7 @@
       <c r="Q19" s="42">
         <v>113</v>
       </c>
-      <c r="R19" s="69"/>
+      <c r="R19" s="79"/>
       <c r="S19" s="46"/>
       <c r="U19" s="39" t="s">
         <v>38</v>
@@ -6669,7 +6683,7 @@
       <c r="V19" s="39">
         <v>145</v>
       </c>
-      <c r="W19" s="67"/>
+      <c r="W19" s="73"/>
       <c r="X19" s="38"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
@@ -6679,7 +6693,7 @@
       <c r="B20" s="33">
         <v>19</v>
       </c>
-      <c r="C20" s="60"/>
+      <c r="C20" s="85"/>
       <c r="D20" s="43"/>
       <c r="F20" s="40" t="s">
         <v>38</v>
@@ -6687,7 +6701,7 @@
       <c r="G20" s="40">
         <v>50</v>
       </c>
-      <c r="H20" s="61"/>
+      <c r="H20" s="82"/>
       <c r="I20" s="44"/>
       <c r="K20" s="41" t="s">
         <v>38</v>
@@ -6695,7 +6709,7 @@
       <c r="L20" s="41">
         <v>82</v>
       </c>
-      <c r="M20" s="65"/>
+      <c r="M20" s="81"/>
       <c r="N20" s="45"/>
       <c r="P20" s="42" t="s">
         <v>38</v>
@@ -6703,7 +6717,7 @@
       <c r="Q20" s="42">
         <v>114</v>
       </c>
-      <c r="R20" s="69"/>
+      <c r="R20" s="79"/>
       <c r="S20" s="46"/>
       <c r="U20" s="39" t="s">
         <v>38</v>
@@ -6711,7 +6725,7 @@
       <c r="V20" s="39">
         <v>146</v>
       </c>
-      <c r="W20" s="67"/>
+      <c r="W20" s="73"/>
       <c r="X20" s="38"/>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
@@ -6721,7 +6735,7 @@
       <c r="B21" s="33">
         <v>20</v>
       </c>
-      <c r="C21" s="60"/>
+      <c r="C21" s="85"/>
       <c r="D21" s="43"/>
       <c r="F21" s="40" t="s">
         <v>38</v>
@@ -6729,7 +6743,7 @@
       <c r="G21" s="40">
         <v>51</v>
       </c>
-      <c r="H21" s="61"/>
+      <c r="H21" s="82"/>
       <c r="I21" s="44"/>
       <c r="K21" s="41" t="s">
         <v>38</v>
@@ -6737,7 +6751,7 @@
       <c r="L21" s="41">
         <v>83</v>
       </c>
-      <c r="M21" s="65"/>
+      <c r="M21" s="81"/>
       <c r="N21" s="45"/>
       <c r="P21" s="42" t="s">
         <v>38</v>
@@ -6745,7 +6759,7 @@
       <c r="Q21" s="42">
         <v>115</v>
       </c>
-      <c r="R21" s="69"/>
+      <c r="R21" s="79"/>
       <c r="S21" s="46"/>
       <c r="U21" s="39" t="s">
         <v>38</v>
@@ -6753,7 +6767,7 @@
       <c r="V21" s="39">
         <v>147</v>
       </c>
-      <c r="W21" s="67"/>
+      <c r="W21" s="73"/>
       <c r="X21" s="38"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
@@ -6763,7 +6777,7 @@
       <c r="B22" s="33">
         <v>21</v>
       </c>
-      <c r="C22" s="60"/>
+      <c r="C22" s="85"/>
       <c r="D22" s="43"/>
       <c r="F22" s="40" t="s">
         <v>38</v>
@@ -6771,7 +6785,7 @@
       <c r="G22" s="40">
         <v>52</v>
       </c>
-      <c r="H22" s="61"/>
+      <c r="H22" s="82"/>
       <c r="I22" s="44"/>
       <c r="K22" s="41" t="s">
         <v>38</v>
@@ -6779,7 +6793,7 @@
       <c r="L22" s="41">
         <v>84</v>
       </c>
-      <c r="M22" s="65"/>
+      <c r="M22" s="81"/>
       <c r="N22" s="45"/>
       <c r="P22" s="42" t="s">
         <v>38</v>
@@ -6787,7 +6801,7 @@
       <c r="Q22" s="42">
         <v>116</v>
       </c>
-      <c r="R22" s="69"/>
+      <c r="R22" s="79"/>
       <c r="S22" s="46"/>
       <c r="U22" s="39" t="s">
         <v>38</v>
@@ -6795,7 +6809,7 @@
       <c r="V22" s="39">
         <v>148</v>
       </c>
-      <c r="W22" s="67"/>
+      <c r="W22" s="73"/>
       <c r="X22" s="38"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
@@ -6805,7 +6819,7 @@
       <c r="B23" s="33">
         <v>22</v>
       </c>
-      <c r="C23" s="60"/>
+      <c r="C23" s="85"/>
       <c r="D23" s="43"/>
       <c r="F23" s="40" t="s">
         <v>38</v>
@@ -6813,7 +6827,7 @@
       <c r="G23" s="40">
         <v>53</v>
       </c>
-      <c r="H23" s="61"/>
+      <c r="H23" s="82"/>
       <c r="I23" s="44"/>
       <c r="K23" s="41" t="s">
         <v>38</v>
@@ -6821,7 +6835,7 @@
       <c r="L23" s="41">
         <v>85</v>
       </c>
-      <c r="M23" s="65"/>
+      <c r="M23" s="81"/>
       <c r="N23" s="45"/>
       <c r="P23" s="42" t="s">
         <v>38</v>
@@ -6829,7 +6843,7 @@
       <c r="Q23" s="42">
         <v>117</v>
       </c>
-      <c r="R23" s="69"/>
+      <c r="R23" s="79"/>
       <c r="S23" s="46"/>
       <c r="U23" s="39" t="s">
         <v>38</v>
@@ -6837,7 +6851,7 @@
       <c r="V23" s="39">
         <v>149</v>
       </c>
-      <c r="W23" s="67"/>
+      <c r="W23" s="73"/>
       <c r="X23" s="38"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
@@ -6847,7 +6861,7 @@
       <c r="B24" s="33">
         <v>23</v>
       </c>
-      <c r="C24" s="60"/>
+      <c r="C24" s="85"/>
       <c r="D24" s="43"/>
       <c r="F24" s="40" t="s">
         <v>38</v>
@@ -6855,7 +6869,7 @@
       <c r="G24" s="40">
         <v>54</v>
       </c>
-      <c r="H24" s="61"/>
+      <c r="H24" s="82"/>
       <c r="I24" s="44"/>
       <c r="K24" s="41" t="s">
         <v>38</v>
@@ -6863,7 +6877,7 @@
       <c r="L24" s="41">
         <v>86</v>
       </c>
-      <c r="M24" s="65"/>
+      <c r="M24" s="81"/>
       <c r="N24" s="45"/>
       <c r="P24" s="42" t="s">
         <v>38</v>
@@ -6871,7 +6885,7 @@
       <c r="Q24" s="42">
         <v>118</v>
       </c>
-      <c r="R24" s="69"/>
+      <c r="R24" s="79"/>
       <c r="S24" s="46"/>
       <c r="U24" s="39" t="s">
         <v>38</v>
@@ -6879,7 +6893,7 @@
       <c r="V24" s="39">
         <v>150</v>
       </c>
-      <c r="W24" s="67"/>
+      <c r="W24" s="73"/>
       <c r="X24" s="38"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
@@ -6889,7 +6903,7 @@
       <c r="B25" s="33">
         <v>24</v>
       </c>
-      <c r="C25" s="60"/>
+      <c r="C25" s="85"/>
       <c r="D25" s="43"/>
       <c r="F25" s="40" t="s">
         <v>38</v>
@@ -6897,7 +6911,7 @@
       <c r="G25" s="40">
         <v>55</v>
       </c>
-      <c r="H25" s="61"/>
+      <c r="H25" s="82"/>
       <c r="I25" s="44"/>
       <c r="K25" s="41" t="s">
         <v>38</v>
@@ -6905,7 +6919,7 @@
       <c r="L25" s="41">
         <v>87</v>
       </c>
-      <c r="M25" s="65"/>
+      <c r="M25" s="81"/>
       <c r="N25" s="45"/>
       <c r="P25" s="42" t="s">
         <v>38</v>
@@ -6913,7 +6927,7 @@
       <c r="Q25" s="42">
         <v>119</v>
       </c>
-      <c r="R25" s="69"/>
+      <c r="R25" s="79"/>
       <c r="S25" s="46"/>
       <c r="U25" s="39" t="s">
         <v>38</v>
@@ -6921,7 +6935,7 @@
       <c r="V25" s="39">
         <v>151</v>
       </c>
-      <c r="W25" s="67"/>
+      <c r="W25" s="73"/>
       <c r="X25" s="38"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
@@ -6931,7 +6945,7 @@
       <c r="B26" s="33">
         <v>25</v>
       </c>
-      <c r="C26" s="60"/>
+      <c r="C26" s="85"/>
       <c r="D26" s="43"/>
       <c r="F26" s="40" t="s">
         <v>38</v>
@@ -6939,7 +6953,7 @@
       <c r="G26" s="40">
         <v>56</v>
       </c>
-      <c r="H26" s="61"/>
+      <c r="H26" s="82"/>
       <c r="I26" s="44"/>
       <c r="K26" s="41" t="s">
         <v>38</v>
@@ -6947,7 +6961,7 @@
       <c r="L26" s="41">
         <v>88</v>
       </c>
-      <c r="M26" s="65"/>
+      <c r="M26" s="81"/>
       <c r="N26" s="45"/>
       <c r="P26" s="42" t="s">
         <v>38</v>
@@ -6955,7 +6969,7 @@
       <c r="Q26" s="42">
         <v>120</v>
       </c>
-      <c r="R26" s="69"/>
+      <c r="R26" s="79"/>
       <c r="S26" s="46"/>
       <c r="U26" s="39" t="s">
         <v>38</v>
@@ -6963,7 +6977,7 @@
       <c r="V26" s="39">
         <v>152</v>
       </c>
-      <c r="W26" s="67"/>
+      <c r="W26" s="73"/>
       <c r="X26" s="38"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
@@ -6973,7 +6987,7 @@
       <c r="B27" s="33">
         <v>26</v>
       </c>
-      <c r="C27" s="60"/>
+      <c r="C27" s="85"/>
       <c r="D27" s="43"/>
       <c r="F27" s="40" t="s">
         <v>38</v>
@@ -6981,7 +6995,7 @@
       <c r="G27" s="40">
         <v>57</v>
       </c>
-      <c r="H27" s="61"/>
+      <c r="H27" s="82"/>
       <c r="I27" s="44"/>
       <c r="K27" s="41" t="s">
         <v>38</v>
@@ -6989,7 +7003,7 @@
       <c r="L27" s="41">
         <v>89</v>
       </c>
-      <c r="M27" s="65"/>
+      <c r="M27" s="81"/>
       <c r="N27" s="45"/>
       <c r="P27" s="42" t="s">
         <v>38</v>
@@ -6997,7 +7011,7 @@
       <c r="Q27" s="42">
         <v>121</v>
       </c>
-      <c r="R27" s="69"/>
+      <c r="R27" s="79"/>
       <c r="S27" s="46"/>
       <c r="U27" s="39" t="s">
         <v>38</v>
@@ -7005,7 +7019,7 @@
       <c r="V27" s="39">
         <v>153</v>
       </c>
-      <c r="W27" s="67"/>
+      <c r="W27" s="73"/>
       <c r="X27" s="38"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
@@ -7015,7 +7029,7 @@
       <c r="B28" s="33">
         <v>27</v>
       </c>
-      <c r="C28" s="60"/>
+      <c r="C28" s="85"/>
       <c r="D28" s="54" t="s">
         <v>35</v>
       </c>
@@ -7025,7 +7039,7 @@
       <c r="G28" s="40">
         <v>58</v>
       </c>
-      <c r="H28" s="61"/>
+      <c r="H28" s="82"/>
       <c r="I28" s="44"/>
       <c r="K28" s="41" t="s">
         <v>38</v>
@@ -7033,7 +7047,7 @@
       <c r="L28" s="41">
         <v>90</v>
       </c>
-      <c r="M28" s="65"/>
+      <c r="M28" s="81"/>
       <c r="N28" s="45"/>
       <c r="P28" s="42" t="s">
         <v>38</v>
@@ -7041,7 +7055,7 @@
       <c r="Q28" s="42">
         <v>122</v>
       </c>
-      <c r="R28" s="69"/>
+      <c r="R28" s="79"/>
       <c r="S28" s="46"/>
       <c r="U28" s="39" t="s">
         <v>38</v>
@@ -7049,7 +7063,7 @@
       <c r="V28" s="39">
         <v>154</v>
       </c>
-      <c r="W28" s="67"/>
+      <c r="W28" s="73"/>
       <c r="X28" s="38"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
@@ -7059,7 +7073,7 @@
       <c r="B29" s="33">
         <v>28</v>
       </c>
-      <c r="C29" s="60"/>
+      <c r="C29" s="85"/>
       <c r="D29" s="43" t="s">
         <v>36</v>
       </c>
@@ -7069,7 +7083,7 @@
       <c r="G29" s="40">
         <v>59</v>
       </c>
-      <c r="H29" s="61"/>
+      <c r="H29" s="82"/>
       <c r="I29" s="44"/>
       <c r="K29" s="41" t="s">
         <v>38</v>
@@ -7077,7 +7091,7 @@
       <c r="L29" s="41">
         <v>91</v>
       </c>
-      <c r="M29" s="65"/>
+      <c r="M29" s="81"/>
       <c r="N29" s="45"/>
       <c r="P29" s="42" t="s">
         <v>38</v>
@@ -7085,7 +7099,7 @@
       <c r="Q29" s="42">
         <v>123</v>
       </c>
-      <c r="R29" s="69"/>
+      <c r="R29" s="79"/>
       <c r="S29" s="46"/>
       <c r="U29" s="39" t="s">
         <v>38</v>
@@ -7093,7 +7107,7 @@
       <c r="V29" s="39">
         <v>155</v>
       </c>
-      <c r="W29" s="67"/>
+      <c r="W29" s="73"/>
       <c r="X29" s="38"/>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
@@ -7103,7 +7117,7 @@
       <c r="B30" s="33">
         <v>29</v>
       </c>
-      <c r="C30" s="60"/>
+      <c r="C30" s="85"/>
       <c r="D30" s="43" t="s">
         <v>37</v>
       </c>
@@ -7113,7 +7127,7 @@
       <c r="G30" s="40">
         <v>60</v>
       </c>
-      <c r="H30" s="61"/>
+      <c r="H30" s="82"/>
       <c r="I30" s="44"/>
       <c r="K30" s="41" t="s">
         <v>38</v>
@@ -7121,7 +7135,7 @@
       <c r="L30" s="41">
         <v>92</v>
       </c>
-      <c r="M30" s="65"/>
+      <c r="M30" s="81"/>
       <c r="N30" s="45"/>
       <c r="P30" s="42" t="s">
         <v>38</v>
@@ -7129,7 +7143,7 @@
       <c r="Q30" s="42">
         <v>124</v>
       </c>
-      <c r="R30" s="69"/>
+      <c r="R30" s="79"/>
       <c r="S30" s="46"/>
       <c r="U30" s="39" t="s">
         <v>38</v>
@@ -7137,7 +7151,7 @@
       <c r="V30" s="39">
         <v>156</v>
       </c>
-      <c r="W30" s="67"/>
+      <c r="W30" s="73"/>
       <c r="X30" s="38"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
@@ -7147,7 +7161,7 @@
       <c r="B31" s="33">
         <v>30</v>
       </c>
-      <c r="C31" s="60"/>
+      <c r="C31" s="85"/>
       <c r="D31" s="43" t="s">
         <v>33</v>
       </c>
@@ -7157,7 +7171,7 @@
       <c r="G31" s="40">
         <v>61</v>
       </c>
-      <c r="H31" s="61"/>
+      <c r="H31" s="82"/>
       <c r="I31" s="44"/>
       <c r="K31" s="41" t="s">
         <v>38</v>
@@ -7165,7 +7179,7 @@
       <c r="L31" s="41">
         <v>93</v>
       </c>
-      <c r="M31" s="65"/>
+      <c r="M31" s="81"/>
       <c r="N31" s="45"/>
       <c r="P31" s="42" t="s">
         <v>38</v>
@@ -7173,7 +7187,7 @@
       <c r="Q31" s="42">
         <v>125</v>
       </c>
-      <c r="R31" s="69"/>
+      <c r="R31" s="79"/>
       <c r="S31" s="46"/>
       <c r="U31" s="39" t="s">
         <v>38</v>
@@ -7181,7 +7195,7 @@
       <c r="V31" s="39">
         <v>157</v>
       </c>
-      <c r="W31" s="67"/>
+      <c r="W31" s="73"/>
       <c r="X31" s="38"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
@@ -7191,7 +7205,7 @@
       <c r="B32" s="33">
         <v>31</v>
       </c>
-      <c r="C32" s="60"/>
+      <c r="C32" s="85"/>
       <c r="D32" s="43" t="s">
         <v>32</v>
       </c>
@@ -7201,7 +7215,7 @@
       <c r="G32" s="40">
         <v>62</v>
       </c>
-      <c r="H32" s="61"/>
+      <c r="H32" s="82"/>
       <c r="I32" s="44" t="s">
         <v>33</v>
       </c>
@@ -7211,7 +7225,7 @@
       <c r="L32" s="41">
         <v>94</v>
       </c>
-      <c r="M32" s="65"/>
+      <c r="M32" s="81"/>
       <c r="N32" s="45" t="s">
         <v>33</v>
       </c>
@@ -7221,7 +7235,7 @@
       <c r="Q32" s="42">
         <v>126</v>
       </c>
-      <c r="R32" s="69"/>
+      <c r="R32" s="79"/>
       <c r="S32" s="46" t="s">
         <v>33</v>
       </c>
@@ -7231,7 +7245,7 @@
       <c r="V32" s="39">
         <v>158</v>
       </c>
-      <c r="W32" s="67"/>
+      <c r="W32" s="73"/>
       <c r="X32" s="38" t="s">
         <v>33</v>
       </c>
@@ -7243,7 +7257,7 @@
       <c r="G33" s="40">
         <v>63</v>
       </c>
-      <c r="H33" s="61"/>
+      <c r="H33" s="82"/>
       <c r="I33" s="44" t="s">
         <v>32</v>
       </c>
@@ -7253,7 +7267,7 @@
       <c r="L33" s="41">
         <v>95</v>
       </c>
-      <c r="M33" s="65"/>
+      <c r="M33" s="81"/>
       <c r="N33" s="45" t="s">
         <v>32</v>
       </c>
@@ -7263,7 +7277,7 @@
       <c r="Q33" s="42">
         <v>127</v>
       </c>
-      <c r="R33" s="69"/>
+      <c r="R33" s="79"/>
       <c r="S33" s="46" t="s">
         <v>32</v>
       </c>
@@ -7273,7 +7287,7 @@
       <c r="V33" s="39">
         <v>159</v>
       </c>
-      <c r="W33" s="68"/>
+      <c r="W33" s="74"/>
       <c r="X33" s="38" t="s">
         <v>32</v>
       </c>
@@ -7285,7 +7299,7 @@
       <c r="B35" s="37">
         <v>160</v>
       </c>
-      <c r="C35" s="74" t="s">
+      <c r="C35" s="66" t="s">
         <v>26</v>
       </c>
       <c r="D35" s="34" t="s">
@@ -7297,7 +7311,7 @@
       <c r="G35" s="37">
         <v>176</v>
       </c>
-      <c r="H35" s="70" t="s">
+      <c r="H35" s="75" t="s">
         <v>27</v>
       </c>
       <c r="I35" s="34" t="s">
@@ -7309,7 +7323,7 @@
       <c r="L35" s="35">
         <v>192</v>
       </c>
-      <c r="M35" s="71" t="s">
+      <c r="M35" s="76" t="s">
         <v>25</v>
       </c>
       <c r="N35" s="36" t="s">
@@ -7321,7 +7335,7 @@
       <c r="Q35" s="32">
         <v>208</v>
       </c>
-      <c r="R35" s="83" t="s">
+      <c r="R35" s="63" t="s">
         <v>34</v>
       </c>
       <c r="S35" s="31" t="s">
@@ -7333,7 +7347,7 @@
       <c r="V35" s="51">
         <v>224</v>
       </c>
-      <c r="W35" s="79" t="s">
+      <c r="W35" s="71" t="s">
         <v>29</v>
       </c>
       <c r="X35" s="48" t="s">
@@ -7347,7 +7361,7 @@
       <c r="B36" s="37">
         <v>161</v>
       </c>
-      <c r="C36" s="75"/>
+      <c r="C36" s="67"/>
       <c r="D36" s="34"/>
       <c r="F36" s="37" t="s">
         <v>38</v>
@@ -7355,7 +7369,7 @@
       <c r="G36" s="37">
         <v>177</v>
       </c>
-      <c r="H36" s="70"/>
+      <c r="H36" s="75"/>
       <c r="I36" s="34"/>
       <c r="K36" s="35" t="s">
         <v>38</v>
@@ -7363,7 +7377,7 @@
       <c r="L36" s="35">
         <v>193</v>
       </c>
-      <c r="M36" s="72"/>
+      <c r="M36" s="77"/>
       <c r="N36" s="36"/>
       <c r="P36" s="32" t="s">
         <v>38</v>
@@ -7371,7 +7385,7 @@
       <c r="Q36" s="32">
         <v>209</v>
       </c>
-      <c r="R36" s="83"/>
+      <c r="R36" s="63"/>
       <c r="S36" s="31" t="s">
         <v>58</v>
       </c>
@@ -7381,7 +7395,7 @@
       <c r="V36" s="51">
         <v>225</v>
       </c>
-      <c r="W36" s="79"/>
+      <c r="W36" s="71"/>
       <c r="X36" s="48"/>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
@@ -7391,7 +7405,7 @@
       <c r="B37" s="37">
         <v>162</v>
       </c>
-      <c r="C37" s="75"/>
+      <c r="C37" s="67"/>
       <c r="D37" s="34"/>
       <c r="F37" s="37" t="s">
         <v>38</v>
@@ -7399,7 +7413,7 @@
       <c r="G37" s="37">
         <v>178</v>
       </c>
-      <c r="H37" s="70"/>
+      <c r="H37" s="75"/>
       <c r="I37" s="34"/>
       <c r="K37" s="35" t="s">
         <v>38</v>
@@ -7407,7 +7421,7 @@
       <c r="L37" s="35">
         <v>194</v>
       </c>
-      <c r="M37" s="72"/>
+      <c r="M37" s="77"/>
       <c r="N37" s="36"/>
       <c r="P37" s="32" t="s">
         <v>38</v>
@@ -7415,7 +7429,7 @@
       <c r="Q37" s="32">
         <v>210</v>
       </c>
-      <c r="R37" s="83"/>
+      <c r="R37" s="63"/>
       <c r="S37" s="31" t="s">
         <v>59</v>
       </c>
@@ -7425,7 +7439,7 @@
       <c r="V37" s="51">
         <v>226</v>
       </c>
-      <c r="W37" s="79"/>
+      <c r="W37" s="71"/>
       <c r="X37" s="48"/>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
@@ -7435,7 +7449,7 @@
       <c r="B38" s="37">
         <v>163</v>
       </c>
-      <c r="C38" s="75"/>
+      <c r="C38" s="67"/>
       <c r="D38" s="34"/>
       <c r="F38" s="37" t="s">
         <v>38</v>
@@ -7443,7 +7457,7 @@
       <c r="G38" s="37">
         <v>179</v>
       </c>
-      <c r="H38" s="70"/>
+      <c r="H38" s="75"/>
       <c r="I38" s="34"/>
       <c r="K38" s="35" t="s">
         <v>38</v>
@@ -7451,7 +7465,7 @@
       <c r="L38" s="35">
         <v>195</v>
       </c>
-      <c r="M38" s="72"/>
+      <c r="M38" s="77"/>
       <c r="N38" s="36"/>
       <c r="P38" s="32" t="s">
         <v>38</v>
@@ -7459,7 +7473,7 @@
       <c r="Q38" s="32">
         <v>211</v>
       </c>
-      <c r="R38" s="83"/>
+      <c r="R38" s="63"/>
       <c r="S38" s="31" t="s">
         <v>60</v>
       </c>
@@ -7469,7 +7483,7 @@
       <c r="V38" s="51">
         <v>227</v>
       </c>
-      <c r="W38" s="79"/>
+      <c r="W38" s="71"/>
       <c r="X38" s="48"/>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
@@ -7479,7 +7493,7 @@
       <c r="B39" s="37">
         <v>164</v>
       </c>
-      <c r="C39" s="75"/>
+      <c r="C39" s="67"/>
       <c r="D39" s="34"/>
       <c r="F39" s="37" t="s">
         <v>38</v>
@@ -7487,7 +7501,7 @@
       <c r="G39" s="37">
         <v>180</v>
       </c>
-      <c r="H39" s="70"/>
+      <c r="H39" s="75"/>
       <c r="I39" s="34"/>
       <c r="K39" s="35" t="s">
         <v>38</v>
@@ -7495,7 +7509,7 @@
       <c r="L39" s="35">
         <v>196</v>
       </c>
-      <c r="M39" s="72"/>
+      <c r="M39" s="77"/>
       <c r="N39" s="36"/>
       <c r="P39" s="32" t="s">
         <v>38</v>
@@ -7503,7 +7517,7 @@
       <c r="Q39" s="32">
         <v>212</v>
       </c>
-      <c r="R39" s="83"/>
+      <c r="R39" s="63"/>
       <c r="S39" s="31"/>
       <c r="U39" s="50" t="s">
         <v>38</v>
@@ -7511,7 +7525,7 @@
       <c r="V39" s="51">
         <v>228</v>
       </c>
-      <c r="W39" s="79"/>
+      <c r="W39" s="71"/>
       <c r="X39" s="48"/>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
@@ -7521,7 +7535,7 @@
       <c r="B40" s="37">
         <v>165</v>
       </c>
-      <c r="C40" s="75"/>
+      <c r="C40" s="67"/>
       <c r="D40" s="34"/>
       <c r="F40" s="37" t="s">
         <v>38</v>
@@ -7529,7 +7543,7 @@
       <c r="G40" s="37">
         <v>181</v>
       </c>
-      <c r="H40" s="70"/>
+      <c r="H40" s="75"/>
       <c r="I40" s="34"/>
       <c r="K40" s="35" t="s">
         <v>38</v>
@@ -7537,7 +7551,7 @@
       <c r="L40" s="35">
         <v>197</v>
       </c>
-      <c r="M40" s="72"/>
+      <c r="M40" s="77"/>
       <c r="N40" s="36"/>
       <c r="P40" s="32" t="s">
         <v>38</v>
@@ -7545,7 +7559,7 @@
       <c r="Q40" s="32">
         <v>213</v>
       </c>
-      <c r="R40" s="83"/>
+      <c r="R40" s="63"/>
       <c r="S40" s="31"/>
       <c r="U40" s="50" t="s">
         <v>38</v>
@@ -7553,7 +7567,7 @@
       <c r="V40" s="51">
         <v>229</v>
       </c>
-      <c r="W40" s="79"/>
+      <c r="W40" s="71"/>
       <c r="X40" s="48"/>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
@@ -7563,7 +7577,7 @@
       <c r="B41" s="37">
         <v>166</v>
       </c>
-      <c r="C41" s="75"/>
+      <c r="C41" s="67"/>
       <c r="D41" s="34"/>
       <c r="F41" s="37" t="s">
         <v>38</v>
@@ -7571,7 +7585,7 @@
       <c r="G41" s="37">
         <v>182</v>
       </c>
-      <c r="H41" s="70"/>
+      <c r="H41" s="75"/>
       <c r="I41" s="34"/>
       <c r="K41" s="35" t="s">
         <v>38</v>
@@ -7579,7 +7593,7 @@
       <c r="L41" s="35">
         <v>198</v>
       </c>
-      <c r="M41" s="72"/>
+      <c r="M41" s="77"/>
       <c r="N41" s="36" t="s">
         <v>33</v>
       </c>
@@ -7589,7 +7603,7 @@
       <c r="Q41" s="32">
         <v>214</v>
       </c>
-      <c r="R41" s="83"/>
+      <c r="R41" s="63"/>
       <c r="S41" s="31"/>
       <c r="U41" s="50" t="s">
         <v>38</v>
@@ -7597,7 +7611,7 @@
       <c r="V41" s="51">
         <v>230</v>
       </c>
-      <c r="W41" s="79"/>
+      <c r="W41" s="71"/>
       <c r="X41" s="48"/>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
@@ -7607,7 +7621,7 @@
       <c r="B42" s="37">
         <v>167</v>
       </c>
-      <c r="C42" s="75"/>
+      <c r="C42" s="67"/>
       <c r="D42" s="34"/>
       <c r="F42" s="37" t="s">
         <v>38</v>
@@ -7615,7 +7629,7 @@
       <c r="G42" s="37">
         <v>183</v>
       </c>
-      <c r="H42" s="70"/>
+      <c r="H42" s="75"/>
       <c r="I42" s="34"/>
       <c r="K42" s="35" t="s">
         <v>38</v>
@@ -7623,7 +7637,7 @@
       <c r="L42" s="35">
         <v>199</v>
       </c>
-      <c r="M42" s="73"/>
+      <c r="M42" s="78"/>
       <c r="N42" s="36" t="s">
         <v>32</v>
       </c>
@@ -7633,7 +7647,7 @@
       <c r="Q42" s="32">
         <v>215</v>
       </c>
-      <c r="R42" s="83"/>
+      <c r="R42" s="63"/>
       <c r="S42" s="31"/>
       <c r="U42" s="50" t="s">
         <v>38</v>
@@ -7641,7 +7655,7 @@
       <c r="V42" s="51">
         <v>231</v>
       </c>
-      <c r="W42" s="79"/>
+      <c r="W42" s="71"/>
       <c r="X42" s="48" t="s">
         <v>32</v>
       </c>
@@ -7653,7 +7667,7 @@
       <c r="B43" s="37">
         <v>168</v>
       </c>
-      <c r="C43" s="75"/>
+      <c r="C43" s="67"/>
       <c r="D43" s="34"/>
       <c r="F43" s="37" t="s">
         <v>38</v>
@@ -7661,7 +7675,7 @@
       <c r="G43" s="37">
         <v>184</v>
       </c>
-      <c r="H43" s="70"/>
+      <c r="H43" s="75"/>
       <c r="I43" s="34"/>
       <c r="P43" s="32" t="s">
         <v>38</v>
@@ -7669,7 +7683,7 @@
       <c r="Q43" s="32">
         <v>216</v>
       </c>
-      <c r="R43" s="83"/>
+      <c r="R43" s="63"/>
       <c r="S43" s="31"/>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
@@ -7679,7 +7693,7 @@
       <c r="B44" s="37">
         <v>169</v>
       </c>
-      <c r="C44" s="75"/>
+      <c r="C44" s="67"/>
       <c r="D44" s="34"/>
       <c r="F44" s="37" t="s">
         <v>38</v>
@@ -7687,7 +7701,7 @@
       <c r="G44" s="37">
         <v>185</v>
       </c>
-      <c r="H44" s="70"/>
+      <c r="H44" s="75"/>
       <c r="I44" s="34"/>
       <c r="K44" s="35" t="s">
         <v>38</v>
@@ -7695,7 +7709,7 @@
       <c r="L44" s="35">
         <v>200</v>
       </c>
-      <c r="M44" s="80" t="s">
+      <c r="M44" s="60" t="s">
         <v>24</v>
       </c>
       <c r="N44" s="36" t="s">
@@ -7707,7 +7721,7 @@
       <c r="Q44" s="32">
         <v>217</v>
       </c>
-      <c r="R44" s="83"/>
+      <c r="R44" s="63"/>
       <c r="S44" s="31"/>
       <c r="U44" s="47" t="s">
         <v>38</v>
@@ -7715,7 +7729,7 @@
       <c r="V44" s="47">
         <v>232</v>
       </c>
-      <c r="W44" s="85" t="s">
+      <c r="W44" s="65" t="s">
         <v>30</v>
       </c>
       <c r="X44" s="49" t="s">
@@ -7729,7 +7743,7 @@
       <c r="B45" s="37">
         <v>170</v>
       </c>
-      <c r="C45" s="75"/>
+      <c r="C45" s="67"/>
       <c r="D45" s="34"/>
       <c r="F45" s="37" t="s">
         <v>38</v>
@@ -7737,7 +7751,7 @@
       <c r="G45" s="37">
         <v>186</v>
       </c>
-      <c r="H45" s="70"/>
+      <c r="H45" s="75"/>
       <c r="I45" s="34"/>
       <c r="K45" s="35" t="s">
         <v>38</v>
@@ -7745,7 +7759,7 @@
       <c r="L45" s="35">
         <v>201</v>
       </c>
-      <c r="M45" s="80"/>
+      <c r="M45" s="60"/>
       <c r="N45" s="36"/>
       <c r="P45" s="32" t="s">
         <v>38</v>
@@ -7753,7 +7767,7 @@
       <c r="Q45" s="32">
         <v>218</v>
       </c>
-      <c r="R45" s="83"/>
+      <c r="R45" s="63"/>
       <c r="S45" s="31"/>
       <c r="U45" s="47" t="s">
         <v>38</v>
@@ -7761,7 +7775,7 @@
       <c r="V45" s="47">
         <v>233</v>
       </c>
-      <c r="W45" s="85"/>
+      <c r="W45" s="65"/>
       <c r="X45" s="49" t="s">
         <v>57</v>
       </c>
@@ -7773,7 +7787,7 @@
       <c r="B46" s="37">
         <v>171</v>
       </c>
-      <c r="C46" s="75"/>
+      <c r="C46" s="67"/>
       <c r="D46" s="34"/>
       <c r="F46" s="37" t="s">
         <v>38</v>
@@ -7781,7 +7795,7 @@
       <c r="G46" s="37">
         <v>187</v>
       </c>
-      <c r="H46" s="70"/>
+      <c r="H46" s="75"/>
       <c r="I46" s="34"/>
       <c r="K46" s="35" t="s">
         <v>38</v>
@@ -7789,7 +7803,7 @@
       <c r="L46" s="35">
         <v>202</v>
       </c>
-      <c r="M46" s="80"/>
+      <c r="M46" s="60"/>
       <c r="N46" s="36"/>
       <c r="P46" s="32" t="s">
         <v>38</v>
@@ -7797,7 +7811,7 @@
       <c r="Q46" s="32">
         <v>219</v>
       </c>
-      <c r="R46" s="83"/>
+      <c r="R46" s="63"/>
       <c r="S46" s="31"/>
       <c r="U46" s="47" t="s">
         <v>38</v>
@@ -7805,7 +7819,7 @@
       <c r="V46" s="47">
         <v>234</v>
       </c>
-      <c r="W46" s="85"/>
+      <c r="W46" s="65"/>
       <c r="X46" s="49" t="s">
         <v>33</v>
       </c>
@@ -7817,7 +7831,7 @@
       <c r="B47" s="37">
         <v>172</v>
       </c>
-      <c r="C47" s="75"/>
+      <c r="C47" s="67"/>
       <c r="D47" s="34"/>
       <c r="F47" s="37" t="s">
         <v>38</v>
@@ -7825,7 +7839,7 @@
       <c r="G47" s="37">
         <v>188</v>
       </c>
-      <c r="H47" s="70"/>
+      <c r="H47" s="75"/>
       <c r="I47" s="34"/>
       <c r="K47" s="35" t="s">
         <v>38</v>
@@ -7833,7 +7847,7 @@
       <c r="L47" s="35">
         <v>203</v>
       </c>
-      <c r="M47" s="80"/>
+      <c r="M47" s="60"/>
       <c r="N47" s="36"/>
       <c r="P47" s="32" t="s">
         <v>38</v>
@@ -7841,7 +7855,7 @@
       <c r="Q47" s="32">
         <v>220</v>
       </c>
-      <c r="R47" s="83"/>
+      <c r="R47" s="63"/>
       <c r="S47" s="31"/>
       <c r="U47" s="47" t="s">
         <v>38</v>
@@ -7849,7 +7863,7 @@
       <c r="V47" s="47">
         <v>235</v>
       </c>
-      <c r="W47" s="85"/>
+      <c r="W47" s="65"/>
       <c r="X47" s="49" t="s">
         <v>32</v>
       </c>
@@ -7861,7 +7875,7 @@
       <c r="B48" s="37">
         <v>173</v>
       </c>
-      <c r="C48" s="75"/>
+      <c r="C48" s="67"/>
       <c r="D48" s="34"/>
       <c r="F48" s="37" t="s">
         <v>38</v>
@@ -7869,7 +7883,7 @@
       <c r="G48" s="37">
         <v>189</v>
       </c>
-      <c r="H48" s="70"/>
+      <c r="H48" s="75"/>
       <c r="I48" s="34"/>
       <c r="K48" s="35" t="s">
         <v>38</v>
@@ -7877,7 +7891,7 @@
       <c r="L48" s="35">
         <v>204</v>
       </c>
-      <c r="M48" s="80"/>
+      <c r="M48" s="60"/>
       <c r="N48" s="36"/>
       <c r="P48" s="32" t="s">
         <v>38</v>
@@ -7885,7 +7899,7 @@
       <c r="Q48" s="32">
         <v>221</v>
       </c>
-      <c r="R48" s="83"/>
+      <c r="R48" s="63"/>
       <c r="S48" s="31"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
@@ -7895,7 +7909,7 @@
       <c r="B49" s="37">
         <v>174</v>
       </c>
-      <c r="C49" s="75"/>
+      <c r="C49" s="67"/>
       <c r="D49" s="34" t="s">
         <v>33</v>
       </c>
@@ -7905,7 +7919,7 @@
       <c r="G49" s="37">
         <v>190</v>
       </c>
-      <c r="H49" s="70"/>
+      <c r="H49" s="75"/>
       <c r="I49" s="34" t="s">
         <v>33</v>
       </c>
@@ -7915,7 +7929,7 @@
       <c r="L49" s="35">
         <v>205</v>
       </c>
-      <c r="M49" s="80"/>
+      <c r="M49" s="60"/>
       <c r="N49" s="36"/>
       <c r="P49" s="32" t="s">
         <v>38</v>
@@ -7923,7 +7937,7 @@
       <c r="Q49" s="32">
         <v>222</v>
       </c>
-      <c r="R49" s="83"/>
+      <c r="R49" s="63"/>
       <c r="S49" s="31"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
@@ -7933,7 +7947,7 @@
       <c r="B50" s="37">
         <v>175</v>
       </c>
-      <c r="C50" s="76"/>
+      <c r="C50" s="68"/>
       <c r="D50" s="34" t="s">
         <v>32</v>
       </c>
@@ -7943,7 +7957,7 @@
       <c r="G50" s="37">
         <v>191</v>
       </c>
-      <c r="H50" s="70"/>
+      <c r="H50" s="75"/>
       <c r="I50" s="34" t="s">
         <v>32</v>
       </c>
@@ -7953,7 +7967,7 @@
       <c r="L50" s="35">
         <v>206</v>
       </c>
-      <c r="M50" s="80"/>
+      <c r="M50" s="60"/>
       <c r="N50" s="36" t="s">
         <v>33</v>
       </c>
@@ -7963,7 +7977,7 @@
       <c r="Q50" s="32">
         <v>223</v>
       </c>
-      <c r="R50" s="83"/>
+      <c r="R50" s="63"/>
       <c r="S50" s="31" t="s">
         <v>32</v>
       </c>
@@ -7975,7 +7989,7 @@
       <c r="L51" s="35">
         <v>207</v>
       </c>
-      <c r="M51" s="80"/>
+      <c r="M51" s="60"/>
       <c r="N51" s="36" t="s">
         <v>32</v>
       </c>
@@ -8259,7 +8273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{094E0344-2B81-4E6D-AD84-5D175246353F}">
   <dimension ref="B2:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>

</xml_diff>